<commit_message>
- tiny fix for one number missing
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D14649-96D5-0B49-A85C-7D220283D9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C9C346-BF4C-134F-95D4-73C2798E2825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -768,7 +768,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
-    <numFmt numFmtId="169" formatCode="0.000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1371,7 +1371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1524,56 +1524,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1641,11 +1593,56 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1954,8 +1951,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="99" workbookViewId="0">
-      <selection activeCell="N116" sqref="N116"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="99" workbookViewId="0">
+      <selection activeCell="J117" sqref="J117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2004,19 +2001,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="70"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="77"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="61"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2027,17 +2024,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="81"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="65"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2066,43 +2063,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="84" t="s">
+      <c r="E5" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="84" t="s">
+      <c r="F5" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="84" t="s">
+      <c r="G5" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="85" t="s">
+      <c r="H5" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="87" t="s">
+      <c r="I5" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="89" t="s">
+      <c r="J5" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="89" t="s">
+      <c r="K5" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="84" t="s">
+      <c r="L5" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="84" t="s">
+      <c r="M5" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="84" t="s">
+      <c r="N5" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="52" t="s">
+      <c r="O5" s="75" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2113,19 +2110,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="53"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="76"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
@@ -2170,7 +2167,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="54"/>
+      <c r="O7" s="77"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2183,35 +2180,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="58" t="s">
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="63" t="s">
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="85"/>
+      <c r="M8" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="64"/>
+      <c r="N8" s="87"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="65" t="s">
+      <c r="P8" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="66"/>
-      <c r="R8" s="67"/>
-      <c r="S8" s="67"/>
-      <c r="T8" s="68"/>
+      <c r="Q8" s="89"/>
+      <c r="R8" s="90"/>
+      <c r="S8" s="90"/>
+      <c r="T8" s="91"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
@@ -2295,7 +2292,7 @@
       <c r="I10" s="43">
         <v>298</v>
       </c>
-      <c r="J10" s="91">
+      <c r="J10" s="52">
         <v>9.5999999999999991E-7</v>
       </c>
       <c r="K10" s="4"/>
@@ -2332,7 +2329,7 @@
       <c r="I11" s="43">
         <v>298</v>
       </c>
-      <c r="J11" s="91">
+      <c r="J11" s="52">
         <v>1.33E-6</v>
       </c>
       <c r="K11" s="4"/>
@@ -2371,7 +2368,7 @@
       <c r="I12" s="43">
         <v>298</v>
       </c>
-      <c r="J12" s="91">
+      <c r="J12" s="52">
         <v>8.8000000000000004E-7</v>
       </c>
       <c r="K12" s="4"/>
@@ -2410,7 +2407,7 @@
       <c r="I13" s="43">
         <v>298</v>
       </c>
-      <c r="J13" s="91">
+      <c r="J13" s="52">
         <v>1.2300000000000001E-6</v>
       </c>
       <c r="K13" s="4"/>
@@ -2447,7 +2444,7 @@
       <c r="I14" s="43">
         <v>298</v>
       </c>
-      <c r="J14" s="91">
+      <c r="J14" s="52">
         <f>P14*9807000</f>
         <v>2069277000</v>
       </c>
@@ -2488,7 +2485,7 @@
       <c r="I15" s="43">
         <v>298</v>
       </c>
-      <c r="J15" s="91">
+      <c r="J15" s="52">
         <f t="shared" ref="J15:J17" si="0">P15*9807000</f>
         <v>2285031000</v>
       </c>
@@ -2531,7 +2528,7 @@
       <c r="I16" s="43">
         <v>298</v>
       </c>
-      <c r="J16" s="91">
+      <c r="J16" s="52">
         <f t="shared" si="0"/>
         <v>2363487000</v>
       </c>
@@ -2574,7 +2571,7 @@
       <c r="I17" s="43">
         <v>298</v>
       </c>
-      <c r="J17" s="91">
+      <c r="J17" s="52">
         <f t="shared" si="0"/>
         <v>2510592000</v>
       </c>
@@ -2615,7 +2612,7 @@
       <c r="I18" s="43">
         <v>298</v>
       </c>
-      <c r="J18" s="91">
+      <c r="J18" s="52">
         <v>773000000</v>
       </c>
       <c r="K18" s="4"/>
@@ -2651,7 +2648,7 @@
       <c r="I19" s="43">
         <v>298</v>
       </c>
-      <c r="J19" s="91">
+      <c r="J19" s="52">
         <v>1001000000</v>
       </c>
       <c r="K19" s="4"/>
@@ -2689,7 +2686,7 @@
       <c r="I20" s="43">
         <v>298</v>
       </c>
-      <c r="J20" s="91">
+      <c r="J20" s="52">
         <v>241000000</v>
       </c>
       <c r="K20" s="4"/>
@@ -2727,7 +2724,7 @@
       <c r="I21" s="43">
         <v>298</v>
       </c>
-      <c r="J21" s="91">
+      <c r="J21" s="52">
         <v>256000000</v>
       </c>
       <c r="K21" s="4"/>
@@ -2763,7 +2760,7 @@
       <c r="I22" s="43">
         <v>298</v>
       </c>
-      <c r="J22" s="91">
+      <c r="J22" s="52">
         <v>1184000000</v>
       </c>
       <c r="K22" s="4"/>
@@ -2799,7 +2796,7 @@
       <c r="I23" s="43">
         <v>298</v>
       </c>
-      <c r="J23" s="91">
+      <c r="J23" s="52">
         <v>1800000000</v>
       </c>
       <c r="K23" s="4"/>
@@ -2837,7 +2834,7 @@
       <c r="I24" s="43">
         <v>298</v>
       </c>
-      <c r="J24" s="91">
+      <c r="J24" s="52">
         <v>1071000000</v>
       </c>
       <c r="K24" s="4"/>
@@ -2875,7 +2872,7 @@
       <c r="I25" s="43">
         <v>298</v>
       </c>
-      <c r="J25" s="91">
+      <c r="J25" s="52">
         <v>1365000000</v>
       </c>
       <c r="K25" s="4"/>
@@ -2911,7 +2908,7 @@
       <c r="I26" s="43">
         <v>298</v>
       </c>
-      <c r="J26" s="91">
+      <c r="J26" s="52">
         <v>17</v>
       </c>
       <c r="K26" s="4"/>
@@ -2947,7 +2944,7 @@
       <c r="I27" s="43">
         <v>298</v>
       </c>
-      <c r="J27" s="91">
+      <c r="J27" s="52">
         <v>21.9</v>
       </c>
       <c r="K27" s="4"/>
@@ -2985,7 +2982,7 @@
       <c r="I28" s="43">
         <v>298</v>
       </c>
-      <c r="J28" s="91">
+      <c r="J28" s="52">
         <v>17.7</v>
       </c>
       <c r="K28" s="4"/>
@@ -3023,7 +3020,7 @@
       <c r="I29" s="43">
         <v>298</v>
       </c>
-      <c r="J29" s="91">
+      <c r="J29" s="52">
         <v>15.7</v>
       </c>
       <c r="K29" s="4"/>
@@ -3063,7 +3060,7 @@
       <c r="I30" s="43">
         <v>298</v>
       </c>
-      <c r="J30" s="91">
+      <c r="J30" s="52">
         <v>1293000000</v>
       </c>
       <c r="K30" s="4"/>
@@ -3103,7 +3100,7 @@
       <c r="I31" s="43">
         <v>298</v>
       </c>
-      <c r="J31" s="91">
+      <c r="J31" s="52">
         <v>1349000000</v>
       </c>
       <c r="K31" s="4"/>
@@ -3143,7 +3140,7 @@
       <c r="I32" s="43">
         <v>298</v>
       </c>
-      <c r="J32" s="91">
+      <c r="J32" s="52">
         <v>1402000000</v>
       </c>
       <c r="K32" s="4"/>
@@ -3183,7 +3180,7 @@
       <c r="I33" s="43">
         <v>298</v>
       </c>
-      <c r="J33" s="91">
+      <c r="J33" s="52">
         <v>1441000000</v>
       </c>
       <c r="K33" s="4"/>
@@ -3223,7 +3220,7 @@
       <c r="I34" s="43">
         <v>298</v>
       </c>
-      <c r="J34" s="91">
+      <c r="J34" s="52">
         <v>32.5</v>
       </c>
       <c r="K34" s="4"/>
@@ -3263,7 +3260,7 @@
       <c r="I35" s="43">
         <v>298</v>
       </c>
-      <c r="J35" s="91">
+      <c r="J35" s="52">
         <v>26.6</v>
       </c>
       <c r="K35" s="4"/>
@@ -3303,7 +3300,7 @@
       <c r="I36" s="43">
         <v>298</v>
       </c>
-      <c r="J36" s="91">
+      <c r="J36" s="52">
         <v>25</v>
       </c>
       <c r="K36" s="4"/>
@@ -3343,7 +3340,7 @@
       <c r="I37" s="43">
         <v>298</v>
       </c>
-      <c r="J37" s="91">
+      <c r="J37" s="52">
         <v>23.6</v>
       </c>
       <c r="K37" s="4"/>
@@ -3383,7 +3380,7 @@
       <c r="I38" s="43">
         <v>298</v>
       </c>
-      <c r="J38" s="91">
+      <c r="J38" s="52">
         <v>2352000000</v>
       </c>
       <c r="K38" s="4"/>
@@ -3423,7 +3420,7 @@
       <c r="I39" s="43">
         <v>298</v>
       </c>
-      <c r="J39" s="91">
+      <c r="J39" s="52">
         <v>2104000000</v>
       </c>
       <c r="K39" s="4"/>
@@ -3463,7 +3460,7 @@
       <c r="I40" s="43">
         <v>298</v>
       </c>
-      <c r="J40" s="91">
+      <c r="J40" s="52">
         <v>2050000000</v>
       </c>
       <c r="K40" s="4"/>
@@ -3503,7 +3500,7 @@
       <c r="I41" s="43">
         <v>298</v>
       </c>
-      <c r="J41" s="91">
+      <c r="J41" s="52">
         <v>2018000000</v>
       </c>
       <c r="K41" s="4"/>
@@ -3543,7 +3540,7 @@
       <c r="I42" s="3">
         <v>100</v>
       </c>
-      <c r="J42" s="91">
+      <c r="J42" s="52">
         <v>8.1000000000000004E-6</v>
       </c>
       <c r="K42" s="4"/>
@@ -3553,7 +3550,7 @@
       <c r="M42" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="N42" s="92" t="s">
+      <c r="N42" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3583,7 +3580,7 @@
       <c r="I43" s="3">
         <v>360</v>
       </c>
-      <c r="J43" s="91">
+      <c r="J43" s="52">
         <v>1.5800000000000001E-5</v>
       </c>
       <c r="K43" s="4"/>
@@ -3593,7 +3590,7 @@
       <c r="M43" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="N43" s="92" t="s">
+      <c r="N43" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3623,7 +3620,7 @@
       <c r="I44" s="3">
         <v>10</v>
       </c>
-      <c r="J44" s="91">
+      <c r="J44" s="52">
         <v>54</v>
       </c>
       <c r="K44" s="4"/>
@@ -3633,7 +3630,7 @@
       <c r="M44" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="N44" s="92" t="s">
+      <c r="N44" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3663,7 +3660,7 @@
       <c r="I45" s="3">
         <v>10</v>
       </c>
-      <c r="J45" s="91">
+      <c r="J45" s="52">
         <v>43</v>
       </c>
       <c r="K45" s="4"/>
@@ -3673,7 +3670,7 @@
       <c r="M45" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="N45" s="92" t="s">
+      <c r="N45" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3703,7 +3700,7 @@
       <c r="I46" s="3">
         <v>10</v>
       </c>
-      <c r="J46" s="91">
+      <c r="J46" s="52">
         <v>45</v>
       </c>
       <c r="K46" s="4"/>
@@ -3713,7 +3710,7 @@
       <c r="M46" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="N46" s="92" t="s">
+      <c r="N46" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3743,7 +3740,7 @@
       <c r="I47" s="3">
         <v>10</v>
       </c>
-      <c r="J47" s="91">
+      <c r="J47" s="52">
         <v>82</v>
       </c>
       <c r="K47" s="4"/>
@@ -3753,7 +3750,7 @@
       <c r="M47" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="N47" s="92" t="s">
+      <c r="N47" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3783,7 +3780,7 @@
       <c r="I48" s="3">
         <v>10</v>
       </c>
-      <c r="J48" s="91">
+      <c r="J48" s="52">
         <v>102</v>
       </c>
       <c r="K48" s="4"/>
@@ -3793,7 +3790,7 @@
       <c r="M48" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="N48" s="92" t="s">
+      <c r="N48" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3823,7 +3820,7 @@
       <c r="I49" s="3">
         <v>298</v>
       </c>
-      <c r="J49" s="91">
+      <c r="J49" s="52">
         <v>1977000000</v>
       </c>
       <c r="K49" s="4"/>
@@ -3833,7 +3830,7 @@
       <c r="M49" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="N49" s="92" t="s">
+      <c r="N49" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3863,7 +3860,7 @@
       <c r="I50" s="3">
         <v>298</v>
       </c>
-      <c r="J50" s="91">
+      <c r="J50" s="52">
         <v>2045000000</v>
       </c>
       <c r="K50" s="4"/>
@@ -3873,7 +3870,7 @@
       <c r="M50" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="N50" s="92" t="s">
+      <c r="N50" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3903,7 +3900,7 @@
       <c r="I51" s="3">
         <v>298</v>
       </c>
-      <c r="J51" s="91">
+      <c r="J51" s="52">
         <v>2057000000</v>
       </c>
       <c r="K51" s="4"/>
@@ -3913,7 +3910,7 @@
       <c r="M51" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="N51" s="92" t="s">
+      <c r="N51" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3943,7 +3940,7 @@
       <c r="I52" s="3">
         <v>298</v>
       </c>
-      <c r="J52" s="91">
+      <c r="J52" s="52">
         <v>4284000000</v>
       </c>
       <c r="K52" s="4"/>
@@ -3953,7 +3950,7 @@
       <c r="M52" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="N52" s="92" t="s">
+      <c r="N52" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3983,7 +3980,7 @@
       <c r="I53" s="3">
         <v>298</v>
       </c>
-      <c r="J53" s="91">
+      <c r="J53" s="52">
         <v>5045000000</v>
       </c>
       <c r="K53" s="4"/>
@@ -3993,7 +3990,7 @@
       <c r="M53" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="N53" s="92" t="s">
+      <c r="N53" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -4023,7 +4020,7 @@
       <c r="I54" s="3">
         <v>10</v>
       </c>
-      <c r="J54" s="91">
+      <c r="J54" s="52">
         <v>46</v>
       </c>
       <c r="K54" s="4"/>
@@ -4033,7 +4030,7 @@
       <c r="M54" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="N54" s="92" t="s">
+      <c r="N54" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -4063,7 +4060,7 @@
       <c r="I55" s="3">
         <v>10</v>
       </c>
-      <c r="J55" s="91">
+      <c r="J55" s="52">
         <v>21</v>
       </c>
       <c r="K55" s="4"/>
@@ -4073,7 +4070,7 @@
       <c r="M55" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="N55" s="92" t="s">
+      <c r="N55" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -4103,7 +4100,7 @@
       <c r="I56" s="3">
         <v>10</v>
       </c>
-      <c r="J56" s="91">
+      <c r="J56" s="52">
         <v>51</v>
       </c>
       <c r="K56" s="4"/>
@@ -4113,7 +4110,7 @@
       <c r="M56" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="N56" s="92" t="s">
+      <c r="N56" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -4143,7 +4140,7 @@
       <c r="I57" s="3">
         <v>10</v>
       </c>
-      <c r="J57" s="91">
+      <c r="J57" s="52">
         <v>98</v>
       </c>
       <c r="K57" s="4"/>
@@ -4153,7 +4150,7 @@
       <c r="M57" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="N57" s="92" t="s">
+      <c r="N57" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -4183,7 +4180,7 @@
       <c r="I58" s="3">
         <v>298</v>
       </c>
-      <c r="J58" s="91">
+      <c r="J58" s="52">
         <v>2084000000</v>
       </c>
       <c r="K58" s="4"/>
@@ -4193,7 +4190,7 @@
       <c r="M58" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="N58" s="92" t="s">
+      <c r="N58" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -4223,7 +4220,7 @@
       <c r="I59" s="3">
         <v>298</v>
       </c>
-      <c r="J59" s="91">
+      <c r="J59" s="52">
         <v>2199000000</v>
       </c>
       <c r="K59" s="4"/>
@@ -4233,7 +4230,7 @@
       <c r="M59" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="N59" s="92" t="s">
+      <c r="N59" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -4263,7 +4260,7 @@
       <c r="I60" s="3">
         <v>298</v>
       </c>
-      <c r="J60" s="91">
+      <c r="J60" s="52">
         <v>2810000000</v>
       </c>
       <c r="K60" s="4"/>
@@ -4273,7 +4270,7 @@
       <c r="M60" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="N60" s="92" t="s">
+      <c r="N60" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -4303,7 +4300,7 @@
       <c r="I61" s="3">
         <v>298</v>
       </c>
-      <c r="J61" s="91">
+      <c r="J61" s="52">
         <v>5288000000</v>
       </c>
       <c r="K61" s="4"/>
@@ -4313,7 +4310,7 @@
       <c r="M61" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="N61" s="92" t="s">
+      <c r="N61" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -4341,7 +4338,7 @@
       <c r="I62" s="3">
         <v>298</v>
       </c>
-      <c r="J62" s="91">
+      <c r="J62" s="52">
         <v>18.14</v>
       </c>
       <c r="K62" s="4"/>
@@ -4379,7 +4376,7 @@
       <c r="I63" s="3">
         <v>298</v>
       </c>
-      <c r="J63" s="91">
+      <c r="J63" s="52">
         <v>147.86000000000001</v>
       </c>
       <c r="K63" s="4"/>
@@ -4417,7 +4414,7 @@
       <c r="I64" s="3">
         <v>298</v>
       </c>
-      <c r="J64" s="91">
+      <c r="J64" s="52">
         <v>1.39</v>
       </c>
       <c r="K64" s="4"/>
@@ -4455,7 +4452,7 @@
       <c r="I65" s="3">
         <v>298</v>
       </c>
-      <c r="J65" s="91">
+      <c r="J65" s="52">
         <v>80.430000000000007</v>
       </c>
       <c r="K65" s="4"/>
@@ -4495,7 +4492,7 @@
       <c r="I66" s="3">
         <v>298</v>
       </c>
-      <c r="J66" s="91">
+      <c r="J66" s="52">
         <v>80.290000000000006</v>
       </c>
       <c r="K66" s="4"/>
@@ -4533,7 +4530,7 @@
       <c r="I67" s="3">
         <v>298</v>
       </c>
-      <c r="J67" s="91">
+      <c r="J67" s="52">
         <v>119</v>
       </c>
       <c r="K67" s="4"/>
@@ -4571,7 +4568,7 @@
       <c r="I68" s="3">
         <v>298</v>
       </c>
-      <c r="J68" s="91">
+      <c r="J68" s="52">
         <v>629</v>
       </c>
       <c r="K68" s="4"/>
@@ -4609,7 +4606,7 @@
       <c r="I69" s="3">
         <v>298</v>
       </c>
-      <c r="J69" s="91">
+      <c r="J69" s="52">
         <v>10804</v>
       </c>
       <c r="K69" s="4"/>
@@ -4647,7 +4644,7 @@
       <c r="I70" s="3">
         <v>298</v>
       </c>
-      <c r="J70" s="91">
+      <c r="J70" s="52">
         <v>915</v>
       </c>
       <c r="K70" s="4"/>
@@ -4687,7 +4684,7 @@
       <c r="I71" s="3">
         <v>298</v>
       </c>
-      <c r="J71" s="91">
+      <c r="J71" s="52">
         <v>3431</v>
       </c>
       <c r="K71" s="4"/>
@@ -4721,7 +4718,7 @@
       <c r="I72" s="3">
         <v>298</v>
       </c>
-      <c r="J72" s="91"/>
+      <c r="J72" s="52"/>
       <c r="K72" s="4"/>
       <c r="L72" s="44"/>
       <c r="M72" s="44" t="s">
@@ -4751,7 +4748,7 @@
       <c r="I73" s="3">
         <v>298</v>
       </c>
-      <c r="J73" s="91"/>
+      <c r="J73" s="52"/>
       <c r="K73" s="4"/>
       <c r="L73" s="44"/>
       <c r="M73" s="44" t="s">
@@ -4779,7 +4776,7 @@
       <c r="I74" s="3">
         <v>298</v>
       </c>
-      <c r="J74" s="91"/>
+      <c r="J74" s="52"/>
       <c r="K74" s="4"/>
       <c r="L74" s="44"/>
       <c r="M74" s="44" t="s">
@@ -4807,7 +4804,7 @@
       <c r="I75" s="3">
         <v>298</v>
       </c>
-      <c r="J75" s="91"/>
+      <c r="J75" s="52"/>
       <c r="K75" s="4"/>
       <c r="L75" s="44"/>
       <c r="M75" s="44" t="s">
@@ -4841,7 +4838,7 @@
       <c r="I76" s="3">
         <v>300</v>
       </c>
-      <c r="J76" s="91">
+      <c r="J76" s="52">
         <v>2.0699999999999998E-5</v>
       </c>
       <c r="K76" s="4"/>
@@ -4873,7 +4870,7 @@
       <c r="G77" s="42"/>
       <c r="H77" s="42"/>
       <c r="I77" s="3"/>
-      <c r="J77" s="91"/>
+      <c r="J77" s="52"/>
       <c r="K77" s="4"/>
       <c r="L77" s="44"/>
       <c r="M77" s="44" t="s">
@@ -4901,7 +4898,7 @@
       <c r="G78" s="42"/>
       <c r="H78" s="42"/>
       <c r="I78" s="3"/>
-      <c r="J78" s="91"/>
+      <c r="J78" s="52"/>
       <c r="K78" s="4"/>
       <c r="L78" s="44"/>
       <c r="M78" s="44" t="s">
@@ -4929,7 +4926,7 @@
       <c r="G79" s="42"/>
       <c r="H79" s="42"/>
       <c r="I79" s="3"/>
-      <c r="J79" s="91"/>
+      <c r="J79" s="52"/>
       <c r="K79" s="4"/>
       <c r="L79" s="44"/>
       <c r="M79" s="44" t="s">
@@ -4957,7 +4954,7 @@
       <c r="G80" s="42"/>
       <c r="H80" s="42"/>
       <c r="I80" s="3"/>
-      <c r="J80" s="91"/>
+      <c r="J80" s="52"/>
       <c r="K80" s="4"/>
       <c r="L80" s="44"/>
       <c r="M80" s="44" t="s">
@@ -4985,7 +4982,7 @@
       <c r="G81" s="42"/>
       <c r="H81" s="42"/>
       <c r="I81" s="3"/>
-      <c r="J81" s="91"/>
+      <c r="J81" s="52"/>
       <c r="K81" s="4"/>
       <c r="L81" s="44"/>
       <c r="M81" s="44" t="s">
@@ -5047,11 +5044,11 @@
       <c r="I83" s="3">
         <v>298</v>
       </c>
-      <c r="J83" s="91">
+      <c r="J83" s="52">
         <f>P83*9807000</f>
         <v>4981956000</v>
       </c>
-      <c r="K83" s="91">
+      <c r="K83" s="52">
         <f>Q83*9807000</f>
         <v>196140000</v>
       </c>
@@ -5093,11 +5090,11 @@
       <c r="I84" s="3">
         <v>298</v>
       </c>
-      <c r="J84" s="91">
+      <c r="J84" s="52">
         <f t="shared" ref="J84:J86" si="1">P84*9807000</f>
         <v>5344815000</v>
       </c>
-      <c r="K84" s="91">
+      <c r="K84" s="52">
         <f t="shared" ref="K84:K86" si="2">Q84*9807000</f>
         <v>98070000</v>
       </c>
@@ -5139,11 +5136,11 @@
       <c r="I85" s="3">
         <v>298</v>
       </c>
-      <c r="J85" s="91">
+      <c r="J85" s="52">
         <f t="shared" si="1"/>
         <v>5629218000</v>
       </c>
-      <c r="K85" s="91">
+      <c r="K85" s="52">
         <f t="shared" si="2"/>
         <v>147105000</v>
       </c>
@@ -5185,11 +5182,11 @@
       <c r="I86" s="3">
         <v>298</v>
       </c>
-      <c r="J86" s="91">
+      <c r="J86" s="52">
         <f t="shared" si="1"/>
         <v>6198024000</v>
       </c>
-      <c r="K86" s="91">
+      <c r="K86" s="52">
         <f t="shared" si="2"/>
         <v>245175000</v>
       </c>
@@ -5383,7 +5380,7 @@
       <c r="I91" s="3">
         <v>298</v>
       </c>
-      <c r="J91" s="91">
+      <c r="J91" s="52">
         <f>P91*9807000</f>
         <v>8934177000</v>
       </c>
@@ -5535,7 +5532,9 @@
       <c r="I95" s="3">
         <v>298</v>
       </c>
-      <c r="J95" s="4"/>
+      <c r="J95" s="4">
+        <v>2.67</v>
+      </c>
       <c r="K95" s="4"/>
       <c r="L95" s="44" t="s">
         <v>66</v>
@@ -10995,6 +10994,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -11009,11 +11013,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted `10.1016/j.mtadv.2020.100101` and updated some data for the previous one
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B625BE0C-5B20-3B4E-8606-E25CD4C32AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94032314-6BE4-6E4A-ADBA-456D9AFCE709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="227">
   <si>
     <t>Metadata</t>
   </si>
@@ -771,13 +771,40 @@
     <t>Bi3In5+In0.2Sn0.8+Ag5Zn8</t>
   </si>
   <si>
-    <t>AC+PM</t>
-  </si>
-  <si>
     <t>micrometer particles with ultrasonic dispersion; example of bad a composition notation</t>
   </si>
   <si>
     <t>remelting of micrometer particles with ultrasonic dispersion; example of bad a composition notation</t>
+  </si>
+  <si>
+    <t>10.1016/j.mtadv.2020.100101</t>
+  </si>
+  <si>
+    <t>solidus temperature</t>
+  </si>
+  <si>
+    <t>liquidus temperature</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>P5624</t>
+  </si>
+  <si>
+    <t>SnBiInZn</t>
+  </si>
+  <si>
+    <t>VIM+PM</t>
+  </si>
+  <si>
+    <t>VIM</t>
+  </si>
+  <si>
+    <t>BCT+InBi+Bi</t>
+  </si>
+  <si>
+    <t>F2</t>
   </si>
 </sst>
 </file>
@@ -1969,8 +1996,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="99" workbookViewId="0">
-      <selection activeCell="N118" sqref="N118"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6307,20 +6334,28 @@
         <v>214</v>
       </c>
       <c r="D115" s="42" t="s">
+        <v>223</v>
+      </c>
+      <c r="E115" s="44" t="s">
         <v>215</v>
       </c>
-      <c r="E115" s="44" t="s">
-        <v>216</v>
-      </c>
-      <c r="F115" s="42"/>
-      <c r="G115" s="42"/>
+      <c r="F115" s="42" t="s">
+        <v>218</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H115" s="42"/>
       <c r="I115" s="3"/>
-      <c r="J115" s="4"/>
+      <c r="J115" s="4">
+        <v>335.95</v>
+      </c>
       <c r="K115" s="4"/>
-      <c r="L115" s="44"/>
+      <c r="L115" s="44" t="s">
+        <v>220</v>
+      </c>
       <c r="M115" s="44" t="s">
-        <v>125</v>
+        <v>221</v>
       </c>
       <c r="N115" s="44" t="s">
         <v>212</v>
@@ -6335,20 +6370,28 @@
         <v>214</v>
       </c>
       <c r="D116" s="42" t="s">
-        <v>64</v>
+        <v>223</v>
       </c>
       <c r="E116" s="44" t="s">
-        <v>217</v>
-      </c>
-      <c r="F116" s="42"/>
-      <c r="G116" s="42"/>
+        <v>215</v>
+      </c>
+      <c r="F116" s="42" t="s">
+        <v>219</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H116" s="42"/>
       <c r="I116" s="3"/>
-      <c r="J116" s="4"/>
+      <c r="J116" s="4">
+        <v>341.74</v>
+      </c>
       <c r="K116" s="4"/>
-      <c r="L116" s="44"/>
+      <c r="L116" s="44" t="s">
+        <v>220</v>
+      </c>
       <c r="M116" s="44" t="s">
-        <v>128</v>
+        <v>221</v>
       </c>
       <c r="N116" s="44" t="s">
         <v>212</v>
@@ -6356,10 +6399,18 @@
     </row>
     <row r="117" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="24"/>
-      <c r="B117" s="44"/>
-      <c r="C117" s="42"/>
-      <c r="D117" s="42"/>
-      <c r="E117" s="44"/>
+      <c r="B117" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="C117" s="42" t="s">
+        <v>214</v>
+      </c>
+      <c r="D117" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="E117" s="44" t="s">
+        <v>216</v>
+      </c>
       <c r="F117" s="42"/>
       <c r="G117" s="42"/>
       <c r="H117" s="42"/>
@@ -6367,24 +6418,46 @@
       <c r="J117" s="4"/>
       <c r="K117" s="4"/>
       <c r="L117" s="44"/>
-      <c r="M117" s="44"/>
-      <c r="N117" s="44"/>
+      <c r="M117" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="N117" s="44" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="118" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="24"/>
-      <c r="B118" s="44"/>
-      <c r="C118" s="42"/>
-      <c r="D118" s="42"/>
+      <c r="B118" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="C118" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="D118" s="42" t="s">
+        <v>224</v>
+      </c>
       <c r="E118" s="44"/>
-      <c r="F118" s="42"/>
-      <c r="G118" s="42"/>
+      <c r="F118" s="42" t="s">
+        <v>218</v>
+      </c>
+      <c r="G118" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H118" s="42"/>
       <c r="I118" s="3"/>
-      <c r="J118" s="4"/>
+      <c r="J118" s="4">
+        <v>351.25</v>
+      </c>
       <c r="K118" s="4"/>
-      <c r="L118" s="44"/>
-      <c r="M118" s="44"/>
-      <c r="N118" s="44"/>
+      <c r="L118" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="M118" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="N118" s="44" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="119" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="24"/>

</xml_diff>

<commit_message>
- typo fix in `10.1007/s11431-017-9073-0`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240B4C86-24E6-4540-BCB1-351191367449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D77A794-CE01-2247-85C6-5D23E6AF93C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2065,8 +2065,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B101" zoomScale="99" workbookViewId="0">
-      <selection activeCell="F136" sqref="F136"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="99" workbookViewId="0">
+      <selection activeCell="G135" sqref="G135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5527,7 +5527,7 @@
         <v>183</v>
       </c>
       <c r="F92" s="42" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
- extracted data from  `10.1016/j.intermet.2022.107495`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D77A794-CE01-2247-85C6-5D23E6AF93C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DD5E47-2B73-4B4C-A298-107CF90E6BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="272">
   <si>
     <t>Metadata</t>
   </si>
@@ -874,6 +874,72 @@
   </si>
   <si>
     <t>10.1016/j.jallcom.2021.160640</t>
+  </si>
+  <si>
+    <t>VEC-18</t>
+  </si>
+  <si>
+    <t>VEC-18.72</t>
+  </si>
+  <si>
+    <t>VEC-17</t>
+  </si>
+  <si>
+    <t>Zn16.67 Fe9.17 Co7.50 Ni16.67 Mn16.67 Sb33.33</t>
+  </si>
+  <si>
+    <t>Zn20.30 Fe11.20 Co9.15 Ni13.00 Mn13.00 Sb33.33</t>
+  </si>
+  <si>
+    <t>Zn25.40 Fe14.00 Co11.50 Ni7.90 Mn7.90 Sb33.33</t>
+  </si>
+  <si>
+    <t>AC+HIP</t>
+  </si>
+  <si>
+    <t>Zn10 Fe10 Co10 Ni10 Mn10 Sb50</t>
+  </si>
+  <si>
+    <t>AC+A</t>
+  </si>
+  <si>
+    <t>annealed at 550*C for 20h</t>
+  </si>
+  <si>
+    <t>Zn16 Fe10 Co8 Ni13 Mn15 Sb39</t>
+  </si>
+  <si>
+    <t>?+?+?</t>
+  </si>
+  <si>
+    <t>HH</t>
+  </si>
+  <si>
+    <t>HH+?+?</t>
+  </si>
+  <si>
+    <t>HH is half-heusler (C1b) phase majority with 2 minor phases; heusler composition refined in another datapoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HH is half-heusler  is C1b; Authors consider the phase to have an XYZ half-Heusler type composition, where Sb occupies the Z site in a NaCl sublattice, which is reasonable since Sb is the most electronegative element in the phase and occupies 1/3 of the sites. The other five elements would then substitute for X and Y in the Heusler composition. </t>
+  </si>
+  <si>
+    <t>seebeck coefficient</t>
+  </si>
+  <si>
+    <t>V/K</t>
+  </si>
+  <si>
+    <t>thermal conductivity</t>
+  </si>
+  <si>
+    <t>W/(Km)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ground into powder; HIP at 973K for 30min; HH is half-heusler  is C1b; Authors consider the phase to have an XYZ half-Heusler type composition, where Sb occupies the Z site in a NaCl sublattice, which is reasonable since Sb is the most electronegative element in the phase and occupies 1/3 of the sites. The other five elements would then substitute for X and Y in the Heusler composition. </t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2022.107495</t>
   </si>
 </sst>
 </file>
@@ -1641,6 +1707,57 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1706,57 +1823,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2065,14 +2131,14 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G135" sqref="G135"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="99" workbookViewId="0">
+      <selection activeCell="H166" sqref="H166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" customWidth="1"/>
     <col min="3" max="4" width="16.33203125" style="48" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.83203125" style="48" bestFit="1" customWidth="1"/>
@@ -2115,19 +2181,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="61"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="78"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2138,17 +2204,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="65"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="82"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2177,43 +2243,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="68" t="s">
+      <c r="F5" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="71" t="s">
+      <c r="I5" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="73" t="s">
+      <c r="J5" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="73" t="s">
+      <c r="K5" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="68" t="s">
+      <c r="L5" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="68" t="s">
+      <c r="M5" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="68" t="s">
+      <c r="N5" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="75" t="s">
+      <c r="O5" s="53" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2224,19 +2290,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="76"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="84"/>
+      <c r="O6" s="54"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
@@ -2281,7 +2347,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="77"/>
+      <c r="O7" s="55"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2294,35 +2360,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="81" t="s">
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="86" t="s">
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="87"/>
+      <c r="N8" s="65"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="88" t="s">
+      <c r="P8" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="89"/>
-      <c r="R8" s="90"/>
-      <c r="S8" s="90"/>
-      <c r="T8" s="91"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="68"/>
+      <c r="T8" s="69"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
@@ -6898,7 +6964,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="24"/>
       <c r="B129" s="44" t="s">
         <v>240</v>
@@ -6936,7 +7002,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="24"/>
       <c r="B130" s="44" t="s">
         <v>241</v>
@@ -6972,12 +7038,22 @@
         <v>249</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="24"/>
-      <c r="B131" s="44"/>
-      <c r="C131" s="42"/>
-      <c r="D131" s="42"/>
-      <c r="E131" s="44"/>
+    <row r="131" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="B131" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="C131" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D131" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E131" s="44" t="s">
+        <v>265</v>
+      </c>
       <c r="F131" s="42"/>
       <c r="G131" s="42"/>
       <c r="H131" s="42"/>
@@ -6985,15 +7061,29 @@
       <c r="J131" s="4"/>
       <c r="K131" s="4"/>
       <c r="L131" s="44"/>
-      <c r="M131" s="44"/>
-      <c r="N131" s="44"/>
-    </row>
-    <row r="132" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="24"/>
-      <c r="B132" s="44"/>
-      <c r="C132" s="42"/>
-      <c r="D132" s="42"/>
-      <c r="E132" s="44"/>
+      <c r="M131" s="44" t="s">
+        <v>152</v>
+      </c>
+      <c r="N131" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="B132" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="C132" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D132" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E132" s="44" t="s">
+        <v>265</v>
+      </c>
       <c r="F132" s="42"/>
       <c r="G132" s="42"/>
       <c r="H132" s="42"/>
@@ -7001,15 +7091,29 @@
       <c r="J132" s="4"/>
       <c r="K132" s="4"/>
       <c r="L132" s="44"/>
-      <c r="M132" s="44"/>
-      <c r="N132" s="44"/>
-    </row>
-    <row r="133" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="24"/>
-      <c r="B133" s="44"/>
-      <c r="C133" s="42"/>
-      <c r="D133" s="42"/>
-      <c r="E133" s="44"/>
+      <c r="M132" s="44" t="s">
+        <v>152</v>
+      </c>
+      <c r="N132" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B133" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="C133" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D133" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E133" s="44" t="s">
+        <v>265</v>
+      </c>
       <c r="F133" s="42"/>
       <c r="G133" s="42"/>
       <c r="H133" s="42"/>
@@ -7017,14 +7121,24 @@
       <c r="J133" s="4"/>
       <c r="K133" s="4"/>
       <c r="L133" s="44"/>
-      <c r="M133" s="44"/>
-      <c r="N133" s="44"/>
-    </row>
-    <row r="134" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M133" s="44" t="s">
+        <v>152</v>
+      </c>
+      <c r="N133" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="24"/>
-      <c r="B134" s="44"/>
-      <c r="C134" s="42"/>
-      <c r="D134" s="42"/>
+      <c r="B134" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="C134" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="D134" s="42" t="s">
+        <v>64</v>
+      </c>
       <c r="E134" s="44"/>
       <c r="F134" s="42"/>
       <c r="G134" s="42"/>
@@ -7033,15 +7147,27 @@
       <c r="J134" s="4"/>
       <c r="K134" s="4"/>
       <c r="L134" s="44"/>
-      <c r="M134" s="44"/>
-      <c r="N134" s="44"/>
-    </row>
-    <row r="135" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M134" s="44" t="s">
+        <v>229</v>
+      </c>
+      <c r="N134" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="24"/>
-      <c r="B135" s="44"/>
-      <c r="C135" s="42"/>
-      <c r="D135" s="42"/>
-      <c r="E135" s="44"/>
+      <c r="B135" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="C135" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="D135" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="E135" s="44" t="s">
+        <v>259</v>
+      </c>
       <c r="F135" s="42"/>
       <c r="G135" s="42"/>
       <c r="H135" s="42"/>
@@ -7049,15 +7175,27 @@
       <c r="J135" s="4"/>
       <c r="K135" s="4"/>
       <c r="L135" s="44"/>
-      <c r="M135" s="44"/>
-      <c r="N135" s="44"/>
-    </row>
-    <row r="136" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M135" s="44" t="s">
+        <v>229</v>
+      </c>
+      <c r="N135" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="24"/>
-      <c r="B136" s="44"/>
-      <c r="C136" s="42"/>
-      <c r="D136" s="42"/>
-      <c r="E136" s="44"/>
+      <c r="B136" s="44" t="s">
+        <v>260</v>
+      </c>
+      <c r="C136" s="42" t="s">
+        <v>263</v>
+      </c>
+      <c r="D136" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E136" s="44" t="s">
+        <v>264</v>
+      </c>
       <c r="F136" s="42"/>
       <c r="G136" s="42"/>
       <c r="H136" s="42"/>
@@ -7065,489 +7203,1168 @@
       <c r="J136" s="4"/>
       <c r="K136" s="4"/>
       <c r="L136" s="44"/>
-      <c r="M136" s="44"/>
-      <c r="N136" s="44"/>
-    </row>
-    <row r="137" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="24"/>
-      <c r="B137" s="44"/>
-      <c r="C137" s="42"/>
-      <c r="D137" s="42"/>
-      <c r="E137" s="44"/>
-      <c r="F137" s="42"/>
-      <c r="G137" s="42"/>
+      <c r="M136" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="N136" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="B137" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="C137" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D137" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E137" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G137" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H137" s="42"/>
-      <c r="I137" s="3"/>
-      <c r="J137" s="4"/>
+      <c r="I137" s="3">
+        <v>300</v>
+      </c>
+      <c r="J137" s="4">
+        <f>1/(100*P137)</f>
+        <v>2.0387359836901123E-6</v>
+      </c>
       <c r="K137" s="4"/>
-      <c r="L137" s="44"/>
-      <c r="M137" s="44"/>
-      <c r="N137" s="44"/>
-    </row>
-    <row r="138" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="24"/>
-      <c r="B138" s="44"/>
-      <c r="C138" s="42"/>
-      <c r="D138" s="42"/>
-      <c r="E138" s="44"/>
-      <c r="F138" s="42"/>
-      <c r="G138" s="42"/>
+      <c r="L137" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M137" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N137" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P137" s="6">
+        <v>4905</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="B138" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="C138" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D138" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E138" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G138" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H138" s="42"/>
-      <c r="I138" s="3"/>
-      <c r="J138" s="4"/>
+      <c r="I138" s="3">
+        <v>300</v>
+      </c>
+      <c r="J138" s="4">
+        <f t="shared" ref="J138:J148" si="3">1/(100*P138)</f>
+        <v>2.6881720430107525E-6</v>
+      </c>
       <c r="K138" s="4"/>
-      <c r="L138" s="44"/>
-      <c r="M138" s="44"/>
-      <c r="N138" s="44"/>
-    </row>
-    <row r="139" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="24"/>
-      <c r="B139" s="44"/>
-      <c r="C139" s="42"/>
-      <c r="D139" s="42"/>
-      <c r="E139" s="44"/>
-      <c r="F139" s="42"/>
-      <c r="G139" s="42"/>
+      <c r="L138" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M138" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N138" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P138" s="6">
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B139" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="C139" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D139" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E139" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G139" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H139" s="42"/>
-      <c r="I139" s="3"/>
-      <c r="J139" s="4"/>
+      <c r="I139" s="3">
+        <v>300</v>
+      </c>
+      <c r="J139" s="4">
+        <f t="shared" si="3"/>
+        <v>3.3863867253640365E-6</v>
+      </c>
       <c r="K139" s="4"/>
-      <c r="L139" s="44"/>
-      <c r="M139" s="44"/>
-      <c r="N139" s="44"/>
-    </row>
-    <row r="140" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="24"/>
-      <c r="B140" s="44"/>
-      <c r="C140" s="42"/>
-      <c r="D140" s="42"/>
-      <c r="E140" s="44"/>
-      <c r="F140" s="42"/>
-      <c r="G140" s="42"/>
+      <c r="L139" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M139" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N139" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P139" s="6">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="B140" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="C140" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D140" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E140" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G140" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H140" s="42"/>
-      <c r="I140" s="3"/>
-      <c r="J140" s="4"/>
+      <c r="I140" s="3">
+        <v>473</v>
+      </c>
+      <c r="J140" s="4">
+        <f t="shared" si="3"/>
+        <v>2.14638334406525E-6</v>
+      </c>
       <c r="K140" s="4"/>
-      <c r="L140" s="44"/>
-      <c r="M140" s="44"/>
-      <c r="N140" s="44"/>
-    </row>
-    <row r="141" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="24"/>
-      <c r="B141" s="44"/>
-      <c r="C141" s="42"/>
-      <c r="D141" s="42"/>
-      <c r="E141" s="44"/>
-      <c r="F141" s="42"/>
-      <c r="G141" s="42"/>
+      <c r="L140" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M140" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N140" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P140" s="6">
+        <v>4659</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="B141" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="C141" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D141" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E141" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G141" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H141" s="42"/>
-      <c r="I141" s="3"/>
-      <c r="J141" s="4"/>
+      <c r="I141" s="3">
+        <v>473</v>
+      </c>
+      <c r="J141" s="4">
+        <f t="shared" si="3"/>
+        <v>2.6274303730951129E-6</v>
+      </c>
       <c r="K141" s="4"/>
-      <c r="L141" s="44"/>
-      <c r="M141" s="44"/>
-      <c r="N141" s="44"/>
-    </row>
-    <row r="142" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="24"/>
-      <c r="B142" s="44"/>
-      <c r="C142" s="42"/>
-      <c r="D142" s="42"/>
-      <c r="E142" s="44"/>
-      <c r="F142" s="42"/>
-      <c r="G142" s="42"/>
+      <c r="L141" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M141" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N141" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P141" s="6">
+        <v>3806</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B142" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="C142" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D142" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E142" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G142" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H142" s="42"/>
-      <c r="I142" s="3"/>
-      <c r="J142" s="4"/>
+      <c r="I142" s="3">
+        <v>473</v>
+      </c>
+      <c r="J142" s="4">
+        <f t="shared" si="3"/>
+        <v>3.1826861871419479E-6</v>
+      </c>
       <c r="K142" s="4"/>
-      <c r="L142" s="44"/>
-      <c r="M142" s="44"/>
-      <c r="N142" s="44"/>
-    </row>
-    <row r="143" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="24"/>
-      <c r="B143" s="44"/>
-      <c r="C143" s="42"/>
-      <c r="D143" s="42"/>
-      <c r="E143" s="44"/>
-      <c r="F143" s="42"/>
-      <c r="G143" s="42"/>
+      <c r="L142" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M142" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N142" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P142" s="6">
+        <v>3142</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="B143" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="C143" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D143" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E143" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G143" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H143" s="42"/>
-      <c r="I143" s="3"/>
-      <c r="J143" s="4"/>
+      <c r="I143" s="3">
+        <v>623</v>
+      </c>
+      <c r="J143" s="4">
+        <f t="shared" si="3"/>
+        <v>2.1079258010118043E-6</v>
+      </c>
       <c r="K143" s="4"/>
-      <c r="L143" s="44"/>
-      <c r="M143" s="44"/>
-      <c r="N143" s="44"/>
-    </row>
-    <row r="144" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="24"/>
-      <c r="B144" s="44"/>
-      <c r="C144" s="42"/>
-      <c r="D144" s="42"/>
-      <c r="E144" s="44"/>
-      <c r="F144" s="42"/>
-      <c r="G144" s="42"/>
+      <c r="L143" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M143" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N143" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P143" s="6">
+        <v>4744</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="B144" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="C144" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D144" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E144" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G144" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H144" s="42"/>
-      <c r="I144" s="3"/>
-      <c r="J144" s="4"/>
+      <c r="I144" s="3">
+        <v>623</v>
+      </c>
+      <c r="J144" s="4">
+        <f t="shared" si="3"/>
+        <v>2.508780732563974E-6</v>
+      </c>
       <c r="K144" s="4"/>
-      <c r="L144" s="44"/>
-      <c r="M144" s="44"/>
-      <c r="N144" s="44"/>
-    </row>
-    <row r="145" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="24"/>
-      <c r="B145" s="44"/>
-      <c r="C145" s="42"/>
-      <c r="D145" s="42"/>
-      <c r="E145" s="44"/>
-      <c r="F145" s="42"/>
-      <c r="G145" s="42"/>
+      <c r="L144" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M144" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N144" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P144" s="6">
+        <v>3986</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B145" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="C145" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D145" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E145" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G145" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H145" s="42"/>
-      <c r="I145" s="3"/>
-      <c r="J145" s="4"/>
+      <c r="I145" s="3">
+        <v>623</v>
+      </c>
+      <c r="J145" s="4">
+        <f t="shared" si="3"/>
+        <v>2.9180040852057195E-6</v>
+      </c>
       <c r="K145" s="4"/>
-      <c r="L145" s="44"/>
-      <c r="M145" s="44"/>
-      <c r="N145" s="44"/>
-    </row>
-    <row r="146" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="24"/>
-      <c r="B146" s="44"/>
-      <c r="C146" s="42"/>
-      <c r="D146" s="42"/>
-      <c r="E146" s="44"/>
-      <c r="F146" s="42"/>
-      <c r="G146" s="42"/>
+      <c r="L145" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M145" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N145" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P145" s="6">
+        <v>3427</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="B146" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="C146" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D146" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E146" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F146" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="G146" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H146" s="42"/>
-      <c r="I146" s="3"/>
-      <c r="J146" s="4"/>
+      <c r="I146" s="3">
+        <v>300</v>
+      </c>
+      <c r="J146" s="4">
+        <f>P146*10^(-6)</f>
+        <v>-9.4700000000000008E-6</v>
+      </c>
       <c r="K146" s="4"/>
-      <c r="L146" s="44"/>
-      <c r="M146" s="44"/>
-      <c r="N146" s="44"/>
-    </row>
-    <row r="147" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="24"/>
-      <c r="B147" s="44"/>
-      <c r="C147" s="42"/>
-      <c r="D147" s="42"/>
-      <c r="E147" s="44"/>
-      <c r="F147" s="42"/>
-      <c r="G147" s="42"/>
+      <c r="L146" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="M146" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N146" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P146" s="6">
+        <v>-9.4700000000000006</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="B147" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="C147" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D147" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E147" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F147" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="G147" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H147" s="42"/>
-      <c r="I147" s="3"/>
-      <c r="J147" s="4"/>
+      <c r="I147" s="3">
+        <v>300</v>
+      </c>
+      <c r="J147" s="4">
+        <f t="shared" ref="J147:J163" si="4">P147*10^(-6)</f>
+        <v>-1.027E-5</v>
+      </c>
       <c r="K147" s="4"/>
-      <c r="L147" s="44"/>
-      <c r="M147" s="44"/>
-      <c r="N147" s="44"/>
-    </row>
-    <row r="148" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="24"/>
-      <c r="B148" s="44"/>
-      <c r="C148" s="42"/>
-      <c r="D148" s="42"/>
-      <c r="E148" s="44"/>
-      <c r="F148" s="42"/>
-      <c r="G148" s="42"/>
+      <c r="L147" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="M147" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N147" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P147" s="6">
+        <v>-10.27</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B148" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="C148" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D148" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E148" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F148" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="G148" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H148" s="42"/>
-      <c r="I148" s="3"/>
-      <c r="J148" s="4"/>
+      <c r="I148" s="3">
+        <v>300</v>
+      </c>
+      <c r="J148" s="4">
+        <f t="shared" si="4"/>
+        <v>-6.6100000000000002E-6</v>
+      </c>
       <c r="K148" s="4"/>
-      <c r="L148" s="44"/>
-      <c r="M148" s="44"/>
-      <c r="N148" s="44"/>
-    </row>
-    <row r="149" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="24"/>
-      <c r="B149" s="44"/>
-      <c r="C149" s="42"/>
-      <c r="D149" s="42"/>
-      <c r="E149" s="44"/>
-      <c r="F149" s="42"/>
-      <c r="G149" s="42"/>
+      <c r="L148" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="M148" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N148" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P148" s="6">
+        <v>-6.61</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="B149" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="C149" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D149" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E149" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F149" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="G149" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H149" s="42"/>
-      <c r="I149" s="3"/>
-      <c r="J149" s="4"/>
+      <c r="I149" s="3">
+        <v>473</v>
+      </c>
+      <c r="J149" s="4">
+        <f t="shared" si="4"/>
+        <v>-1.096E-5</v>
+      </c>
       <c r="K149" s="4"/>
-      <c r="L149" s="44"/>
-      <c r="M149" s="44"/>
-      <c r="N149" s="44"/>
-    </row>
-    <row r="150" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="24"/>
-      <c r="B150" s="44"/>
-      <c r="C150" s="42"/>
-      <c r="D150" s="42"/>
-      <c r="E150" s="44"/>
-      <c r="F150" s="42"/>
-      <c r="G150" s="42"/>
+      <c r="L149" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="M149" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N149" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P149" s="6">
+        <v>-10.96</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="B150" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="C150" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D150" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E150" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F150" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="G150" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H150" s="42"/>
-      <c r="I150" s="3"/>
-      <c r="J150" s="4"/>
+      <c r="I150" s="3">
+        <v>473</v>
+      </c>
+      <c r="J150" s="4">
+        <f t="shared" si="4"/>
+        <v>-1.363E-5</v>
+      </c>
       <c r="K150" s="4"/>
-      <c r="L150" s="44"/>
-      <c r="M150" s="44"/>
-      <c r="N150" s="44"/>
-    </row>
-    <row r="151" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="24"/>
-      <c r="B151" s="44"/>
-      <c r="C151" s="42"/>
-      <c r="D151" s="42"/>
-      <c r="E151" s="44"/>
-      <c r="F151" s="42"/>
-      <c r="G151" s="42"/>
+      <c r="L150" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="M150" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N150" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P150" s="6">
+        <v>-13.63</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B151" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="C151" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D151" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E151" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F151" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="G151" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H151" s="42"/>
-      <c r="I151" s="3"/>
-      <c r="J151" s="4"/>
+      <c r="I151" s="3">
+        <v>473</v>
+      </c>
+      <c r="J151" s="4">
+        <f t="shared" si="4"/>
+        <v>-9.7799999999999995E-6</v>
+      </c>
       <c r="K151" s="4"/>
-      <c r="L151" s="44"/>
-      <c r="M151" s="44"/>
-      <c r="N151" s="44"/>
-    </row>
-    <row r="152" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="24"/>
-      <c r="B152" s="44"/>
-      <c r="C152" s="42"/>
-      <c r="D152" s="42"/>
-      <c r="E152" s="44"/>
-      <c r="F152" s="42"/>
-      <c r="G152" s="42"/>
+      <c r="L151" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="M151" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N151" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P151" s="6">
+        <v>-9.7799999999999994</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="B152" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="C152" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D152" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E152" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F152" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="G152" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H152" s="42"/>
-      <c r="I152" s="3"/>
-      <c r="J152" s="4"/>
+      <c r="I152" s="3">
+        <v>623</v>
+      </c>
+      <c r="J152" s="4">
+        <f t="shared" si="4"/>
+        <v>-1.2639999999999999E-5</v>
+      </c>
       <c r="K152" s="4"/>
-      <c r="L152" s="44"/>
-      <c r="M152" s="44"/>
-      <c r="N152" s="44"/>
-    </row>
-    <row r="153" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="24"/>
-      <c r="B153" s="44"/>
-      <c r="C153" s="42"/>
-      <c r="D153" s="42"/>
-      <c r="E153" s="44"/>
-      <c r="F153" s="42"/>
-      <c r="G153" s="42"/>
+      <c r="L152" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="M152" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N152" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P152" s="6">
+        <v>-12.64</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="B153" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="C153" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D153" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E153" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F153" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="G153" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H153" s="42"/>
-      <c r="I153" s="3"/>
-      <c r="J153" s="4"/>
+      <c r="I153" s="3">
+        <v>623</v>
+      </c>
+      <c r="J153" s="4">
+        <f t="shared" si="4"/>
+        <v>-1.6309999999999998E-5</v>
+      </c>
       <c r="K153" s="4"/>
-      <c r="L153" s="44"/>
-      <c r="M153" s="44"/>
-      <c r="N153" s="44"/>
-    </row>
-    <row r="154" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="24"/>
-      <c r="B154" s="44"/>
-      <c r="C154" s="42"/>
-      <c r="D154" s="42"/>
-      <c r="E154" s="44"/>
-      <c r="F154" s="42"/>
-      <c r="G154" s="42"/>
+      <c r="L153" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="M153" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N153" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P153" s="6">
+        <v>-16.309999999999999</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B154" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="C154" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D154" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E154" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F154" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="G154" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H154" s="42"/>
-      <c r="I154" s="3"/>
-      <c r="J154" s="4"/>
+      <c r="I154" s="3">
+        <v>623</v>
+      </c>
+      <c r="J154" s="4">
+        <f t="shared" si="4"/>
+        <v>-1.3689999999999999E-5</v>
+      </c>
       <c r="K154" s="4"/>
-      <c r="L154" s="44"/>
-      <c r="M154" s="44"/>
-      <c r="N154" s="44"/>
-    </row>
-    <row r="155" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="24"/>
-      <c r="B155" s="44"/>
-      <c r="C155" s="42"/>
-      <c r="D155" s="42"/>
-      <c r="E155" s="44"/>
-      <c r="F155" s="42"/>
-      <c r="G155" s="42"/>
+      <c r="L154" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="M154" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N154" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="P154" s="6">
+        <v>-13.69</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="B155" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="C155" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D155" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E155" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F155" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="G155" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H155" s="42"/>
-      <c r="I155" s="3"/>
-      <c r="J155" s="4"/>
+      <c r="I155" s="3">
+        <v>300</v>
+      </c>
+      <c r="J155" s="6">
+        <v>5.76</v>
+      </c>
       <c r="K155" s="4"/>
-      <c r="L155" s="44"/>
-      <c r="M155" s="44"/>
-      <c r="N155" s="44"/>
-    </row>
-    <row r="156" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="24"/>
-      <c r="B156" s="44"/>
-      <c r="C156" s="42"/>
-      <c r="D156" s="42"/>
-      <c r="E156" s="44"/>
-      <c r="F156" s="42"/>
-      <c r="G156" s="42"/>
+      <c r="L155" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="M155" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="N155" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="B156" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="C156" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D156" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E156" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F156" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="G156" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H156" s="42"/>
-      <c r="I156" s="3"/>
-      <c r="J156" s="4"/>
+      <c r="I156" s="3">
+        <v>300</v>
+      </c>
+      <c r="J156" s="6">
+        <v>5.38</v>
+      </c>
       <c r="K156" s="4"/>
-      <c r="L156" s="44"/>
-      <c r="M156" s="44"/>
-      <c r="N156" s="44"/>
-    </row>
-    <row r="157" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="24"/>
-      <c r="B157" s="44"/>
-      <c r="C157" s="42"/>
-      <c r="D157" s="42"/>
-      <c r="E157" s="44"/>
-      <c r="F157" s="42"/>
-      <c r="G157" s="42"/>
+      <c r="L156" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="M156" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="N156" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B157" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="C157" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D157" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E157" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F157" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="G157" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H157" s="42"/>
-      <c r="I157" s="3"/>
-      <c r="J157" s="4"/>
+      <c r="I157" s="3">
+        <v>300</v>
+      </c>
+      <c r="J157" s="6">
+        <v>4.32</v>
+      </c>
       <c r="K157" s="4"/>
-      <c r="L157" s="44"/>
-      <c r="M157" s="44"/>
-      <c r="N157" s="44"/>
-    </row>
-    <row r="158" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="24"/>
-      <c r="B158" s="44"/>
-      <c r="C158" s="42"/>
-      <c r="D158" s="42"/>
-      <c r="E158" s="44"/>
-      <c r="F158" s="42"/>
-      <c r="G158" s="42"/>
+      <c r="L157" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="M157" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="N157" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="B158" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="C158" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D158" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E158" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F158" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="G158" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H158" s="42"/>
-      <c r="I158" s="3"/>
-      <c r="J158" s="4"/>
+      <c r="I158" s="3">
+        <v>473</v>
+      </c>
+      <c r="J158" s="6">
+        <v>8.6</v>
+      </c>
       <c r="K158" s="4"/>
-      <c r="L158" s="44"/>
-      <c r="M158" s="44"/>
-      <c r="N158" s="44"/>
-    </row>
-    <row r="159" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="24"/>
-      <c r="B159" s="44"/>
-      <c r="C159" s="42"/>
-      <c r="D159" s="42"/>
-      <c r="E159" s="44"/>
-      <c r="F159" s="42"/>
-      <c r="G159" s="42"/>
+      <c r="L158" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="M158" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="N158" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="B159" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="C159" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D159" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E159" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F159" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="G159" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H159" s="42"/>
-      <c r="I159" s="3"/>
-      <c r="J159" s="4"/>
+      <c r="I159" s="3">
+        <v>473</v>
+      </c>
+      <c r="J159" s="6">
+        <v>8.6</v>
+      </c>
       <c r="K159" s="4"/>
-      <c r="L159" s="44"/>
-      <c r="M159" s="44"/>
-      <c r="N159" s="44"/>
-    </row>
-    <row r="160" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A160" s="24"/>
-      <c r="B160" s="44"/>
-      <c r="C160" s="42"/>
-      <c r="D160" s="42"/>
-      <c r="E160" s="44"/>
-      <c r="F160" s="42"/>
-      <c r="G160" s="42"/>
+      <c r="L159" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="M159" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="N159" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B160" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="C160" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D160" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E160" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F160" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="G160" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H160" s="42"/>
-      <c r="I160" s="3"/>
-      <c r="J160" s="4"/>
+      <c r="I160" s="3">
+        <v>473</v>
+      </c>
+      <c r="J160" s="6">
+        <v>7.39</v>
+      </c>
       <c r="K160" s="4"/>
-      <c r="L160" s="44"/>
-      <c r="M160" s="44"/>
-      <c r="N160" s="44"/>
+      <c r="L160" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="M160" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="N160" s="44" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="161" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="24"/>
-      <c r="B161" s="44"/>
-      <c r="C161" s="42"/>
-      <c r="D161" s="42"/>
-      <c r="E161" s="44"/>
-      <c r="F161" s="42"/>
-      <c r="G161" s="42"/>
+      <c r="A161" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="B161" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="C161" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D161" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E161" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F161" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="G161" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H161" s="42"/>
-      <c r="I161" s="3"/>
-      <c r="J161" s="4"/>
+      <c r="I161" s="3">
+        <v>623</v>
+      </c>
+      <c r="J161" s="6">
+        <v>11.43</v>
+      </c>
       <c r="K161" s="4"/>
-      <c r="L161" s="44"/>
-      <c r="M161" s="44"/>
-      <c r="N161" s="44"/>
+      <c r="L161" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="M161" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="N161" s="44" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="162" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="24"/>
-      <c r="B162" s="44"/>
-      <c r="C162" s="42"/>
-      <c r="D162" s="42"/>
-      <c r="E162" s="44"/>
-      <c r="F162" s="42"/>
-      <c r="G162" s="42"/>
+      <c r="A162" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="B162" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="C162" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D162" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E162" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F162" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="G162" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H162" s="42"/>
-      <c r="I162" s="3"/>
-      <c r="J162" s="4"/>
+      <c r="I162" s="3">
+        <v>623</v>
+      </c>
+      <c r="J162" s="6">
+        <v>10.65</v>
+      </c>
       <c r="K162" s="4"/>
-      <c r="L162" s="44"/>
-      <c r="M162" s="44"/>
-      <c r="N162" s="44"/>
+      <c r="L162" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="M162" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="N162" s="44" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="163" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="24"/>
-      <c r="B163" s="44"/>
-      <c r="C163" s="42"/>
-      <c r="D163" s="42"/>
-      <c r="E163" s="44"/>
-      <c r="F163" s="42"/>
-      <c r="G163" s="42"/>
+      <c r="A163" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B163" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="C163" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D163" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="E163" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F163" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="G163" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H163" s="42"/>
-      <c r="I163" s="3"/>
-      <c r="J163" s="4"/>
+      <c r="I163" s="3">
+        <v>623</v>
+      </c>
+      <c r="J163" s="6">
+        <v>9.3699999999999992</v>
+      </c>
       <c r="K163" s="4"/>
-      <c r="L163" s="44"/>
-      <c r="M163" s="44"/>
-      <c r="N163" s="44"/>
-    </row>
-    <row r="164" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="24"/>
-      <c r="B164" s="44"/>
-      <c r="C164" s="42"/>
-      <c r="D164" s="42"/>
-      <c r="E164" s="44"/>
-      <c r="F164" s="42"/>
-      <c r="G164" s="42"/>
-      <c r="H164" s="42"/>
-      <c r="I164" s="3"/>
-      <c r="J164" s="4"/>
-      <c r="K164" s="4"/>
-      <c r="L164" s="44"/>
-      <c r="M164" s="44"/>
-      <c r="N164" s="44"/>
-    </row>
-    <row r="165" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A165" s="24"/>
-      <c r="B165" s="44"/>
-      <c r="C165" s="42"/>
-      <c r="D165" s="42"/>
-      <c r="E165" s="44"/>
-      <c r="F165" s="42"/>
-      <c r="G165" s="42"/>
-      <c r="H165" s="42"/>
-      <c r="I165" s="3"/>
-      <c r="J165" s="4"/>
-      <c r="K165" s="4"/>
-      <c r="L165" s="44"/>
-      <c r="M165" s="44"/>
-      <c r="N165" s="44"/>
-    </row>
-    <row r="166" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A166" s="24"/>
-      <c r="B166" s="44"/>
-      <c r="C166" s="42"/>
-      <c r="D166" s="42"/>
-      <c r="E166" s="44"/>
-      <c r="F166" s="42"/>
-      <c r="G166" s="42"/>
-      <c r="H166" s="42"/>
-      <c r="I166" s="3"/>
-      <c r="J166" s="4"/>
-      <c r="K166" s="4"/>
-      <c r="L166" s="44"/>
-      <c r="M166" s="44"/>
-      <c r="N166" s="44"/>
-    </row>
+      <c r="L163" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="M163" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="N163" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="167" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="24"/>
       <c r="B167" s="44"/>
@@ -11430,11 +12247,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -11449,6 +12261,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted data from  `10.1016/j.scriptamat.2020.05.033`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DD5E47-2B73-4B4C-A298-107CF90E6BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1864B0CB-F07B-8249-809C-0D9C05B69E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="276">
   <si>
     <t>Metadata</t>
   </si>
@@ -940,6 +940,19 @@
   </si>
   <si>
     <t>10.1016/j.intermet.2022.107495</t>
+  </si>
+  <si>
+    <t>Ti Zr Hf Y La0.2</t>
+  </si>
+  <si>
+    <t>designed based on the concept of the LPS and segregation for
+enhancing the immiscibility of the constituent elements</t>
+  </si>
+  <si>
+    <t>P245</t>
+  </si>
+  <si>
+    <t>10.1016/j.scriptamat.2020.05.033</t>
   </si>
 </sst>
 </file>
@@ -1551,7 +1564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1707,57 +1720,6 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1823,6 +1785,63 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2131,8 +2150,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="99" workbookViewId="0">
-      <selection activeCell="H166" sqref="H166"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="99" workbookViewId="0">
+      <selection activeCell="M174" sqref="M174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2181,19 +2200,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="71"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="78"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="61"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2204,17 +2223,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="82"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="65"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2243,43 +2262,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="85" t="s">
+      <c r="D5" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="85" t="s">
+      <c r="E5" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="85" t="s">
+      <c r="F5" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="85" t="s">
+      <c r="G5" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="86" t="s">
+      <c r="H5" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="88" t="s">
+      <c r="I5" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="90" t="s">
+      <c r="J5" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="90" t="s">
+      <c r="K5" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="85" t="s">
+      <c r="L5" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="85" t="s">
+      <c r="M5" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="85" t="s">
+      <c r="N5" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="53" t="s">
+      <c r="O5" s="75" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2290,19 +2309,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="84"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="54"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="76"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
@@ -2347,7 +2366,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="55"/>
+      <c r="O7" s="77"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2360,35 +2379,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="59" t="s">
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="63"/>
-      <c r="M8" s="64" t="s">
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="85"/>
+      <c r="M8" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="65"/>
+      <c r="N8" s="87"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="66" t="s">
+      <c r="P8" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="67"/>
-      <c r="R8" s="68"/>
-      <c r="S8" s="68"/>
-      <c r="T8" s="69"/>
+      <c r="Q8" s="89"/>
+      <c r="R8" s="90"/>
+      <c r="S8" s="90"/>
+      <c r="T8" s="91"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
@@ -7281,7 +7300,7 @@
         <v>300</v>
       </c>
       <c r="J138" s="4">
-        <f t="shared" ref="J138:J148" si="3">1/(100*P138)</f>
+        <f t="shared" ref="J138:J145" si="3">1/(100*P138)</f>
         <v>2.6881720430107525E-6</v>
       </c>
       <c r="K138" s="4"/>
@@ -7677,7 +7696,7 @@
         <v>300</v>
       </c>
       <c r="J147" s="4">
-        <f t="shared" ref="J147:J163" si="4">P147*10^(-6)</f>
+        <f t="shared" ref="J147:J154" si="4">P147*10^(-6)</f>
         <v>-1.027E-5</v>
       </c>
       <c r="K147" s="4"/>
@@ -8242,7 +8261,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="24" t="s">
         <v>251</v>
       </c>
@@ -8282,7 +8301,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="24" t="s">
         <v>250</v>
       </c>
@@ -8322,7 +8341,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="24" t="s">
         <v>252</v>
       </c>
@@ -8362,10 +8381,48 @@
         <v>271</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="167" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B164" s="92" t="s">
+        <v>272</v>
+      </c>
+      <c r="C164" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="D164" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E164" s="93" t="s">
+        <v>273</v>
+      </c>
+      <c r="F164" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G164" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="I164" s="49">
+        <v>298</v>
+      </c>
+      <c r="J164" s="50">
+        <f>P164*9807000</f>
+        <v>2628276000</v>
+      </c>
+      <c r="L164" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M164" s="51" t="s">
+        <v>274</v>
+      </c>
+      <c r="N164" s="51" t="s">
+        <v>275</v>
+      </c>
+      <c r="P164" s="6">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="24"/>
       <c r="B167" s="44"/>
       <c r="C167" s="42"/>
@@ -8381,7 +8438,7 @@
       <c r="M167" s="44"/>
       <c r="N167" s="44"/>
     </row>
-    <row r="168" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="24"/>
       <c r="B168" s="44"/>
       <c r="C168" s="42"/>
@@ -8397,7 +8454,7 @@
       <c r="M168" s="44"/>
       <c r="N168" s="44"/>
     </row>
-    <row r="169" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="24"/>
       <c r="B169" s="44"/>
       <c r="C169" s="42"/>
@@ -8413,7 +8470,7 @@
       <c r="M169" s="44"/>
       <c r="N169" s="44"/>
     </row>
-    <row r="170" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="24"/>
       <c r="B170" s="44"/>
       <c r="C170" s="42"/>
@@ -8429,7 +8486,7 @@
       <c r="M170" s="44"/>
       <c r="N170" s="44"/>
     </row>
-    <row r="171" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="24"/>
       <c r="B171" s="44"/>
       <c r="C171" s="42"/>
@@ -8445,7 +8502,7 @@
       <c r="M171" s="44"/>
       <c r="N171" s="44"/>
     </row>
-    <row r="172" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="24"/>
       <c r="B172" s="44"/>
       <c r="C172" s="42"/>
@@ -8461,7 +8518,7 @@
       <c r="M172" s="44"/>
       <c r="N172" s="44"/>
     </row>
-    <row r="173" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="24"/>
       <c r="B173" s="44"/>
       <c r="C173" s="42"/>
@@ -8477,7 +8534,7 @@
       <c r="M173" s="44"/>
       <c r="N173" s="44"/>
     </row>
-    <row r="174" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="24"/>
       <c r="B174" s="44"/>
       <c r="C174" s="42"/>
@@ -8493,7 +8550,7 @@
       <c r="M174" s="44"/>
       <c r="N174" s="44"/>
     </row>
-    <row r="175" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="24"/>
       <c r="B175" s="44"/>
       <c r="C175" s="42"/>
@@ -8509,7 +8566,7 @@
       <c r="M175" s="44"/>
       <c r="N175" s="44"/>
     </row>
-    <row r="176" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="24"/>
       <c r="B176" s="44"/>
       <c r="C176" s="42"/>
@@ -12247,6 +12304,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -12261,11 +12323,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted data from  `10.1016/j.jallcom.2021.159918`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1864B0CB-F07B-8249-809C-0D9C05B69E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0707BB11-CE4E-B24C-9132-BAD66C4E1986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="285">
   <si>
     <t>Metadata</t>
   </si>
@@ -953,6 +953,33 @@
   </si>
   <si>
     <t>10.1016/j.scriptamat.2020.05.033</t>
+  </si>
+  <si>
+    <t>GdTbHoEr</t>
+  </si>
+  <si>
+    <t>GdTbHoErLa</t>
+  </si>
+  <si>
+    <t>GdTbHoErLaY</t>
+  </si>
+  <si>
+    <t>GdTbHoErPr</t>
+  </si>
+  <si>
+    <t>neel temperature</t>
+  </si>
+  <si>
+    <t>curie temperature</t>
+  </si>
+  <si>
+    <t>peak magnetic entropy change</t>
+  </si>
+  <si>
+    <t>J / (kg K)</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2021.159918</t>
   </si>
 </sst>
 </file>
@@ -2150,8 +2177,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="99" workbookViewId="0">
-      <selection activeCell="M174" sqref="M174"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="99" workbookViewId="0">
+      <selection activeCell="N175" sqref="N175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8420,103 +8447,265 @@
         <v>268</v>
       </c>
     </row>
-    <row r="165" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B165" s="92" t="s">
+        <v>276</v>
+      </c>
+      <c r="C165" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D165" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F165" s="48" t="s">
+        <v>280</v>
+      </c>
+      <c r="G165" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="J165" s="50">
+        <v>190</v>
+      </c>
+      <c r="L165" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="M165" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N165" s="51" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B166" s="92" t="s">
+        <v>277</v>
+      </c>
+      <c r="C166" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D166" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F166" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="G166" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="J166" s="50">
+        <v>127</v>
+      </c>
+      <c r="L166" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="M166" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N166" s="51" t="s">
+        <v>284</v>
+      </c>
+    </row>
     <row r="167" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="24"/>
-      <c r="B167" s="44"/>
-      <c r="C167" s="42"/>
-      <c r="D167" s="42"/>
+      <c r="B167" s="44" t="s">
+        <v>278</v>
+      </c>
+      <c r="C167" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D167" s="48" t="s">
+        <v>89</v>
+      </c>
       <c r="E167" s="44"/>
-      <c r="F167" s="42"/>
-      <c r="G167" s="42"/>
+      <c r="F167" s="48" t="s">
+        <v>280</v>
+      </c>
+      <c r="G167" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H167" s="42"/>
       <c r="I167" s="3"/>
-      <c r="J167" s="4"/>
+      <c r="J167" s="4">
+        <v>120</v>
+      </c>
       <c r="K167" s="4"/>
-      <c r="L167" s="44"/>
-      <c r="M167" s="44"/>
-      <c r="N167" s="44"/>
+      <c r="L167" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="M167" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N167" s="51" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="168" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="24"/>
-      <c r="B168" s="44"/>
-      <c r="C168" s="42"/>
-      <c r="D168" s="42"/>
+      <c r="B168" s="44" t="s">
+        <v>279</v>
+      </c>
+      <c r="C168" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D168" s="48" t="s">
+        <v>89</v>
+      </c>
       <c r="E168" s="44"/>
-      <c r="F168" s="42"/>
-      <c r="G168" s="42"/>
+      <c r="F168" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="G168" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H168" s="42"/>
       <c r="I168" s="3"/>
-      <c r="J168" s="4"/>
+      <c r="J168" s="4">
+        <v>135</v>
+      </c>
       <c r="K168" s="4"/>
-      <c r="L168" s="44"/>
-      <c r="M168" s="44"/>
-      <c r="N168" s="44"/>
+      <c r="L168" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="M168" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N168" s="51" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="169" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="24"/>
-      <c r="B169" s="44"/>
-      <c r="C169" s="42"/>
-      <c r="D169" s="42"/>
-      <c r="E169" s="44"/>
-      <c r="F169" s="42"/>
-      <c r="G169" s="42"/>
+      <c r="B169" s="92" t="s">
+        <v>276</v>
+      </c>
+      <c r="C169" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D169" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F169" s="48" t="s">
+        <v>282</v>
+      </c>
+      <c r="G169" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H169" s="42"/>
       <c r="I169" s="3"/>
-      <c r="J169" s="4"/>
+      <c r="J169" s="4">
+        <v>8.64</v>
+      </c>
       <c r="K169" s="4"/>
-      <c r="L169" s="44"/>
-      <c r="M169" s="44"/>
-      <c r="N169" s="44"/>
+      <c r="L169" s="44" t="s">
+        <v>283</v>
+      </c>
+      <c r="M169" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N169" s="51" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="170" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="24"/>
-      <c r="B170" s="44"/>
-      <c r="C170" s="42"/>
-      <c r="D170" s="42"/>
-      <c r="E170" s="44"/>
-      <c r="F170" s="42"/>
-      <c r="G170" s="42"/>
+      <c r="B170" s="92" t="s">
+        <v>277</v>
+      </c>
+      <c r="C170" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D170" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F170" s="48" t="s">
+        <v>282</v>
+      </c>
+      <c r="G170" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H170" s="42"/>
       <c r="I170" s="3"/>
-      <c r="J170" s="4"/>
+      <c r="J170" s="4">
+        <v>5.92</v>
+      </c>
       <c r="K170" s="4"/>
-      <c r="L170" s="44"/>
-      <c r="M170" s="44"/>
-      <c r="N170" s="44"/>
+      <c r="L170" s="44" t="s">
+        <v>283</v>
+      </c>
+      <c r="M170" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N170" s="51" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="171" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="24"/>
-      <c r="B171" s="44"/>
-      <c r="C171" s="42"/>
-      <c r="D171" s="42"/>
+      <c r="B171" s="44" t="s">
+        <v>278</v>
+      </c>
+      <c r="C171" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D171" s="48" t="s">
+        <v>89</v>
+      </c>
       <c r="E171" s="44"/>
-      <c r="F171" s="42"/>
-      <c r="G171" s="42"/>
+      <c r="F171" s="48" t="s">
+        <v>282</v>
+      </c>
+      <c r="G171" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H171" s="42"/>
       <c r="I171" s="3"/>
-      <c r="J171" s="4"/>
+      <c r="J171" s="4">
+        <v>5.85</v>
+      </c>
       <c r="K171" s="4"/>
-      <c r="L171" s="44"/>
-      <c r="M171" s="44"/>
-      <c r="N171" s="44"/>
+      <c r="L171" s="44" t="s">
+        <v>283</v>
+      </c>
+      <c r="M171" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N171" s="51" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="172" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="24"/>
-      <c r="B172" s="44"/>
-      <c r="C172" s="42"/>
-      <c r="D172" s="42"/>
+      <c r="B172" s="44" t="s">
+        <v>279</v>
+      </c>
+      <c r="C172" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D172" s="48" t="s">
+        <v>89</v>
+      </c>
       <c r="E172" s="44"/>
-      <c r="F172" s="42"/>
-      <c r="G172" s="42"/>
+      <c r="F172" s="48" t="s">
+        <v>282</v>
+      </c>
+      <c r="G172" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H172" s="42"/>
       <c r="I172" s="3"/>
-      <c r="J172" s="4"/>
+      <c r="J172" s="4">
+        <v>6.92</v>
+      </c>
       <c r="K172" s="4"/>
-      <c r="L172" s="44"/>
-      <c r="M172" s="44"/>
-      <c r="N172" s="44"/>
+      <c r="L172" s="44" t="s">
+        <v>283</v>
+      </c>
+      <c r="M172" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N172" s="51" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="173" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="24"/>

</xml_diff>

<commit_message>
- extracted data from  `10.1016/j.matdes.2016.01.149`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0707BB11-CE4E-B24C-9132-BAD66C4E1986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC28D3A4-795D-8242-87A5-AFD85E6DF382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="287">
   <si>
     <t>Metadata</t>
   </si>
@@ -980,6 +980,12 @@
   </si>
   <si>
     <t>10.1016/j.jallcom.2021.159918</t>
+  </si>
+  <si>
+    <t>GdHoLaTbY</t>
+  </si>
+  <si>
+    <t>10.1016/j.matdes.2016.01.149</t>
   </si>
 </sst>
 </file>
@@ -2177,8 +2183,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="99" workbookViewId="0">
-      <selection activeCell="N175" sqref="N175"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="99" workbookViewId="0">
+      <selection activeCell="O178" sqref="O178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8709,67 +8715,143 @@
     </row>
     <row r="173" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="24"/>
-      <c r="B173" s="44"/>
-      <c r="C173" s="42"/>
-      <c r="D173" s="42"/>
+      <c r="B173" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C173" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D173" s="42" t="s">
+        <v>64</v>
+      </c>
       <c r="E173" s="44"/>
-      <c r="F173" s="42"/>
-      <c r="G173" s="42"/>
+      <c r="F173" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G173" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H173" s="42"/>
       <c r="I173" s="3"/>
-      <c r="J173" s="4"/>
+      <c r="J173" s="4">
+        <v>880000000</v>
+      </c>
       <c r="K173" s="4"/>
-      <c r="L173" s="44"/>
-      <c r="M173" s="44"/>
-      <c r="N173" s="44"/>
+      <c r="L173" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M173" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N173" s="44" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="174" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="24"/>
-      <c r="B174" s="44"/>
-      <c r="C174" s="42"/>
-      <c r="D174" s="42"/>
+      <c r="B174" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C174" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D174" s="42" t="s">
+        <v>64</v>
+      </c>
       <c r="E174" s="44"/>
-      <c r="F174" s="42"/>
-      <c r="G174" s="42"/>
+      <c r="F174" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="G174" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H174" s="42"/>
       <c r="I174" s="3"/>
-      <c r="J174" s="4"/>
+      <c r="J174" s="4">
+        <v>108000000</v>
+      </c>
       <c r="K174" s="4"/>
-      <c r="L174" s="44"/>
-      <c r="M174" s="44"/>
-      <c r="N174" s="44"/>
+      <c r="L174" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M174" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N174" s="44" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="175" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="24"/>
-      <c r="B175" s="44"/>
-      <c r="C175" s="42"/>
-      <c r="D175" s="42"/>
+      <c r="B175" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C175" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D175" s="42" t="s">
+        <v>64</v>
+      </c>
       <c r="E175" s="44"/>
-      <c r="F175" s="42"/>
-      <c r="G175" s="42"/>
+      <c r="F175" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G175" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H175" s="42"/>
       <c r="I175" s="3"/>
-      <c r="J175" s="4"/>
+      <c r="J175" s="4">
+        <v>21.8</v>
+      </c>
       <c r="K175" s="4"/>
-      <c r="L175" s="44"/>
-      <c r="M175" s="44"/>
-      <c r="N175" s="44"/>
+      <c r="L175" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M175" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N175" s="44" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="176" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="24"/>
-      <c r="B176" s="44"/>
-      <c r="C176" s="42"/>
-      <c r="D176" s="42"/>
+      <c r="B176" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="C176" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D176" s="42" t="s">
+        <v>64</v>
+      </c>
       <c r="E176" s="44"/>
-      <c r="F176" s="42"/>
-      <c r="G176" s="42"/>
+      <c r="F176" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G176" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H176" s="42"/>
       <c r="I176" s="3"/>
-      <c r="J176" s="4"/>
+      <c r="J176" s="50">
+        <f>P176*9807000</f>
+        <v>941472000</v>
+      </c>
       <c r="K176" s="4"/>
-      <c r="L176" s="44"/>
-      <c r="M176" s="44"/>
-      <c r="N176" s="44"/>
+      <c r="L176" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M176" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N176" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="P176" s="6">
+        <v>96</v>
+      </c>
     </row>
     <row r="177" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="24"/>

</xml_diff>

<commit_message>
- extracted data from  `10.1063/1.5051514`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC28D3A4-795D-8242-87A5-AFD85E6DF382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5584F65F-7008-E647-BEC1-8908E8FA17AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="293">
   <si>
     <t>Metadata</t>
   </si>
@@ -986,6 +986,24 @@
   </si>
   <si>
     <t>10.1016/j.matdes.2016.01.149</t>
+  </si>
+  <si>
+    <t>10.1063/1.5051514</t>
+  </si>
+  <si>
+    <t>ErGdHoLaTbY</t>
+  </si>
+  <si>
+    <t>DyGdHoLaTbY</t>
+  </si>
+  <si>
+    <t>DyErGdHoLuScTbY</t>
+  </si>
+  <si>
+    <t>strong O contamination concentrated in the grain boundaries</t>
+  </si>
+  <si>
+    <t>strong O contamination concentrated in the FCC (around 50% O)</t>
   </si>
 </sst>
 </file>
@@ -2184,7 +2202,7 @@
   <dimension ref="A1:T430"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A155" zoomScale="99" workbookViewId="0">
-      <selection activeCell="O178" sqref="O178"/>
+      <selection activeCell="H191" sqref="H191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8855,147 +8873,327 @@
     </row>
     <row r="177" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="24"/>
-      <c r="B177" s="44"/>
-      <c r="C177" s="42"/>
-      <c r="D177" s="42"/>
-      <c r="E177" s="44"/>
-      <c r="F177" s="42"/>
-      <c r="G177" s="42"/>
+      <c r="B177" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="C177" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D177" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E177" s="44" t="s">
+        <v>291</v>
+      </c>
+      <c r="F177" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="G177" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H177" s="42"/>
       <c r="I177" s="3"/>
-      <c r="J177" s="4"/>
+      <c r="J177" s="4">
+        <v>245000000</v>
+      </c>
       <c r="K177" s="4"/>
-      <c r="L177" s="44"/>
-      <c r="M177" s="44"/>
-      <c r="N177" s="44"/>
+      <c r="L177" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M177" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N177" s="44" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="178" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="24"/>
-      <c r="B178" s="44"/>
-      <c r="C178" s="42"/>
-      <c r="D178" s="42"/>
-      <c r="E178" s="44"/>
-      <c r="F178" s="42"/>
-      <c r="G178" s="42"/>
+      <c r="B178" s="92" t="s">
+        <v>289</v>
+      </c>
+      <c r="C178" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="D178" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E178" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="F178" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="G178" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H178" s="42"/>
       <c r="I178" s="3"/>
-      <c r="J178" s="4"/>
+      <c r="J178" s="4">
+        <v>205000000</v>
+      </c>
       <c r="K178" s="4"/>
-      <c r="L178" s="44"/>
-      <c r="M178" s="44"/>
-      <c r="N178" s="44"/>
+      <c r="L178" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M178" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N178" s="44" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="179" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="24"/>
-      <c r="B179" s="44"/>
-      <c r="C179" s="42"/>
-      <c r="D179" s="42"/>
-      <c r="E179" s="44"/>
-      <c r="F179" s="42"/>
-      <c r="G179" s="42"/>
+      <c r="B179" s="44" t="s">
+        <v>290</v>
+      </c>
+      <c r="C179" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="D179" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E179" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="F179" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="G179" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H179" s="42"/>
       <c r="I179" s="3"/>
-      <c r="J179" s="4"/>
+      <c r="J179" s="4">
+        <v>360000000</v>
+      </c>
       <c r="K179" s="4"/>
-      <c r="L179" s="44"/>
-      <c r="M179" s="44"/>
-      <c r="N179" s="44"/>
+      <c r="L179" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M179" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N179" s="44" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="180" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="24"/>
-      <c r="B180" s="44"/>
-      <c r="C180" s="42"/>
-      <c r="D180" s="42"/>
-      <c r="E180" s="44"/>
-      <c r="F180" s="42"/>
-      <c r="G180" s="42"/>
+      <c r="B180" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="C180" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D180" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E180" s="44" t="s">
+        <v>291</v>
+      </c>
+      <c r="F180" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G180" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H180" s="42"/>
       <c r="I180" s="3"/>
-      <c r="J180" s="4"/>
+      <c r="J180" s="4">
+        <v>869000000</v>
+      </c>
       <c r="K180" s="4"/>
-      <c r="L180" s="44"/>
-      <c r="M180" s="44"/>
-      <c r="N180" s="44"/>
+      <c r="L180" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M180" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N180" s="44" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="181" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="24"/>
-      <c r="B181" s="44"/>
-      <c r="C181" s="42"/>
-      <c r="D181" s="42"/>
-      <c r="E181" s="44"/>
-      <c r="F181" s="42"/>
-      <c r="G181" s="42"/>
+      <c r="B181" s="92" t="s">
+        <v>289</v>
+      </c>
+      <c r="C181" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="D181" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E181" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="F181" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G181" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H181" s="42"/>
       <c r="I181" s="3"/>
-      <c r="J181" s="4"/>
+      <c r="J181" s="4">
+        <v>863000000</v>
+      </c>
       <c r="K181" s="4"/>
-      <c r="L181" s="44"/>
-      <c r="M181" s="44"/>
-      <c r="N181" s="44"/>
+      <c r="L181" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M181" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N181" s="44" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="182" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="24"/>
-      <c r="B182" s="44"/>
-      <c r="C182" s="42"/>
-      <c r="D182" s="42"/>
-      <c r="E182" s="44"/>
-      <c r="F182" s="42"/>
-      <c r="G182" s="42"/>
+      <c r="B182" s="44" t="s">
+        <v>290</v>
+      </c>
+      <c r="C182" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="D182" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E182" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="F182" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G182" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H182" s="42"/>
       <c r="I182" s="3"/>
-      <c r="J182" s="4"/>
+      <c r="J182" s="4">
+        <v>850000000</v>
+      </c>
       <c r="K182" s="4"/>
-      <c r="L182" s="44"/>
-      <c r="M182" s="44"/>
-      <c r="N182" s="44"/>
+      <c r="L182" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M182" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N182" s="44" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="183" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="24"/>
-      <c r="B183" s="44"/>
-      <c r="C183" s="42"/>
-      <c r="D183" s="42"/>
-      <c r="E183" s="44"/>
-      <c r="F183" s="42"/>
-      <c r="G183" s="42"/>
+      <c r="B183" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="C183" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D183" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E183" s="44" t="s">
+        <v>291</v>
+      </c>
+      <c r="F183" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G183" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H183" s="42"/>
       <c r="I183" s="3"/>
-      <c r="J183" s="4"/>
+      <c r="J183" s="4">
+        <v>17</v>
+      </c>
       <c r="K183" s="4"/>
-      <c r="L183" s="44"/>
-      <c r="M183" s="44"/>
-      <c r="N183" s="44"/>
+      <c r="L183" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M183" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N183" s="44" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="184" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="24"/>
-      <c r="B184" s="44"/>
-      <c r="C184" s="42"/>
-      <c r="D184" s="42"/>
-      <c r="E184" s="44"/>
-      <c r="F184" s="42"/>
-      <c r="G184" s="42"/>
+      <c r="B184" s="92" t="s">
+        <v>289</v>
+      </c>
+      <c r="C184" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="D184" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E184" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="F184" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G184" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H184" s="42"/>
       <c r="I184" s="3"/>
-      <c r="J184" s="4"/>
+      <c r="J184" s="4">
+        <v>20</v>
+      </c>
       <c r="K184" s="4"/>
-      <c r="L184" s="44"/>
-      <c r="M184" s="44"/>
-      <c r="N184" s="44"/>
+      <c r="L184" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M184" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N184" s="44" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="185" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="24"/>
-      <c r="B185" s="44"/>
-      <c r="C185" s="42"/>
-      <c r="D185" s="42"/>
-      <c r="E185" s="44"/>
-      <c r="F185" s="42"/>
-      <c r="G185" s="42"/>
+      <c r="B185" s="44" t="s">
+        <v>290</v>
+      </c>
+      <c r="C185" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="D185" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E185" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="F185" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G185" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H185" s="42"/>
       <c r="I185" s="3"/>
-      <c r="J185" s="4"/>
+      <c r="J185" s="4">
+        <v>27</v>
+      </c>
       <c r="K185" s="4"/>
-      <c r="L185" s="44"/>
-      <c r="M185" s="44"/>
-      <c r="N185" s="44"/>
+      <c r="L185" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M185" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N185" s="44" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="186" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="24"/>

</xml_diff>

<commit_message>
- extracted data from  `10.1063/1.4813688`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5584F65F-7008-E647-BEC1-8908E8FA17AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9380CA-23DA-6F45-B4BD-49B9F4128F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="298">
   <si>
     <t>Metadata</t>
   </si>
@@ -1004,6 +1004,21 @@
   </si>
   <si>
     <t>strong O contamination concentrated in the FCC (around 50% O)</t>
+  </si>
+  <si>
+    <t>10.1063/1.4813688</t>
+  </si>
+  <si>
+    <t>Ag0.5CoCrCuFeNi</t>
+  </si>
+  <si>
+    <t>compression at a rate of 4e-4/s</t>
+  </si>
+  <si>
+    <t>in liquid nitrogen</t>
+  </si>
+  <si>
+    <t>in helium vapor</t>
   </si>
 </sst>
 </file>
@@ -2201,8 +2216,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="99" workbookViewId="0">
-      <selection activeCell="H191" sqref="H191"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="99" workbookViewId="0">
+      <selection activeCell="L193" sqref="L193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8892,7 +8907,9 @@
         <v>29</v>
       </c>
       <c r="H177" s="42"/>
-      <c r="I177" s="3"/>
+      <c r="I177" s="3">
+        <v>298</v>
+      </c>
       <c r="J177" s="4">
         <v>245000000</v>
       </c>
@@ -8928,7 +8945,9 @@
         <v>29</v>
       </c>
       <c r="H178" s="42"/>
-      <c r="I178" s="3"/>
+      <c r="I178" s="3">
+        <v>298</v>
+      </c>
       <c r="J178" s="4">
         <v>205000000</v>
       </c>
@@ -8964,7 +8983,9 @@
         <v>29</v>
       </c>
       <c r="H179" s="42"/>
-      <c r="I179" s="3"/>
+      <c r="I179" s="3">
+        <v>298</v>
+      </c>
       <c r="J179" s="4">
         <v>360000000</v>
       </c>
@@ -9000,7 +9021,9 @@
         <v>29</v>
       </c>
       <c r="H180" s="42"/>
-      <c r="I180" s="3"/>
+      <c r="I180" s="3">
+        <v>298</v>
+      </c>
       <c r="J180" s="4">
         <v>869000000</v>
       </c>
@@ -9036,7 +9059,9 @@
         <v>29</v>
       </c>
       <c r="H181" s="42"/>
-      <c r="I181" s="3"/>
+      <c r="I181" s="3">
+        <v>298</v>
+      </c>
       <c r="J181" s="4">
         <v>863000000</v>
       </c>
@@ -9072,7 +9097,9 @@
         <v>29</v>
       </c>
       <c r="H182" s="42"/>
-      <c r="I182" s="3"/>
+      <c r="I182" s="3">
+        <v>298</v>
+      </c>
       <c r="J182" s="4">
         <v>850000000</v>
       </c>
@@ -9108,7 +9135,9 @@
         <v>29</v>
       </c>
       <c r="H183" s="42"/>
-      <c r="I183" s="3"/>
+      <c r="I183" s="3">
+        <v>298</v>
+      </c>
       <c r="J183" s="4">
         <v>17</v>
       </c>
@@ -9144,7 +9173,9 @@
         <v>29</v>
       </c>
       <c r="H184" s="42"/>
-      <c r="I184" s="3"/>
+      <c r="I184" s="3">
+        <v>298</v>
+      </c>
       <c r="J184" s="4">
         <v>20</v>
       </c>
@@ -9180,7 +9211,9 @@
         <v>29</v>
       </c>
       <c r="H185" s="42"/>
-      <c r="I185" s="3"/>
+      <c r="I185" s="3">
+        <v>298</v>
+      </c>
       <c r="J185" s="4">
         <v>27</v>
       </c>
@@ -9197,51 +9230,121 @@
     </row>
     <row r="186" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="24"/>
-      <c r="B186" s="44"/>
+      <c r="B186" s="44" t="s">
+        <v>294</v>
+      </c>
       <c r="C186" s="42"/>
-      <c r="D186" s="42"/>
+      <c r="D186" s="42" t="s">
+        <v>89</v>
+      </c>
       <c r="E186" s="44"/>
-      <c r="F186" s="42"/>
-      <c r="G186" s="42"/>
-      <c r="H186" s="42"/>
-      <c r="I186" s="3"/>
-      <c r="J186" s="4"/>
-      <c r="K186" s="4"/>
-      <c r="L186" s="44"/>
-      <c r="M186" s="44"/>
-      <c r="N186" s="44"/>
+      <c r="F186" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="G186" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H186" s="42" t="s">
+        <v>295</v>
+      </c>
+      <c r="I186" s="3">
+        <v>300</v>
+      </c>
+      <c r="J186" s="4">
+        <v>450000000</v>
+      </c>
+      <c r="K186" s="4">
+        <v>40000000</v>
+      </c>
+      <c r="L186" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M186" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="N186" s="44" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="187" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="24"/>
-      <c r="B187" s="44"/>
+      <c r="B187" s="44" t="s">
+        <v>294</v>
+      </c>
       <c r="C187" s="42"/>
-      <c r="D187" s="42"/>
-      <c r="E187" s="44"/>
-      <c r="F187" s="42"/>
-      <c r="G187" s="42"/>
-      <c r="H187" s="42"/>
-      <c r="I187" s="3"/>
-      <c r="J187" s="4"/>
-      <c r="K187" s="4"/>
-      <c r="L187" s="44"/>
-      <c r="M187" s="44"/>
-      <c r="N187" s="44"/>
+      <c r="D187" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E187" s="44" t="s">
+        <v>296</v>
+      </c>
+      <c r="F187" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="G187" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H187" s="42" t="s">
+        <v>295</v>
+      </c>
+      <c r="I187" s="3">
+        <v>177</v>
+      </c>
+      <c r="J187" s="4">
+        <v>530000000</v>
+      </c>
+      <c r="K187" s="4">
+        <v>20000000</v>
+      </c>
+      <c r="L187" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M187" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="N187" s="44" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="188" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="24"/>
-      <c r="B188" s="44"/>
+      <c r="B188" s="44" t="s">
+        <v>294</v>
+      </c>
       <c r="C188" s="42"/>
-      <c r="D188" s="42"/>
-      <c r="E188" s="44"/>
-      <c r="F188" s="42"/>
-      <c r="G188" s="42"/>
-      <c r="H188" s="42"/>
-      <c r="I188" s="3"/>
-      <c r="J188" s="4"/>
-      <c r="K188" s="4"/>
-      <c r="L188" s="44"/>
-      <c r="M188" s="44"/>
-      <c r="N188" s="44"/>
+      <c r="D188" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E188" s="44" t="s">
+        <v>297</v>
+      </c>
+      <c r="F188" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="G188" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H188" s="42" t="s">
+        <v>295</v>
+      </c>
+      <c r="I188" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="J188" s="4">
+        <v>750000000</v>
+      </c>
+      <c r="K188" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="L188" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M188" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="N188" s="44" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="189" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="24"/>

</xml_diff>

<commit_message>
- extracted data from  `10.1016/j.intermet.2018.10.014`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9380CA-23DA-6F45-B4BD-49B9F4128F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B7D1A1-408B-E148-87D6-A65D8B9C9F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="301">
   <si>
     <t>Metadata</t>
   </si>
@@ -1019,6 +1019,15 @@
   </si>
   <si>
     <t>in helium vapor</t>
+  </si>
+  <si>
+    <t>Gd Tb Dy Ho Lu</t>
+  </si>
+  <si>
+    <t>levitation melting in argon</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2018.10.014</t>
   </si>
 </sst>
 </file>
@@ -2216,8 +2225,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="99" workbookViewId="0">
-      <selection activeCell="L193" sqref="L193"/>
+    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="99" workbookViewId="0">
+      <selection activeCell="N195" sqref="N195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9348,67 +9357,153 @@
     </row>
     <row r="189" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="24"/>
-      <c r="B189" s="44"/>
-      <c r="C189" s="42"/>
-      <c r="D189" s="42"/>
-      <c r="E189" s="44"/>
-      <c r="F189" s="42"/>
-      <c r="G189" s="42"/>
+      <c r="B189" s="44" t="s">
+        <v>298</v>
+      </c>
+      <c r="C189" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D189" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="E189" s="44" t="s">
+        <v>299</v>
+      </c>
+      <c r="F189" s="42" t="s">
+        <v>280</v>
+      </c>
+      <c r="G189" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H189" s="42"/>
       <c r="I189" s="3"/>
-      <c r="J189" s="4"/>
+      <c r="J189" s="4">
+        <v>174</v>
+      </c>
       <c r="K189" s="4"/>
-      <c r="L189" s="44"/>
-      <c r="M189" s="44"/>
-      <c r="N189" s="44"/>
+      <c r="L189" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="M189" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="N189" s="44" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="190" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="24"/>
-      <c r="B190" s="44"/>
-      <c r="C190" s="42"/>
-      <c r="D190" s="42"/>
-      <c r="E190" s="44"/>
-      <c r="F190" s="42"/>
-      <c r="G190" s="42"/>
+      <c r="B190" s="44" t="s">
+        <v>298</v>
+      </c>
+      <c r="C190" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D190" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="E190" s="44" t="s">
+        <v>299</v>
+      </c>
+      <c r="F190" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="G190" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H190" s="42"/>
-      <c r="I190" s="3"/>
-      <c r="J190" s="4"/>
+      <c r="I190" s="3">
+        <v>2</v>
+      </c>
+      <c r="J190" s="4">
+        <v>4.7E-7</v>
+      </c>
       <c r="K190" s="4"/>
-      <c r="L190" s="44"/>
-      <c r="M190" s="44"/>
-      <c r="N190" s="44"/>
+      <c r="L190" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M190" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="N190" s="44" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="191" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="24"/>
-      <c r="B191" s="44"/>
-      <c r="C191" s="42"/>
-      <c r="D191" s="42"/>
-      <c r="E191" s="44"/>
-      <c r="F191" s="42"/>
-      <c r="G191" s="42"/>
+      <c r="B191" s="44" t="s">
+        <v>298</v>
+      </c>
+      <c r="C191" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D191" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="E191" s="44" t="s">
+        <v>299</v>
+      </c>
+      <c r="F191" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="G191" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H191" s="42"/>
-      <c r="I191" s="3"/>
-      <c r="J191" s="4"/>
+      <c r="I191" s="3">
+        <v>300</v>
+      </c>
+      <c r="J191" s="4">
+        <v>1.19E-6</v>
+      </c>
       <c r="K191" s="4"/>
-      <c r="L191" s="44"/>
-      <c r="M191" s="44"/>
-      <c r="N191" s="44"/>
+      <c r="L191" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M191" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="N191" s="44" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="192" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="24"/>
-      <c r="B192" s="44"/>
-      <c r="C192" s="42"/>
-      <c r="D192" s="42"/>
-      <c r="E192" s="44"/>
-      <c r="F192" s="42"/>
-      <c r="G192" s="42"/>
+      <c r="B192" s="44" t="s">
+        <v>298</v>
+      </c>
+      <c r="C192" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D192" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="E192" s="44" t="s">
+        <v>299</v>
+      </c>
+      <c r="F192" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="G192" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H192" s="42"/>
-      <c r="I192" s="3"/>
-      <c r="J192" s="4"/>
+      <c r="I192" s="3">
+        <v>2</v>
+      </c>
+      <c r="J192" s="4">
+        <v>0.23200000000000001</v>
+      </c>
       <c r="K192" s="4"/>
-      <c r="L192" s="44"/>
-      <c r="M192" s="44"/>
-      <c r="N192" s="44"/>
+      <c r="L192" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="M192" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="N192" s="44" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="193" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="24"/>

</xml_diff>

<commit_message>
- extracted data from  `10.1016/j.mtcomm.2024.111088`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B7D1A1-408B-E148-87D6-A65D8B9C9F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F7D1B0-71A3-8740-B869-0EAE46B943AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1851" uniqueCount="311">
   <si>
     <t>Metadata</t>
   </si>
@@ -1029,6 +1029,36 @@
   <si>
     <t>10.1016/j.intermet.2018.10.014</t>
   </si>
+  <si>
+    <t>NiMnCrMoW0.2</t>
+  </si>
+  <si>
+    <t>NiMnCrMoW0.4</t>
+  </si>
+  <si>
+    <t>NiMnCrMoW0.6</t>
+  </si>
+  <si>
+    <t>NiMnCrMoW0.8</t>
+  </si>
+  <si>
+    <t>NiMnCrMoW1.0</t>
+  </si>
+  <si>
+    <t>complex multi-phase structure in the reference if needed</t>
+  </si>
+  <si>
+    <t>UCS</t>
+  </si>
+  <si>
+    <t>annealed at 1473K for 2h; complex multi-phase structure in the reference if needed</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>10.1016/j.mtcomm.2024.111088</t>
+  </si>
 </sst>
 </file>
 
@@ -1038,7 +1068,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1125,6 +1155,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1639,7 +1676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1795,6 +1832,60 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1861,62 +1952,11 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2225,8 +2265,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="99" workbookViewId="0">
-      <selection activeCell="N195" sqref="N195"/>
+    <sheetView tabSelected="1" topLeftCell="D183" zoomScale="99" workbookViewId="0">
+      <selection activeCell="N220" sqref="N220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2275,19 +2315,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="61"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="79"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2298,17 +2338,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="65"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="83"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2337,43 +2377,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="68" t="s">
+      <c r="F5" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="71" t="s">
+      <c r="I5" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="73" t="s">
+      <c r="J5" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="73" t="s">
+      <c r="K5" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="68" t="s">
+      <c r="L5" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="68" t="s">
+      <c r="M5" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="68" t="s">
+      <c r="N5" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="75" t="s">
+      <c r="O5" s="54" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2384,19 +2424,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="76"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="92"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85"/>
+      <c r="O6" s="55"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
@@ -2441,7 +2481,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="77"/>
+      <c r="O7" s="56"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2454,35 +2494,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="81" t="s">
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="86" t="s">
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="87"/>
+      <c r="N8" s="66"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="88" t="s">
+      <c r="P8" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="89"/>
-      <c r="R8" s="90"/>
-      <c r="S8" s="90"/>
-      <c r="T8" s="91"/>
+      <c r="Q8" s="68"/>
+      <c r="R8" s="69"/>
+      <c r="S8" s="69"/>
+      <c r="T8" s="70"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
@@ -8457,7 +8497,7 @@
       </c>
     </row>
     <row r="164" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B164" s="92" t="s">
+      <c r="B164" s="44" t="s">
         <v>272</v>
       </c>
       <c r="C164" s="48" t="s">
@@ -8466,7 +8506,7 @@
       <c r="D164" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="E164" s="93" t="s">
+      <c r="E164" s="53" t="s">
         <v>273</v>
       </c>
       <c r="F164" s="48" t="s">
@@ -8496,7 +8536,7 @@
       </c>
     </row>
     <row r="165" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B165" s="92" t="s">
+      <c r="B165" s="44" t="s">
         <v>276</v>
       </c>
       <c r="C165" s="48" t="s">
@@ -8525,7 +8565,7 @@
       </c>
     </row>
     <row r="166" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B166" s="92" t="s">
+      <c r="B166" s="44" t="s">
         <v>277</v>
       </c>
       <c r="C166" s="48" t="s">
@@ -8623,7 +8663,7 @@
     </row>
     <row r="169" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="24"/>
-      <c r="B169" s="92" t="s">
+      <c r="B169" s="44" t="s">
         <v>276</v>
       </c>
       <c r="C169" s="48" t="s">
@@ -8656,7 +8696,7 @@
     </row>
     <row r="170" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="24"/>
-      <c r="B170" s="92" t="s">
+      <c r="B170" s="44" t="s">
         <v>277</v>
       </c>
       <c r="C170" s="48" t="s">
@@ -8935,7 +8975,7 @@
     </row>
     <row r="178" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="24"/>
-      <c r="B178" s="92" t="s">
+      <c r="B178" s="44" t="s">
         <v>289</v>
       </c>
       <c r="C178" s="42" t="s">
@@ -9049,7 +9089,7 @@
     </row>
     <row r="181" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="24"/>
-      <c r="B181" s="92" t="s">
+      <c r="B181" s="44" t="s">
         <v>289</v>
       </c>
       <c r="C181" s="42" t="s">
@@ -9163,7 +9203,7 @@
     </row>
     <row r="184" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="24"/>
-      <c r="B184" s="92" t="s">
+      <c r="B184" s="44" t="s">
         <v>289</v>
       </c>
       <c r="C184" s="42" t="s">
@@ -9505,327 +9545,767 @@
         <v>300</v>
       </c>
     </row>
-    <row r="193" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="24"/>
-      <c r="B193" s="44"/>
+      <c r="B193" s="44" t="s">
+        <v>301</v>
+      </c>
       <c r="C193" s="42"/>
-      <c r="D193" s="42"/>
-      <c r="E193" s="44"/>
-      <c r="F193" s="42"/>
-      <c r="G193" s="42"/>
+      <c r="D193" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E193" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="F193" s="42" t="s">
+        <v>307</v>
+      </c>
+      <c r="G193" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H193" s="42"/>
-      <c r="I193" s="3"/>
-      <c r="J193" s="4"/>
+      <c r="I193" s="3">
+        <v>298</v>
+      </c>
+      <c r="J193" s="4">
+        <v>1524000000</v>
+      </c>
       <c r="K193" s="4"/>
-      <c r="L193" s="44"/>
-      <c r="M193" s="44"/>
-      <c r="N193" s="44"/>
-    </row>
-    <row r="194" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L193" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M193" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N193" s="44" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="194" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="24"/>
-      <c r="B194" s="44"/>
+      <c r="B194" s="44" t="s">
+        <v>302</v>
+      </c>
       <c r="C194" s="42"/>
-      <c r="D194" s="42"/>
-      <c r="E194" s="44"/>
-      <c r="F194" s="42"/>
-      <c r="G194" s="42"/>
+      <c r="D194" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E194" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="F194" s="42" t="s">
+        <v>307</v>
+      </c>
+      <c r="G194" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H194" s="42"/>
-      <c r="I194" s="3"/>
-      <c r="J194" s="4"/>
+      <c r="I194" s="3">
+        <v>298</v>
+      </c>
+      <c r="J194" s="4">
+        <v>1608000000</v>
+      </c>
       <c r="K194" s="4"/>
-      <c r="L194" s="44"/>
-      <c r="M194" s="44"/>
-      <c r="N194" s="44"/>
-    </row>
-    <row r="195" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L194" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M194" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N194" s="44" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="195" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="24"/>
-      <c r="B195" s="44"/>
+      <c r="B195" s="44" t="s">
+        <v>303</v>
+      </c>
       <c r="C195" s="42"/>
-      <c r="D195" s="42"/>
-      <c r="E195" s="44"/>
-      <c r="F195" s="42"/>
-      <c r="G195" s="42"/>
+      <c r="D195" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E195" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="F195" s="42" t="s">
+        <v>307</v>
+      </c>
+      <c r="G195" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H195" s="42"/>
-      <c r="I195" s="3"/>
-      <c r="J195" s="4"/>
+      <c r="I195" s="3">
+        <v>298</v>
+      </c>
+      <c r="J195" s="4">
+        <v>1617000000</v>
+      </c>
       <c r="K195" s="4"/>
-      <c r="L195" s="44"/>
-      <c r="M195" s="44"/>
-      <c r="N195" s="44"/>
-    </row>
-    <row r="196" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L195" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M195" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N195" s="44" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="24"/>
-      <c r="B196" s="44"/>
+      <c r="B196" s="44" t="s">
+        <v>304</v>
+      </c>
       <c r="C196" s="42"/>
-      <c r="D196" s="42"/>
-      <c r="E196" s="44"/>
-      <c r="F196" s="42"/>
-      <c r="G196" s="42"/>
+      <c r="D196" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E196" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="F196" s="42" t="s">
+        <v>307</v>
+      </c>
+      <c r="G196" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H196" s="42"/>
-      <c r="I196" s="3"/>
-      <c r="J196" s="4"/>
+      <c r="I196" s="3">
+        <v>298</v>
+      </c>
+      <c r="J196" s="4">
+        <v>1240000000</v>
+      </c>
       <c r="K196" s="4"/>
-      <c r="L196" s="44"/>
-      <c r="M196" s="44"/>
-      <c r="N196" s="44"/>
-    </row>
-    <row r="197" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L196" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M196" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N196" s="44" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="197" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="24"/>
-      <c r="B197" s="44"/>
+      <c r="B197" s="44" t="s">
+        <v>305</v>
+      </c>
       <c r="C197" s="42"/>
-      <c r="D197" s="42"/>
-      <c r="E197" s="44"/>
-      <c r="F197" s="42"/>
-      <c r="G197" s="42"/>
+      <c r="D197" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E197" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="F197" s="42" t="s">
+        <v>307</v>
+      </c>
+      <c r="G197" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H197" s="42"/>
-      <c r="I197" s="3"/>
-      <c r="J197" s="4"/>
+      <c r="I197" s="3">
+        <v>298</v>
+      </c>
+      <c r="J197" s="4">
+        <v>1146000000</v>
+      </c>
       <c r="K197" s="4"/>
-      <c r="L197" s="44"/>
-      <c r="M197" s="44"/>
-      <c r="N197" s="44"/>
-    </row>
-    <row r="198" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L197" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M197" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N197" s="44" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="198" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="24"/>
-      <c r="B198" s="44"/>
+      <c r="B198" s="44" t="s">
+        <v>301</v>
+      </c>
       <c r="C198" s="42"/>
-      <c r="D198" s="42"/>
-      <c r="E198" s="44"/>
-      <c r="F198" s="42"/>
-      <c r="G198" s="42"/>
+      <c r="D198" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E198" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="F198" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G198" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H198" s="42"/>
-      <c r="I198" s="3"/>
-      <c r="J198" s="4"/>
+      <c r="I198" s="3">
+        <v>298</v>
+      </c>
+      <c r="J198" s="4">
+        <v>19.21</v>
+      </c>
       <c r="K198" s="4"/>
-      <c r="L198" s="44"/>
-      <c r="M198" s="44"/>
-      <c r="N198" s="44"/>
-    </row>
-    <row r="199" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L198" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M198" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N198" s="44" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="199" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="24"/>
-      <c r="B199" s="44"/>
+      <c r="B199" s="44" t="s">
+        <v>302</v>
+      </c>
       <c r="C199" s="42"/>
-      <c r="D199" s="42"/>
-      <c r="E199" s="44"/>
-      <c r="F199" s="42"/>
-      <c r="G199" s="42"/>
+      <c r="D199" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E199" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="F199" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G199" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H199" s="42"/>
-      <c r="I199" s="3"/>
-      <c r="J199" s="4"/>
+      <c r="I199" s="3">
+        <v>298</v>
+      </c>
+      <c r="J199" s="4">
+        <v>17.38</v>
+      </c>
       <c r="K199" s="4"/>
-      <c r="L199" s="44"/>
-      <c r="M199" s="44"/>
-      <c r="N199" s="44"/>
-    </row>
-    <row r="200" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L199" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M199" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N199" s="44" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="200" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="24"/>
-      <c r="B200" s="44"/>
+      <c r="B200" s="44" t="s">
+        <v>303</v>
+      </c>
       <c r="C200" s="42"/>
-      <c r="D200" s="42"/>
-      <c r="E200" s="44"/>
-      <c r="F200" s="42"/>
-      <c r="G200" s="42"/>
+      <c r="D200" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E200" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="F200" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G200" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H200" s="42"/>
-      <c r="I200" s="3"/>
-      <c r="J200" s="4"/>
+      <c r="I200" s="3">
+        <v>298</v>
+      </c>
+      <c r="J200" s="4">
+        <v>9.6999999999999993</v>
+      </c>
       <c r="K200" s="4"/>
-      <c r="L200" s="44"/>
-      <c r="M200" s="44"/>
-      <c r="N200" s="44"/>
-    </row>
-    <row r="201" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L200" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M200" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N200" s="44" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="201" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="24"/>
-      <c r="B201" s="44"/>
+      <c r="B201" s="44" t="s">
+        <v>304</v>
+      </c>
       <c r="C201" s="42"/>
-      <c r="D201" s="42"/>
-      <c r="E201" s="44"/>
-      <c r="F201" s="42"/>
-      <c r="G201" s="42"/>
+      <c r="D201" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E201" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="F201" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G201" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H201" s="42"/>
-      <c r="I201" s="3"/>
-      <c r="J201" s="4"/>
+      <c r="I201" s="3">
+        <v>298</v>
+      </c>
+      <c r="J201" s="4">
+        <v>6.64</v>
+      </c>
       <c r="K201" s="4"/>
-      <c r="L201" s="44"/>
-      <c r="M201" s="44"/>
-      <c r="N201" s="44"/>
-    </row>
-    <row r="202" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L201" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M201" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N201" s="44" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="202" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="24"/>
-      <c r="B202" s="44"/>
+      <c r="B202" s="44" t="s">
+        <v>305</v>
+      </c>
       <c r="C202" s="42"/>
-      <c r="D202" s="42"/>
-      <c r="E202" s="44"/>
-      <c r="F202" s="42"/>
-      <c r="G202" s="42"/>
+      <c r="D202" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E202" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="F202" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G202" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H202" s="42"/>
-      <c r="I202" s="3"/>
-      <c r="J202" s="4"/>
+      <c r="I202" s="3">
+        <v>298</v>
+      </c>
+      <c r="J202" s="4">
+        <v>6.08</v>
+      </c>
       <c r="K202" s="4"/>
-      <c r="L202" s="44"/>
-      <c r="M202" s="44"/>
-      <c r="N202" s="44"/>
-    </row>
-    <row r="203" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L202" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M202" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N202" s="44" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="203" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="24"/>
-      <c r="B203" s="44"/>
+      <c r="B203" s="44" t="s">
+        <v>301</v>
+      </c>
       <c r="C203" s="42"/>
-      <c r="D203" s="42"/>
-      <c r="E203" s="44"/>
-      <c r="F203" s="42"/>
-      <c r="G203" s="42"/>
+      <c r="D203" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E203" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="F203" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G203" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H203" s="42"/>
-      <c r="I203" s="3"/>
-      <c r="J203" s="4"/>
+      <c r="I203" s="3">
+        <v>298</v>
+      </c>
+      <c r="J203" s="50">
+        <f>P203*9807000</f>
+        <v>5972463000</v>
+      </c>
       <c r="K203" s="4"/>
-      <c r="L203" s="44"/>
-      <c r="M203" s="44"/>
-      <c r="N203" s="44"/>
-    </row>
-    <row r="204" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L203" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M203" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="N203" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="P203" s="6">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="204" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="24"/>
-      <c r="B204" s="44"/>
+      <c r="B204" s="44" t="s">
+        <v>302</v>
+      </c>
       <c r="C204" s="42"/>
-      <c r="D204" s="42"/>
-      <c r="E204" s="44"/>
-      <c r="F204" s="42"/>
-      <c r="G204" s="42"/>
+      <c r="D204" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E204" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="F204" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G204" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H204" s="42"/>
-      <c r="I204" s="3"/>
-      <c r="J204" s="4"/>
+      <c r="I204" s="3">
+        <v>298</v>
+      </c>
+      <c r="J204" s="50">
+        <f t="shared" ref="J204:J212" si="5">P204*9807000</f>
+        <v>6247059000</v>
+      </c>
       <c r="K204" s="4"/>
-      <c r="L204" s="44"/>
-      <c r="M204" s="44"/>
-      <c r="N204" s="44"/>
-    </row>
-    <row r="205" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L204" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M204" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="N204" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="P204" s="6">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="24"/>
-      <c r="B205" s="44"/>
+      <c r="B205" s="44" t="s">
+        <v>303</v>
+      </c>
       <c r="C205" s="42"/>
-      <c r="D205" s="42"/>
-      <c r="E205" s="44"/>
-      <c r="F205" s="42"/>
-      <c r="G205" s="42"/>
+      <c r="D205" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E205" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="F205" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G205" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H205" s="42"/>
-      <c r="I205" s="3"/>
-      <c r="J205" s="4"/>
+      <c r="I205" s="3">
+        <v>298</v>
+      </c>
+      <c r="J205" s="50">
+        <f t="shared" si="5"/>
+        <v>6433392000</v>
+      </c>
       <c r="K205" s="4"/>
-      <c r="L205" s="44"/>
-      <c r="M205" s="44"/>
-      <c r="N205" s="44"/>
-    </row>
-    <row r="206" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L205" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M205" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="N205" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="P205" s="6">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="206" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="24"/>
-      <c r="B206" s="44"/>
+      <c r="B206" s="44" t="s">
+        <v>304</v>
+      </c>
       <c r="C206" s="42"/>
-      <c r="D206" s="42"/>
-      <c r="E206" s="44"/>
-      <c r="F206" s="42"/>
-      <c r="G206" s="42"/>
+      <c r="D206" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E206" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="F206" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G206" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H206" s="42"/>
-      <c r="I206" s="3"/>
-      <c r="J206" s="4"/>
+      <c r="I206" s="3">
+        <v>298</v>
+      </c>
+      <c r="J206" s="50">
+        <f t="shared" si="5"/>
+        <v>6217638000</v>
+      </c>
       <c r="K206" s="4"/>
-      <c r="L206" s="44"/>
-      <c r="M206" s="44"/>
-      <c r="N206" s="44"/>
-    </row>
-    <row r="207" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L206" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M206" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="N206" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="P206" s="6">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="207" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="24"/>
-      <c r="B207" s="44"/>
+      <c r="B207" s="44" t="s">
+        <v>305</v>
+      </c>
       <c r="C207" s="42"/>
-      <c r="D207" s="42"/>
-      <c r="E207" s="44"/>
-      <c r="F207" s="42"/>
-      <c r="G207" s="42"/>
+      <c r="D207" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E207" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="F207" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G207" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H207" s="42"/>
-      <c r="I207" s="3"/>
-      <c r="J207" s="4"/>
+      <c r="I207" s="3">
+        <v>298</v>
+      </c>
+      <c r="J207" s="50">
+        <f t="shared" si="5"/>
+        <v>5923428000</v>
+      </c>
       <c r="K207" s="4"/>
-      <c r="L207" s="44"/>
-      <c r="M207" s="44"/>
-      <c r="N207" s="44"/>
-    </row>
-    <row r="208" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L207" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M207" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="N207" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="P207" s="6">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="208" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="24"/>
-      <c r="B208" s="44"/>
-      <c r="C208" s="42"/>
-      <c r="D208" s="42"/>
-      <c r="E208" s="44"/>
-      <c r="F208" s="42"/>
-      <c r="G208" s="42"/>
+      <c r="B208" s="93" t="s">
+        <v>301</v>
+      </c>
+      <c r="C208" s="94"/>
+      <c r="D208" s="94" t="s">
+        <v>158</v>
+      </c>
+      <c r="E208" s="93" t="s">
+        <v>308</v>
+      </c>
+      <c r="F208" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G208" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H208" s="42"/>
-      <c r="I208" s="3"/>
-      <c r="J208" s="4"/>
+      <c r="I208" s="3">
+        <v>298</v>
+      </c>
+      <c r="J208" s="50">
+        <f t="shared" si="5"/>
+        <v>7100268000</v>
+      </c>
       <c r="K208" s="4"/>
-      <c r="L208" s="44"/>
-      <c r="M208" s="44"/>
-      <c r="N208" s="44"/>
-    </row>
-    <row r="209" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L208" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M208" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="N208" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="P208" s="6">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="209" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="24"/>
-      <c r="B209" s="44"/>
-      <c r="C209" s="42"/>
-      <c r="D209" s="42"/>
-      <c r="E209" s="44"/>
-      <c r="F209" s="42"/>
-      <c r="G209" s="42"/>
+      <c r="B209" s="93" t="s">
+        <v>302</v>
+      </c>
+      <c r="C209" s="94"/>
+      <c r="D209" s="94" t="s">
+        <v>158</v>
+      </c>
+      <c r="E209" s="93" t="s">
+        <v>308</v>
+      </c>
+      <c r="F209" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G209" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H209" s="42"/>
-      <c r="I209" s="3"/>
-      <c r="J209" s="4"/>
+      <c r="I209" s="3">
+        <v>298</v>
+      </c>
+      <c r="J209" s="50">
+        <f t="shared" si="5"/>
+        <v>7247373000</v>
+      </c>
       <c r="K209" s="4"/>
-      <c r="L209" s="44"/>
-      <c r="M209" s="44"/>
-      <c r="N209" s="44"/>
-    </row>
-    <row r="210" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L209" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M209" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="N209" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="P209" s="6">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="210" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="24"/>
-      <c r="B210" s="44"/>
-      <c r="C210" s="42"/>
-      <c r="D210" s="42"/>
-      <c r="E210" s="44"/>
-      <c r="F210" s="42"/>
-      <c r="G210" s="42"/>
+      <c r="B210" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="C210" s="94"/>
+      <c r="D210" s="94" t="s">
+        <v>158</v>
+      </c>
+      <c r="E210" s="93" t="s">
+        <v>308</v>
+      </c>
+      <c r="F210" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G210" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H210" s="42"/>
-      <c r="I210" s="3"/>
-      <c r="J210" s="4"/>
+      <c r="I210" s="3">
+        <v>298</v>
+      </c>
+      <c r="J210" s="50">
+        <f t="shared" si="5"/>
+        <v>7266987000</v>
+      </c>
       <c r="K210" s="4"/>
-      <c r="L210" s="44"/>
-      <c r="M210" s="44"/>
-      <c r="N210" s="44"/>
-    </row>
-    <row r="211" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L210" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M210" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="N210" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="P210" s="6">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="211" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="24"/>
-      <c r="B211" s="44"/>
-      <c r="C211" s="42"/>
-      <c r="D211" s="42"/>
-      <c r="E211" s="44"/>
-      <c r="F211" s="42"/>
-      <c r="G211" s="42"/>
+      <c r="B211" s="93" t="s">
+        <v>304</v>
+      </c>
+      <c r="C211" s="94"/>
+      <c r="D211" s="94" t="s">
+        <v>158</v>
+      </c>
+      <c r="E211" s="93" t="s">
+        <v>308</v>
+      </c>
+      <c r="F211" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G211" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H211" s="42"/>
-      <c r="I211" s="3"/>
-      <c r="J211" s="4"/>
+      <c r="I211" s="3">
+        <v>298</v>
+      </c>
+      <c r="J211" s="50">
+        <f t="shared" si="5"/>
+        <v>7139496000</v>
+      </c>
       <c r="K211" s="4"/>
-      <c r="L211" s="44"/>
-      <c r="M211" s="44"/>
-      <c r="N211" s="44"/>
-    </row>
-    <row r="212" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L211" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M211" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="N211" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="P211" s="6">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="212" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="24"/>
-      <c r="B212" s="44"/>
-      <c r="C212" s="42"/>
-      <c r="D212" s="42"/>
-      <c r="E212" s="44"/>
-      <c r="F212" s="42"/>
-      <c r="G212" s="42"/>
+      <c r="B212" s="93" t="s">
+        <v>305</v>
+      </c>
+      <c r="C212" s="94"/>
+      <c r="D212" s="94" t="s">
+        <v>158</v>
+      </c>
+      <c r="E212" s="93" t="s">
+        <v>308</v>
+      </c>
+      <c r="F212" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G212" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H212" s="42"/>
-      <c r="I212" s="3"/>
-      <c r="J212" s="4"/>
+      <c r="I212" s="3">
+        <v>298</v>
+      </c>
+      <c r="J212" s="50">
+        <f t="shared" si="5"/>
+        <v>6698181000</v>
+      </c>
       <c r="K212" s="4"/>
-      <c r="L212" s="44"/>
-      <c r="M212" s="44"/>
-      <c r="N212" s="44"/>
-    </row>
-    <row r="213" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L212" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M212" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="N212" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="P212" s="6">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="213" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="24"/>
       <c r="B213" s="44"/>
       <c r="C213" s="42"/>
@@ -9841,7 +10321,7 @@
       <c r="M213" s="44"/>
       <c r="N213" s="44"/>
     </row>
-    <row r="214" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="24"/>
       <c r="B214" s="44"/>
       <c r="C214" s="42"/>
@@ -9857,7 +10337,7 @@
       <c r="M214" s="44"/>
       <c r="N214" s="44"/>
     </row>
-    <row r="215" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="24"/>
       <c r="B215" s="44"/>
       <c r="C215" s="42"/>
@@ -9873,7 +10353,7 @@
       <c r="M215" s="44"/>
       <c r="N215" s="44"/>
     </row>
-    <row r="216" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="24"/>
       <c r="B216" s="44"/>
       <c r="C216" s="42"/>
@@ -9889,7 +10369,7 @@
       <c r="M216" s="44"/>
       <c r="N216" s="44"/>
     </row>
-    <row r="217" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="24"/>
       <c r="B217" s="44"/>
       <c r="C217" s="42"/>
@@ -9905,7 +10385,7 @@
       <c r="M217" s="44"/>
       <c r="N217" s="44"/>
     </row>
-    <row r="218" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="24"/>
       <c r="B218" s="44"/>
       <c r="C218" s="42"/>
@@ -9921,7 +10401,7 @@
       <c r="M218" s="44"/>
       <c r="N218" s="44"/>
     </row>
-    <row r="219" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="24"/>
       <c r="B219" s="44"/>
       <c r="C219" s="42"/>
@@ -9937,7 +10417,7 @@
       <c r="M219" s="44"/>
       <c r="N219" s="44"/>
     </row>
-    <row r="220" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="24"/>
       <c r="B220" s="44"/>
       <c r="C220" s="42"/>
@@ -9953,7 +10433,7 @@
       <c r="M220" s="44"/>
       <c r="N220" s="44"/>
     </row>
-    <row r="221" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="24"/>
       <c r="B221" s="44"/>
       <c r="C221" s="42"/>
@@ -9969,7 +10449,7 @@
       <c r="M221" s="44"/>
       <c r="N221" s="44"/>
     </row>
-    <row r="222" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="24"/>
       <c r="B222" s="44"/>
       <c r="C222" s="42"/>
@@ -9985,7 +10465,7 @@
       <c r="M222" s="44"/>
       <c r="N222" s="44"/>
     </row>
-    <row r="223" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="24"/>
       <c r="B223" s="44"/>
       <c r="C223" s="42"/>
@@ -10001,7 +10481,7 @@
       <c r="M223" s="44"/>
       <c r="N223" s="44"/>
     </row>
-    <row r="224" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="24"/>
       <c r="B224" s="44"/>
       <c r="C224" s="42"/>
@@ -12971,11 +13451,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -12990,6 +13465,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted data from  `10.1016/j.ijrmhm.2021.105568`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F7D1B0-71A3-8740-B869-0EAE46B943AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA21E03-96BD-A047-9717-08BCD895D980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1851" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="318">
   <si>
     <t>Metadata</t>
   </si>
@@ -1058,6 +1058,27 @@
   </si>
   <si>
     <t>10.1016/j.mtcomm.2024.111088</t>
+  </si>
+  <si>
+    <t>HfMoScTaZr</t>
+  </si>
+  <si>
+    <t>BCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quenched from 800*C </t>
+  </si>
+  <si>
+    <t xml:space="preserve">quenched from 1200*C </t>
+  </si>
+  <si>
+    <t>g / cm^3</t>
+  </si>
+  <si>
+    <t>minimum compressive ductility</t>
+  </si>
+  <si>
+    <t>10.1016/j.ijrmhm.2021.105568</t>
   </si>
 </sst>
 </file>
@@ -1676,7 +1697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1835,55 +1856,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1952,11 +1928,59 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2265,8 +2289,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D183" zoomScale="99" workbookViewId="0">
-      <selection activeCell="N220" sqref="N220"/>
+    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="99" workbookViewId="0">
+      <selection activeCell="N227" sqref="N227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2315,19 +2339,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="72"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="79"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="64"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2338,17 +2362,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="83"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="68"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2377,43 +2401,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="86" t="s">
+      <c r="D5" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="E5" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="86" t="s">
+      <c r="F5" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="86" t="s">
+      <c r="G5" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="87" t="s">
+      <c r="H5" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="89" t="s">
+      <c r="I5" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="91" t="s">
+      <c r="J5" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="91" t="s">
+      <c r="K5" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="86" t="s">
+      <c r="L5" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="86" t="s">
+      <c r="M5" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="86" t="s">
+      <c r="N5" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="54" t="s">
+      <c r="O5" s="78" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2424,19 +2448,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="85"/>
-      <c r="M6" s="85"/>
-      <c r="N6" s="85"/>
-      <c r="O6" s="55"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
+      <c r="O6" s="79"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
@@ -2481,7 +2505,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="56"/>
+      <c r="O7" s="80"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2494,35 +2518,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60" t="s">
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="63"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="65" t="s">
+      <c r="G8" s="85"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="66"/>
+      <c r="N8" s="90"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="67" t="s">
+      <c r="P8" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="68"/>
-      <c r="R8" s="69"/>
-      <c r="S8" s="69"/>
-      <c r="T8" s="70"/>
+      <c r="Q8" s="92"/>
+      <c r="R8" s="93"/>
+      <c r="S8" s="93"/>
+      <c r="T8" s="94"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
@@ -10107,14 +10131,14 @@
     </row>
     <row r="208" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="24"/>
-      <c r="B208" s="93" t="s">
+      <c r="B208" s="54" t="s">
         <v>301</v>
       </c>
-      <c r="C208" s="94"/>
-      <c r="D208" s="94" t="s">
+      <c r="C208" s="55"/>
+      <c r="D208" s="55" t="s">
         <v>158</v>
       </c>
-      <c r="E208" s="93" t="s">
+      <c r="E208" s="54" t="s">
         <v>308</v>
       </c>
       <c r="F208" s="42" t="s">
@@ -10147,14 +10171,14 @@
     </row>
     <row r="209" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="24"/>
-      <c r="B209" s="93" t="s">
+      <c r="B209" s="54" t="s">
         <v>302</v>
       </c>
-      <c r="C209" s="94"/>
-      <c r="D209" s="94" t="s">
+      <c r="C209" s="55"/>
+      <c r="D209" s="55" t="s">
         <v>158</v>
       </c>
-      <c r="E209" s="93" t="s">
+      <c r="E209" s="54" t="s">
         <v>308</v>
       </c>
       <c r="F209" s="42" t="s">
@@ -10187,14 +10211,14 @@
     </row>
     <row r="210" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="24"/>
-      <c r="B210" s="93" t="s">
+      <c r="B210" s="54" t="s">
         <v>303</v>
       </c>
-      <c r="C210" s="94"/>
-      <c r="D210" s="94" t="s">
+      <c r="C210" s="55"/>
+      <c r="D210" s="55" t="s">
         <v>158</v>
       </c>
-      <c r="E210" s="93" t="s">
+      <c r="E210" s="54" t="s">
         <v>308</v>
       </c>
       <c r="F210" s="42" t="s">
@@ -10227,14 +10251,14 @@
     </row>
     <row r="211" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="24"/>
-      <c r="B211" s="93" t="s">
+      <c r="B211" s="54" t="s">
         <v>304</v>
       </c>
-      <c r="C211" s="94"/>
-      <c r="D211" s="94" t="s">
+      <c r="C211" s="55"/>
+      <c r="D211" s="55" t="s">
         <v>158</v>
       </c>
-      <c r="E211" s="93" t="s">
+      <c r="E211" s="54" t="s">
         <v>308</v>
       </c>
       <c r="F211" s="42" t="s">
@@ -10267,14 +10291,14 @@
     </row>
     <row r="212" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="24"/>
-      <c r="B212" s="93" t="s">
+      <c r="B212" s="54" t="s">
         <v>305</v>
       </c>
-      <c r="C212" s="94"/>
-      <c r="D212" s="94" t="s">
+      <c r="C212" s="55"/>
+      <c r="D212" s="55" t="s">
         <v>158</v>
       </c>
-      <c r="E212" s="93" t="s">
+      <c r="E212" s="54" t="s">
         <v>308</v>
       </c>
       <c r="F212" s="42" t="s">
@@ -10307,10 +10331,18 @@
     </row>
     <row r="213" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="24"/>
-      <c r="B213" s="44"/>
-      <c r="C213" s="42"/>
-      <c r="D213" s="42"/>
-      <c r="E213" s="44"/>
+      <c r="B213" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="C213" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="D213" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="E213" s="44" t="s">
+        <v>313</v>
+      </c>
       <c r="F213" s="42"/>
       <c r="G213" s="42"/>
       <c r="H213" s="42"/>
@@ -10319,14 +10351,24 @@
       <c r="K213" s="4"/>
       <c r="L213" s="44"/>
       <c r="M213" s="44"/>
-      <c r="N213" s="44"/>
+      <c r="N213" s="95" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="214" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="24"/>
-      <c r="B214" s="44"/>
-      <c r="C214" s="42"/>
-      <c r="D214" s="42"/>
-      <c r="E214" s="44"/>
+      <c r="B214" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="C214" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="D214" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="E214" s="44" t="s">
+        <v>314</v>
+      </c>
       <c r="F214" s="42"/>
       <c r="G214" s="42"/>
       <c r="H214" s="42"/>
@@ -10335,167 +10377,372 @@
       <c r="K214" s="4"/>
       <c r="L214" s="44"/>
       <c r="M214" s="44"/>
-      <c r="N214" s="44"/>
+      <c r="N214" s="95" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="215" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="24"/>
-      <c r="B215" s="44"/>
-      <c r="C215" s="42"/>
-      <c r="D215" s="42"/>
+      <c r="B215" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="C215" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="D215" s="42" t="s">
+        <v>88</v>
+      </c>
       <c r="E215" s="44"/>
-      <c r="F215" s="42"/>
-      <c r="G215" s="42"/>
+      <c r="F215" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="G215" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H215" s="42"/>
-      <c r="I215" s="3"/>
-      <c r="J215" s="4"/>
+      <c r="I215" s="3">
+        <v>298</v>
+      </c>
+      <c r="J215" s="4">
+        <v>9.2799999999999994</v>
+      </c>
       <c r="K215" s="4"/>
-      <c r="L215" s="44"/>
+      <c r="L215" s="44" t="s">
+        <v>315</v>
+      </c>
       <c r="M215" s="44"/>
-      <c r="N215" s="44"/>
+      <c r="N215" s="95" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="216" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="24"/>
-      <c r="B216" s="44"/>
-      <c r="C216" s="42"/>
-      <c r="D216" s="42"/>
-      <c r="E216" s="44"/>
-      <c r="F216" s="42"/>
-      <c r="G216" s="42"/>
+      <c r="B216" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="C216" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="D216" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F216" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="G216" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H216" s="42"/>
-      <c r="I216" s="3"/>
-      <c r="J216" s="4"/>
+      <c r="I216" s="3">
+        <v>298</v>
+      </c>
+      <c r="J216" s="4">
+        <v>1778000000</v>
+      </c>
       <c r="K216" s="4"/>
-      <c r="L216" s="44"/>
-      <c r="M216" s="44"/>
-      <c r="N216" s="44"/>
+      <c r="L216" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M216" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N216" s="95" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="217" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="24"/>
-      <c r="B217" s="44"/>
-      <c r="C217" s="42"/>
-      <c r="D217" s="42"/>
+      <c r="B217" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="C217" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="D217" s="42" t="s">
+        <v>88</v>
+      </c>
       <c r="E217" s="44"/>
-      <c r="F217" s="42"/>
-      <c r="G217" s="42"/>
+      <c r="F217" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="G217" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H217" s="42"/>
-      <c r="I217" s="3"/>
-      <c r="J217" s="4"/>
+      <c r="I217" s="3">
+        <f>273+800</f>
+        <v>1073</v>
+      </c>
+      <c r="J217" s="4">
+        <v>1118000000</v>
+      </c>
       <c r="K217" s="4"/>
-      <c r="L217" s="44"/>
-      <c r="M217" s="44"/>
-      <c r="N217" s="44"/>
+      <c r="L217" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M217" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N217" s="95" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="218" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="24"/>
-      <c r="B218" s="44"/>
-      <c r="C218" s="42"/>
-      <c r="D218" s="42"/>
+      <c r="B218" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="C218" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="D218" s="42" t="s">
+        <v>88</v>
+      </c>
       <c r="E218" s="44"/>
-      <c r="F218" s="42"/>
-      <c r="G218" s="42"/>
+      <c r="F218" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="G218" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H218" s="42"/>
-      <c r="I218" s="3"/>
-      <c r="J218" s="4"/>
+      <c r="I218" s="3">
+        <f>273+1000</f>
+        <v>1273</v>
+      </c>
+      <c r="J218" s="4">
+        <v>963000000</v>
+      </c>
       <c r="K218" s="4"/>
-      <c r="L218" s="44"/>
-      <c r="M218" s="44"/>
-      <c r="N218" s="44"/>
+      <c r="L218" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M218" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N218" s="95" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="219" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="24"/>
-      <c r="B219" s="44"/>
-      <c r="C219" s="42"/>
-      <c r="D219" s="42"/>
+      <c r="B219" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="C219" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="D219" s="42" t="s">
+        <v>88</v>
+      </c>
       <c r="E219" s="44"/>
-      <c r="F219" s="42"/>
-      <c r="G219" s="42"/>
+      <c r="F219" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="G219" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H219" s="42"/>
-      <c r="I219" s="3"/>
-      <c r="J219" s="4"/>
+      <c r="I219" s="3">
+        <f>273+1200</f>
+        <v>1473</v>
+      </c>
+      <c r="J219" s="4">
+        <v>498000000</v>
+      </c>
       <c r="K219" s="4"/>
-      <c r="L219" s="44"/>
-      <c r="M219" s="44"/>
-      <c r="N219" s="44"/>
+      <c r="L219" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M219" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N219" s="95" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="220" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="24"/>
-      <c r="B220" s="44"/>
-      <c r="C220" s="42"/>
-      <c r="D220" s="42"/>
+      <c r="B220" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="C220" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="D220" s="42" t="s">
+        <v>88</v>
+      </c>
       <c r="E220" s="44"/>
-      <c r="F220" s="42"/>
-      <c r="G220" s="42"/>
+      <c r="F220" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G220" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H220" s="42"/>
-      <c r="I220" s="3"/>
-      <c r="J220" s="4"/>
+      <c r="I220" s="3">
+        <v>298</v>
+      </c>
+      <c r="J220" s="4">
+        <v>27</v>
+      </c>
       <c r="K220" s="4"/>
-      <c r="L220" s="44"/>
-      <c r="M220" s="44"/>
-      <c r="N220" s="44"/>
+      <c r="L220" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M220" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N220" s="95" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="221" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="24"/>
-      <c r="B221" s="44"/>
-      <c r="C221" s="42"/>
-      <c r="D221" s="42"/>
+      <c r="B221" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="C221" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="D221" s="42" t="s">
+        <v>88</v>
+      </c>
       <c r="E221" s="44"/>
-      <c r="F221" s="42"/>
-      <c r="G221" s="42"/>
+      <c r="F221" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G221" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H221" s="42"/>
-      <c r="I221" s="3"/>
-      <c r="J221" s="4"/>
+      <c r="I221" s="3">
+        <f>273+800</f>
+        <v>1073</v>
+      </c>
+      <c r="J221" s="4">
+        <v>35</v>
+      </c>
       <c r="K221" s="4"/>
-      <c r="L221" s="44"/>
-      <c r="M221" s="44"/>
-      <c r="N221" s="44"/>
+      <c r="L221" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M221" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N221" s="95" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="222" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="24"/>
-      <c r="B222" s="44"/>
-      <c r="C222" s="42"/>
-      <c r="D222" s="42"/>
+      <c r="B222" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="C222" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="D222" s="42" t="s">
+        <v>88</v>
+      </c>
       <c r="E222" s="44"/>
-      <c r="F222" s="42"/>
-      <c r="G222" s="42"/>
+      <c r="F222" s="42" t="s">
+        <v>316</v>
+      </c>
+      <c r="G222" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H222" s="42"/>
-      <c r="I222" s="3"/>
-      <c r="J222" s="4"/>
+      <c r="I222" s="3">
+        <f>273+1000</f>
+        <v>1273</v>
+      </c>
+      <c r="J222" s="4">
+        <v>42</v>
+      </c>
       <c r="K222" s="4"/>
-      <c r="L222" s="44"/>
-      <c r="M222" s="44"/>
-      <c r="N222" s="44"/>
+      <c r="L222" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M222" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N222" s="95" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="223" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="24"/>
-      <c r="B223" s="44"/>
-      <c r="C223" s="42"/>
-      <c r="D223" s="42"/>
+      <c r="B223" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="C223" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="D223" s="42" t="s">
+        <v>88</v>
+      </c>
       <c r="E223" s="44"/>
-      <c r="F223" s="42"/>
-      <c r="G223" s="42"/>
+      <c r="F223" s="42" t="s">
+        <v>316</v>
+      </c>
+      <c r="G223" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H223" s="42"/>
-      <c r="I223" s="3"/>
-      <c r="J223" s="4"/>
+      <c r="I223" s="3">
+        <f>273+1200</f>
+        <v>1473</v>
+      </c>
+      <c r="J223" s="4">
+        <v>42</v>
+      </c>
       <c r="K223" s="4"/>
-      <c r="L223" s="44"/>
-      <c r="M223" s="44"/>
-      <c r="N223" s="44"/>
+      <c r="L223" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M223" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N223" s="95" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="224" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="24"/>
-      <c r="B224" s="44"/>
-      <c r="C224" s="42"/>
-      <c r="D224" s="42"/>
+      <c r="B224" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="C224" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="D224" s="42" t="s">
+        <v>88</v>
+      </c>
       <c r="E224" s="44"/>
-      <c r="F224" s="42"/>
-      <c r="G224" s="42"/>
+      <c r="F224" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G224" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H224" s="42"/>
-      <c r="I224" s="3"/>
-      <c r="J224" s="4"/>
+      <c r="I224" s="3">
+        <v>298</v>
+      </c>
+      <c r="J224" s="4">
+        <v>9400000000</v>
+      </c>
       <c r="K224" s="4"/>
-      <c r="L224" s="44"/>
-      <c r="M224" s="44"/>
-      <c r="N224" s="44"/>
+      <c r="L224" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M224" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N224" s="95" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="225" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="24"/>
@@ -13451,6 +13698,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -13465,11 +13717,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted data from  `10.1007/s40843-018-9365-8`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA21E03-96BD-A047-9717-08BCD895D980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC92980E-E84C-5E44-9C87-72AC189799CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1958" uniqueCount="325">
   <si>
     <t>Metadata</t>
   </si>
@@ -1080,6 +1080,27 @@
   <si>
     <t>10.1016/j.ijrmhm.2021.105568</t>
   </si>
+  <si>
+    <t>Al Zn0.4 Li0.2 Mg0.2 Cu0.2</t>
+  </si>
+  <si>
+    <t>FCC+C14+C16</t>
+  </si>
+  <si>
+    <t>VIM+supergravity</t>
+  </si>
+  <si>
+    <t>VIM+A</t>
+  </si>
+  <si>
+    <t>remelted at 680*C and slowly cooled</t>
+  </si>
+  <si>
+    <t>remelted at 680*C with resistance heating and high gravity of 500g; centriguged in molten state for 5min; centrifuged during cooling for 5min</t>
+  </si>
+  <si>
+    <t>10.1007/s40843-018-9365-8</t>
+  </si>
 </sst>
 </file>
 
@@ -1089,7 +1110,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1186,6 +1207,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="-webkit-standard"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1862,6 +1888,57 @@
     <xf numFmtId="3" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1928,60 +2005,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2289,11 +2313,11 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="99" workbookViewId="0">
-      <selection activeCell="N227" sqref="N227"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="N236" sqref="N236"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.1640625" style="47" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.1640625" customWidth="1"/>
@@ -2315,7 +2339,7 @@
     <col min="19" max="20" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="21" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2331,7 +2355,7 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="23.25" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -2339,22 +2363,22 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="64"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="81"/>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="22.5" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
@@ -2362,20 +2386,20 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="68"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="85"/>
       <c r="O3" s="9"/>
     </row>
-    <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
@@ -2394,75 +2418,75 @@
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="28.5" customHeight="1">
       <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="71" t="s">
+      <c r="D5" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="71" t="s">
+      <c r="E5" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="71" t="s">
+      <c r="F5" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="71" t="s">
+      <c r="G5" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="72" t="s">
+      <c r="H5" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="74" t="s">
+      <c r="I5" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="76" t="s">
+      <c r="J5" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="76" t="s">
+      <c r="K5" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="71" t="s">
+      <c r="L5" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="71" t="s">
+      <c r="M5" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="71" t="s">
+      <c r="N5" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="78" t="s">
+      <c r="O5" s="56" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="28.5" customHeight="1">
       <c r="A6" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="70"/>
-      <c r="O6" s="79"/>
-    </row>
-    <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="90"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="87"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="57"/>
+    </row>
+    <row r="7" spans="1:20" ht="23.5" customHeight="1">
       <c r="A7" s="17" t="s">
         <v>23</v>
       </c>
@@ -2505,7 +2529,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="80"/>
+      <c r="O7" s="58"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2516,39 +2540,39 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="84" t="s">
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="86"/>
-      <c r="J8" s="87"/>
-      <c r="K8" s="87"/>
-      <c r="L8" s="88"/>
-      <c r="M8" s="89" t="s">
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="90"/>
+      <c r="N8" s="68"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="91" t="s">
+      <c r="P8" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="92"/>
-      <c r="R8" s="93"/>
-      <c r="S8" s="93"/>
-      <c r="T8" s="94"/>
-    </row>
-    <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q8" s="70"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="71"/>
+      <c r="T8" s="72"/>
+    </row>
+    <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="26" t="s">
         <v>44</v>
       </c>
@@ -2608,7 +2632,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="24"/>
       <c r="B10" s="9" t="s">
         <v>71</v>
@@ -2645,7 +2669,7 @@
       </c>
       <c r="O10" s="44"/>
     </row>
-    <row r="11" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="24"/>
       <c r="B11" s="9" t="s">
         <v>72</v>
@@ -2682,7 +2706,7 @@
       </c>
       <c r="O11" s="44"/>
     </row>
-    <row r="12" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="24"/>
       <c r="B12" s="9" t="s">
         <v>73</v>
@@ -2721,7 +2745,7 @@
       </c>
       <c r="O12" s="45"/>
     </row>
-    <row r="13" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="24"/>
       <c r="B13" s="9" t="s">
         <v>74</v>
@@ -2760,7 +2784,7 @@
       </c>
       <c r="O13" s="44"/>
     </row>
-    <row r="14" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="24"/>
       <c r="B14" s="9" t="s">
         <v>71</v>
@@ -2801,7 +2825,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="9" t="s">
         <v>72</v>
@@ -2842,7 +2866,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="24"/>
       <c r="B16" s="9" t="s">
         <v>73</v>
@@ -2885,7 +2909,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="18.75" customHeight="1">
       <c r="A17" s="24"/>
       <c r="B17" s="9" t="s">
         <v>74</v>
@@ -2928,7 +2952,7 @@
       </c>
       <c r="Q17" s="46"/>
     </row>
-    <row r="18" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="18.75" customHeight="1">
       <c r="A18" s="24"/>
       <c r="B18" s="9" t="s">
         <v>71</v>
@@ -2964,7 +2988,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="18.75" customHeight="1">
       <c r="A19" s="24"/>
       <c r="B19" s="9" t="s">
         <v>72</v>
@@ -3000,7 +3024,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="18.75" customHeight="1">
       <c r="A20" s="24"/>
       <c r="B20" s="9" t="s">
         <v>73</v>
@@ -3038,7 +3062,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="18.75" customHeight="1">
       <c r="A21" s="24"/>
       <c r="B21" s="9" t="s">
         <v>74</v>
@@ -3076,7 +3100,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="18.75" customHeight="1">
       <c r="A22" s="24"/>
       <c r="B22" s="9" t="s">
         <v>71</v>
@@ -3112,7 +3136,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="18.75" customHeight="1">
       <c r="A23" s="24"/>
       <c r="B23" s="9" t="s">
         <v>72</v>
@@ -3148,7 +3172,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="18.75" customHeight="1">
       <c r="A24" s="24"/>
       <c r="B24" s="9" t="s">
         <v>73</v>
@@ -3186,7 +3210,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="18.75" customHeight="1">
       <c r="A25" s="24"/>
       <c r="B25" s="9" t="s">
         <v>74</v>
@@ -3224,7 +3248,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="18.75" customHeight="1">
       <c r="A26" s="24"/>
       <c r="B26" s="9" t="s">
         <v>71</v>
@@ -3260,7 +3284,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" ht="18.75" customHeight="1">
       <c r="A27" s="24"/>
       <c r="B27" s="9" t="s">
         <v>72</v>
@@ -3296,7 +3320,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" ht="18.75" customHeight="1">
       <c r="A28" s="24"/>
       <c r="B28" s="9" t="s">
         <v>73</v>
@@ -3334,7 +3358,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" ht="18.75" customHeight="1">
       <c r="A29" s="24"/>
       <c r="B29" s="9" t="s">
         <v>74</v>
@@ -3372,7 +3396,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" ht="18.75" customHeight="1">
       <c r="A30" s="24" t="s">
         <v>92</v>
       </c>
@@ -3412,7 +3436,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="18.75" customHeight="1">
       <c r="A31" s="24" t="s">
         <v>93</v>
       </c>
@@ -3452,7 +3476,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" ht="18.75" customHeight="1">
       <c r="A32" s="24" t="s">
         <v>94</v>
       </c>
@@ -3492,7 +3516,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="18.75" customHeight="1">
       <c r="A33" s="24" t="s">
         <v>95</v>
       </c>
@@ -3532,7 +3556,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="18.75" customHeight="1">
       <c r="A34" s="24" t="s">
         <v>92</v>
       </c>
@@ -3572,7 +3596,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="18.75" customHeight="1">
       <c r="A35" s="24" t="s">
         <v>93</v>
       </c>
@@ -3612,7 +3636,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="18.75" customHeight="1">
       <c r="A36" s="24" t="s">
         <v>94</v>
       </c>
@@ -3652,7 +3676,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="18.75" customHeight="1">
       <c r="A37" s="24" t="s">
         <v>95</v>
       </c>
@@ -3692,7 +3716,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="18.75" customHeight="1">
       <c r="A38" s="24" t="s">
         <v>92</v>
       </c>
@@ -3732,7 +3756,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="18.75" customHeight="1">
       <c r="A39" s="24" t="s">
         <v>93</v>
       </c>
@@ -3772,7 +3796,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="18.75" customHeight="1">
       <c r="A40" s="24" t="s">
         <v>94</v>
       </c>
@@ -3812,7 +3836,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="18.75" customHeight="1">
       <c r="A41" s="24" t="s">
         <v>95</v>
       </c>
@@ -3852,7 +3876,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" ht="18.75" customHeight="1">
       <c r="A42" s="24" t="s">
         <v>113</v>
       </c>
@@ -3892,7 +3916,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" ht="18" customHeight="1">
       <c r="A43" s="24" t="s">
         <v>113</v>
       </c>
@@ -3932,7 +3956,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" ht="18" customHeight="1">
       <c r="A44" s="24" t="s">
         <v>112</v>
       </c>
@@ -3972,7 +3996,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="18" customHeight="1">
       <c r="A45" s="24" t="s">
         <v>113</v>
       </c>
@@ -4012,7 +4036,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="18" customHeight="1">
       <c r="A46" s="24" t="s">
         <v>114</v>
       </c>
@@ -4052,7 +4076,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" ht="18" customHeight="1">
       <c r="A47" s="24" t="s">
         <v>115</v>
       </c>
@@ -4092,7 +4116,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" ht="18" customHeight="1">
       <c r="A48" s="24" t="s">
         <v>116</v>
       </c>
@@ -4132,7 +4156,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="18" customHeight="1">
       <c r="A49" s="24" t="s">
         <v>112</v>
       </c>
@@ -4172,7 +4196,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" ht="18" customHeight="1">
       <c r="A50" s="24" t="s">
         <v>113</v>
       </c>
@@ -4212,7 +4236,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" ht="18" customHeight="1">
       <c r="A51" s="24" t="s">
         <v>114</v>
       </c>
@@ -4252,7 +4276,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="18" customHeight="1">
       <c r="A52" s="24" t="s">
         <v>115</v>
       </c>
@@ -4292,7 +4316,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="18" customHeight="1">
       <c r="A53" s="24" t="s">
         <v>116</v>
       </c>
@@ -4332,7 +4356,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="18" customHeight="1">
       <c r="A54" s="24" t="s">
         <v>129</v>
       </c>
@@ -4372,7 +4396,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="18" customHeight="1">
       <c r="A55" s="24" t="s">
         <v>130</v>
       </c>
@@ -4412,7 +4436,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="18" customHeight="1">
       <c r="A56" s="24" t="s">
         <v>131</v>
       </c>
@@ -4452,7 +4476,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" ht="18" customHeight="1">
       <c r="A57" s="24" t="s">
         <v>132</v>
       </c>
@@ -4492,7 +4516,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="18" customHeight="1">
       <c r="A58" s="24" t="s">
         <v>129</v>
       </c>
@@ -4532,7 +4556,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="18" customHeight="1">
       <c r="A59" s="24" t="s">
         <v>130</v>
       </c>
@@ -4572,7 +4596,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="18" customHeight="1">
       <c r="A60" s="24" t="s">
         <v>131</v>
       </c>
@@ -4612,7 +4636,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="18" customHeight="1">
       <c r="A61" s="24" t="s">
         <v>132</v>
       </c>
@@ -4652,7 +4676,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="18" customHeight="1">
       <c r="A62" s="24" t="s">
         <v>112</v>
       </c>
@@ -4690,7 +4714,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="18" customHeight="1">
       <c r="A63" s="24" t="s">
         <v>144</v>
       </c>
@@ -4728,7 +4752,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" ht="18" customHeight="1">
       <c r="A64" s="24" t="s">
         <v>145</v>
       </c>
@@ -4766,7 +4790,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="18" customHeight="1">
       <c r="A65" s="24" t="s">
         <v>146</v>
       </c>
@@ -4804,7 +4828,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="18" customHeight="1">
       <c r="A66" s="24" t="s">
         <v>147</v>
       </c>
@@ -4844,7 +4868,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" ht="18" customHeight="1">
       <c r="A67" s="24" t="s">
         <v>112</v>
       </c>
@@ -4882,7 +4906,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" ht="18" customHeight="1">
       <c r="A68" s="24" t="s">
         <v>144</v>
       </c>
@@ -4920,7 +4944,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" ht="18" customHeight="1">
       <c r="A69" s="24" t="s">
         <v>145</v>
       </c>
@@ -4958,7 +4982,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" ht="18" customHeight="1">
       <c r="A70" s="24" t="s">
         <v>146</v>
       </c>
@@ -4996,7 +5020,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" ht="18" customHeight="1">
       <c r="A71" s="24" t="s">
         <v>147</v>
       </c>
@@ -5036,7 +5060,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" ht="18" customHeight="1">
       <c r="A72" s="24"/>
       <c r="B72" s="44" t="s">
         <v>156</v>
@@ -5066,7 +5090,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" ht="18" customHeight="1">
       <c r="A73" s="24"/>
       <c r="B73" s="44" t="s">
         <v>157</v>
@@ -5096,7 +5120,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" ht="18" customHeight="1">
       <c r="A74" s="24"/>
       <c r="B74" s="44" t="s">
         <v>156</v>
@@ -5124,7 +5148,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" ht="18" customHeight="1">
       <c r="A75" s="24"/>
       <c r="B75" s="44" t="s">
         <v>157</v>
@@ -5152,7 +5176,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" ht="18" customHeight="1">
       <c r="A76" s="24"/>
       <c r="B76" s="44" t="s">
         <v>164</v>
@@ -5190,7 +5214,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" ht="18" customHeight="1">
       <c r="A77" s="24"/>
       <c r="B77" s="44" t="s">
         <v>165</v>
@@ -5218,7 +5242,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" ht="18" customHeight="1">
       <c r="A78" s="24"/>
       <c r="B78" s="44" t="s">
         <v>166</v>
@@ -5246,7 +5270,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" ht="18" customHeight="1">
       <c r="A79" s="24"/>
       <c r="B79" s="44" t="s">
         <v>167</v>
@@ -5274,7 +5298,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" ht="18" customHeight="1">
       <c r="A80" s="24"/>
       <c r="B80" s="44" t="s">
         <v>168</v>
@@ -5302,7 +5326,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="81" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" ht="18" customHeight="1">
       <c r="A81" s="24"/>
       <c r="B81" s="44" t="s">
         <v>174</v>
@@ -5330,7 +5354,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="82" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" ht="18" customHeight="1">
       <c r="A82" s="24"/>
       <c r="B82" s="44" t="s">
         <v>174</v>
@@ -5358,7 +5382,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="83" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" ht="18" customHeight="1">
       <c r="A83" s="24"/>
       <c r="B83" s="9" t="s">
         <v>90</v>
@@ -5404,7 +5428,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" ht="18" customHeight="1">
       <c r="A84" s="24"/>
       <c r="B84" s="9" t="s">
         <v>91</v>
@@ -5450,7 +5474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" ht="18" customHeight="1">
       <c r="A85" s="24"/>
       <c r="B85" s="9" t="s">
         <v>96</v>
@@ -5496,7 +5520,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" ht="18" customHeight="1">
       <c r="A86" s="24"/>
       <c r="B86" s="9" t="s">
         <v>97</v>
@@ -5542,7 +5566,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" ht="18" customHeight="1">
       <c r="A87" s="24"/>
       <c r="B87" s="9" t="s">
         <v>90</v>
@@ -5580,7 +5604,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="88" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" ht="18" customHeight="1">
       <c r="A88" s="24"/>
       <c r="B88" s="9" t="s">
         <v>91</v>
@@ -5618,7 +5642,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="89" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" ht="18" customHeight="1">
       <c r="A89" s="24"/>
       <c r="B89" s="9" t="s">
         <v>96</v>
@@ -5656,7 +5680,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="90" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" ht="18" customHeight="1">
       <c r="A90" s="24"/>
       <c r="B90" s="9" t="s">
         <v>97</v>
@@ -5694,7 +5718,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="91" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" ht="18" customHeight="1">
       <c r="A91" s="24"/>
       <c r="B91" s="44" t="s">
         <v>181</v>
@@ -5736,7 +5760,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="92" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" ht="18" customHeight="1">
       <c r="A92" s="24"/>
       <c r="B92" s="44" t="s">
         <v>181</v>
@@ -5774,7 +5798,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="93" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17" ht="18" customHeight="1">
       <c r="A93" s="24"/>
       <c r="B93" s="44" t="s">
         <v>187</v>
@@ -5810,7 +5834,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="94" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" ht="18" customHeight="1">
       <c r="A94" s="24"/>
       <c r="B94" s="44" t="s">
         <v>187</v>
@@ -5846,7 +5870,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="95" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" ht="18" customHeight="1">
       <c r="A95" s="24"/>
       <c r="B95" s="44" t="s">
         <v>187</v>
@@ -5882,7 +5906,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="96" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" ht="18" customHeight="1">
       <c r="A96" s="24"/>
       <c r="B96" s="44" t="s">
         <v>191</v>
@@ -5918,7 +5942,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" ht="18" customHeight="1">
       <c r="A97" s="24"/>
       <c r="B97" s="44" t="s">
         <v>191</v>
@@ -5954,7 +5978,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" ht="18" customHeight="1">
       <c r="A98" s="24"/>
       <c r="B98" s="44" t="s">
         <v>191</v>
@@ -5990,7 +6014,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" ht="18" customHeight="1">
       <c r="A99" s="24"/>
       <c r="B99" s="44" t="s">
         <v>196</v>
@@ -6028,7 +6052,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" ht="18" customHeight="1">
       <c r="A100" s="24"/>
       <c r="B100" s="44" t="s">
         <v>197</v>
@@ -6066,7 +6090,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" ht="18" customHeight="1">
       <c r="A101" s="24"/>
       <c r="B101" s="44" t="s">
         <v>198</v>
@@ -6104,7 +6128,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" ht="18" customHeight="1">
       <c r="A102" s="24"/>
       <c r="B102" s="44" t="s">
         <v>199</v>
@@ -6142,7 +6166,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" ht="18" customHeight="1">
       <c r="A103" s="24"/>
       <c r="B103" s="44" t="s">
         <v>200</v>
@@ -6180,7 +6204,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" ht="18" customHeight="1">
       <c r="A104" s="24"/>
       <c r="B104" s="44" t="s">
         <v>201</v>
@@ -6218,7 +6242,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" ht="18" customHeight="1">
       <c r="A105" s="24"/>
       <c r="B105" s="44" t="s">
         <v>196</v>
@@ -6258,7 +6282,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" ht="18" customHeight="1">
       <c r="A106" s="24"/>
       <c r="B106" s="44" t="s">
         <v>200</v>
@@ -6298,7 +6322,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" ht="18" customHeight="1">
       <c r="A107" s="24"/>
       <c r="B107" s="44" t="s">
         <v>201</v>
@@ -6338,7 +6362,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14" ht="18" customHeight="1">
       <c r="A108" s="24"/>
       <c r="B108" s="44" t="s">
         <v>196</v>
@@ -6378,7 +6402,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" ht="18" customHeight="1">
       <c r="A109" s="24"/>
       <c r="B109" s="44" t="s">
         <v>197</v>
@@ -6418,7 +6442,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14" ht="18" customHeight="1">
       <c r="A110" s="24"/>
       <c r="B110" s="44" t="s">
         <v>200</v>
@@ -6458,7 +6482,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14" ht="18" customHeight="1">
       <c r="A111" s="24"/>
       <c r="B111" s="44" t="s">
         <v>201</v>
@@ -6498,7 +6522,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" ht="18" customHeight="1">
       <c r="A112" s="24"/>
       <c r="B112" s="44" t="s">
         <v>196</v>
@@ -6538,7 +6562,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" ht="18" customHeight="1">
       <c r="A113" s="24"/>
       <c r="B113" s="44" t="s">
         <v>200</v>
@@ -6578,7 +6602,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" ht="18" customHeight="1">
       <c r="A114" s="24"/>
       <c r="B114" s="44" t="s">
         <v>201</v>
@@ -6618,7 +6642,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" ht="18" customHeight="1">
       <c r="A115" s="24"/>
       <c r="B115" s="44" t="s">
         <v>213</v>
@@ -6654,7 +6678,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" ht="18" customHeight="1">
       <c r="A116" s="24"/>
       <c r="B116" s="44" t="s">
         <v>213</v>
@@ -6690,7 +6714,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" ht="18" customHeight="1">
       <c r="A117" s="24"/>
       <c r="B117" s="44" t="s">
         <v>213</v>
@@ -6718,7 +6742,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14" ht="18" customHeight="1">
       <c r="A118" s="24"/>
       <c r="B118" s="44" t="s">
         <v>222</v>
@@ -6752,7 +6776,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" ht="18" customHeight="1">
       <c r="A119" s="24"/>
       <c r="B119" s="44" t="s">
         <v>227</v>
@@ -6788,7 +6812,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" ht="18" customHeight="1">
       <c r="A120" s="24"/>
       <c r="B120" s="44" t="s">
         <v>227</v>
@@ -6826,7 +6850,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" ht="18" customHeight="1">
       <c r="A121" s="24"/>
       <c r="B121" s="44" t="s">
         <v>227</v>
@@ -6864,7 +6888,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14" ht="18" customHeight="1">
       <c r="A122" s="24"/>
       <c r="B122" s="44" t="s">
         <v>236</v>
@@ -6892,7 +6916,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14" ht="18" customHeight="1">
       <c r="A123" s="24"/>
       <c r="B123" s="44" t="s">
         <v>240</v>
@@ -6932,7 +6956,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:14" ht="18" customHeight="1">
       <c r="A124" s="24"/>
       <c r="B124" s="44" t="s">
         <v>241</v>
@@ -6970,7 +6994,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:14" ht="18" customHeight="1">
       <c r="A125" s="24"/>
       <c r="B125" s="44" t="s">
         <v>240</v>
@@ -7010,7 +7034,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14" ht="18" customHeight="1">
       <c r="A126" s="24"/>
       <c r="B126" s="44" t="s">
         <v>241</v>
@@ -7048,7 +7072,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:14" ht="18" customHeight="1">
       <c r="A127" s="24"/>
       <c r="B127" s="44" t="s">
         <v>240</v>
@@ -7086,7 +7110,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:14" ht="18" customHeight="1">
       <c r="A128" s="24"/>
       <c r="B128" s="44" t="s">
         <v>241</v>
@@ -7122,7 +7146,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="129" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" ht="18" customHeight="1">
       <c r="A129" s="24"/>
       <c r="B129" s="44" t="s">
         <v>240</v>
@@ -7160,7 +7184,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="130" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" ht="18" customHeight="1">
       <c r="A130" s="24"/>
       <c r="B130" s="44" t="s">
         <v>241</v>
@@ -7196,7 +7220,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="131" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" ht="18" customHeight="1">
       <c r="A131" s="24" t="s">
         <v>251</v>
       </c>
@@ -7226,7 +7250,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" ht="18" customHeight="1">
       <c r="A132" s="24" t="s">
         <v>250</v>
       </c>
@@ -7256,7 +7280,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="133" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" ht="18" customHeight="1">
       <c r="A133" s="24" t="s">
         <v>252</v>
       </c>
@@ -7286,7 +7310,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" ht="18" customHeight="1">
       <c r="A134" s="24"/>
       <c r="B134" s="44" t="s">
         <v>257</v>
@@ -7312,7 +7336,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="135" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:16" ht="18" customHeight="1">
       <c r="A135" s="24"/>
       <c r="B135" s="44" t="s">
         <v>257</v>
@@ -7340,7 +7364,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="136" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16" ht="18" customHeight="1">
       <c r="A136" s="24"/>
       <c r="B136" s="44" t="s">
         <v>260</v>
@@ -7368,7 +7392,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="137" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:16" ht="18" customHeight="1">
       <c r="A137" s="24" t="s">
         <v>251</v>
       </c>
@@ -7412,7 +7436,7 @@
         <v>4905</v>
       </c>
     </row>
-    <row r="138" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16" ht="18" customHeight="1">
       <c r="A138" s="24" t="s">
         <v>250</v>
       </c>
@@ -7456,7 +7480,7 @@
         <v>3720</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16" ht="18" customHeight="1">
       <c r="A139" s="24" t="s">
         <v>252</v>
       </c>
@@ -7500,7 +7524,7 @@
         <v>2953</v>
       </c>
     </row>
-    <row r="140" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:16" ht="18" customHeight="1">
       <c r="A140" s="24" t="s">
         <v>251</v>
       </c>
@@ -7544,7 +7568,7 @@
         <v>4659</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:16" ht="18" customHeight="1">
       <c r="A141" s="24" t="s">
         <v>250</v>
       </c>
@@ -7588,7 +7612,7 @@
         <v>3806</v>
       </c>
     </row>
-    <row r="142" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" ht="18" customHeight="1">
       <c r="A142" s="24" t="s">
         <v>252</v>
       </c>
@@ -7632,7 +7656,7 @@
         <v>3142</v>
       </c>
     </row>
-    <row r="143" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16" ht="18" customHeight="1">
       <c r="A143" s="24" t="s">
         <v>251</v>
       </c>
@@ -7676,7 +7700,7 @@
         <v>4744</v>
       </c>
     </row>
-    <row r="144" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:16" ht="18" customHeight="1">
       <c r="A144" s="24" t="s">
         <v>250</v>
       </c>
@@ -7720,7 +7744,7 @@
         <v>3986</v>
       </c>
     </row>
-    <row r="145" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:16" ht="18" customHeight="1">
       <c r="A145" s="24" t="s">
         <v>252</v>
       </c>
@@ -7764,7 +7788,7 @@
         <v>3427</v>
       </c>
     </row>
-    <row r="146" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16" ht="18" customHeight="1">
       <c r="A146" s="24" t="s">
         <v>251</v>
       </c>
@@ -7808,7 +7832,7 @@
         <v>-9.4700000000000006</v>
       </c>
     </row>
-    <row r="147" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:16" ht="18" customHeight="1">
       <c r="A147" s="24" t="s">
         <v>250</v>
       </c>
@@ -7852,7 +7876,7 @@
         <v>-10.27</v>
       </c>
     </row>
-    <row r="148" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:16" ht="18" customHeight="1">
       <c r="A148" s="24" t="s">
         <v>252</v>
       </c>
@@ -7896,7 +7920,7 @@
         <v>-6.61</v>
       </c>
     </row>
-    <row r="149" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:16" ht="18" customHeight="1">
       <c r="A149" s="24" t="s">
         <v>251</v>
       </c>
@@ -7940,7 +7964,7 @@
         <v>-10.96</v>
       </c>
     </row>
-    <row r="150" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:16" ht="18" customHeight="1">
       <c r="A150" s="24" t="s">
         <v>250</v>
       </c>
@@ -7984,7 +8008,7 @@
         <v>-13.63</v>
       </c>
     </row>
-    <row r="151" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:16" ht="18" customHeight="1">
       <c r="A151" s="24" t="s">
         <v>252</v>
       </c>
@@ -8028,7 +8052,7 @@
         <v>-9.7799999999999994</v>
       </c>
     </row>
-    <row r="152" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:16" ht="18" customHeight="1">
       <c r="A152" s="24" t="s">
         <v>251</v>
       </c>
@@ -8072,7 +8096,7 @@
         <v>-12.64</v>
       </c>
     </row>
-    <row r="153" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:16" ht="18" customHeight="1">
       <c r="A153" s="24" t="s">
         <v>250</v>
       </c>
@@ -8116,7 +8140,7 @@
         <v>-16.309999999999999</v>
       </c>
     </row>
-    <row r="154" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:16" ht="18" customHeight="1">
       <c r="A154" s="24" t="s">
         <v>252</v>
       </c>
@@ -8160,7 +8184,7 @@
         <v>-13.69</v>
       </c>
     </row>
-    <row r="155" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:16" ht="18" customHeight="1">
       <c r="A155" s="24" t="s">
         <v>251</v>
       </c>
@@ -8200,7 +8224,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="156" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:16" ht="18" customHeight="1">
       <c r="A156" s="24" t="s">
         <v>250</v>
       </c>
@@ -8240,7 +8264,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="157" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:16" ht="18" customHeight="1">
       <c r="A157" s="24" t="s">
         <v>252</v>
       </c>
@@ -8280,7 +8304,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="158" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:16" ht="18" customHeight="1">
       <c r="A158" s="24" t="s">
         <v>251</v>
       </c>
@@ -8320,7 +8344,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="159" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:16" ht="18" customHeight="1">
       <c r="A159" s="24" t="s">
         <v>250</v>
       </c>
@@ -8360,7 +8384,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="160" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:16" ht="18" customHeight="1">
       <c r="A160" s="24" t="s">
         <v>252</v>
       </c>
@@ -8400,7 +8424,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="161" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:16" ht="18" customHeight="1">
       <c r="A161" s="24" t="s">
         <v>251</v>
       </c>
@@ -8440,7 +8464,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="162" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:16" ht="18" customHeight="1">
       <c r="A162" s="24" t="s">
         <v>250</v>
       </c>
@@ -8480,7 +8504,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="163" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:16" ht="18" customHeight="1">
       <c r="A163" s="24" t="s">
         <v>252</v>
       </c>
@@ -8520,7 +8544,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="164" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:16" ht="18" customHeight="1">
       <c r="B164" s="44" t="s">
         <v>272</v>
       </c>
@@ -8559,7 +8583,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="165" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:16" ht="18" customHeight="1">
       <c r="B165" s="44" t="s">
         <v>276</v>
       </c>
@@ -8588,7 +8612,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="166" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:16" ht="18" customHeight="1">
       <c r="B166" s="44" t="s">
         <v>277</v>
       </c>
@@ -8617,7 +8641,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="167" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:16" ht="18" customHeight="1">
       <c r="A167" s="24"/>
       <c r="B167" s="44" t="s">
         <v>278</v>
@@ -8651,7 +8675,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="168" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:16" ht="18" customHeight="1">
       <c r="A168" s="24"/>
       <c r="B168" s="44" t="s">
         <v>279</v>
@@ -8685,7 +8709,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="169" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:16" ht="18" customHeight="1">
       <c r="A169" s="24"/>
       <c r="B169" s="44" t="s">
         <v>276</v>
@@ -8718,7 +8742,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="170" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:16" ht="18" customHeight="1">
       <c r="A170" s="24"/>
       <c r="B170" s="44" t="s">
         <v>277</v>
@@ -8751,7 +8775,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="171" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:16" ht="18" customHeight="1">
       <c r="A171" s="24"/>
       <c r="B171" s="44" t="s">
         <v>278</v>
@@ -8785,7 +8809,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="172" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:16" ht="18" customHeight="1">
       <c r="A172" s="24"/>
       <c r="B172" s="44" t="s">
         <v>279</v>
@@ -8819,7 +8843,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="173" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:16" ht="18" customHeight="1">
       <c r="A173" s="24"/>
       <c r="B173" s="44" t="s">
         <v>285</v>
@@ -8853,7 +8877,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="174" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:16" ht="18" customHeight="1">
       <c r="A174" s="24"/>
       <c r="B174" s="44" t="s">
         <v>285</v>
@@ -8887,7 +8911,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="175" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:16" ht="18" customHeight="1">
       <c r="A175" s="24"/>
       <c r="B175" s="44" t="s">
         <v>285</v>
@@ -8921,7 +8945,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="176" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:16" ht="18" customHeight="1">
       <c r="A176" s="24"/>
       <c r="B176" s="44" t="s">
         <v>285</v>
@@ -8959,7 +8983,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:14" ht="18" customHeight="1">
       <c r="A177" s="24"/>
       <c r="B177" s="44" t="s">
         <v>288</v>
@@ -8997,7 +9021,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:14" ht="18" customHeight="1">
       <c r="A178" s="24"/>
       <c r="B178" s="44" t="s">
         <v>289</v>
@@ -9035,7 +9059,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:14" ht="18" customHeight="1">
       <c r="A179" s="24"/>
       <c r="B179" s="44" t="s">
         <v>290</v>
@@ -9073,7 +9097,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:14" ht="18" customHeight="1">
       <c r="A180" s="24"/>
       <c r="B180" s="44" t="s">
         <v>288</v>
@@ -9111,7 +9135,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="181" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:14" ht="18" customHeight="1">
       <c r="A181" s="24"/>
       <c r="B181" s="44" t="s">
         <v>289</v>
@@ -9149,7 +9173,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="182" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:14" ht="18" customHeight="1">
       <c r="A182" s="24"/>
       <c r="B182" s="44" t="s">
         <v>290</v>
@@ -9187,7 +9211,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="183" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:14" ht="18" customHeight="1">
       <c r="A183" s="24"/>
       <c r="B183" s="44" t="s">
         <v>288</v>
@@ -9225,7 +9249,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="184" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:14" ht="18" customHeight="1">
       <c r="A184" s="24"/>
       <c r="B184" s="44" t="s">
         <v>289</v>
@@ -9263,7 +9287,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="185" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:14" ht="18" customHeight="1">
       <c r="A185" s="24"/>
       <c r="B185" s="44" t="s">
         <v>290</v>
@@ -9301,7 +9325,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="186" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:14" ht="18" customHeight="1">
       <c r="A186" s="24"/>
       <c r="B186" s="44" t="s">
         <v>294</v>
@@ -9339,7 +9363,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:14" ht="18" customHeight="1">
       <c r="A187" s="24"/>
       <c r="B187" s="44" t="s">
         <v>294</v>
@@ -9379,7 +9403,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="188" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:14" ht="18" customHeight="1">
       <c r="A188" s="24"/>
       <c r="B188" s="44" t="s">
         <v>294</v>
@@ -9419,7 +9443,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="189" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:14" ht="18" customHeight="1">
       <c r="A189" s="24"/>
       <c r="B189" s="44" t="s">
         <v>298</v>
@@ -9455,7 +9479,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="190" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:14" ht="18" customHeight="1">
       <c r="A190" s="24"/>
       <c r="B190" s="44" t="s">
         <v>298</v>
@@ -9493,7 +9517,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="191" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:14" ht="18" customHeight="1">
       <c r="A191" s="24"/>
       <c r="B191" s="44" t="s">
         <v>298</v>
@@ -9531,7 +9555,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="192" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:14" ht="18" customHeight="1">
       <c r="A192" s="24"/>
       <c r="B192" s="44" t="s">
         <v>298</v>
@@ -9569,7 +9593,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="193" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:16" ht="18" customHeight="1">
       <c r="A193" s="24"/>
       <c r="B193" s="44" t="s">
         <v>301</v>
@@ -9605,7 +9629,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="194" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:16" ht="18" customHeight="1">
       <c r="A194" s="24"/>
       <c r="B194" s="44" t="s">
         <v>302</v>
@@ -9641,7 +9665,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="195" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:16" ht="18" customHeight="1">
       <c r="A195" s="24"/>
       <c r="B195" s="44" t="s">
         <v>303</v>
@@ -9677,7 +9701,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="196" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:16" ht="18" customHeight="1">
       <c r="A196" s="24"/>
       <c r="B196" s="44" t="s">
         <v>304</v>
@@ -9713,7 +9737,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="197" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:16" ht="18" customHeight="1">
       <c r="A197" s="24"/>
       <c r="B197" s="44" t="s">
         <v>305</v>
@@ -9749,7 +9773,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="198" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:16" ht="18" customHeight="1">
       <c r="A198" s="24"/>
       <c r="B198" s="44" t="s">
         <v>301</v>
@@ -9785,7 +9809,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="199" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:16" ht="18" customHeight="1">
       <c r="A199" s="24"/>
       <c r="B199" s="44" t="s">
         <v>302</v>
@@ -9821,7 +9845,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="200" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:16" ht="18" customHeight="1">
       <c r="A200" s="24"/>
       <c r="B200" s="44" t="s">
         <v>303</v>
@@ -9857,7 +9881,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="201" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:16" ht="18" customHeight="1">
       <c r="A201" s="24"/>
       <c r="B201" s="44" t="s">
         <v>304</v>
@@ -9893,7 +9917,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="202" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:16" ht="18" customHeight="1">
       <c r="A202" s="24"/>
       <c r="B202" s="44" t="s">
         <v>305</v>
@@ -9929,7 +9953,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="203" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:16" ht="18" customHeight="1">
       <c r="A203" s="24"/>
       <c r="B203" s="44" t="s">
         <v>301</v>
@@ -9969,7 +9993,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="204" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:16" ht="18" customHeight="1">
       <c r="A204" s="24"/>
       <c r="B204" s="44" t="s">
         <v>302</v>
@@ -10009,7 +10033,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="205" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:16" ht="18" customHeight="1">
       <c r="A205" s="24"/>
       <c r="B205" s="44" t="s">
         <v>303</v>
@@ -10049,7 +10073,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="206" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:16" ht="18" customHeight="1">
       <c r="A206" s="24"/>
       <c r="B206" s="44" t="s">
         <v>304</v>
@@ -10089,7 +10113,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="207" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:16" ht="18" customHeight="1">
       <c r="A207" s="24"/>
       <c r="B207" s="44" t="s">
         <v>305</v>
@@ -10129,7 +10153,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="208" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:16" ht="18" customHeight="1">
       <c r="A208" s="24"/>
       <c r="B208" s="54" t="s">
         <v>301</v>
@@ -10169,7 +10193,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="209" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:16" ht="18" customHeight="1">
       <c r="A209" s="24"/>
       <c r="B209" s="54" t="s">
         <v>302</v>
@@ -10209,7 +10233,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="210" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:16" ht="18" customHeight="1">
       <c r="A210" s="24"/>
       <c r="B210" s="54" t="s">
         <v>303</v>
@@ -10249,7 +10273,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="211" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:16" ht="18" customHeight="1">
       <c r="A211" s="24"/>
       <c r="B211" s="54" t="s">
         <v>304</v>
@@ -10289,7 +10313,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="212" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:16" ht="18" customHeight="1">
       <c r="A212" s="24"/>
       <c r="B212" s="54" t="s">
         <v>305</v>
@@ -10329,7 +10353,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="213" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:16" ht="18" customHeight="1">
       <c r="A213" s="24"/>
       <c r="B213" s="44" t="s">
         <v>311</v>
@@ -10351,11 +10375,11 @@
       <c r="K213" s="4"/>
       <c r="L213" s="44"/>
       <c r="M213" s="44"/>
-      <c r="N213" s="95" t="s">
+      <c r="N213" s="44" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="214" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:16" ht="18" customHeight="1">
       <c r="A214" s="24"/>
       <c r="B214" s="44" t="s">
         <v>311</v>
@@ -10377,11 +10401,11 @@
       <c r="K214" s="4"/>
       <c r="L214" s="44"/>
       <c r="M214" s="44"/>
-      <c r="N214" s="95" t="s">
+      <c r="N214" s="44" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="215" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:16" ht="18" customHeight="1">
       <c r="A215" s="24"/>
       <c r="B215" s="44" t="s">
         <v>311</v>
@@ -10411,11 +10435,11 @@
         <v>315</v>
       </c>
       <c r="M215" s="44"/>
-      <c r="N215" s="95" t="s">
+      <c r="N215" s="44" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="216" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:16" ht="18" customHeight="1">
       <c r="A216" s="24"/>
       <c r="B216" s="44" t="s">
         <v>311</v>
@@ -10446,11 +10470,11 @@
       <c r="M216" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="N216" s="95" t="s">
+      <c r="N216" s="44" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="217" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:16" ht="18" customHeight="1">
       <c r="A217" s="24"/>
       <c r="B217" s="44" t="s">
         <v>311</v>
@@ -10483,11 +10507,11 @@
       <c r="M217" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="N217" s="95" t="s">
+      <c r="N217" s="44" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="218" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:16" ht="18" customHeight="1">
       <c r="A218" s="24"/>
       <c r="B218" s="44" t="s">
         <v>311</v>
@@ -10520,11 +10544,11 @@
       <c r="M218" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="N218" s="95" t="s">
+      <c r="N218" s="44" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="219" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:16" ht="18" customHeight="1">
       <c r="A219" s="24"/>
       <c r="B219" s="44" t="s">
         <v>311</v>
@@ -10557,11 +10581,11 @@
       <c r="M219" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="N219" s="95" t="s">
+      <c r="N219" s="44" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="220" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:16" ht="18" customHeight="1">
       <c r="A220" s="24"/>
       <c r="B220" s="44" t="s">
         <v>311</v>
@@ -10593,11 +10617,11 @@
       <c r="M220" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="N220" s="95" t="s">
+      <c r="N220" s="44" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="221" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:16" ht="18" customHeight="1">
       <c r="A221" s="24"/>
       <c r="B221" s="44" t="s">
         <v>311</v>
@@ -10630,11 +10654,11 @@
       <c r="M221" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="N221" s="95" t="s">
+      <c r="N221" s="44" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="222" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:16" ht="18" customHeight="1">
       <c r="A222" s="24"/>
       <c r="B222" s="44" t="s">
         <v>311</v>
@@ -10667,11 +10691,11 @@
       <c r="M222" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="N222" s="95" t="s">
+      <c r="N222" s="44" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="223" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:16" ht="18" customHeight="1">
       <c r="A223" s="24"/>
       <c r="B223" s="44" t="s">
         <v>311</v>
@@ -10704,11 +10728,11 @@
       <c r="M223" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="N223" s="95" t="s">
+      <c r="N223" s="44" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="224" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:16" ht="18" customHeight="1">
       <c r="A224" s="24"/>
       <c r="B224" s="44" t="s">
         <v>311</v>
@@ -10740,43 +10764,101 @@
       <c r="M224" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="N224" s="95" t="s">
+      <c r="N224" s="44" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="225" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:17" ht="18" customHeight="1">
       <c r="A225" s="24"/>
-      <c r="B225" s="44"/>
-      <c r="C225" s="42"/>
-      <c r="D225" s="42"/>
-      <c r="E225" s="44"/>
-      <c r="F225" s="42"/>
-      <c r="G225" s="42"/>
+      <c r="B225" s="44" t="s">
+        <v>318</v>
+      </c>
+      <c r="C225" s="42" t="s">
+        <v>319</v>
+      </c>
+      <c r="D225" s="42" t="s">
+        <v>321</v>
+      </c>
+      <c r="E225" s="44" t="s">
+        <v>322</v>
+      </c>
+      <c r="F225" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G225" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H225" s="42"/>
-      <c r="I225" s="3"/>
-      <c r="J225" s="4"/>
-      <c r="K225" s="4"/>
-      <c r="L225" s="44"/>
-      <c r="M225" s="44"/>
-      <c r="N225" s="44"/>
-    </row>
-    <row r="226" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I225" s="3">
+        <v>299</v>
+      </c>
+      <c r="J225" s="50">
+        <f>P225*9807000</f>
+        <v>2138906700</v>
+      </c>
+      <c r="K225" s="50">
+        <f>Q225*9807000</f>
+        <v>15691200</v>
+      </c>
+      <c r="L225" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M225" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="N225" s="44" t="s">
+        <v>324</v>
+      </c>
+      <c r="P225" s="95">
+        <v>218.1</v>
+      </c>
+      <c r="Q225" s="6">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="226" spans="1:17" ht="18" customHeight="1">
       <c r="A226" s="24"/>
-      <c r="B226" s="44"/>
-      <c r="C226" s="42"/>
-      <c r="D226" s="42"/>
-      <c r="E226" s="44"/>
-      <c r="F226" s="42"/>
-      <c r="G226" s="42"/>
+      <c r="B226" s="44" t="s">
+        <v>318</v>
+      </c>
+      <c r="C226" s="42" t="s">
+        <v>319</v>
+      </c>
+      <c r="D226" s="42" t="s">
+        <v>320</v>
+      </c>
+      <c r="E226" s="44" t="s">
+        <v>323</v>
+      </c>
+      <c r="F226" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G226" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H226" s="42"/>
-      <c r="I226" s="3"/>
-      <c r="J226" s="4"/>
+      <c r="I226" s="3">
+        <v>300</v>
+      </c>
+      <c r="J226" s="50">
+        <f>P226*9807000</f>
+        <v>2788130100</v>
+      </c>
       <c r="K226" s="4"/>
-      <c r="L226" s="44"/>
-      <c r="M226" s="44"/>
-      <c r="N226" s="44"/>
-    </row>
-    <row r="227" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L226" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M226" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="N226" s="44" t="s">
+        <v>324</v>
+      </c>
+      <c r="P226" s="6">
+        <v>284.3</v>
+      </c>
+    </row>
+    <row r="227" spans="1:17" ht="18" customHeight="1">
       <c r="A227" s="24"/>
       <c r="B227" s="44"/>
       <c r="C227" s="42"/>
@@ -10792,7 +10874,7 @@
       <c r="M227" s="44"/>
       <c r="N227" s="44"/>
     </row>
-    <row r="228" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:17" ht="18" customHeight="1">
       <c r="A228" s="24"/>
       <c r="B228" s="44"/>
       <c r="C228" s="42"/>
@@ -10808,7 +10890,7 @@
       <c r="M228" s="44"/>
       <c r="N228" s="44"/>
     </row>
-    <row r="229" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:17" ht="18" customHeight="1">
       <c r="A229" s="24"/>
       <c r="B229" s="44"/>
       <c r="C229" s="42"/>
@@ -10824,7 +10906,7 @@
       <c r="M229" s="44"/>
       <c r="N229" s="44"/>
     </row>
-    <row r="230" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:17" ht="18" customHeight="1">
       <c r="A230" s="24"/>
       <c r="B230" s="44"/>
       <c r="C230" s="42"/>
@@ -10840,7 +10922,7 @@
       <c r="M230" s="44"/>
       <c r="N230" s="44"/>
     </row>
-    <row r="231" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:17" ht="18" customHeight="1">
       <c r="A231" s="24"/>
       <c r="B231" s="44"/>
       <c r="C231" s="42"/>
@@ -10856,7 +10938,7 @@
       <c r="M231" s="44"/>
       <c r="N231" s="44"/>
     </row>
-    <row r="232" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:17" ht="18" customHeight="1">
       <c r="A232" s="24"/>
       <c r="B232" s="44"/>
       <c r="C232" s="42"/>
@@ -10872,7 +10954,7 @@
       <c r="M232" s="44"/>
       <c r="N232" s="44"/>
     </row>
-    <row r="233" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:17" ht="18" customHeight="1">
       <c r="A233" s="24"/>
       <c r="B233" s="44"/>
       <c r="C233" s="42"/>
@@ -10888,7 +10970,7 @@
       <c r="M233" s="44"/>
       <c r="N233" s="44"/>
     </row>
-    <row r="234" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:17" ht="18" customHeight="1">
       <c r="A234" s="24"/>
       <c r="B234" s="44"/>
       <c r="C234" s="42"/>
@@ -10904,7 +10986,7 @@
       <c r="M234" s="44"/>
       <c r="N234" s="44"/>
     </row>
-    <row r="235" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:17" ht="18" customHeight="1">
       <c r="A235" s="24"/>
       <c r="B235" s="44"/>
       <c r="C235" s="42"/>
@@ -10920,7 +11002,7 @@
       <c r="M235" s="44"/>
       <c r="N235" s="44"/>
     </row>
-    <row r="236" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:17" ht="18" customHeight="1">
       <c r="A236" s="24"/>
       <c r="B236" s="44"/>
       <c r="C236" s="42"/>
@@ -10936,7 +11018,7 @@
       <c r="M236" s="44"/>
       <c r="N236" s="44"/>
     </row>
-    <row r="237" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:17" ht="18" customHeight="1">
       <c r="A237" s="24"/>
       <c r="B237" s="44"/>
       <c r="C237" s="42"/>
@@ -10952,7 +11034,7 @@
       <c r="M237" s="44"/>
       <c r="N237" s="44"/>
     </row>
-    <row r="238" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:17" ht="18" customHeight="1">
       <c r="A238" s="24"/>
       <c r="B238" s="44"/>
       <c r="C238" s="42"/>
@@ -10968,7 +11050,7 @@
       <c r="M238" s="44"/>
       <c r="N238" s="44"/>
     </row>
-    <row r="239" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:17" ht="18" customHeight="1">
       <c r="A239" s="24"/>
       <c r="B239" s="44"/>
       <c r="C239" s="42"/>
@@ -10984,7 +11066,7 @@
       <c r="M239" s="44"/>
       <c r="N239" s="44"/>
     </row>
-    <row r="240" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:17" ht="18" customHeight="1">
       <c r="A240" s="24"/>
       <c r="B240" s="44"/>
       <c r="C240" s="42"/>
@@ -11000,7 +11082,7 @@
       <c r="M240" s="44"/>
       <c r="N240" s="44"/>
     </row>
-    <row r="241" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:14" ht="18" customHeight="1">
       <c r="A241" s="24"/>
       <c r="B241" s="44"/>
       <c r="C241" s="42"/>
@@ -11016,7 +11098,7 @@
       <c r="M241" s="44"/>
       <c r="N241" s="44"/>
     </row>
-    <row r="242" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:14" ht="18" customHeight="1">
       <c r="A242" s="24"/>
       <c r="B242" s="44"/>
       <c r="C242" s="42"/>
@@ -11032,7 +11114,7 @@
       <c r="M242" s="44"/>
       <c r="N242" s="44"/>
     </row>
-    <row r="243" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:14" ht="18" customHeight="1">
       <c r="A243" s="24"/>
       <c r="B243" s="44"/>
       <c r="C243" s="42"/>
@@ -11048,7 +11130,7 @@
       <c r="M243" s="44"/>
       <c r="N243" s="44"/>
     </row>
-    <row r="244" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:14" ht="18" customHeight="1">
       <c r="A244" s="24"/>
       <c r="B244" s="44"/>
       <c r="C244" s="42"/>
@@ -11064,7 +11146,7 @@
       <c r="M244" s="44"/>
       <c r="N244" s="44"/>
     </row>
-    <row r="245" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:14" ht="18" customHeight="1">
       <c r="A245" s="24"/>
       <c r="B245" s="44"/>
       <c r="C245" s="42"/>
@@ -11080,7 +11162,7 @@
       <c r="M245" s="44"/>
       <c r="N245" s="44"/>
     </row>
-    <row r="246" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:14" ht="18" customHeight="1">
       <c r="A246" s="24"/>
       <c r="B246" s="44"/>
       <c r="C246" s="42"/>
@@ -11096,7 +11178,7 @@
       <c r="M246" s="44"/>
       <c r="N246" s="44"/>
     </row>
-    <row r="247" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:14" ht="18" customHeight="1">
       <c r="A247" s="24"/>
       <c r="B247" s="44"/>
       <c r="C247" s="42"/>
@@ -11112,7 +11194,7 @@
       <c r="M247" s="44"/>
       <c r="N247" s="44"/>
     </row>
-    <row r="248" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:14" ht="18" customHeight="1">
       <c r="A248" s="24"/>
       <c r="B248" s="44"/>
       <c r="C248" s="42"/>
@@ -11128,7 +11210,7 @@
       <c r="M248" s="44"/>
       <c r="N248" s="44"/>
     </row>
-    <row r="249" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:14" ht="18" customHeight="1">
       <c r="A249" s="24"/>
       <c r="B249" s="44"/>
       <c r="C249" s="42"/>
@@ -11144,7 +11226,7 @@
       <c r="M249" s="44"/>
       <c r="N249" s="44"/>
     </row>
-    <row r="250" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:14" ht="18" customHeight="1">
       <c r="A250" s="24"/>
       <c r="B250" s="44"/>
       <c r="C250" s="42"/>
@@ -11160,7 +11242,7 @@
       <c r="M250" s="44"/>
       <c r="N250" s="44"/>
     </row>
-    <row r="251" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:14" ht="18" customHeight="1">
       <c r="A251" s="24"/>
       <c r="B251" s="44"/>
       <c r="C251" s="42"/>
@@ -11176,7 +11258,7 @@
       <c r="M251" s="44"/>
       <c r="N251" s="44"/>
     </row>
-    <row r="252" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:14" ht="18" customHeight="1">
       <c r="A252" s="24"/>
       <c r="B252" s="44"/>
       <c r="C252" s="42"/>
@@ -11192,7 +11274,7 @@
       <c r="M252" s="44"/>
       <c r="N252" s="44"/>
     </row>
-    <row r="253" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:14" ht="18" customHeight="1">
       <c r="A253" s="24"/>
       <c r="B253" s="44"/>
       <c r="C253" s="42"/>
@@ -11208,7 +11290,7 @@
       <c r="M253" s="44"/>
       <c r="N253" s="44"/>
     </row>
-    <row r="254" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:14" ht="18" customHeight="1">
       <c r="A254" s="24"/>
       <c r="B254" s="44"/>
       <c r="C254" s="42"/>
@@ -11224,7 +11306,7 @@
       <c r="M254" s="44"/>
       <c r="N254" s="44"/>
     </row>
-    <row r="255" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:14" ht="18" customHeight="1">
       <c r="A255" s="24"/>
       <c r="B255" s="44"/>
       <c r="C255" s="42"/>
@@ -11240,7 +11322,7 @@
       <c r="M255" s="44"/>
       <c r="N255" s="44"/>
     </row>
-    <row r="256" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:14" ht="18" customHeight="1">
       <c r="A256" s="24"/>
       <c r="B256" s="44"/>
       <c r="C256" s="42"/>
@@ -11256,7 +11338,7 @@
       <c r="M256" s="44"/>
       <c r="N256" s="44"/>
     </row>
-    <row r="257" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:14" ht="18" customHeight="1">
       <c r="A257" s="24"/>
       <c r="B257" s="44"/>
       <c r="C257" s="42"/>
@@ -11272,7 +11354,7 @@
       <c r="M257" s="44"/>
       <c r="N257" s="44"/>
     </row>
-    <row r="258" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:14" ht="18" customHeight="1">
       <c r="A258" s="24"/>
       <c r="B258" s="44"/>
       <c r="C258" s="42"/>
@@ -11288,7 +11370,7 @@
       <c r="M258" s="44"/>
       <c r="N258" s="44"/>
     </row>
-    <row r="259" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:14" ht="18" customHeight="1">
       <c r="A259" s="24"/>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
@@ -11302,7 +11384,7 @@
       <c r="M259" s="44"/>
       <c r="N259" s="44"/>
     </row>
-    <row r="260" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:14" ht="18" customHeight="1">
       <c r="A260" s="24"/>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
@@ -11316,7 +11398,7 @@
       <c r="M260" s="44"/>
       <c r="N260" s="44"/>
     </row>
-    <row r="261" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:14" ht="18" customHeight="1">
       <c r="A261" s="24"/>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
@@ -11330,7 +11412,7 @@
       <c r="M261" s="44"/>
       <c r="N261" s="44"/>
     </row>
-    <row r="262" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:14" ht="18" customHeight="1">
       <c r="A262" s="24"/>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
@@ -11344,7 +11426,7 @@
       <c r="M262" s="44"/>
       <c r="N262" s="44"/>
     </row>
-    <row r="263" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:14" ht="18" customHeight="1">
       <c r="A263" s="24"/>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
@@ -11358,7 +11440,7 @@
       <c r="M263" s="44"/>
       <c r="N263" s="44"/>
     </row>
-    <row r="264" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:14" ht="18" customHeight="1">
       <c r="A264" s="24"/>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
@@ -11372,7 +11454,7 @@
       <c r="M264" s="44"/>
       <c r="N264" s="44"/>
     </row>
-    <row r="265" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:14" ht="18" customHeight="1">
       <c r="A265" s="24"/>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
@@ -11386,7 +11468,7 @@
       <c r="M265" s="44"/>
       <c r="N265" s="44"/>
     </row>
-    <row r="266" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:14" ht="18" customHeight="1">
       <c r="A266" s="24"/>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
@@ -11400,7 +11482,7 @@
       <c r="M266" s="44"/>
       <c r="N266" s="44"/>
     </row>
-    <row r="267" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:14" ht="18" customHeight="1">
       <c r="A267" s="24"/>
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
@@ -11414,7 +11496,7 @@
       <c r="M267" s="44"/>
       <c r="N267" s="44"/>
     </row>
-    <row r="268" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:14" ht="18" customHeight="1">
       <c r="A268" s="24"/>
       <c r="C268" s="2"/>
       <c r="D268" s="2"/>
@@ -11428,7 +11510,7 @@
       <c r="M268" s="44"/>
       <c r="N268" s="44"/>
     </row>
-    <row r="269" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:14" ht="18" customHeight="1">
       <c r="A269" s="24"/>
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
@@ -11442,7 +11524,7 @@
       <c r="M269" s="44"/>
       <c r="N269" s="44"/>
     </row>
-    <row r="270" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:14" ht="18" customHeight="1">
       <c r="A270" s="24"/>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
@@ -11456,7 +11538,7 @@
       <c r="M270" s="44"/>
       <c r="N270" s="44"/>
     </row>
-    <row r="271" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:14" ht="18" customHeight="1">
       <c r="A271" s="24"/>
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
@@ -11470,7 +11552,7 @@
       <c r="M271" s="44"/>
       <c r="N271" s="44"/>
     </row>
-    <row r="272" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:14" ht="18" customHeight="1">
       <c r="A272" s="24"/>
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
@@ -11484,7 +11566,7 @@
       <c r="M272" s="44"/>
       <c r="N272" s="44"/>
     </row>
-    <row r="273" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:14" ht="18" customHeight="1">
       <c r="A273" s="24"/>
       <c r="C273" s="2"/>
       <c r="D273" s="2"/>
@@ -11498,7 +11580,7 @@
       <c r="M273" s="44"/>
       <c r="N273" s="44"/>
     </row>
-    <row r="274" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:14" ht="18" customHeight="1">
       <c r="A274" s="24"/>
       <c r="C274" s="2"/>
       <c r="D274" s="2"/>
@@ -11512,7 +11594,7 @@
       <c r="M274" s="44"/>
       <c r="N274" s="44"/>
     </row>
-    <row r="275" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:14" ht="18" customHeight="1">
       <c r="A275" s="24"/>
       <c r="C275" s="2"/>
       <c r="D275" s="2"/>
@@ -11526,7 +11608,7 @@
       <c r="M275" s="44"/>
       <c r="N275" s="44"/>
     </row>
-    <row r="276" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:14" ht="18" customHeight="1">
       <c r="A276" s="24"/>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
@@ -11540,7 +11622,7 @@
       <c r="M276" s="44"/>
       <c r="N276" s="44"/>
     </row>
-    <row r="277" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:14" ht="18" customHeight="1">
       <c r="A277" s="24"/>
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
@@ -11554,7 +11636,7 @@
       <c r="M277" s="44"/>
       <c r="N277" s="44"/>
     </row>
-    <row r="278" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:14" ht="18" customHeight="1">
       <c r="A278" s="24"/>
       <c r="C278" s="2"/>
       <c r="D278" s="2"/>
@@ -11568,7 +11650,7 @@
       <c r="M278" s="44"/>
       <c r="N278" s="44"/>
     </row>
-    <row r="279" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:14" ht="18" customHeight="1">
       <c r="A279" s="24"/>
       <c r="C279" s="2"/>
       <c r="D279" s="2"/>
@@ -11582,7 +11664,7 @@
       <c r="M279" s="44"/>
       <c r="N279" s="44"/>
     </row>
-    <row r="280" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:14" ht="18" customHeight="1">
       <c r="A280" s="24"/>
       <c r="C280" s="2"/>
       <c r="D280" s="2"/>
@@ -11596,7 +11678,7 @@
       <c r="M280" s="44"/>
       <c r="N280" s="44"/>
     </row>
-    <row r="281" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:14" ht="18" customHeight="1">
       <c r="A281" s="24"/>
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
@@ -11610,7 +11692,7 @@
       <c r="M281" s="44"/>
       <c r="N281" s="44"/>
     </row>
-    <row r="282" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:14" ht="18" customHeight="1">
       <c r="A282" s="24"/>
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
@@ -11624,7 +11706,7 @@
       <c r="M282" s="44"/>
       <c r="N282" s="44"/>
     </row>
-    <row r="283" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:14" ht="18" customHeight="1">
       <c r="A283" s="24"/>
       <c r="C283" s="2"/>
       <c r="D283" s="2"/>
@@ -11638,7 +11720,7 @@
       <c r="M283" s="44"/>
       <c r="N283" s="44"/>
     </row>
-    <row r="284" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:14" ht="18" customHeight="1">
       <c r="A284" s="24"/>
       <c r="C284" s="2"/>
       <c r="D284" s="2"/>
@@ -11652,7 +11734,7 @@
       <c r="M284" s="44"/>
       <c r="N284" s="44"/>
     </row>
-    <row r="285" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:14" ht="18" customHeight="1">
       <c r="A285" s="24"/>
       <c r="C285" s="2"/>
       <c r="D285" s="2"/>
@@ -11666,7 +11748,7 @@
       <c r="M285" s="44"/>
       <c r="N285" s="44"/>
     </row>
-    <row r="286" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:14" ht="18" customHeight="1">
       <c r="A286" s="24"/>
       <c r="C286" s="2"/>
       <c r="D286" s="2"/>
@@ -11680,7 +11762,7 @@
       <c r="M286" s="44"/>
       <c r="N286" s="44"/>
     </row>
-    <row r="287" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:14" ht="18" customHeight="1">
       <c r="A287" s="24"/>
       <c r="C287" s="2"/>
       <c r="D287" s="2"/>
@@ -11694,7 +11776,7 @@
       <c r="M287" s="44"/>
       <c r="N287" s="44"/>
     </row>
-    <row r="288" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:14" ht="18" customHeight="1">
       <c r="A288" s="24"/>
       <c r="C288" s="2"/>
       <c r="D288" s="2"/>
@@ -11708,7 +11790,7 @@
       <c r="M288" s="44"/>
       <c r="N288" s="44"/>
     </row>
-    <row r="289" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:14" ht="18" customHeight="1">
       <c r="A289" s="24"/>
       <c r="C289" s="2"/>
       <c r="D289" s="2"/>
@@ -11722,7 +11804,7 @@
       <c r="M289" s="44"/>
       <c r="N289" s="44"/>
     </row>
-    <row r="290" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:14" ht="18" customHeight="1">
       <c r="A290" s="24"/>
       <c r="C290" s="2"/>
       <c r="D290" s="2"/>
@@ -11736,7 +11818,7 @@
       <c r="M290" s="44"/>
       <c r="N290" s="44"/>
     </row>
-    <row r="291" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:14" ht="18" customHeight="1">
       <c r="A291" s="24"/>
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
@@ -11750,7 +11832,7 @@
       <c r="M291" s="44"/>
       <c r="N291" s="44"/>
     </row>
-    <row r="292" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:14" ht="18" customHeight="1">
       <c r="A292" s="24"/>
       <c r="C292" s="2"/>
       <c r="D292" s="2"/>
@@ -11764,7 +11846,7 @@
       <c r="M292" s="44"/>
       <c r="N292" s="44"/>
     </row>
-    <row r="293" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:14" ht="18" customHeight="1">
       <c r="A293" s="24"/>
       <c r="C293" s="2"/>
       <c r="D293" s="2"/>
@@ -11778,7 +11860,7 @@
       <c r="M293" s="44"/>
       <c r="N293" s="44"/>
     </row>
-    <row r="294" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:14" ht="18" customHeight="1">
       <c r="A294" s="24"/>
       <c r="C294" s="2"/>
       <c r="D294" s="2"/>
@@ -11792,7 +11874,7 @@
       <c r="M294" s="44"/>
       <c r="N294" s="44"/>
     </row>
-    <row r="295" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:14" ht="18" customHeight="1">
       <c r="A295" s="24"/>
       <c r="C295" s="2"/>
       <c r="D295" s="2"/>
@@ -11806,7 +11888,7 @@
       <c r="M295" s="44"/>
       <c r="N295" s="44"/>
     </row>
-    <row r="296" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:14" ht="18" customHeight="1">
       <c r="A296" s="24"/>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
@@ -11820,7 +11902,7 @@
       <c r="M296" s="44"/>
       <c r="N296" s="44"/>
     </row>
-    <row r="297" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:14" ht="18" customHeight="1">
       <c r="A297" s="24"/>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
@@ -11834,7 +11916,7 @@
       <c r="M297" s="44"/>
       <c r="N297" s="44"/>
     </row>
-    <row r="298" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:14" ht="18" customHeight="1">
       <c r="A298" s="24"/>
       <c r="C298" s="2"/>
       <c r="D298" s="2"/>
@@ -11848,7 +11930,7 @@
       <c r="M298" s="44"/>
       <c r="N298" s="44"/>
     </row>
-    <row r="299" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:14" ht="18" customHeight="1">
       <c r="A299" s="24"/>
       <c r="C299" s="2"/>
       <c r="D299" s="2"/>
@@ -11862,7 +11944,7 @@
       <c r="M299" s="44"/>
       <c r="N299" s="44"/>
     </row>
-    <row r="300" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:14" ht="18" customHeight="1">
       <c r="A300" s="24"/>
       <c r="C300" s="2"/>
       <c r="D300" s="2"/>
@@ -11876,7 +11958,7 @@
       <c r="M300" s="44"/>
       <c r="N300" s="44"/>
     </row>
-    <row r="301" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:14" ht="18" customHeight="1">
       <c r="A301" s="24"/>
       <c r="C301" s="2"/>
       <c r="D301" s="2"/>
@@ -11890,7 +11972,7 @@
       <c r="M301" s="44"/>
       <c r="N301" s="44"/>
     </row>
-    <row r="302" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:14" ht="18" customHeight="1">
       <c r="A302" s="24"/>
       <c r="C302" s="2"/>
       <c r="D302" s="2"/>
@@ -11904,7 +11986,7 @@
       <c r="M302" s="44"/>
       <c r="N302" s="44"/>
     </row>
-    <row r="303" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:14" ht="18" customHeight="1">
       <c r="A303" s="24"/>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
@@ -11918,7 +12000,7 @@
       <c r="M303" s="44"/>
       <c r="N303" s="44"/>
     </row>
-    <row r="304" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:14" ht="18" customHeight="1">
       <c r="A304" s="24"/>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
@@ -11932,7 +12014,7 @@
       <c r="M304" s="44"/>
       <c r="N304" s="44"/>
     </row>
-    <row r="305" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:14" ht="18" customHeight="1">
       <c r="A305" s="24"/>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
@@ -11946,7 +12028,7 @@
       <c r="M305" s="44"/>
       <c r="N305" s="44"/>
     </row>
-    <row r="306" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:14" ht="18" customHeight="1">
       <c r="A306" s="44"/>
       <c r="C306" s="2"/>
       <c r="D306" s="2"/>
@@ -11960,7 +12042,7 @@
       <c r="M306" s="44"/>
       <c r="N306" s="44"/>
     </row>
-    <row r="307" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:14" ht="18" customHeight="1">
       <c r="A307" s="44"/>
       <c r="C307" s="2"/>
       <c r="D307" s="2"/>
@@ -11974,7 +12056,7 @@
       <c r="M307" s="44"/>
       <c r="N307" s="44"/>
     </row>
-    <row r="308" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:14" ht="18" customHeight="1">
       <c r="A308" s="44"/>
       <c r="C308" s="2"/>
       <c r="D308" s="2"/>
@@ -11988,7 +12070,7 @@
       <c r="M308" s="44"/>
       <c r="N308" s="44"/>
     </row>
-    <row r="309" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:14" ht="18" customHeight="1">
       <c r="A309" s="44"/>
       <c r="C309" s="2"/>
       <c r="D309" s="2"/>
@@ -12002,7 +12084,7 @@
       <c r="M309" s="44"/>
       <c r="N309" s="44"/>
     </row>
-    <row r="310" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:14" ht="18" customHeight="1">
       <c r="A310" s="44"/>
       <c r="C310" s="2"/>
       <c r="D310" s="2"/>
@@ -12016,7 +12098,7 @@
       <c r="M310" s="44"/>
       <c r="N310" s="44"/>
     </row>
-    <row r="311" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:14" ht="18" customHeight="1">
       <c r="A311" s="44"/>
       <c r="C311" s="2"/>
       <c r="D311" s="2"/>
@@ -12030,7 +12112,7 @@
       <c r="M311" s="44"/>
       <c r="N311" s="44"/>
     </row>
-    <row r="312" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:14" ht="18" customHeight="1">
       <c r="A312" s="44"/>
       <c r="C312" s="2"/>
       <c r="D312" s="2"/>
@@ -12044,7 +12126,7 @@
       <c r="M312" s="44"/>
       <c r="N312" s="44"/>
     </row>
-    <row r="313" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:14" ht="18" customHeight="1">
       <c r="A313" s="44"/>
       <c r="C313" s="2"/>
       <c r="D313" s="2"/>
@@ -12058,7 +12140,7 @@
       <c r="M313" s="44"/>
       <c r="N313" s="44"/>
     </row>
-    <row r="314" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:14" ht="18" customHeight="1">
       <c r="A314" s="44"/>
       <c r="C314" s="2"/>
       <c r="D314" s="2"/>
@@ -12072,7 +12154,7 @@
       <c r="M314" s="44"/>
       <c r="N314" s="44"/>
     </row>
-    <row r="315" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:14" ht="18" customHeight="1">
       <c r="A315" s="44"/>
       <c r="C315" s="2"/>
       <c r="D315" s="2"/>
@@ -12086,7 +12168,7 @@
       <c r="M315" s="44"/>
       <c r="N315" s="44"/>
     </row>
-    <row r="316" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:14" ht="18" customHeight="1">
       <c r="A316" s="44"/>
       <c r="C316" s="2"/>
       <c r="D316" s="2"/>
@@ -12100,7 +12182,7 @@
       <c r="M316" s="44"/>
       <c r="N316" s="44"/>
     </row>
-    <row r="317" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:14" ht="18" customHeight="1">
       <c r="A317" s="44"/>
       <c r="C317" s="2"/>
       <c r="D317" s="2"/>
@@ -12114,7 +12196,7 @@
       <c r="M317" s="44"/>
       <c r="N317" s="44"/>
     </row>
-    <row r="318" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:14" ht="18" customHeight="1">
       <c r="A318" s="44"/>
       <c r="C318" s="2"/>
       <c r="D318" s="2"/>
@@ -12128,7 +12210,7 @@
       <c r="M318" s="44"/>
       <c r="N318" s="44"/>
     </row>
-    <row r="319" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:14" ht="18" customHeight="1">
       <c r="A319" s="44"/>
       <c r="C319" s="2"/>
       <c r="D319" s="2"/>
@@ -12142,7 +12224,7 @@
       <c r="M319" s="44"/>
       <c r="N319" s="44"/>
     </row>
-    <row r="320" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:14" ht="18" customHeight="1">
       <c r="A320" s="44"/>
       <c r="C320" s="2"/>
       <c r="D320" s="2"/>
@@ -12156,7 +12238,7 @@
       <c r="M320" s="44"/>
       <c r="N320" s="44"/>
     </row>
-    <row r="321" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:14" ht="18" customHeight="1">
       <c r="A321" s="44"/>
       <c r="C321" s="2"/>
       <c r="D321" s="2"/>
@@ -12170,7 +12252,7 @@
       <c r="M321" s="44"/>
       <c r="N321" s="44"/>
     </row>
-    <row r="322" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:14" ht="18" customHeight="1">
       <c r="A322" s="44"/>
       <c r="C322" s="2"/>
       <c r="D322" s="2"/>
@@ -12184,7 +12266,7 @@
       <c r="M322" s="44"/>
       <c r="N322" s="44"/>
     </row>
-    <row r="323" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:14" ht="18" customHeight="1">
       <c r="A323" s="44"/>
       <c r="C323" s="2"/>
       <c r="D323" s="2"/>
@@ -12198,7 +12280,7 @@
       <c r="M323" s="44"/>
       <c r="N323" s="44"/>
     </row>
-    <row r="324" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:14" ht="18" customHeight="1">
       <c r="A324" s="44"/>
       <c r="C324" s="2"/>
       <c r="D324" s="2"/>
@@ -12212,7 +12294,7 @@
       <c r="M324" s="44"/>
       <c r="N324" s="44"/>
     </row>
-    <row r="325" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:14" ht="18" customHeight="1">
       <c r="A325" s="44"/>
       <c r="C325" s="2"/>
       <c r="D325" s="2"/>
@@ -12226,7 +12308,7 @@
       <c r="M325" s="44"/>
       <c r="N325" s="44"/>
     </row>
-    <row r="326" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:14" ht="18" customHeight="1">
       <c r="A326" s="44"/>
       <c r="C326" s="2"/>
       <c r="D326" s="2"/>
@@ -12240,7 +12322,7 @@
       <c r="M326" s="44"/>
       <c r="N326" s="44"/>
     </row>
-    <row r="327" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:14" ht="18" customHeight="1">
       <c r="A327" s="44"/>
       <c r="C327" s="2"/>
       <c r="D327" s="2"/>
@@ -12254,7 +12336,7 @@
       <c r="M327" s="44"/>
       <c r="N327" s="44"/>
     </row>
-    <row r="328" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:14" ht="18" customHeight="1">
       <c r="A328" s="44"/>
       <c r="C328" s="2"/>
       <c r="D328" s="2"/>
@@ -12268,7 +12350,7 @@
       <c r="M328" s="44"/>
       <c r="N328" s="44"/>
     </row>
-    <row r="329" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:14" ht="18" customHeight="1">
       <c r="A329" s="44"/>
       <c r="C329" s="2"/>
       <c r="D329" s="2"/>
@@ -12282,7 +12364,7 @@
       <c r="M329" s="44"/>
       <c r="N329" s="44"/>
     </row>
-    <row r="330" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:14" ht="18" customHeight="1">
       <c r="A330" s="44"/>
       <c r="C330" s="2"/>
       <c r="D330" s="2"/>
@@ -12296,7 +12378,7 @@
       <c r="M330" s="44"/>
       <c r="N330" s="44"/>
     </row>
-    <row r="331" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:14" ht="18" customHeight="1">
       <c r="A331" s="44"/>
       <c r="C331" s="2"/>
       <c r="D331" s="2"/>
@@ -12310,7 +12392,7 @@
       <c r="M331" s="44"/>
       <c r="N331" s="44"/>
     </row>
-    <row r="332" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:14" ht="18" customHeight="1">
       <c r="A332" s="44"/>
       <c r="C332" s="2"/>
       <c r="D332" s="2"/>
@@ -12324,7 +12406,7 @@
       <c r="M332" s="44"/>
       <c r="N332" s="44"/>
     </row>
-    <row r="333" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:14" ht="18" customHeight="1">
       <c r="A333" s="44"/>
       <c r="C333" s="2"/>
       <c r="D333" s="2"/>
@@ -12338,7 +12420,7 @@
       <c r="M333" s="44"/>
       <c r="N333" s="44"/>
     </row>
-    <row r="334" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:14" ht="18" customHeight="1">
       <c r="A334" s="44"/>
       <c r="C334" s="2"/>
       <c r="D334" s="2"/>
@@ -12352,7 +12434,7 @@
       <c r="M334" s="44"/>
       <c r="N334" s="44"/>
     </row>
-    <row r="335" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:14" ht="18" customHeight="1">
       <c r="A335" s="44"/>
       <c r="C335" s="2"/>
       <c r="D335" s="2"/>
@@ -12366,7 +12448,7 @@
       <c r="M335" s="44"/>
       <c r="N335" s="44"/>
     </row>
-    <row r="336" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:14" ht="18" customHeight="1">
       <c r="A336" s="44"/>
       <c r="C336" s="2"/>
       <c r="D336" s="2"/>
@@ -12380,7 +12462,7 @@
       <c r="M336" s="44"/>
       <c r="N336" s="44"/>
     </row>
-    <row r="337" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:14" ht="18" customHeight="1">
       <c r="A337" s="44"/>
       <c r="C337" s="2"/>
       <c r="D337" s="2"/>
@@ -12394,7 +12476,7 @@
       <c r="M337" s="44"/>
       <c r="N337" s="44"/>
     </row>
-    <row r="338" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:14" ht="18" customHeight="1">
       <c r="A338" s="44"/>
       <c r="C338" s="2"/>
       <c r="D338" s="2"/>
@@ -12408,7 +12490,7 @@
       <c r="M338" s="44"/>
       <c r="N338" s="44"/>
     </row>
-    <row r="339" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:14" ht="18" customHeight="1">
       <c r="A339" s="44"/>
       <c r="C339" s="2"/>
       <c r="D339" s="2"/>
@@ -12422,7 +12504,7 @@
       <c r="M339" s="44"/>
       <c r="N339" s="44"/>
     </row>
-    <row r="340" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:14" ht="18" customHeight="1">
       <c r="A340" s="44"/>
       <c r="C340" s="2"/>
       <c r="D340" s="2"/>
@@ -12436,7 +12518,7 @@
       <c r="M340" s="44"/>
       <c r="N340" s="44"/>
     </row>
-    <row r="341" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:14" ht="18" customHeight="1">
       <c r="A341" s="44"/>
       <c r="C341" s="2"/>
       <c r="D341" s="2"/>
@@ -12450,7 +12532,7 @@
       <c r="M341" s="44"/>
       <c r="N341" s="44"/>
     </row>
-    <row r="342" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:14" ht="18" customHeight="1">
       <c r="A342" s="44"/>
       <c r="C342" s="2"/>
       <c r="D342" s="2"/>
@@ -12464,7 +12546,7 @@
       <c r="M342" s="44"/>
       <c r="N342" s="44"/>
     </row>
-    <row r="343" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:14" ht="18" customHeight="1">
       <c r="A343" s="44"/>
       <c r="C343" s="2"/>
       <c r="D343" s="2"/>
@@ -12478,7 +12560,7 @@
       <c r="M343" s="44"/>
       <c r="N343" s="44"/>
     </row>
-    <row r="344" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:14" ht="18" customHeight="1">
       <c r="A344" s="44"/>
       <c r="C344" s="2"/>
       <c r="D344" s="2"/>
@@ -12492,7 +12574,7 @@
       <c r="M344" s="44"/>
       <c r="N344" s="44"/>
     </row>
-    <row r="345" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:14" ht="18" customHeight="1">
       <c r="A345" s="44"/>
       <c r="C345" s="2"/>
       <c r="D345" s="2"/>
@@ -12506,7 +12588,7 @@
       <c r="M345" s="44"/>
       <c r="N345" s="44"/>
     </row>
-    <row r="346" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:14" ht="18" customHeight="1">
       <c r="A346" s="44"/>
       <c r="C346" s="2"/>
       <c r="D346" s="2"/>
@@ -12520,7 +12602,7 @@
       <c r="M346" s="44"/>
       <c r="N346" s="44"/>
     </row>
-    <row r="347" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:14" ht="18" customHeight="1">
       <c r="A347" s="44"/>
       <c r="C347" s="2"/>
       <c r="D347" s="2"/>
@@ -12534,7 +12616,7 @@
       <c r="M347" s="44"/>
       <c r="N347" s="44"/>
     </row>
-    <row r="348" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:14" ht="18" customHeight="1">
       <c r="A348" s="44"/>
       <c r="C348" s="2"/>
       <c r="D348" s="2"/>
@@ -12548,7 +12630,7 @@
       <c r="M348" s="44"/>
       <c r="N348" s="44"/>
     </row>
-    <row r="349" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:14" ht="18" customHeight="1">
       <c r="A349" s="44"/>
       <c r="C349" s="2"/>
       <c r="D349" s="2"/>
@@ -12562,7 +12644,7 @@
       <c r="M349" s="44"/>
       <c r="N349" s="44"/>
     </row>
-    <row r="350" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:14" ht="18" customHeight="1">
       <c r="A350" s="44"/>
       <c r="C350" s="2"/>
       <c r="D350" s="2"/>
@@ -12576,7 +12658,7 @@
       <c r="M350" s="44"/>
       <c r="N350" s="44"/>
     </row>
-    <row r="351" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:14" ht="18" customHeight="1">
       <c r="A351" s="44"/>
       <c r="C351" s="2"/>
       <c r="D351" s="2"/>
@@ -12590,7 +12672,7 @@
       <c r="M351" s="44"/>
       <c r="N351" s="44"/>
     </row>
-    <row r="352" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:14" ht="18" customHeight="1">
       <c r="A352" s="44"/>
       <c r="C352" s="2"/>
       <c r="D352" s="2"/>
@@ -12604,7 +12686,7 @@
       <c r="M352" s="44"/>
       <c r="N352" s="44"/>
     </row>
-    <row r="353" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:14" ht="18" customHeight="1">
       <c r="A353" s="44"/>
       <c r="C353" s="2"/>
       <c r="D353" s="2"/>
@@ -12618,7 +12700,7 @@
       <c r="M353" s="44"/>
       <c r="N353" s="44"/>
     </row>
-    <row r="354" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:14" ht="18" customHeight="1">
       <c r="A354" s="44"/>
       <c r="C354" s="2"/>
       <c r="D354" s="2"/>
@@ -12632,7 +12714,7 @@
       <c r="M354" s="44"/>
       <c r="N354" s="44"/>
     </row>
-    <row r="355" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:14" ht="18" customHeight="1">
       <c r="A355" s="44"/>
       <c r="C355" s="2"/>
       <c r="D355" s="2"/>
@@ -12646,7 +12728,7 @@
       <c r="M355" s="44"/>
       <c r="N355" s="44"/>
     </row>
-    <row r="356" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:14" ht="18" customHeight="1">
       <c r="A356" s="44"/>
       <c r="C356" s="2"/>
       <c r="D356" s="2"/>
@@ -12660,7 +12742,7 @@
       <c r="M356" s="44"/>
       <c r="N356" s="44"/>
     </row>
-    <row r="357" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:14" ht="18" customHeight="1">
       <c r="A357" s="44"/>
       <c r="C357" s="2"/>
       <c r="D357" s="2"/>
@@ -12674,7 +12756,7 @@
       <c r="M357" s="44"/>
       <c r="N357" s="44"/>
     </row>
-    <row r="358" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:14" ht="18" customHeight="1">
       <c r="A358" s="44"/>
       <c r="C358" s="2"/>
       <c r="D358" s="2"/>
@@ -12688,7 +12770,7 @@
       <c r="M358" s="44"/>
       <c r="N358" s="44"/>
     </row>
-    <row r="359" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:14" ht="18" customHeight="1">
       <c r="A359" s="44"/>
       <c r="C359" s="2"/>
       <c r="D359" s="2"/>
@@ -12702,7 +12784,7 @@
       <c r="M359" s="44"/>
       <c r="N359" s="44"/>
     </row>
-    <row r="360" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:14" ht="18" customHeight="1">
       <c r="A360" s="44"/>
       <c r="C360" s="2"/>
       <c r="D360" s="2"/>
@@ -12716,7 +12798,7 @@
       <c r="M360" s="44"/>
       <c r="N360" s="44"/>
     </row>
-    <row r="361" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:14" ht="18" customHeight="1">
       <c r="A361" s="44"/>
       <c r="C361" s="2"/>
       <c r="D361" s="2"/>
@@ -12730,7 +12812,7 @@
       <c r="M361" s="44"/>
       <c r="N361" s="44"/>
     </row>
-    <row r="362" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:14" ht="18" customHeight="1">
       <c r="A362" s="44"/>
       <c r="C362" s="2"/>
       <c r="D362" s="2"/>
@@ -12744,7 +12826,7 @@
       <c r="M362" s="44"/>
       <c r="N362" s="44"/>
     </row>
-    <row r="363" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:14" ht="18" customHeight="1">
       <c r="A363" s="44"/>
       <c r="C363" s="2"/>
       <c r="D363" s="2"/>
@@ -12758,7 +12840,7 @@
       <c r="M363" s="44"/>
       <c r="N363" s="44"/>
     </row>
-    <row r="364" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:14" ht="18" customHeight="1">
       <c r="A364" s="44"/>
       <c r="C364" s="2"/>
       <c r="D364" s="2"/>
@@ -12772,7 +12854,7 @@
       <c r="M364" s="44"/>
       <c r="N364" s="44"/>
     </row>
-    <row r="365" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:14" ht="18" customHeight="1">
       <c r="A365" s="44"/>
       <c r="C365" s="2"/>
       <c r="D365" s="2"/>
@@ -12786,7 +12868,7 @@
       <c r="M365" s="44"/>
       <c r="N365" s="44"/>
     </row>
-    <row r="366" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:14" ht="18" customHeight="1">
       <c r="A366" s="44"/>
       <c r="C366" s="2"/>
       <c r="D366" s="2"/>
@@ -12800,7 +12882,7 @@
       <c r="M366" s="44"/>
       <c r="N366" s="44"/>
     </row>
-    <row r="367" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:14" ht="18" customHeight="1">
       <c r="A367" s="44"/>
       <c r="C367" s="2"/>
       <c r="D367" s="2"/>
@@ -12814,7 +12896,7 @@
       <c r="M367" s="44"/>
       <c r="N367" s="44"/>
     </row>
-    <row r="368" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:14" ht="18" customHeight="1">
       <c r="A368" s="44"/>
       <c r="C368" s="2"/>
       <c r="D368" s="2"/>
@@ -12828,7 +12910,7 @@
       <c r="M368" s="44"/>
       <c r="N368" s="44"/>
     </row>
-    <row r="369" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:14" ht="18" customHeight="1">
       <c r="A369" s="44"/>
       <c r="C369" s="2"/>
       <c r="D369" s="2"/>
@@ -12842,7 +12924,7 @@
       <c r="M369" s="44"/>
       <c r="N369" s="44"/>
     </row>
-    <row r="370" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:14" ht="18" customHeight="1">
       <c r="A370" s="44"/>
       <c r="C370" s="2"/>
       <c r="D370" s="2"/>
@@ -12856,7 +12938,7 @@
       <c r="M370" s="44"/>
       <c r="N370" s="44"/>
     </row>
-    <row r="371" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:14" ht="18" customHeight="1">
       <c r="A371" s="44"/>
       <c r="C371" s="2"/>
       <c r="D371" s="2"/>
@@ -12870,7 +12952,7 @@
       <c r="M371" s="44"/>
       <c r="N371" s="44"/>
     </row>
-    <row r="372" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:14" ht="18" customHeight="1">
       <c r="A372" s="44"/>
       <c r="C372" s="2"/>
       <c r="D372" s="2"/>
@@ -12884,7 +12966,7 @@
       <c r="M372" s="44"/>
       <c r="N372" s="44"/>
     </row>
-    <row r="373" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:14" ht="18" customHeight="1">
       <c r="A373" s="44"/>
       <c r="C373" s="2"/>
       <c r="D373" s="2"/>
@@ -12898,7 +12980,7 @@
       <c r="M373" s="44"/>
       <c r="N373" s="44"/>
     </row>
-    <row r="374" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:14" ht="18" customHeight="1">
       <c r="A374" s="44"/>
       <c r="C374" s="2"/>
       <c r="D374" s="2"/>
@@ -12912,7 +12994,7 @@
       <c r="M374" s="44"/>
       <c r="N374" s="44"/>
     </row>
-    <row r="375" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:14" ht="18" customHeight="1">
       <c r="A375" s="44"/>
       <c r="C375" s="2"/>
       <c r="D375" s="2"/>
@@ -12926,7 +13008,7 @@
       <c r="M375" s="44"/>
       <c r="N375" s="44"/>
     </row>
-    <row r="376" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:14" ht="18" customHeight="1">
       <c r="A376" s="44"/>
       <c r="C376" s="2"/>
       <c r="D376" s="2"/>
@@ -12940,7 +13022,7 @@
       <c r="M376" s="44"/>
       <c r="N376" s="44"/>
     </row>
-    <row r="377" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:14" ht="18" customHeight="1">
       <c r="A377" s="44"/>
       <c r="C377" s="2"/>
       <c r="D377" s="2"/>
@@ -12954,7 +13036,7 @@
       <c r="M377" s="44"/>
       <c r="N377" s="44"/>
     </row>
-    <row r="378" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:14" ht="18" customHeight="1">
       <c r="A378" s="44"/>
       <c r="C378" s="2"/>
       <c r="D378" s="2"/>
@@ -12968,7 +13050,7 @@
       <c r="M378" s="44"/>
       <c r="N378" s="44"/>
     </row>
-    <row r="379" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:14" ht="18" customHeight="1">
       <c r="A379" s="44"/>
       <c r="C379" s="2"/>
       <c r="D379" s="2"/>
@@ -12982,7 +13064,7 @@
       <c r="M379" s="44"/>
       <c r="N379" s="44"/>
     </row>
-    <row r="380" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:14" ht="18" customHeight="1">
       <c r="A380" s="44"/>
       <c r="C380" s="2"/>
       <c r="D380" s="2"/>
@@ -12996,7 +13078,7 @@
       <c r="M380" s="44"/>
       <c r="N380" s="44"/>
     </row>
-    <row r="381" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:14" ht="18" customHeight="1">
       <c r="A381" s="44"/>
       <c r="C381" s="2"/>
       <c r="D381" s="2"/>
@@ -13010,7 +13092,7 @@
       <c r="M381" s="44"/>
       <c r="N381" s="44"/>
     </row>
-    <row r="382" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:14" ht="18" customHeight="1">
       <c r="A382" s="44"/>
       <c r="C382" s="2"/>
       <c r="D382" s="2"/>
@@ -13024,7 +13106,7 @@
       <c r="M382" s="44"/>
       <c r="N382" s="44"/>
     </row>
-    <row r="383" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:14" ht="18" customHeight="1">
       <c r="A383" s="44"/>
       <c r="C383" s="2"/>
       <c r="D383" s="2"/>
@@ -13038,7 +13120,7 @@
       <c r="M383" s="44"/>
       <c r="N383" s="44"/>
     </row>
-    <row r="384" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:14" ht="18" customHeight="1">
       <c r="A384" s="44"/>
       <c r="C384" s="2"/>
       <c r="D384" s="2"/>
@@ -13052,7 +13134,7 @@
       <c r="M384" s="44"/>
       <c r="N384" s="44"/>
     </row>
-    <row r="385" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:14" ht="18" customHeight="1">
       <c r="A385" s="44"/>
       <c r="C385" s="2"/>
       <c r="D385" s="2"/>
@@ -13066,7 +13148,7 @@
       <c r="M385" s="44"/>
       <c r="N385" s="44"/>
     </row>
-    <row r="386" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:14" ht="18" customHeight="1">
       <c r="A386" s="44"/>
       <c r="C386" s="2"/>
       <c r="D386" s="2"/>
@@ -13080,7 +13162,7 @@
       <c r="M386" s="44"/>
       <c r="N386" s="44"/>
     </row>
-    <row r="387" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:14" ht="18" customHeight="1">
       <c r="A387" s="44"/>
       <c r="C387" s="2"/>
       <c r="D387" s="2"/>
@@ -13094,7 +13176,7 @@
       <c r="M387" s="44"/>
       <c r="N387" s="44"/>
     </row>
-    <row r="388" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:14" ht="18" customHeight="1">
       <c r="A388" s="44"/>
       <c r="C388" s="2"/>
       <c r="D388" s="2"/>
@@ -13108,7 +13190,7 @@
       <c r="M388" s="44"/>
       <c r="N388" s="44"/>
     </row>
-    <row r="389" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:14" ht="18" customHeight="1">
       <c r="A389" s="44"/>
       <c r="C389" s="2"/>
       <c r="D389" s="2"/>
@@ -13122,7 +13204,7 @@
       <c r="M389" s="44"/>
       <c r="N389" s="44"/>
     </row>
-    <row r="390" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:14" ht="18" customHeight="1">
       <c r="A390" s="44"/>
       <c r="C390" s="2"/>
       <c r="D390" s="2"/>
@@ -13136,7 +13218,7 @@
       <c r="M390" s="44"/>
       <c r="N390" s="44"/>
     </row>
-    <row r="391" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:14" ht="18" customHeight="1">
       <c r="A391" s="44"/>
       <c r="C391" s="2"/>
       <c r="D391" s="2"/>
@@ -13150,7 +13232,7 @@
       <c r="M391" s="44"/>
       <c r="N391" s="44"/>
     </row>
-    <row r="392" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:14" ht="18" customHeight="1">
       <c r="A392" s="44"/>
       <c r="C392" s="2"/>
       <c r="D392" s="2"/>
@@ -13164,7 +13246,7 @@
       <c r="M392" s="44"/>
       <c r="N392" s="44"/>
     </row>
-    <row r="393" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:14" ht="18" customHeight="1">
       <c r="A393" s="44"/>
       <c r="C393" s="2"/>
       <c r="D393" s="2"/>
@@ -13178,7 +13260,7 @@
       <c r="M393" s="44"/>
       <c r="N393" s="44"/>
     </row>
-    <row r="394" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:14" ht="18" customHeight="1">
       <c r="A394" s="44"/>
       <c r="C394" s="2"/>
       <c r="D394" s="2"/>
@@ -13192,7 +13274,7 @@
       <c r="M394" s="44"/>
       <c r="N394" s="44"/>
     </row>
-    <row r="395" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:14" ht="18" customHeight="1">
       <c r="A395" s="44"/>
       <c r="C395" s="2"/>
       <c r="D395" s="2"/>
@@ -13206,7 +13288,7 @@
       <c r="M395" s="44"/>
       <c r="N395" s="44"/>
     </row>
-    <row r="396" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:14" ht="18" customHeight="1">
       <c r="A396" s="44"/>
       <c r="C396" s="2"/>
       <c r="D396" s="2"/>
@@ -13220,7 +13302,7 @@
       <c r="M396" s="44"/>
       <c r="N396" s="44"/>
     </row>
-    <row r="397" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:14" ht="18" customHeight="1">
       <c r="A397" s="44"/>
       <c r="C397" s="2"/>
       <c r="D397" s="2"/>
@@ -13234,7 +13316,7 @@
       <c r="M397" s="44"/>
       <c r="N397" s="44"/>
     </row>
-    <row r="398" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:14" ht="18" customHeight="1">
       <c r="A398" s="44"/>
       <c r="C398" s="2"/>
       <c r="D398" s="2"/>
@@ -13248,7 +13330,7 @@
       <c r="M398" s="44"/>
       <c r="N398" s="44"/>
     </row>
-    <row r="399" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:14" ht="18" customHeight="1">
       <c r="A399" s="44"/>
       <c r="C399" s="2"/>
       <c r="D399" s="2"/>
@@ -13262,7 +13344,7 @@
       <c r="M399" s="44"/>
       <c r="N399" s="44"/>
     </row>
-    <row r="400" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:14" ht="18" customHeight="1">
       <c r="A400" s="44"/>
       <c r="C400" s="2"/>
       <c r="D400" s="2"/>
@@ -13276,7 +13358,7 @@
       <c r="M400" s="44"/>
       <c r="N400" s="44"/>
     </row>
-    <row r="401" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:14" ht="18" customHeight="1">
       <c r="A401" s="44"/>
       <c r="C401" s="2"/>
       <c r="D401" s="2"/>
@@ -13290,7 +13372,7 @@
       <c r="M401" s="44"/>
       <c r="N401" s="44"/>
     </row>
-    <row r="402" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:14" ht="18" customHeight="1">
       <c r="A402" s="44"/>
       <c r="C402" s="2"/>
       <c r="D402" s="2"/>
@@ -13304,7 +13386,7 @@
       <c r="M402" s="44"/>
       <c r="N402" s="44"/>
     </row>
-    <row r="403" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:14" ht="18" customHeight="1">
       <c r="A403" s="44"/>
       <c r="C403" s="2"/>
       <c r="D403" s="2"/>
@@ -13318,7 +13400,7 @@
       <c r="M403" s="44"/>
       <c r="N403" s="44"/>
     </row>
-    <row r="404" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:14" ht="18" customHeight="1">
       <c r="A404" s="44"/>
       <c r="C404" s="2"/>
       <c r="D404" s="2"/>
@@ -13332,7 +13414,7 @@
       <c r="M404" s="44"/>
       <c r="N404" s="44"/>
     </row>
-    <row r="405" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:14" ht="18" customHeight="1">
       <c r="A405" s="44"/>
       <c r="C405" s="2"/>
       <c r="D405" s="2"/>
@@ -13346,7 +13428,7 @@
       <c r="M405" s="44"/>
       <c r="N405" s="44"/>
     </row>
-    <row r="406" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:14" ht="18" customHeight="1">
       <c r="A406" s="44"/>
       <c r="C406" s="2"/>
       <c r="D406" s="2"/>
@@ -13360,7 +13442,7 @@
       <c r="M406" s="44"/>
       <c r="N406" s="44"/>
     </row>
-    <row r="407" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:14" ht="18" customHeight="1">
       <c r="A407" s="44"/>
       <c r="C407" s="2"/>
       <c r="D407" s="2"/>
@@ -13374,7 +13456,7 @@
       <c r="M407" s="44"/>
       <c r="N407" s="44"/>
     </row>
-    <row r="408" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:14" ht="18" customHeight="1">
       <c r="A408" s="44"/>
       <c r="C408" s="2"/>
       <c r="D408" s="2"/>
@@ -13388,7 +13470,7 @@
       <c r="M408" s="44"/>
       <c r="N408" s="44"/>
     </row>
-    <row r="409" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:14" ht="18" customHeight="1">
       <c r="A409" s="44"/>
       <c r="C409" s="2"/>
       <c r="D409" s="2"/>
@@ -13402,7 +13484,7 @@
       <c r="M409" s="44"/>
       <c r="N409" s="44"/>
     </row>
-    <row r="410" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:14" ht="18" customHeight="1">
       <c r="A410" s="44"/>
       <c r="C410" s="2"/>
       <c r="D410" s="2"/>
@@ -13416,7 +13498,7 @@
       <c r="M410" s="44"/>
       <c r="N410" s="44"/>
     </row>
-    <row r="411" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:14" ht="18" customHeight="1">
       <c r="A411" s="44"/>
       <c r="C411" s="2"/>
       <c r="D411" s="2"/>
@@ -13430,7 +13512,7 @@
       <c r="M411" s="44"/>
       <c r="N411" s="44"/>
     </row>
-    <row r="412" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:14" ht="18" customHeight="1">
       <c r="A412" s="44"/>
       <c r="C412" s="2"/>
       <c r="D412" s="2"/>
@@ -13444,7 +13526,7 @@
       <c r="M412" s="44"/>
       <c r="N412" s="44"/>
     </row>
-    <row r="413" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:14" ht="18" customHeight="1">
       <c r="A413" s="44"/>
       <c r="C413" s="2"/>
       <c r="D413" s="2"/>
@@ -13458,7 +13540,7 @@
       <c r="M413" s="44"/>
       <c r="N413" s="44"/>
     </row>
-    <row r="414" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:14" ht="18" customHeight="1">
       <c r="A414" s="44"/>
       <c r="C414" s="2"/>
       <c r="D414" s="2"/>
@@ -13472,7 +13554,7 @@
       <c r="M414" s="44"/>
       <c r="N414" s="44"/>
     </row>
-    <row r="415" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:14" ht="18" customHeight="1">
       <c r="A415" s="44"/>
       <c r="C415" s="2"/>
       <c r="D415" s="2"/>
@@ -13486,7 +13568,7 @@
       <c r="M415" s="44"/>
       <c r="N415" s="44"/>
     </row>
-    <row r="416" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:14" ht="18" customHeight="1">
       <c r="A416" s="44"/>
       <c r="C416" s="2"/>
       <c r="D416" s="2"/>
@@ -13500,7 +13582,7 @@
       <c r="M416" s="44"/>
       <c r="N416" s="44"/>
     </row>
-    <row r="417" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:14" ht="18" customHeight="1">
       <c r="A417" s="44"/>
       <c r="C417" s="2"/>
       <c r="D417" s="2"/>
@@ -13514,7 +13596,7 @@
       <c r="M417" s="44"/>
       <c r="N417" s="44"/>
     </row>
-    <row r="418" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:14" ht="18" customHeight="1">
       <c r="A418" s="44"/>
       <c r="C418" s="2"/>
       <c r="D418" s="2"/>
@@ -13528,7 +13610,7 @@
       <c r="M418" s="44"/>
       <c r="N418" s="44"/>
     </row>
-    <row r="419" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:14" ht="18" customHeight="1">
       <c r="A419" s="44"/>
       <c r="C419" s="2"/>
       <c r="D419" s="2"/>
@@ -13542,7 +13624,7 @@
       <c r="M419" s="44"/>
       <c r="N419" s="44"/>
     </row>
-    <row r="420" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:14" ht="18" customHeight="1">
       <c r="A420" s="44"/>
       <c r="C420" s="2"/>
       <c r="D420" s="2"/>
@@ -13556,7 +13638,7 @@
       <c r="M420" s="44"/>
       <c r="N420" s="44"/>
     </row>
-    <row r="421" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:14" ht="18" customHeight="1">
       <c r="A421" s="44"/>
       <c r="C421" s="2"/>
       <c r="D421" s="2"/>
@@ -13570,7 +13652,7 @@
       <c r="M421" s="44"/>
       <c r="N421" s="44"/>
     </row>
-    <row r="422" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:14" ht="18" customHeight="1">
       <c r="A422" s="44"/>
       <c r="C422" s="2"/>
       <c r="D422" s="2"/>
@@ -13584,7 +13666,7 @@
       <c r="M422" s="44"/>
       <c r="N422" s="44"/>
     </row>
-    <row r="423" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:14" ht="18" customHeight="1">
       <c r="A423" s="44"/>
       <c r="C423" s="2"/>
       <c r="D423" s="2"/>
@@ -13598,7 +13680,7 @@
       <c r="M423" s="44"/>
       <c r="N423" s="44"/>
     </row>
-    <row r="424" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:14" ht="18" customHeight="1">
       <c r="A424" s="44"/>
       <c r="C424" s="2"/>
       <c r="D424" s="2"/>
@@ -13612,7 +13694,7 @@
       <c r="M424" s="44"/>
       <c r="N424" s="44"/>
     </row>
-    <row r="425" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:14" ht="18" customHeight="1">
       <c r="A425" s="44"/>
       <c r="C425" s="2"/>
       <c r="D425" s="2"/>
@@ -13626,7 +13708,7 @@
       <c r="M425" s="44"/>
       <c r="N425" s="44"/>
     </row>
-    <row r="426" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:14" ht="18" customHeight="1">
       <c r="A426" s="44"/>
       <c r="C426" s="2"/>
       <c r="D426" s="2"/>
@@ -13640,7 +13722,7 @@
       <c r="M426" s="44"/>
       <c r="N426" s="44"/>
     </row>
-    <row r="427" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:14" ht="18" customHeight="1">
       <c r="A427" s="44"/>
       <c r="C427" s="2"/>
       <c r="D427" s="2"/>
@@ -13654,7 +13736,7 @@
       <c r="M427" s="44"/>
       <c r="N427" s="44"/>
     </row>
-    <row r="428" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:14" ht="18" customHeight="1">
       <c r="A428" s="44"/>
       <c r="C428" s="2"/>
       <c r="D428" s="2"/>
@@ -13668,7 +13750,7 @@
       <c r="M428" s="44"/>
       <c r="N428" s="44"/>
     </row>
-    <row r="429" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:14" ht="18" customHeight="1">
       <c r="A429" s="44"/>
       <c r="C429" s="2"/>
       <c r="D429" s="2"/>
@@ -13682,7 +13764,7 @@
       <c r="M429" s="44"/>
       <c r="N429" s="44"/>
     </row>
-    <row r="430" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:14" ht="18" customHeight="1">
       <c r="A430" s="44"/>
       <c r="C430" s="2"/>
       <c r="D430" s="2"/>
@@ -13698,11 +13780,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -13717,6 +13794,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1016/j.jallcom.2016.04.248`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC92980E-E84C-5E44-9C87-72AC189799CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811A1768-DB38-D649-9838-CF3D64AE04A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1958" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="348">
   <si>
     <t>Metadata</t>
   </si>
@@ -1100,6 +1100,75 @@
   </si>
   <si>
     <t>10.1007/s40843-018-9365-8</t>
+  </si>
+  <si>
+    <t>CoCrNiFe0.8</t>
+  </si>
+  <si>
+    <t>CoCrNiFe1.0</t>
+  </si>
+  <si>
+    <t>CoCrNiFe1.2</t>
+  </si>
+  <si>
+    <t>AC+A+WQ</t>
+  </si>
+  <si>
+    <t>CoCrFeNiPd0.5</t>
+  </si>
+  <si>
+    <t>CoCrFeNiPd0.8</t>
+  </si>
+  <si>
+    <t>CoCrFeNiPd1.0</t>
+  </si>
+  <si>
+    <t>CoCrFeNiPd1.2</t>
+  </si>
+  <si>
+    <t>CoCrFeNiPd1.5</t>
+  </si>
+  <si>
+    <t>FCC+monoclinic</t>
+  </si>
+  <si>
+    <t>phase stability investigation through standard X-ray diffraction (XRD), high-energy X-ray diffraction (HEXRD), and neutron diffraction (ND); measured over 4 slices from different parts of sample; noted as single FCC to be compatible with other data but actually 2-3 similar phases</t>
+  </si>
+  <si>
+    <t>phase stability investigation through standard X-ray diffraction (XRD), high-energy X-ray diffraction (HEXRD), and neutron diffraction (ND); measured over 4 slices from different parts of sample; annealed for 3h in 1373K and water quenched; noted as single FCC to be compatible with other data but actually 2-3 similar</t>
+  </si>
+  <si>
+    <t>phase stability investigation through standard X-ray diffraction (XRD), high-energy X-ray diffraction (HEXRD), and neutron diffraction (ND); measured over 4 slices from different parts of sample; annealed for 3h in 1373K; noted as single FCC to be compatible with other data but actually 2-3 similar</t>
+  </si>
+  <si>
+    <t>phase stability investigation through standard X-ray diffraction (XRD), high-energy X-ray diffraction (HEXRD), and neutron diffraction (ND); measured over 4 slices from different parts of sample; annealed for 3h in 673K and water quenched; noted as single FCC to be compatible with other data but actually 2-3 similar</t>
+  </si>
+  <si>
+    <t>phase stability investigation through standard X-ray diffraction (XRD), high-energy X-ray diffraction (HEXRD), and neutron diffraction (ND); measured over 4 slices from different parts of sample; annealed for 3h in 973K and water quenched; noted as single FCC to be compatible with other data but actually 2-3 similar</t>
+  </si>
+  <si>
+    <t>phase stability investigation through standard X-ray diffraction (XRD), high-energy X-ray diffraction (HEXRD), and neutron diffraction (ND); measured over 4 slices from different parts of sample; noted as single FCC to be compatible with other data but actually 3-4 similar</t>
+  </si>
+  <si>
+    <t>phase stability investigation through standard X-ray diffraction (XRD), high-energy X-ray diffraction (HEXRD), and neutron diffraction (ND); measured over 4 slices from different parts of sample; annealed for 3h in 1373K and water quenched; noted as single FCC to be compatible with other data but actually 3-4 similar phases</t>
+  </si>
+  <si>
+    <t>phase stability investigation through standard X-ray diffraction (XRD), high-energy X-ray diffraction (HEXRD), and neutron diffraction (ND); measured over 4 slices from different parts of sample; annealed for 3h in 973K and water quenched; noted as single FCC to be compatible with other data but actually 3-4 similar phases</t>
+  </si>
+  <si>
+    <t>phase stability investigation through standard X-ray diffraction (XRD), high-energy X-ray diffraction (HEXRD), and neutron diffraction (ND); measured over 4 slices from different parts of sample; annealed for 3h in 973K and water quenched; noted only one FCC to be compatible with other data but actually 2-3 similar FCC phases</t>
+  </si>
+  <si>
+    <t>AC+A+WQ+A+WQ</t>
+  </si>
+  <si>
+    <t>FCC+FCC+FCC</t>
+  </si>
+  <si>
+    <t>phase stability investigation through standard X-ray diffraction (XRD), high-energy X-ray diffraction (HEXRD), and neutron diffraction (ND); measured over 4 slices from different parts of sample; annealed for 3h in 1373K and water quenched and then annealed again at 973K for 3h and water quenched</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2016.04.248</t>
   </si>
 </sst>
 </file>
@@ -1888,57 +1957,7 @@
     <xf numFmtId="3" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2005,7 +2024,57 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2311,10 +2380,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T430"/>
+  <dimension ref="A1:T424"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="N236" sqref="N236"/>
+      <selection activeCell="N255" sqref="N255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2363,19 +2432,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="81"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="65"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1">
@@ -2386,17 +2455,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="85"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="69"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1">
@@ -2425,43 +2494,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="86" t="s">
+      <c r="C5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="88" t="s">
+      <c r="D5" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="88" t="s">
+      <c r="E5" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="88" t="s">
+      <c r="F5" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="88" t="s">
+      <c r="G5" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="89" t="s">
+      <c r="H5" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="91" t="s">
+      <c r="I5" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="93" t="s">
+      <c r="J5" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="93" t="s">
+      <c r="K5" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="88" t="s">
+      <c r="L5" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="88" t="s">
+      <c r="M5" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="88" t="s">
+      <c r="N5" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="56" t="s">
+      <c r="O5" s="79" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2472,19 +2541,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="94"/>
-      <c r="K6" s="94"/>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
-      <c r="N6" s="87"/>
-      <c r="O6" s="57"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
+      <c r="N6" s="71"/>
+      <c r="O6" s="80"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1">
       <c r="A7" s="17" t="s">
@@ -2529,7 +2598,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="58"/>
+      <c r="O7" s="81"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2542,35 +2611,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="62" t="s">
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="67" t="s">
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="89"/>
+      <c r="M8" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="68"/>
+      <c r="N8" s="91"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="69" t="s">
+      <c r="P8" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="70"/>
-      <c r="R8" s="71"/>
-      <c r="S8" s="71"/>
-      <c r="T8" s="72"/>
+      <c r="Q8" s="93"/>
+      <c r="R8" s="94"/>
+      <c r="S8" s="94"/>
+      <c r="T8" s="95"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="26" t="s">
@@ -10809,7 +10878,7 @@
       <c r="N225" s="44" t="s">
         <v>324</v>
       </c>
-      <c r="P225" s="95">
+      <c r="P225" s="56">
         <v>218.1</v>
       </c>
       <c r="Q225" s="6">
@@ -10860,11 +10929,18 @@
     </row>
     <row r="227" spans="1:17" ht="18" customHeight="1">
       <c r="A227" s="24"/>
-      <c r="B227" s="44"/>
-      <c r="C227" s="42"/>
-      <c r="D227" s="42"/>
-      <c r="E227" s="44"/>
-      <c r="F227" s="42"/>
+      <c r="B227" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="C227" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D227" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E227" s="42" t="s">
+        <v>335</v>
+      </c>
       <c r="G227" s="42"/>
       <c r="H227" s="42"/>
       <c r="I227" s="3"/>
@@ -10872,15 +10948,24 @@
       <c r="K227" s="4"/>
       <c r="L227" s="44"/>
       <c r="M227" s="44"/>
-      <c r="N227" s="44"/>
+      <c r="N227" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="228" spans="1:17" ht="18" customHeight="1">
       <c r="A228" s="24"/>
-      <c r="B228" s="44"/>
-      <c r="C228" s="42"/>
-      <c r="D228" s="42"/>
-      <c r="E228" s="44"/>
-      <c r="F228" s="42"/>
+      <c r="B228" s="44" t="s">
+        <v>326</v>
+      </c>
+      <c r="C228" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D228" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E228" s="42" t="s">
+        <v>335</v>
+      </c>
       <c r="G228" s="42"/>
       <c r="H228" s="42"/>
       <c r="I228" s="3"/>
@@ -10888,15 +10973,24 @@
       <c r="K228" s="4"/>
       <c r="L228" s="44"/>
       <c r="M228" s="44"/>
-      <c r="N228" s="44"/>
+      <c r="N228" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="229" spans="1:17" ht="18" customHeight="1">
       <c r="A229" s="24"/>
-      <c r="B229" s="44"/>
-      <c r="C229" s="42"/>
-      <c r="D229" s="42"/>
-      <c r="E229" s="44"/>
-      <c r="F229" s="42"/>
+      <c r="B229" s="44" t="s">
+        <v>327</v>
+      </c>
+      <c r="C229" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D229" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E229" s="42" t="s">
+        <v>335</v>
+      </c>
       <c r="G229" s="42"/>
       <c r="H229" s="42"/>
       <c r="I229" s="3"/>
@@ -10904,14 +10998,24 @@
       <c r="K229" s="4"/>
       <c r="L229" s="44"/>
       <c r="M229" s="44"/>
-      <c r="N229" s="44"/>
+      <c r="N229" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="230" spans="1:17" ht="18" customHeight="1">
       <c r="A230" s="24"/>
-      <c r="B230" s="44"/>
-      <c r="C230" s="42"/>
-      <c r="D230" s="42"/>
-      <c r="E230" s="44"/>
+      <c r="B230" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="C230" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D230" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E230" s="42" t="s">
+        <v>336</v>
+      </c>
       <c r="F230" s="42"/>
       <c r="G230" s="42"/>
       <c r="H230" s="42"/>
@@ -10920,14 +11024,24 @@
       <c r="K230" s="4"/>
       <c r="L230" s="44"/>
       <c r="M230" s="44"/>
-      <c r="N230" s="44"/>
+      <c r="N230" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="231" spans="1:17" ht="18" customHeight="1">
       <c r="A231" s="24"/>
-      <c r="B231" s="44"/>
-      <c r="C231" s="42"/>
-      <c r="D231" s="42"/>
-      <c r="E231" s="44"/>
+      <c r="B231" s="44" t="s">
+        <v>326</v>
+      </c>
+      <c r="C231" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D231" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E231" s="42" t="s">
+        <v>336</v>
+      </c>
       <c r="F231" s="42"/>
       <c r="G231" s="42"/>
       <c r="H231" s="42"/>
@@ -10936,14 +11050,24 @@
       <c r="K231" s="4"/>
       <c r="L231" s="44"/>
       <c r="M231" s="44"/>
-      <c r="N231" s="44"/>
+      <c r="N231" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="232" spans="1:17" ht="18" customHeight="1">
       <c r="A232" s="24"/>
-      <c r="B232" s="44"/>
-      <c r="C232" s="42"/>
-      <c r="D232" s="42"/>
-      <c r="E232" s="44"/>
+      <c r="B232" s="44" t="s">
+        <v>327</v>
+      </c>
+      <c r="C232" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D232" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E232" s="42" t="s">
+        <v>336</v>
+      </c>
       <c r="F232" s="42"/>
       <c r="G232" s="42"/>
       <c r="H232" s="42"/>
@@ -10952,14 +11076,24 @@
       <c r="K232" s="4"/>
       <c r="L232" s="44"/>
       <c r="M232" s="44"/>
-      <c r="N232" s="44"/>
+      <c r="N232" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="233" spans="1:17" ht="18" customHeight="1">
       <c r="A233" s="24"/>
-      <c r="B233" s="44"/>
-      <c r="C233" s="42"/>
-      <c r="D233" s="42"/>
-      <c r="E233" s="44"/>
+      <c r="B233" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="C233" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D233" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="E233" s="42" t="s">
+        <v>337</v>
+      </c>
       <c r="F233" s="42"/>
       <c r="G233" s="42"/>
       <c r="H233" s="42"/>
@@ -10968,14 +11102,24 @@
       <c r="K233" s="4"/>
       <c r="L233" s="44"/>
       <c r="M233" s="44"/>
-      <c r="N233" s="44"/>
+      <c r="N233" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="234" spans="1:17" ht="18" customHeight="1">
       <c r="A234" s="24"/>
-      <c r="B234" s="44"/>
-      <c r="C234" s="42"/>
-      <c r="D234" s="42"/>
-      <c r="E234" s="44"/>
+      <c r="B234" s="44" t="s">
+        <v>326</v>
+      </c>
+      <c r="C234" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D234" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="E234" s="42" t="s">
+        <v>337</v>
+      </c>
       <c r="F234" s="42"/>
       <c r="G234" s="42"/>
       <c r="H234" s="42"/>
@@ -10984,14 +11128,24 @@
       <c r="K234" s="4"/>
       <c r="L234" s="44"/>
       <c r="M234" s="44"/>
-      <c r="N234" s="44"/>
+      <c r="N234" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="235" spans="1:17" ht="18" customHeight="1">
       <c r="A235" s="24"/>
-      <c r="B235" s="44"/>
-      <c r="C235" s="42"/>
-      <c r="D235" s="42"/>
-      <c r="E235" s="44"/>
+      <c r="B235" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="C235" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D235" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E235" s="42" t="s">
+        <v>338</v>
+      </c>
       <c r="F235" s="42"/>
       <c r="G235" s="42"/>
       <c r="H235" s="42"/>
@@ -11000,14 +11154,24 @@
       <c r="K235" s="4"/>
       <c r="L235" s="44"/>
       <c r="M235" s="44"/>
-      <c r="N235" s="44"/>
+      <c r="N235" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="236" spans="1:17" ht="18" customHeight="1">
       <c r="A236" s="24"/>
-      <c r="B236" s="44"/>
-      <c r="C236" s="42"/>
-      <c r="D236" s="42"/>
-      <c r="E236" s="44"/>
+      <c r="B236" s="44" t="s">
+        <v>326</v>
+      </c>
+      <c r="C236" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D236" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E236" s="42" t="s">
+        <v>338</v>
+      </c>
       <c r="F236" s="42"/>
       <c r="G236" s="42"/>
       <c r="H236" s="42"/>
@@ -11016,14 +11180,24 @@
       <c r="K236" s="4"/>
       <c r="L236" s="44"/>
       <c r="M236" s="44"/>
-      <c r="N236" s="44"/>
+      <c r="N236" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="237" spans="1:17" ht="18" customHeight="1">
       <c r="A237" s="24"/>
-      <c r="B237" s="44"/>
-      <c r="C237" s="42"/>
-      <c r="D237" s="42"/>
-      <c r="E237" s="44"/>
+      <c r="B237" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="C237" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D237" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E237" s="42" t="s">
+        <v>339</v>
+      </c>
       <c r="F237" s="42"/>
       <c r="G237" s="42"/>
       <c r="H237" s="42"/>
@@ -11032,14 +11206,24 @@
       <c r="K237" s="4"/>
       <c r="L237" s="44"/>
       <c r="M237" s="44"/>
-      <c r="N237" s="44"/>
+      <c r="N237" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="238" spans="1:17" ht="18" customHeight="1">
       <c r="A238" s="24"/>
-      <c r="B238" s="44"/>
-      <c r="C238" s="42"/>
-      <c r="D238" s="42"/>
-      <c r="E238" s="44"/>
+      <c r="B238" s="44" t="s">
+        <v>326</v>
+      </c>
+      <c r="C238" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D238" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E238" s="42" t="s">
+        <v>339</v>
+      </c>
       <c r="F238" s="42"/>
       <c r="G238" s="42"/>
       <c r="H238" s="42"/>
@@ -11048,14 +11232,24 @@
       <c r="K238" s="4"/>
       <c r="L238" s="44"/>
       <c r="M238" s="44"/>
-      <c r="N238" s="44"/>
+      <c r="N238" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="239" spans="1:17" ht="18" customHeight="1">
       <c r="A239" s="24"/>
-      <c r="B239" s="44"/>
-      <c r="C239" s="42"/>
-      <c r="D239" s="42"/>
-      <c r="E239" s="44"/>
+      <c r="B239" s="44" t="s">
+        <v>327</v>
+      </c>
+      <c r="C239" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D239" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E239" s="42" t="s">
+        <v>339</v>
+      </c>
       <c r="F239" s="42"/>
       <c r="G239" s="42"/>
       <c r="H239" s="42"/>
@@ -11064,14 +11258,24 @@
       <c r="K239" s="4"/>
       <c r="L239" s="44"/>
       <c r="M239" s="44"/>
-      <c r="N239" s="44"/>
+      <c r="N239" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="240" spans="1:17" ht="18" customHeight="1">
       <c r="A240" s="24"/>
-      <c r="B240" s="44"/>
-      <c r="C240" s="42"/>
-      <c r="D240" s="42"/>
-      <c r="E240" s="44"/>
+      <c r="B240" s="44" t="s">
+        <v>329</v>
+      </c>
+      <c r="C240" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D240" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E240" s="42" t="s">
+        <v>340</v>
+      </c>
       <c r="F240" s="42"/>
       <c r="G240" s="42"/>
       <c r="H240" s="42"/>
@@ -11080,14 +11284,24 @@
       <c r="K240" s="4"/>
       <c r="L240" s="44"/>
       <c r="M240" s="44"/>
-      <c r="N240" s="44"/>
+      <c r="N240" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="241" spans="1:14" ht="18" customHeight="1">
       <c r="A241" s="24"/>
-      <c r="B241" s="44"/>
-      <c r="C241" s="42"/>
-      <c r="D241" s="42"/>
-      <c r="E241" s="44"/>
+      <c r="B241" s="44" t="s">
+        <v>330</v>
+      </c>
+      <c r="C241" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D241" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E241" s="42" t="s">
+        <v>340</v>
+      </c>
       <c r="F241" s="42"/>
       <c r="G241" s="42"/>
       <c r="H241" s="42"/>
@@ -11096,14 +11310,24 @@
       <c r="K241" s="4"/>
       <c r="L241" s="44"/>
       <c r="M241" s="44"/>
-      <c r="N241" s="44"/>
+      <c r="N241" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="242" spans="1:14" ht="18" customHeight="1">
       <c r="A242" s="24"/>
-      <c r="B242" s="44"/>
-      <c r="C242" s="42"/>
-      <c r="D242" s="42"/>
-      <c r="E242" s="44"/>
+      <c r="B242" s="44" t="s">
+        <v>331</v>
+      </c>
+      <c r="C242" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D242" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E242" s="42" t="s">
+        <v>340</v>
+      </c>
       <c r="F242" s="42"/>
       <c r="G242" s="42"/>
       <c r="H242" s="42"/>
@@ -11112,14 +11336,24 @@
       <c r="K242" s="4"/>
       <c r="L242" s="44"/>
       <c r="M242" s="44"/>
-      <c r="N242" s="44"/>
+      <c r="N242" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="243" spans="1:14" ht="18" customHeight="1">
       <c r="A243" s="24"/>
-      <c r="B243" s="44"/>
-      <c r="C243" s="42"/>
-      <c r="D243" s="42"/>
-      <c r="E243" s="44"/>
+      <c r="B243" s="44" t="s">
+        <v>332</v>
+      </c>
+      <c r="C243" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D243" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E243" s="42" t="s">
+        <v>340</v>
+      </c>
       <c r="F243" s="42"/>
       <c r="G243" s="42"/>
       <c r="H243" s="42"/>
@@ -11128,14 +11362,24 @@
       <c r="K243" s="4"/>
       <c r="L243" s="44"/>
       <c r="M243" s="44"/>
-      <c r="N243" s="44"/>
+      <c r="N243" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="244" spans="1:14" ht="18" customHeight="1">
       <c r="A244" s="24"/>
-      <c r="B244" s="44"/>
-      <c r="C244" s="42"/>
-      <c r="D244" s="42"/>
-      <c r="E244" s="44"/>
+      <c r="B244" s="44" t="s">
+        <v>333</v>
+      </c>
+      <c r="C244" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D244" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E244" s="42" t="s">
+        <v>340</v>
+      </c>
       <c r="F244" s="42"/>
       <c r="G244" s="42"/>
       <c r="H244" s="42"/>
@@ -11144,14 +11388,24 @@
       <c r="K244" s="4"/>
       <c r="L244" s="44"/>
       <c r="M244" s="44"/>
-      <c r="N244" s="44"/>
+      <c r="N244" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="245" spans="1:14" ht="18" customHeight="1">
       <c r="A245" s="24"/>
-      <c r="B245" s="44"/>
-      <c r="C245" s="42"/>
-      <c r="D245" s="42"/>
-      <c r="E245" s="44"/>
+      <c r="B245" s="44" t="s">
+        <v>330</v>
+      </c>
+      <c r="C245" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D245" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E245" s="42" t="s">
+        <v>341</v>
+      </c>
       <c r="F245" s="42"/>
       <c r="G245" s="42"/>
       <c r="H245" s="42"/>
@@ -11160,14 +11414,24 @@
       <c r="K245" s="4"/>
       <c r="L245" s="44"/>
       <c r="M245" s="44"/>
-      <c r="N245" s="44"/>
+      <c r="N245" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="246" spans="1:14" ht="18" customHeight="1">
       <c r="A246" s="24"/>
-      <c r="B246" s="44"/>
-      <c r="C246" s="42"/>
-      <c r="D246" s="42"/>
-      <c r="E246" s="44"/>
+      <c r="B246" s="44" t="s">
+        <v>331</v>
+      </c>
+      <c r="C246" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D246" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E246" s="42" t="s">
+        <v>341</v>
+      </c>
       <c r="F246" s="42"/>
       <c r="G246" s="42"/>
       <c r="H246" s="42"/>
@@ -11176,14 +11440,24 @@
       <c r="K246" s="4"/>
       <c r="L246" s="44"/>
       <c r="M246" s="44"/>
-      <c r="N246" s="44"/>
+      <c r="N246" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="247" spans="1:14" ht="18" customHeight="1">
       <c r="A247" s="24"/>
-      <c r="B247" s="44"/>
-      <c r="C247" s="42"/>
-      <c r="D247" s="42"/>
-      <c r="E247" s="44"/>
+      <c r="B247" s="44" t="s">
+        <v>332</v>
+      </c>
+      <c r="C247" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D247" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E247" s="42" t="s">
+        <v>341</v>
+      </c>
       <c r="F247" s="42"/>
       <c r="G247" s="42"/>
       <c r="H247" s="42"/>
@@ -11192,14 +11466,24 @@
       <c r="K247" s="4"/>
       <c r="L247" s="44"/>
       <c r="M247" s="44"/>
-      <c r="N247" s="44"/>
+      <c r="N247" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="248" spans="1:14" ht="18" customHeight="1">
       <c r="A248" s="24"/>
-      <c r="B248" s="44"/>
-      <c r="C248" s="42"/>
-      <c r="D248" s="42"/>
-      <c r="E248" s="44"/>
+      <c r="B248" s="44" t="s">
+        <v>330</v>
+      </c>
+      <c r="C248" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D248" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E248" s="42" t="s">
+        <v>342</v>
+      </c>
       <c r="F248" s="42"/>
       <c r="G248" s="42"/>
       <c r="H248" s="42"/>
@@ -11208,14 +11492,24 @@
       <c r="K248" s="4"/>
       <c r="L248" s="44"/>
       <c r="M248" s="44"/>
-      <c r="N248" s="44"/>
+      <c r="N248" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="249" spans="1:14" ht="18" customHeight="1">
       <c r="A249" s="24"/>
-      <c r="B249" s="44"/>
-      <c r="C249" s="42"/>
-      <c r="D249" s="42"/>
-      <c r="E249" s="44"/>
+      <c r="B249" s="44" t="s">
+        <v>331</v>
+      </c>
+      <c r="C249" s="42" t="s">
+        <v>334</v>
+      </c>
+      <c r="D249" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E249" s="42" t="s">
+        <v>343</v>
+      </c>
       <c r="F249" s="42"/>
       <c r="G249" s="42"/>
       <c r="H249" s="42"/>
@@ -11224,14 +11518,24 @@
       <c r="K249" s="4"/>
       <c r="L249" s="44"/>
       <c r="M249" s="44"/>
-      <c r="N249" s="44"/>
+      <c r="N249" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="250" spans="1:14" ht="18" customHeight="1">
       <c r="A250" s="24"/>
-      <c r="B250" s="44"/>
-      <c r="C250" s="42"/>
-      <c r="D250" s="42"/>
-      <c r="E250" s="44"/>
+      <c r="B250" s="44" t="s">
+        <v>332</v>
+      </c>
+      <c r="C250" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D250" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E250" s="42" t="s">
+        <v>342</v>
+      </c>
       <c r="F250" s="42"/>
       <c r="G250" s="42"/>
       <c r="H250" s="42"/>
@@ -11240,14 +11544,24 @@
       <c r="K250" s="4"/>
       <c r="L250" s="44"/>
       <c r="M250" s="44"/>
-      <c r="N250" s="44"/>
+      <c r="N250" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="251" spans="1:14" ht="18" customHeight="1">
       <c r="A251" s="24"/>
-      <c r="B251" s="44"/>
-      <c r="C251" s="42"/>
-      <c r="D251" s="42"/>
-      <c r="E251" s="44"/>
+      <c r="B251" s="44" t="s">
+        <v>331</v>
+      </c>
+      <c r="C251" s="42" t="s">
+        <v>345</v>
+      </c>
+      <c r="D251" s="42" t="s">
+        <v>344</v>
+      </c>
+      <c r="E251" s="42" t="s">
+        <v>346</v>
+      </c>
       <c r="F251" s="42"/>
       <c r="G251" s="42"/>
       <c r="H251" s="42"/>
@@ -11256,7 +11570,9 @@
       <c r="K251" s="4"/>
       <c r="L251" s="44"/>
       <c r="M251" s="44"/>
-      <c r="N251" s="44"/>
+      <c r="N251" s="44" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="252" spans="1:14" ht="18" customHeight="1">
       <c r="A252" s="24"/>
@@ -11276,13 +11592,11 @@
     </row>
     <row r="253" spans="1:14" ht="18" customHeight="1">
       <c r="A253" s="24"/>
-      <c r="B253" s="44"/>
-      <c r="C253" s="42"/>
-      <c r="D253" s="42"/>
-      <c r="E253" s="44"/>
-      <c r="F253" s="42"/>
-      <c r="G253" s="42"/>
-      <c r="H253" s="42"/>
+      <c r="C253" s="2"/>
+      <c r="D253" s="2"/>
+      <c r="F253" s="2"/>
+      <c r="G253" s="2"/>
+      <c r="H253" s="2"/>
       <c r="I253" s="3"/>
       <c r="J253" s="4"/>
       <c r="K253" s="4"/>
@@ -11292,13 +11606,11 @@
     </row>
     <row r="254" spans="1:14" ht="18" customHeight="1">
       <c r="A254" s="24"/>
-      <c r="B254" s="44"/>
-      <c r="C254" s="42"/>
-      <c r="D254" s="42"/>
-      <c r="E254" s="44"/>
-      <c r="F254" s="42"/>
-      <c r="G254" s="42"/>
-      <c r="H254" s="42"/>
+      <c r="C254" s="2"/>
+      <c r="D254" s="2"/>
+      <c r="F254" s="2"/>
+      <c r="G254" s="2"/>
+      <c r="H254" s="2"/>
       <c r="I254" s="3"/>
       <c r="J254" s="4"/>
       <c r="K254" s="4"/>
@@ -11308,13 +11620,11 @@
     </row>
     <row r="255" spans="1:14" ht="18" customHeight="1">
       <c r="A255" s="24"/>
-      <c r="B255" s="44"/>
-      <c r="C255" s="42"/>
-      <c r="D255" s="42"/>
-      <c r="E255" s="44"/>
-      <c r="F255" s="42"/>
-      <c r="G255" s="42"/>
-      <c r="H255" s="42"/>
+      <c r="C255" s="2"/>
+      <c r="D255" s="2"/>
+      <c r="F255" s="2"/>
+      <c r="G255" s="2"/>
+      <c r="H255" s="2"/>
       <c r="I255" s="3"/>
       <c r="J255" s="4"/>
       <c r="K255" s="4"/>
@@ -11324,13 +11634,11 @@
     </row>
     <row r="256" spans="1:14" ht="18" customHeight="1">
       <c r="A256" s="24"/>
-      <c r="B256" s="44"/>
-      <c r="C256" s="42"/>
-      <c r="D256" s="42"/>
-      <c r="E256" s="44"/>
-      <c r="F256" s="42"/>
-      <c r="G256" s="42"/>
-      <c r="H256" s="42"/>
+      <c r="C256" s="2"/>
+      <c r="D256" s="2"/>
+      <c r="F256" s="2"/>
+      <c r="G256" s="2"/>
+      <c r="H256" s="2"/>
       <c r="I256" s="3"/>
       <c r="J256" s="4"/>
       <c r="K256" s="4"/>
@@ -11340,13 +11648,11 @@
     </row>
     <row r="257" spans="1:14" ht="18" customHeight="1">
       <c r="A257" s="24"/>
-      <c r="B257" s="44"/>
-      <c r="C257" s="42"/>
-      <c r="D257" s="42"/>
-      <c r="E257" s="44"/>
-      <c r="F257" s="42"/>
-      <c r="G257" s="42"/>
-      <c r="H257" s="42"/>
+      <c r="C257" s="2"/>
+      <c r="D257" s="2"/>
+      <c r="F257" s="2"/>
+      <c r="G257" s="2"/>
+      <c r="H257" s="2"/>
       <c r="I257" s="3"/>
       <c r="J257" s="4"/>
       <c r="K257" s="4"/>
@@ -11356,13 +11662,11 @@
     </row>
     <row r="258" spans="1:14" ht="18" customHeight="1">
       <c r="A258" s="24"/>
-      <c r="B258" s="44"/>
-      <c r="C258" s="42"/>
-      <c r="D258" s="42"/>
-      <c r="E258" s="44"/>
-      <c r="F258" s="42"/>
-      <c r="G258" s="42"/>
-      <c r="H258" s="42"/>
+      <c r="C258" s="2"/>
+      <c r="D258" s="2"/>
+      <c r="F258" s="2"/>
+      <c r="G258" s="2"/>
+      <c r="H258" s="2"/>
       <c r="I258" s="3"/>
       <c r="J258" s="4"/>
       <c r="K258" s="4"/>
@@ -11945,7 +12249,7 @@
       <c r="N299" s="44"/>
     </row>
     <row r="300" spans="1:14" ht="18" customHeight="1">
-      <c r="A300" s="24"/>
+      <c r="A300" s="44"/>
       <c r="C300" s="2"/>
       <c r="D300" s="2"/>
       <c r="F300" s="2"/>
@@ -11959,7 +12263,7 @@
       <c r="N300" s="44"/>
     </row>
     <row r="301" spans="1:14" ht="18" customHeight="1">
-      <c r="A301" s="24"/>
+      <c r="A301" s="44"/>
       <c r="C301" s="2"/>
       <c r="D301" s="2"/>
       <c r="F301" s="2"/>
@@ -11973,7 +12277,7 @@
       <c r="N301" s="44"/>
     </row>
     <row r="302" spans="1:14" ht="18" customHeight="1">
-      <c r="A302" s="24"/>
+      <c r="A302" s="44"/>
       <c r="C302" s="2"/>
       <c r="D302" s="2"/>
       <c r="F302" s="2"/>
@@ -11987,7 +12291,7 @@
       <c r="N302" s="44"/>
     </row>
     <row r="303" spans="1:14" ht="18" customHeight="1">
-      <c r="A303" s="24"/>
+      <c r="A303" s="44"/>
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
       <c r="F303" s="2"/>
@@ -12001,7 +12305,7 @@
       <c r="N303" s="44"/>
     </row>
     <row r="304" spans="1:14" ht="18" customHeight="1">
-      <c r="A304" s="24"/>
+      <c r="A304" s="44"/>
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
       <c r="F304" s="2"/>
@@ -12015,7 +12319,7 @@
       <c r="N304" s="44"/>
     </row>
     <row r="305" spans="1:14" ht="18" customHeight="1">
-      <c r="A305" s="24"/>
+      <c r="A305" s="44"/>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
       <c r="F305" s="2"/>
@@ -13694,92 +13998,13 @@
       <c r="M424" s="44"/>
       <c r="N424" s="44"/>
     </row>
-    <row r="425" spans="1:14" ht="18" customHeight="1">
-      <c r="A425" s="44"/>
-      <c r="C425" s="2"/>
-      <c r="D425" s="2"/>
-      <c r="F425" s="2"/>
-      <c r="G425" s="2"/>
-      <c r="H425" s="2"/>
-      <c r="I425" s="3"/>
-      <c r="J425" s="4"/>
-      <c r="K425" s="4"/>
-      <c r="L425" s="44"/>
-      <c r="M425" s="44"/>
-      <c r="N425" s="44"/>
-    </row>
-    <row r="426" spans="1:14" ht="18" customHeight="1">
-      <c r="A426" s="44"/>
-      <c r="C426" s="2"/>
-      <c r="D426" s="2"/>
-      <c r="F426" s="2"/>
-      <c r="G426" s="2"/>
-      <c r="H426" s="2"/>
-      <c r="I426" s="3"/>
-      <c r="J426" s="4"/>
-      <c r="K426" s="4"/>
-      <c r="L426" s="44"/>
-      <c r="M426" s="44"/>
-      <c r="N426" s="44"/>
-    </row>
-    <row r="427" spans="1:14" ht="18" customHeight="1">
-      <c r="A427" s="44"/>
-      <c r="C427" s="2"/>
-      <c r="D427" s="2"/>
-      <c r="F427" s="2"/>
-      <c r="G427" s="2"/>
-      <c r="H427" s="2"/>
-      <c r="I427" s="3"/>
-      <c r="J427" s="4"/>
-      <c r="K427" s="4"/>
-      <c r="L427" s="44"/>
-      <c r="M427" s="44"/>
-      <c r="N427" s="44"/>
-    </row>
-    <row r="428" spans="1:14" ht="18" customHeight="1">
-      <c r="A428" s="44"/>
-      <c r="C428" s="2"/>
-      <c r="D428" s="2"/>
-      <c r="F428" s="2"/>
-      <c r="G428" s="2"/>
-      <c r="H428" s="2"/>
-      <c r="I428" s="3"/>
-      <c r="J428" s="4"/>
-      <c r="K428" s="4"/>
-      <c r="L428" s="44"/>
-      <c r="M428" s="44"/>
-      <c r="N428" s="44"/>
-    </row>
-    <row r="429" spans="1:14" ht="18" customHeight="1">
-      <c r="A429" s="44"/>
-      <c r="C429" s="2"/>
-      <c r="D429" s="2"/>
-      <c r="F429" s="2"/>
-      <c r="G429" s="2"/>
-      <c r="H429" s="2"/>
-      <c r="I429" s="3"/>
-      <c r="J429" s="4"/>
-      <c r="K429" s="4"/>
-      <c r="L429" s="44"/>
-      <c r="M429" s="44"/>
-      <c r="N429" s="44"/>
-    </row>
-    <row r="430" spans="1:14" ht="18" customHeight="1">
-      <c r="A430" s="44"/>
-      <c r="C430" s="2"/>
-      <c r="D430" s="2"/>
-      <c r="F430" s="2"/>
-      <c r="G430" s="2"/>
-      <c r="H430" s="2"/>
-      <c r="I430" s="3"/>
-      <c r="J430" s="4"/>
-      <c r="K430" s="4"/>
-      <c r="L430" s="44"/>
-      <c r="M430" s="44"/>
-      <c r="N430" s="44"/>
-    </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -13794,11 +14019,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1021/acscatal.9b04302`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811A1768-DB38-D649-9838-CF3D64AE04A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FF93C3-65E6-9D45-A64A-D9517A23E576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="352">
   <si>
     <t>Metadata</t>
   </si>
@@ -1169,6 +1169,18 @@
   </si>
   <si>
     <t>10.1016/j.jallcom.2016.04.248</t>
+  </si>
+  <si>
+    <t>AuAgPtPdCu</t>
+  </si>
+  <si>
+    <t>AC+BM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cryomilled into nanopowder on the oder of 16nm </t>
+  </si>
+  <si>
+    <t>10.1021/acscatal.9b04302</t>
   </si>
 </sst>
 </file>
@@ -1958,6 +1970,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2023,57 +2086,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2383,7 +2395,7 @@
   <dimension ref="A1:T424"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="N255" sqref="N255"/>
+      <selection activeCell="K259" sqref="K259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2432,19 +2444,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="58"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="65"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="82"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1">
@@ -2455,17 +2467,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="69"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="86"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1">
@@ -2494,43 +2506,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="70" t="s">
+      <c r="C5" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="72" t="s">
+      <c r="D5" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="72" t="s">
+      <c r="F5" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="72" t="s">
+      <c r="G5" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="75" t="s">
+      <c r="I5" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="77" t="s">
+      <c r="J5" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="77" t="s">
+      <c r="K5" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="72" t="s">
+      <c r="L5" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="72" t="s">
+      <c r="M5" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="72" t="s">
+      <c r="N5" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="79" t="s">
+      <c r="O5" s="57" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2541,19 +2553,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="80"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="93"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="88"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="58"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1">
       <c r="A7" s="17" t="s">
@@ -2598,7 +2610,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="81"/>
+      <c r="O7" s="59"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2611,35 +2623,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="82" t="s">
+      <c r="B8" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="85" t="s">
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="86"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="87"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="90" t="s">
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="91"/>
+      <c r="N8" s="69"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="92" t="s">
+      <c r="P8" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="93"/>
-      <c r="R8" s="94"/>
-      <c r="S8" s="94"/>
-      <c r="T8" s="95"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="72"/>
+      <c r="S8" s="72"/>
+      <c r="T8" s="73"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="26" t="s">
@@ -11576,10 +11588,18 @@
     </row>
     <row r="252" spans="1:14" ht="18" customHeight="1">
       <c r="A252" s="24"/>
-      <c r="B252" s="44"/>
-      <c r="C252" s="42"/>
-      <c r="D252" s="42"/>
-      <c r="E252" s="44"/>
+      <c r="B252" s="44" t="s">
+        <v>348</v>
+      </c>
+      <c r="C252" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D252" s="42" t="s">
+        <v>349</v>
+      </c>
+      <c r="E252" s="44" t="s">
+        <v>350</v>
+      </c>
       <c r="F252" s="42"/>
       <c r="G252" s="42"/>
       <c r="H252" s="42"/>
@@ -11588,7 +11608,9 @@
       <c r="K252" s="4"/>
       <c r="L252" s="44"/>
       <c r="M252" s="44"/>
-      <c r="N252" s="44"/>
+      <c r="N252" s="44" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="253" spans="1:14" ht="18" customHeight="1">
       <c r="A253" s="24"/>
@@ -14000,11 +14022,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -14019,6 +14036,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1016/j.jallcom.2008.12.055`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FF93C3-65E6-9D45-A64A-D9517A23E576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6323BE40-6BB0-9F4E-ABE2-BD60BF1C11C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2108" uniqueCount="359">
   <si>
     <t>Metadata</t>
   </si>
@@ -1177,10 +1177,31 @@
     <t>AC+BM</t>
   </si>
   <si>
-    <t xml:space="preserve">cryomilled into nanopowder on the oder of 16nm </t>
-  </si>
-  <si>
     <t>10.1021/acscatal.9b04302</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Pt22 Fe14 Co15 Ni14 Cu18 Ag17</t>
+  </si>
+  <si>
+    <t>Pt29 Fe14 Co15 Ni15 Cu13 Ag14</t>
+  </si>
+  <si>
+    <t>Pt52 Fe11 Co10 Ni11 Cu10 Ag8</t>
+  </si>
+  <si>
+    <t>Pt56 Fe7 Co8 Ni10 Cu9 Ag10</t>
+  </si>
+  <si>
+    <t>thin films obtained by RF sputter deposition; designed as PtxFe(100−x)/5Co(100−x)/5Ni(100−x)/5Cu(100−x)/5Ag(100−x)/5; paper has data on catalytic activity</t>
+  </si>
+  <si>
+    <t>cryomilled into nanopowder on the oder of 16nm; paper has data on catalytic activity</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2008.12.055</t>
   </si>
 </sst>
 </file>
@@ -1804,7 +1825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2086,6 +2107,12 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2394,8 +2421,8 @@
   </sheetPr>
   <dimension ref="A1:T424"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="K259" sqref="K259"/>
+    <sheetView tabSelected="1" topLeftCell="A229" zoomScale="99" workbookViewId="0">
+      <selection activeCell="N260" sqref="N260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -11598,7 +11625,7 @@
         <v>349</v>
       </c>
       <c r="E252" s="44" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="F252" s="42"/>
       <c r="G252" s="42"/>
@@ -11609,13 +11636,23 @@
       <c r="L252" s="44"/>
       <c r="M252" s="44"/>
       <c r="N252" s="44" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="253" spans="1:14" ht="18" customHeight="1">
       <c r="A253" s="24"/>
-      <c r="C253" s="2"/>
-      <c r="D253" s="2"/>
+      <c r="B253" s="97" t="s">
+        <v>352</v>
+      </c>
+      <c r="C253" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D253" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E253" s="96" t="s">
+        <v>356</v>
+      </c>
       <c r="F253" s="2"/>
       <c r="G253" s="2"/>
       <c r="H253" s="2"/>
@@ -11624,12 +11661,24 @@
       <c r="K253" s="4"/>
       <c r="L253" s="44"/>
       <c r="M253" s="44"/>
-      <c r="N253" s="44"/>
+      <c r="N253" s="44" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="254" spans="1:14" ht="18" customHeight="1">
       <c r="A254" s="24"/>
-      <c r="C254" s="2"/>
-      <c r="D254" s="2"/>
+      <c r="B254" s="97" t="s">
+        <v>353</v>
+      </c>
+      <c r="C254" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D254" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E254" s="96" t="s">
+        <v>356</v>
+      </c>
       <c r="F254" s="2"/>
       <c r="G254" s="2"/>
       <c r="H254" s="2"/>
@@ -11638,12 +11687,24 @@
       <c r="K254" s="4"/>
       <c r="L254" s="44"/>
       <c r="M254" s="44"/>
-      <c r="N254" s="44"/>
+      <c r="N254" s="44" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="255" spans="1:14" ht="18" customHeight="1">
       <c r="A255" s="24"/>
-      <c r="C255" s="2"/>
-      <c r="D255" s="2"/>
+      <c r="B255" s="97" t="s">
+        <v>354</v>
+      </c>
+      <c r="C255" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D255" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E255" s="96" t="s">
+        <v>356</v>
+      </c>
       <c r="F255" s="2"/>
       <c r="G255" s="2"/>
       <c r="H255" s="2"/>
@@ -11652,12 +11713,24 @@
       <c r="K255" s="4"/>
       <c r="L255" s="44"/>
       <c r="M255" s="44"/>
-      <c r="N255" s="44"/>
+      <c r="N255" s="44" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="256" spans="1:14" ht="18" customHeight="1">
       <c r="A256" s="24"/>
-      <c r="C256" s="2"/>
-      <c r="D256" s="2"/>
+      <c r="B256" s="97" t="s">
+        <v>355</v>
+      </c>
+      <c r="C256" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D256" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E256" s="96" t="s">
+        <v>356</v>
+      </c>
       <c r="F256" s="2"/>
       <c r="G256" s="2"/>
       <c r="H256" s="2"/>
@@ -11666,7 +11739,9 @@
       <c r="K256" s="4"/>
       <c r="L256" s="44"/>
       <c r="M256" s="44"/>
-      <c r="N256" s="44"/>
+      <c r="N256" s="44" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="257" spans="1:14" ht="18" customHeight="1">
       <c r="A257" s="24"/>

</xml_diff>

<commit_message>
- extracted data from `10.1038/s41586-019-1617-1`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9DB259-BD4D-F54C-93E8-D0842FC10EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCCE68C-E4DE-234A-891C-641AF700C239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2133" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="382">
   <si>
     <t>Metadata</t>
   </si>
@@ -1232,6 +1232,45 @@
   </si>
   <si>
     <t>called nanoalloys (NAs); nanoparticles; spHEAs were prepared by thermal decomposition of single-source precursors at 473K for 24h; heated from 300K to 1000K and measured at 1000K</t>
+  </si>
+  <si>
+    <t>CrMnFeCoNi</t>
+  </si>
+  <si>
+    <t>CrFeCoNiPd</t>
+  </si>
+  <si>
+    <t>VAM+H</t>
+  </si>
+  <si>
+    <t>homogenized at 1473K for 24h</t>
+  </si>
+  <si>
+    <t>VAM+H+RX</t>
+  </si>
+  <si>
+    <t>homogenized at 1473K for 24h; recrystallized at 1150*C for 20min in vacuum; 5micrometer grain size</t>
+  </si>
+  <si>
+    <t>homogenized at 1473K for 24h; recrystallized at 1150*C for 60min in vacuum; 130micrometer grain size</t>
+  </si>
+  <si>
+    <t>tensile yield strength</t>
+  </si>
+  <si>
+    <t>EDT1</t>
+  </si>
+  <si>
+    <t>F6c</t>
+  </si>
+  <si>
+    <t>strain rate 1e-3/s</t>
+  </si>
+  <si>
+    <t>F4a</t>
+  </si>
+  <si>
+    <t>10.1038/s41586-019-1617-1</t>
   </si>
 </sst>
 </file>
@@ -2021,57 +2060,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2138,11 +2126,62 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2451,8 +2490,8 @@
   </sheetPr>
   <dimension ref="A1:T424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" zoomScale="99" workbookViewId="0">
-      <selection activeCell="H268" sqref="H268"/>
+    <sheetView tabSelected="1" topLeftCell="A259" zoomScale="99" workbookViewId="0">
+      <selection activeCell="O280" sqref="O280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2501,19 +2540,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="75"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="82"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="65"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1">
@@ -2524,17 +2563,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="86"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="69"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1">
@@ -2563,43 +2602,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="87" t="s">
+      <c r="C5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="89" t="s">
+      <c r="D5" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="89" t="s">
+      <c r="E5" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="89" t="s">
+      <c r="F5" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="89" t="s">
+      <c r="G5" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="90" t="s">
+      <c r="H5" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="92" t="s">
+      <c r="I5" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="94" t="s">
+      <c r="J5" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="94" t="s">
+      <c r="K5" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="89" t="s">
+      <c r="L5" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="89" t="s">
+      <c r="M5" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="89" t="s">
+      <c r="N5" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="57" t="s">
+      <c r="O5" s="79" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2610,19 +2649,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="91"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="88"/>
-      <c r="M6" s="88"/>
-      <c r="N6" s="88"/>
-      <c r="O6" s="58"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
+      <c r="N6" s="71"/>
+      <c r="O6" s="80"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1">
       <c r="A7" s="17" t="s">
@@ -2667,7 +2706,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="59"/>
+      <c r="O7" s="81"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2680,35 +2719,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="63" t="s">
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="68" t="s">
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="89"/>
+      <c r="M8" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="69"/>
+      <c r="N8" s="91"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="70" t="s">
+      <c r="P8" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="71"/>
-      <c r="R8" s="72"/>
-      <c r="S8" s="72"/>
-      <c r="T8" s="73"/>
+      <c r="Q8" s="93"/>
+      <c r="R8" s="94"/>
+      <c r="S8" s="94"/>
+      <c r="T8" s="95"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="26" t="s">
@@ -11671,7 +11710,7 @@
     </row>
     <row r="253" spans="1:14" ht="18" customHeight="1">
       <c r="A253" s="24"/>
-      <c r="B253" s="97" t="s">
+      <c r="B253" s="44" t="s">
         <v>351</v>
       </c>
       <c r="C253" s="42" t="s">
@@ -11680,7 +11719,7 @@
       <c r="D253" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="E253" s="96" t="s">
+      <c r="E253" s="42" t="s">
         <v>355</v>
       </c>
       <c r="F253" s="2"/>
@@ -11697,7 +11736,7 @@
     </row>
     <row r="254" spans="1:14" ht="18" customHeight="1">
       <c r="A254" s="24"/>
-      <c r="B254" s="97" t="s">
+      <c r="B254" s="44" t="s">
         <v>352</v>
       </c>
       <c r="C254" s="42" t="s">
@@ -11706,7 +11745,7 @@
       <c r="D254" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="E254" s="96" t="s">
+      <c r="E254" s="42" t="s">
         <v>355</v>
       </c>
       <c r="F254" s="2"/>
@@ -11723,7 +11762,7 @@
     </row>
     <row r="255" spans="1:14" ht="18" customHeight="1">
       <c r="A255" s="24"/>
-      <c r="B255" s="97" t="s">
+      <c r="B255" s="44" t="s">
         <v>353</v>
       </c>
       <c r="C255" s="42" t="s">
@@ -11732,7 +11771,7 @@
       <c r="D255" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="E255" s="96" t="s">
+      <c r="E255" s="42" t="s">
         <v>355</v>
       </c>
       <c r="F255" s="2"/>
@@ -11749,7 +11788,7 @@
     </row>
     <row r="256" spans="1:14" ht="18" customHeight="1">
       <c r="A256" s="24"/>
-      <c r="B256" s="97" t="s">
+      <c r="B256" s="44" t="s">
         <v>354</v>
       </c>
       <c r="C256" s="42" t="s">
@@ -11758,7 +11797,7 @@
       <c r="D256" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="E256" s="96" t="s">
+      <c r="E256" s="42" t="s">
         <v>355</v>
       </c>
       <c r="F256" s="2"/>
@@ -11775,7 +11814,7 @@
     </row>
     <row r="257" spans="1:14" ht="18" customHeight="1">
       <c r="A257" s="24"/>
-      <c r="B257" s="97" t="s">
+      <c r="B257" s="44" t="s">
         <v>359</v>
       </c>
       <c r="C257" s="2" t="s">
@@ -11784,7 +11823,7 @@
       <c r="D257" s="42" t="s">
         <v>358</v>
       </c>
-      <c r="E257" s="96" t="s">
+      <c r="E257" s="42" t="s">
         <v>366</v>
       </c>
       <c r="F257" s="2"/>
@@ -11801,7 +11840,7 @@
     </row>
     <row r="258" spans="1:14" ht="18" customHeight="1">
       <c r="A258" s="24"/>
-      <c r="B258" s="97" t="s">
+      <c r="B258" s="44" t="s">
         <v>360</v>
       </c>
       <c r="C258" s="2" t="s">
@@ -11810,7 +11849,7 @@
       <c r="D258" s="42" t="s">
         <v>358</v>
       </c>
-      <c r="E258" s="96" t="s">
+      <c r="E258" s="42" t="s">
         <v>366</v>
       </c>
       <c r="F258" s="2"/>
@@ -11827,7 +11866,7 @@
     </row>
     <row r="259" spans="1:14" ht="18" customHeight="1">
       <c r="A259" s="24"/>
-      <c r="B259" s="97" t="s">
+      <c r="B259" s="44" t="s">
         <v>361</v>
       </c>
       <c r="C259" s="2" t="s">
@@ -11836,7 +11875,7 @@
       <c r="D259" s="42" t="s">
         <v>358</v>
       </c>
-      <c r="E259" s="96" t="s">
+      <c r="E259" s="42" t="s">
         <v>366</v>
       </c>
       <c r="F259" s="2"/>
@@ -11853,7 +11892,7 @@
     </row>
     <row r="260" spans="1:14" ht="18" customHeight="1">
       <c r="A260" s="24"/>
-      <c r="B260" s="97" t="s">
+      <c r="B260" s="44" t="s">
         <v>362</v>
       </c>
       <c r="C260" s="2" t="s">
@@ -11862,7 +11901,7 @@
       <c r="D260" s="42" t="s">
         <v>358</v>
       </c>
-      <c r="E260" s="96" t="s">
+      <c r="E260" s="42" t="s">
         <v>367</v>
       </c>
       <c r="F260" s="2"/>
@@ -11879,7 +11918,7 @@
     </row>
     <row r="261" spans="1:14" ht="18" customHeight="1">
       <c r="A261" s="24"/>
-      <c r="B261" s="97" t="s">
+      <c r="B261" s="44" t="s">
         <v>362</v>
       </c>
       <c r="C261" s="2" t="s">
@@ -11888,7 +11927,7 @@
       <c r="D261" s="42" t="s">
         <v>363</v>
       </c>
-      <c r="E261" s="96" t="s">
+      <c r="E261" s="42" t="s">
         <v>368</v>
       </c>
       <c r="F261" s="2"/>
@@ -11905,8 +11944,18 @@
     </row>
     <row r="262" spans="1:14" ht="18" customHeight="1">
       <c r="A262" s="24"/>
-      <c r="C262" s="2"/>
-      <c r="D262" s="2"/>
+      <c r="B262" s="96" t="s">
+        <v>369</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D262" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E262" s="97" t="s">
+        <v>372</v>
+      </c>
       <c r="F262" s="2"/>
       <c r="G262" s="2"/>
       <c r="H262" s="2"/>
@@ -11915,12 +11964,24 @@
       <c r="K262" s="4"/>
       <c r="L262" s="44"/>
       <c r="M262" s="44"/>
-      <c r="N262" s="44"/>
+      <c r="N262" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="263" spans="1:14" ht="18" customHeight="1">
       <c r="A263" s="24"/>
-      <c r="C263" s="2"/>
-      <c r="D263" s="2"/>
+      <c r="B263" s="96" t="s">
+        <v>370</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D263" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E263" s="97" t="s">
+        <v>372</v>
+      </c>
       <c r="F263" s="2"/>
       <c r="G263" s="2"/>
       <c r="H263" s="2"/>
@@ -11929,40 +11990,104 @@
       <c r="K263" s="4"/>
       <c r="L263" s="44"/>
       <c r="M263" s="44"/>
-      <c r="N263" s="44"/>
+      <c r="N263" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="264" spans="1:14" ht="18" customHeight="1">
       <c r="A264" s="24"/>
-      <c r="C264" s="2"/>
-      <c r="D264" s="2"/>
-      <c r="F264" s="2"/>
-      <c r="G264" s="2"/>
-      <c r="H264" s="2"/>
-      <c r="I264" s="3"/>
-      <c r="J264" s="4"/>
+      <c r="B264" s="96" t="s">
+        <v>369</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D264" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E264" s="97" t="s">
+        <v>374</v>
+      </c>
+      <c r="F264" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G264" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H264" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I264" s="3">
+        <v>298</v>
+      </c>
+      <c r="J264" s="4">
+        <v>400000000</v>
+      </c>
       <c r="K264" s="4"/>
-      <c r="L264" s="44"/>
-      <c r="M264" s="44"/>
-      <c r="N264" s="44"/>
+      <c r="L264" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M264" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N264" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="265" spans="1:14" ht="18" customHeight="1">
       <c r="A265" s="24"/>
-      <c r="C265" s="2"/>
-      <c r="D265" s="2"/>
-      <c r="F265" s="2"/>
-      <c r="G265" s="2"/>
-      <c r="H265" s="2"/>
-      <c r="I265" s="3"/>
-      <c r="J265" s="4"/>
+      <c r="B265" s="96" t="s">
+        <v>370</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D265" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E265" s="97" t="s">
+        <v>374</v>
+      </c>
+      <c r="F265" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G265" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H265" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I265" s="3">
+        <v>298</v>
+      </c>
+      <c r="J265" s="4">
+        <v>604000000</v>
+      </c>
       <c r="K265" s="4"/>
-      <c r="L265" s="44"/>
-      <c r="M265" s="44"/>
-      <c r="N265" s="44"/>
+      <c r="L265" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M265" s="44" t="s">
+        <v>377</v>
+      </c>
+      <c r="N265" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="266" spans="1:14" ht="18" customHeight="1">
       <c r="A266" s="24"/>
-      <c r="C266" s="2"/>
-      <c r="D266" s="2"/>
+      <c r="B266" s="96" t="s">
+        <v>369</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D266" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E266" s="97" t="s">
+        <v>374</v>
+      </c>
       <c r="F266" s="2"/>
       <c r="G266" s="2"/>
       <c r="H266" s="2"/>
@@ -11971,166 +12096,464 @@
       <c r="K266" s="4"/>
       <c r="L266" s="44"/>
       <c r="M266" s="44"/>
-      <c r="N266" s="44"/>
+      <c r="N266" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="267" spans="1:14" ht="18" customHeight="1">
       <c r="A267" s="24"/>
-      <c r="C267" s="2"/>
-      <c r="D267" s="2"/>
-      <c r="F267" s="2"/>
-      <c r="G267" s="2"/>
-      <c r="H267" s="2"/>
-      <c r="I267" s="3"/>
-      <c r="J267" s="4"/>
+      <c r="B267" s="96" t="s">
+        <v>370</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D267" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E267" s="97" t="s">
+        <v>374</v>
+      </c>
+      <c r="F267" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G267" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H267" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I267" s="3">
+        <v>77</v>
+      </c>
+      <c r="J267" s="4">
+        <v>900000000</v>
+      </c>
       <c r="K267" s="4"/>
-      <c r="L267" s="44"/>
-      <c r="M267" s="44"/>
-      <c r="N267" s="44"/>
+      <c r="L267" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M267" s="44" t="s">
+        <v>377</v>
+      </c>
+      <c r="N267" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="268" spans="1:14" ht="18" customHeight="1">
       <c r="A268" s="24"/>
-      <c r="C268" s="2"/>
-      <c r="D268" s="2"/>
-      <c r="F268" s="2"/>
-      <c r="G268" s="2"/>
-      <c r="H268" s="2"/>
-      <c r="I268" s="3"/>
-      <c r="J268" s="4"/>
+      <c r="B268" s="96" t="s">
+        <v>369</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D268" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E268" s="97" t="s">
+        <v>374</v>
+      </c>
+      <c r="F268" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G268" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H268" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I268" s="3">
+        <v>298</v>
+      </c>
+      <c r="J268" s="4">
+        <v>786000000</v>
+      </c>
       <c r="K268" s="4"/>
-      <c r="L268" s="44"/>
-      <c r="M268" s="44"/>
-      <c r="N268" s="44"/>
+      <c r="L268" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M268" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N268" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="269" spans="1:14" ht="18" customHeight="1">
       <c r="A269" s="24"/>
-      <c r="C269" s="2"/>
-      <c r="D269" s="2"/>
-      <c r="F269" s="2"/>
-      <c r="G269" s="2"/>
-      <c r="H269" s="2"/>
-      <c r="I269" s="3"/>
-      <c r="J269" s="4"/>
+      <c r="B269" s="96" t="s">
+        <v>370</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D269" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E269" s="97" t="s">
+        <v>374</v>
+      </c>
+      <c r="F269" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G269" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H269" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I269" s="3">
+        <v>298</v>
+      </c>
+      <c r="J269" s="4">
+        <v>871000000</v>
+      </c>
       <c r="K269" s="4"/>
-      <c r="L269" s="44"/>
-      <c r="M269" s="44"/>
-      <c r="N269" s="44"/>
+      <c r="L269" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M269" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N269" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="270" spans="1:14" ht="18" customHeight="1">
       <c r="A270" s="24"/>
-      <c r="C270" s="2"/>
-      <c r="D270" s="2"/>
-      <c r="F270" s="2"/>
-      <c r="G270" s="2"/>
-      <c r="H270" s="2"/>
-      <c r="I270" s="3"/>
-      <c r="J270" s="4"/>
+      <c r="B270" s="96" t="s">
+        <v>369</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D270" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E270" s="97" t="s">
+        <v>374</v>
+      </c>
+      <c r="F270" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G270" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H270" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I270" s="3">
+        <v>77</v>
+      </c>
+      <c r="J270" s="4">
+        <v>1333000000</v>
+      </c>
       <c r="K270" s="4"/>
-      <c r="L270" s="44"/>
-      <c r="M270" s="44"/>
-      <c r="N270" s="44"/>
+      <c r="L270" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M270" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N270" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="271" spans="1:14" ht="18" customHeight="1">
       <c r="A271" s="24"/>
-      <c r="C271" s="2"/>
-      <c r="D271" s="2"/>
-      <c r="F271" s="2"/>
-      <c r="G271" s="2"/>
-      <c r="H271" s="2"/>
-      <c r="I271" s="3"/>
-      <c r="J271" s="4"/>
+      <c r="B271" s="96" t="s">
+        <v>370</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D271" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E271" s="97" t="s">
+        <v>374</v>
+      </c>
+      <c r="F271" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G271" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H271" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I271" s="3">
+        <v>77</v>
+      </c>
+      <c r="J271" s="4">
+        <v>1294000000</v>
+      </c>
       <c r="K271" s="4"/>
-      <c r="L271" s="44"/>
-      <c r="M271" s="44"/>
-      <c r="N271" s="44"/>
+      <c r="L271" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M271" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N271" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="272" spans="1:14" ht="18" customHeight="1">
       <c r="A272" s="24"/>
-      <c r="C272" s="2"/>
-      <c r="D272" s="2"/>
-      <c r="F272" s="2"/>
-      <c r="G272" s="2"/>
-      <c r="H272" s="2"/>
-      <c r="I272" s="3"/>
-      <c r="J272" s="4"/>
+      <c r="B272" s="96" t="s">
+        <v>369</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D272" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E272" s="97" t="s">
+        <v>374</v>
+      </c>
+      <c r="F272" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G272" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H272" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I272" s="3">
+        <v>298</v>
+      </c>
+      <c r="J272" s="4">
+        <v>52</v>
+      </c>
       <c r="K272" s="4"/>
-      <c r="L272" s="44"/>
-      <c r="M272" s="44"/>
-      <c r="N272" s="44"/>
+      <c r="L272" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M272" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N272" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="273" spans="1:14" ht="18" customHeight="1">
       <c r="A273" s="24"/>
-      <c r="C273" s="2"/>
-      <c r="D273" s="2"/>
-      <c r="F273" s="2"/>
-      <c r="G273" s="2"/>
-      <c r="H273" s="2"/>
-      <c r="I273" s="3"/>
-      <c r="J273" s="4"/>
+      <c r="B273" s="96" t="s">
+        <v>370</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D273" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E273" s="97" t="s">
+        <v>374</v>
+      </c>
+      <c r="F273" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G273" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H273" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I273" s="3">
+        <v>298</v>
+      </c>
+      <c r="J273" s="4">
+        <v>42</v>
+      </c>
       <c r="K273" s="4"/>
-      <c r="L273" s="44"/>
-      <c r="M273" s="44"/>
-      <c r="N273" s="44"/>
+      <c r="L273" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M273" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N273" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="274" spans="1:14" ht="18" customHeight="1">
       <c r="A274" s="24"/>
-      <c r="C274" s="2"/>
-      <c r="D274" s="2"/>
-      <c r="F274" s="2"/>
-      <c r="G274" s="2"/>
-      <c r="H274" s="2"/>
-      <c r="I274" s="3"/>
-      <c r="J274" s="4"/>
+      <c r="B274" s="96" t="s">
+        <v>369</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D274" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E274" s="97" t="s">
+        <v>374</v>
+      </c>
+      <c r="F274" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G274" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H274" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I274" s="3">
+        <v>77</v>
+      </c>
+      <c r="J274" s="4">
+        <v>74</v>
+      </c>
       <c r="K274" s="4"/>
-      <c r="L274" s="44"/>
-      <c r="M274" s="44"/>
-      <c r="N274" s="44"/>
+      <c r="L274" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M274" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N274" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="275" spans="1:14" ht="18" customHeight="1">
       <c r="A275" s="24"/>
-      <c r="C275" s="2"/>
-      <c r="D275" s="2"/>
-      <c r="F275" s="2"/>
-      <c r="G275" s="2"/>
-      <c r="H275" s="2"/>
-      <c r="I275" s="3"/>
-      <c r="J275" s="4"/>
+      <c r="B275" s="96" t="s">
+        <v>370</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D275" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E275" s="97" t="s">
+        <v>374</v>
+      </c>
+      <c r="F275" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G275" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H275" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I275" s="3">
+        <v>77</v>
+      </c>
+      <c r="J275" s="4">
+        <v>55</v>
+      </c>
       <c r="K275" s="4"/>
-      <c r="L275" s="44"/>
-      <c r="M275" s="44"/>
-      <c r="N275" s="44"/>
+      <c r="L275" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M275" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N275" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="276" spans="1:14" ht="18" customHeight="1">
       <c r="A276" s="24"/>
-      <c r="C276" s="2"/>
-      <c r="D276" s="2"/>
-      <c r="F276" s="2"/>
-      <c r="G276" s="2"/>
-      <c r="H276" s="2"/>
-      <c r="I276" s="3"/>
-      <c r="J276" s="4"/>
+      <c r="B276" s="96" t="s">
+        <v>369</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D276" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E276" s="97" t="s">
+        <v>375</v>
+      </c>
+      <c r="F276" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G276" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H276" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I276" s="3">
+        <v>298</v>
+      </c>
+      <c r="J276" s="4">
+        <v>170000000</v>
+      </c>
       <c r="K276" s="4"/>
-      <c r="L276" s="44"/>
-      <c r="M276" s="44"/>
-      <c r="N276" s="44"/>
+      <c r="L276" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M276" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N276" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="277" spans="1:14" ht="18" customHeight="1">
       <c r="A277" s="24"/>
-      <c r="C277" s="2"/>
-      <c r="D277" s="2"/>
-      <c r="F277" s="2"/>
-      <c r="G277" s="2"/>
-      <c r="H277" s="2"/>
-      <c r="I277" s="3"/>
-      <c r="J277" s="4"/>
+      <c r="B277" s="96" t="s">
+        <v>370</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D277" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E277" s="97" t="s">
+        <v>375</v>
+      </c>
+      <c r="F277" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G277" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H277" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I277" s="3">
+        <v>298</v>
+      </c>
+      <c r="J277" s="4">
+        <v>410000000</v>
+      </c>
       <c r="K277" s="4"/>
-      <c r="L277" s="44"/>
-      <c r="M277" s="44"/>
-      <c r="N277" s="44"/>
+      <c r="L277" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M277" s="44" t="s">
+        <v>377</v>
+      </c>
+      <c r="N277" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="278" spans="1:14" ht="18" customHeight="1">
       <c r="A278" s="24"/>
-      <c r="C278" s="2"/>
-      <c r="D278" s="2"/>
+      <c r="B278" s="96" t="s">
+        <v>369</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D278" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E278" s="97" t="s">
+        <v>375</v>
+      </c>
       <c r="F278" s="2"/>
       <c r="G278" s="2"/>
       <c r="H278" s="2"/>
@@ -12139,133 +12562,369 @@
       <c r="K278" s="4"/>
       <c r="L278" s="44"/>
       <c r="M278" s="44"/>
-      <c r="N278" s="44"/>
+      <c r="N278" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="279" spans="1:14" ht="18" customHeight="1">
       <c r="A279" s="24"/>
-      <c r="C279" s="2"/>
-      <c r="D279" s="2"/>
-      <c r="F279" s="2"/>
-      <c r="G279" s="2"/>
-      <c r="H279" s="2"/>
-      <c r="I279" s="3"/>
-      <c r="J279" s="4"/>
+      <c r="B279" s="96" t="s">
+        <v>370</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D279" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E279" s="97" t="s">
+        <v>375</v>
+      </c>
+      <c r="F279" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G279" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H279" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I279" s="3">
+        <v>77</v>
+      </c>
+      <c r="J279" s="4">
+        <v>666000000</v>
+      </c>
       <c r="K279" s="4"/>
-      <c r="L279" s="44"/>
-      <c r="M279" s="44"/>
-      <c r="N279" s="44"/>
+      <c r="L279" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M279" s="44" t="s">
+        <v>377</v>
+      </c>
+      <c r="N279" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="280" spans="1:14" ht="18" customHeight="1">
       <c r="A280" s="24"/>
-      <c r="C280" s="2"/>
-      <c r="D280" s="2"/>
-      <c r="F280" s="2"/>
-      <c r="G280" s="2"/>
-      <c r="H280" s="2"/>
-      <c r="I280" s="3"/>
-      <c r="J280" s="4"/>
+      <c r="B280" s="96" t="s">
+        <v>369</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D280" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E280" s="97" t="s">
+        <v>375</v>
+      </c>
+      <c r="F280" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G280" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H280" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I280" s="3">
+        <v>298</v>
+      </c>
+      <c r="J280" s="4">
+        <v>538000000</v>
+      </c>
       <c r="K280" s="4"/>
-      <c r="L280" s="44"/>
-      <c r="M280" s="44"/>
-      <c r="N280" s="44"/>
+      <c r="L280" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M280" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N280" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="281" spans="1:14" ht="18" customHeight="1">
       <c r="A281" s="24"/>
-      <c r="C281" s="2"/>
-      <c r="D281" s="2"/>
-      <c r="F281" s="2"/>
-      <c r="G281" s="2"/>
-      <c r="H281" s="2"/>
-      <c r="I281" s="3"/>
-      <c r="J281" s="4"/>
+      <c r="B281" s="96" t="s">
+        <v>370</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D281" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E281" s="97" t="s">
+        <v>375</v>
+      </c>
+      <c r="F281" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G281" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H281" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I281" s="3">
+        <v>298</v>
+      </c>
+      <c r="J281" s="4">
+        <v>709000000</v>
+      </c>
       <c r="K281" s="4"/>
-      <c r="L281" s="44"/>
-      <c r="M281" s="44"/>
-      <c r="N281" s="44"/>
+      <c r="L281" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M281" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N281" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="282" spans="1:14" ht="18" customHeight="1">
       <c r="A282" s="24"/>
-      <c r="C282" s="2"/>
-      <c r="D282" s="2"/>
-      <c r="F282" s="2"/>
-      <c r="G282" s="2"/>
-      <c r="H282" s="2"/>
-      <c r="I282" s="3"/>
-      <c r="J282" s="4"/>
+      <c r="B282" s="96" t="s">
+        <v>369</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D282" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E282" s="97" t="s">
+        <v>375</v>
+      </c>
+      <c r="F282" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G282" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H282" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I282" s="3">
+        <v>77</v>
+      </c>
+      <c r="J282" s="4">
+        <v>914000000</v>
+      </c>
       <c r="K282" s="4"/>
-      <c r="L282" s="44"/>
-      <c r="M282" s="44"/>
-      <c r="N282" s="44"/>
+      <c r="L282" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M282" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N282" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="283" spans="1:14" ht="18" customHeight="1">
       <c r="A283" s="24"/>
-      <c r="C283" s="2"/>
-      <c r="D283" s="2"/>
-      <c r="F283" s="2"/>
-      <c r="G283" s="2"/>
-      <c r="H283" s="2"/>
-      <c r="I283" s="3"/>
-      <c r="J283" s="4"/>
+      <c r="B283" s="96" t="s">
+        <v>370</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D283" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E283" s="97" t="s">
+        <v>375</v>
+      </c>
+      <c r="F283" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G283" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H283" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I283" s="3">
+        <v>77</v>
+      </c>
+      <c r="J283" s="4">
+        <v>1012000000</v>
+      </c>
       <c r="K283" s="4"/>
-      <c r="L283" s="44"/>
-      <c r="M283" s="44"/>
-      <c r="N283" s="44"/>
+      <c r="L283" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M283" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N283" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="284" spans="1:14" ht="18" customHeight="1">
       <c r="A284" s="24"/>
-      <c r="C284" s="2"/>
-      <c r="D284" s="2"/>
-      <c r="F284" s="2"/>
-      <c r="G284" s="2"/>
-      <c r="H284" s="2"/>
-      <c r="I284" s="3"/>
-      <c r="J284" s="4"/>
+      <c r="B284" s="96" t="s">
+        <v>369</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D284" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E284" s="97" t="s">
+        <v>375</v>
+      </c>
+      <c r="F284" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G284" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H284" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I284" s="3">
+        <v>298</v>
+      </c>
+      <c r="J284" s="4">
+        <v>78</v>
+      </c>
       <c r="K284" s="4"/>
-      <c r="L284" s="44"/>
-      <c r="M284" s="44"/>
-      <c r="N284" s="44"/>
+      <c r="L284" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M284" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N284" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="285" spans="1:14" ht="18" customHeight="1">
       <c r="A285" s="24"/>
-      <c r="C285" s="2"/>
-      <c r="D285" s="2"/>
-      <c r="F285" s="2"/>
-      <c r="G285" s="2"/>
-      <c r="H285" s="2"/>
-      <c r="I285" s="3"/>
-      <c r="J285" s="4"/>
+      <c r="B285" s="96" t="s">
+        <v>370</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D285" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E285" s="97" t="s">
+        <v>375</v>
+      </c>
+      <c r="F285" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G285" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H285" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I285" s="3">
+        <v>298</v>
+      </c>
+      <c r="J285" s="4">
+        <v>54</v>
+      </c>
       <c r="K285" s="4"/>
-      <c r="L285" s="44"/>
-      <c r="M285" s="44"/>
-      <c r="N285" s="44"/>
+      <c r="L285" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M285" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N285" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="286" spans="1:14" ht="18" customHeight="1">
       <c r="A286" s="24"/>
-      <c r="C286" s="2"/>
-      <c r="D286" s="2"/>
-      <c r="F286" s="2"/>
-      <c r="G286" s="2"/>
-      <c r="H286" s="2"/>
-      <c r="I286" s="3"/>
-      <c r="J286" s="4"/>
+      <c r="B286" s="96" t="s">
+        <v>369</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D286" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E286" s="97" t="s">
+        <v>375</v>
+      </c>
+      <c r="F286" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G286" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H286" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I286" s="3">
+        <v>77</v>
+      </c>
+      <c r="J286" s="4">
+        <v>107</v>
+      </c>
       <c r="K286" s="4"/>
-      <c r="L286" s="44"/>
-      <c r="M286" s="44"/>
-      <c r="N286" s="44"/>
+      <c r="L286" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M286" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N286" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="287" spans="1:14" ht="18" customHeight="1">
       <c r="A287" s="24"/>
-      <c r="C287" s="2"/>
-      <c r="D287" s="2"/>
-      <c r="F287" s="2"/>
-      <c r="G287" s="2"/>
-      <c r="H287" s="2"/>
-      <c r="I287" s="3"/>
-      <c r="J287" s="4"/>
+      <c r="B287" s="96" t="s">
+        <v>370</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D287" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E287" s="97" t="s">
+        <v>375</v>
+      </c>
+      <c r="F287" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G287" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H287" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I287" s="3">
+        <v>77</v>
+      </c>
+      <c r="J287" s="4">
+        <v>70</v>
+      </c>
       <c r="K287" s="4"/>
-      <c r="L287" s="44"/>
-      <c r="M287" s="44"/>
-      <c r="N287" s="44"/>
+      <c r="L287" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M287" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="N287" s="44" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="288" spans="1:14" ht="18" customHeight="1">
       <c r="A288" s="24"/>
@@ -14187,6 +14846,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -14201,11 +14865,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1016/j.physc.2019.1353520`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCCE68C-E4DE-234A-891C-641AF700C239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B09371-8B85-5545-BDBE-E391502038C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2418" uniqueCount="396">
   <si>
     <t>Metadata</t>
   </si>
@@ -1271,6 +1271,48 @@
   </si>
   <si>
     <t>10.1038/s41586-019-1617-1</t>
+  </si>
+  <si>
+    <t>MoReRu</t>
+  </si>
+  <si>
+    <t>MoReRuRh</t>
+  </si>
+  <si>
+    <t>Ti0.05(MoReRuRh)0.2375</t>
+  </si>
+  <si>
+    <t>Ti0.1(MoReRuRh)0.225</t>
+  </si>
+  <si>
+    <t>Ti0.15 (MoReRh)0.1 Ru0.55</t>
+  </si>
+  <si>
+    <t>Ti0.15 (MoReRh)0.1 Ru0.5</t>
+  </si>
+  <si>
+    <t>Ti0.15 (MoReRh)0.1 Ru0.4</t>
+  </si>
+  <si>
+    <t>Ti0.15 (MoReRh)0.1 Ru0.15</t>
+  </si>
+  <si>
+    <t>VAM+BM</t>
+  </si>
+  <si>
+    <t>Ti0.15(MoReRuRh)0.2125</t>
+  </si>
+  <si>
+    <t>HCP+B2</t>
+  </si>
+  <si>
+    <t>HCP+B2+sigma</t>
+  </si>
+  <si>
+    <t>as-cast samples cryomilled into powder</t>
+  </si>
+  <si>
+    <t>10.1016/j.physc.2019.1353520</t>
   </si>
 </sst>
 </file>
@@ -2060,6 +2102,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2125,57 +2218,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2490,8 +2532,8 @@
   </sheetPr>
   <dimension ref="A1:T424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" zoomScale="99" workbookViewId="0">
-      <selection activeCell="O280" sqref="O280"/>
+    <sheetView tabSelected="1" topLeftCell="A266" zoomScale="89" workbookViewId="0">
+      <selection activeCell="B303" sqref="B303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2540,19 +2582,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="58"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="65"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="82"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1">
@@ -2563,17 +2605,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="69"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="86"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1">
@@ -2602,43 +2644,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="70" t="s">
+      <c r="C5" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="72" t="s">
+      <c r="D5" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="72" t="s">
+      <c r="F5" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="72" t="s">
+      <c r="G5" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="75" t="s">
+      <c r="I5" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="77" t="s">
+      <c r="J5" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="77" t="s">
+      <c r="K5" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="72" t="s">
+      <c r="L5" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="72" t="s">
+      <c r="M5" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="72" t="s">
+      <c r="N5" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="79" t="s">
+      <c r="O5" s="57" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2649,19 +2691,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="80"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="93"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="88"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="58"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1">
       <c r="A7" s="17" t="s">
@@ -2706,7 +2748,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="81"/>
+      <c r="O7" s="59"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2719,35 +2761,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="82" t="s">
+      <c r="B8" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="85" t="s">
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="86"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="87"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="90" t="s">
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="91"/>
+      <c r="N8" s="69"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="92" t="s">
+      <c r="P8" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="93"/>
-      <c r="R8" s="94"/>
-      <c r="S8" s="94"/>
-      <c r="T8" s="95"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="72"/>
+      <c r="S8" s="72"/>
+      <c r="T8" s="73"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="26" t="s">
@@ -11944,7 +11986,7 @@
     </row>
     <row r="262" spans="1:14" ht="18" customHeight="1">
       <c r="A262" s="24"/>
-      <c r="B262" s="96" t="s">
+      <c r="B262" s="44" t="s">
         <v>369</v>
       </c>
       <c r="C262" s="2" t="s">
@@ -11953,7 +11995,7 @@
       <c r="D262" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="E262" s="97" t="s">
+      <c r="E262" s="42" t="s">
         <v>372</v>
       </c>
       <c r="F262" s="2"/>
@@ -11970,7 +12012,7 @@
     </row>
     <row r="263" spans="1:14" ht="18" customHeight="1">
       <c r="A263" s="24"/>
-      <c r="B263" s="96" t="s">
+      <c r="B263" s="44" t="s">
         <v>370</v>
       </c>
       <c r="C263" s="2" t="s">
@@ -11979,7 +12021,7 @@
       <c r="D263" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="E263" s="97" t="s">
+      <c r="E263" s="42" t="s">
         <v>372</v>
       </c>
       <c r="F263" s="2"/>
@@ -11996,7 +12038,7 @@
     </row>
     <row r="264" spans="1:14" ht="18" customHeight="1">
       <c r="A264" s="24"/>
-      <c r="B264" s="96" t="s">
+      <c r="B264" s="44" t="s">
         <v>369</v>
       </c>
       <c r="C264" s="2" t="s">
@@ -12005,7 +12047,7 @@
       <c r="D264" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E264" s="97" t="s">
+      <c r="E264" s="42" t="s">
         <v>374</v>
       </c>
       <c r="F264" s="2" t="s">
@@ -12036,7 +12078,7 @@
     </row>
     <row r="265" spans="1:14" ht="18" customHeight="1">
       <c r="A265" s="24"/>
-      <c r="B265" s="96" t="s">
+      <c r="B265" s="44" t="s">
         <v>370</v>
       </c>
       <c r="C265" s="2" t="s">
@@ -12045,7 +12087,7 @@
       <c r="D265" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E265" s="97" t="s">
+      <c r="E265" s="42" t="s">
         <v>374</v>
       </c>
       <c r="F265" s="2" t="s">
@@ -12076,7 +12118,7 @@
     </row>
     <row r="266" spans="1:14" ht="18" customHeight="1">
       <c r="A266" s="24"/>
-      <c r="B266" s="96" t="s">
+      <c r="B266" s="44" t="s">
         <v>369</v>
       </c>
       <c r="C266" s="2" t="s">
@@ -12085,7 +12127,7 @@
       <c r="D266" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E266" s="97" t="s">
+      <c r="E266" s="42" t="s">
         <v>374</v>
       </c>
       <c r="F266" s="2"/>
@@ -12102,7 +12144,7 @@
     </row>
     <row r="267" spans="1:14" ht="18" customHeight="1">
       <c r="A267" s="24"/>
-      <c r="B267" s="96" t="s">
+      <c r="B267" s="44" t="s">
         <v>370</v>
       </c>
       <c r="C267" s="2" t="s">
@@ -12111,7 +12153,7 @@
       <c r="D267" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E267" s="97" t="s">
+      <c r="E267" s="42" t="s">
         <v>374</v>
       </c>
       <c r="F267" s="2" t="s">
@@ -12142,7 +12184,7 @@
     </row>
     <row r="268" spans="1:14" ht="18" customHeight="1">
       <c r="A268" s="24"/>
-      <c r="B268" s="96" t="s">
+      <c r="B268" s="44" t="s">
         <v>369</v>
       </c>
       <c r="C268" s="2" t="s">
@@ -12151,7 +12193,7 @@
       <c r="D268" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E268" s="97" t="s">
+      <c r="E268" s="42" t="s">
         <v>374</v>
       </c>
       <c r="F268" s="2" t="s">
@@ -12182,7 +12224,7 @@
     </row>
     <row r="269" spans="1:14" ht="18" customHeight="1">
       <c r="A269" s="24"/>
-      <c r="B269" s="96" t="s">
+      <c r="B269" s="44" t="s">
         <v>370</v>
       </c>
       <c r="C269" s="2" t="s">
@@ -12191,7 +12233,7 @@
       <c r="D269" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E269" s="97" t="s">
+      <c r="E269" s="42" t="s">
         <v>374</v>
       </c>
       <c r="F269" s="2" t="s">
@@ -12222,7 +12264,7 @@
     </row>
     <row r="270" spans="1:14" ht="18" customHeight="1">
       <c r="A270" s="24"/>
-      <c r="B270" s="96" t="s">
+      <c r="B270" s="44" t="s">
         <v>369</v>
       </c>
       <c r="C270" s="2" t="s">
@@ -12231,7 +12273,7 @@
       <c r="D270" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E270" s="97" t="s">
+      <c r="E270" s="42" t="s">
         <v>374</v>
       </c>
       <c r="F270" s="2" t="s">
@@ -12262,7 +12304,7 @@
     </row>
     <row r="271" spans="1:14" ht="18" customHeight="1">
       <c r="A271" s="24"/>
-      <c r="B271" s="96" t="s">
+      <c r="B271" s="44" t="s">
         <v>370</v>
       </c>
       <c r="C271" s="2" t="s">
@@ -12271,7 +12313,7 @@
       <c r="D271" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E271" s="97" t="s">
+      <c r="E271" s="42" t="s">
         <v>374</v>
       </c>
       <c r="F271" s="2" t="s">
@@ -12302,7 +12344,7 @@
     </row>
     <row r="272" spans="1:14" ht="18" customHeight="1">
       <c r="A272" s="24"/>
-      <c r="B272" s="96" t="s">
+      <c r="B272" s="44" t="s">
         <v>369</v>
       </c>
       <c r="C272" s="2" t="s">
@@ -12311,7 +12353,7 @@
       <c r="D272" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E272" s="97" t="s">
+      <c r="E272" s="42" t="s">
         <v>374</v>
       </c>
       <c r="F272" s="2" t="s">
@@ -12342,7 +12384,7 @@
     </row>
     <row r="273" spans="1:14" ht="18" customHeight="1">
       <c r="A273" s="24"/>
-      <c r="B273" s="96" t="s">
+      <c r="B273" s="44" t="s">
         <v>370</v>
       </c>
       <c r="C273" s="2" t="s">
@@ -12351,7 +12393,7 @@
       <c r="D273" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E273" s="97" t="s">
+      <c r="E273" s="42" t="s">
         <v>374</v>
       </c>
       <c r="F273" s="2" t="s">
@@ -12382,7 +12424,7 @@
     </row>
     <row r="274" spans="1:14" ht="18" customHeight="1">
       <c r="A274" s="24"/>
-      <c r="B274" s="96" t="s">
+      <c r="B274" s="44" t="s">
         <v>369</v>
       </c>
       <c r="C274" s="2" t="s">
@@ -12391,7 +12433,7 @@
       <c r="D274" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E274" s="97" t="s">
+      <c r="E274" s="42" t="s">
         <v>374</v>
       </c>
       <c r="F274" s="2" t="s">
@@ -12422,7 +12464,7 @@
     </row>
     <row r="275" spans="1:14" ht="18" customHeight="1">
       <c r="A275" s="24"/>
-      <c r="B275" s="96" t="s">
+      <c r="B275" s="44" t="s">
         <v>370</v>
       </c>
       <c r="C275" s="2" t="s">
@@ -12431,7 +12473,7 @@
       <c r="D275" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E275" s="97" t="s">
+      <c r="E275" s="42" t="s">
         <v>374</v>
       </c>
       <c r="F275" s="2" t="s">
@@ -12462,7 +12504,7 @@
     </row>
     <row r="276" spans="1:14" ht="18" customHeight="1">
       <c r="A276" s="24"/>
-      <c r="B276" s="96" t="s">
+      <c r="B276" s="44" t="s">
         <v>369</v>
       </c>
       <c r="C276" s="2" t="s">
@@ -12471,7 +12513,7 @@
       <c r="D276" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E276" s="97" t="s">
+      <c r="E276" s="42" t="s">
         <v>375</v>
       </c>
       <c r="F276" s="2" t="s">
@@ -12502,7 +12544,7 @@
     </row>
     <row r="277" spans="1:14" ht="18" customHeight="1">
       <c r="A277" s="24"/>
-      <c r="B277" s="96" t="s">
+      <c r="B277" s="44" t="s">
         <v>370</v>
       </c>
       <c r="C277" s="2" t="s">
@@ -12511,7 +12553,7 @@
       <c r="D277" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E277" s="97" t="s">
+      <c r="E277" s="42" t="s">
         <v>375</v>
       </c>
       <c r="F277" s="2" t="s">
@@ -12542,7 +12584,7 @@
     </row>
     <row r="278" spans="1:14" ht="18" customHeight="1">
       <c r="A278" s="24"/>
-      <c r="B278" s="96" t="s">
+      <c r="B278" s="44" t="s">
         <v>369</v>
       </c>
       <c r="C278" s="2" t="s">
@@ -12551,7 +12593,7 @@
       <c r="D278" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E278" s="97" t="s">
+      <c r="E278" s="42" t="s">
         <v>375</v>
       </c>
       <c r="F278" s="2"/>
@@ -12568,7 +12610,7 @@
     </row>
     <row r="279" spans="1:14" ht="18" customHeight="1">
       <c r="A279" s="24"/>
-      <c r="B279" s="96" t="s">
+      <c r="B279" s="44" t="s">
         <v>370</v>
       </c>
       <c r="C279" s="2" t="s">
@@ -12577,7 +12619,7 @@
       <c r="D279" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E279" s="97" t="s">
+      <c r="E279" s="42" t="s">
         <v>375</v>
       </c>
       <c r="F279" s="2" t="s">
@@ -12608,7 +12650,7 @@
     </row>
     <row r="280" spans="1:14" ht="18" customHeight="1">
       <c r="A280" s="24"/>
-      <c r="B280" s="96" t="s">
+      <c r="B280" s="44" t="s">
         <v>369</v>
       </c>
       <c r="C280" s="2" t="s">
@@ -12617,7 +12659,7 @@
       <c r="D280" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E280" s="97" t="s">
+      <c r="E280" s="42" t="s">
         <v>375</v>
       </c>
       <c r="F280" s="2" t="s">
@@ -12648,7 +12690,7 @@
     </row>
     <row r="281" spans="1:14" ht="18" customHeight="1">
       <c r="A281" s="24"/>
-      <c r="B281" s="96" t="s">
+      <c r="B281" s="44" t="s">
         <v>370</v>
       </c>
       <c r="C281" s="2" t="s">
@@ -12657,7 +12699,7 @@
       <c r="D281" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E281" s="97" t="s">
+      <c r="E281" s="42" t="s">
         <v>375</v>
       </c>
       <c r="F281" s="2" t="s">
@@ -12688,7 +12730,7 @@
     </row>
     <row r="282" spans="1:14" ht="18" customHeight="1">
       <c r="A282" s="24"/>
-      <c r="B282" s="96" t="s">
+      <c r="B282" s="44" t="s">
         <v>369</v>
       </c>
       <c r="C282" s="2" t="s">
@@ -12697,7 +12739,7 @@
       <c r="D282" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E282" s="97" t="s">
+      <c r="E282" s="42" t="s">
         <v>375</v>
       </c>
       <c r="F282" s="2" t="s">
@@ -12728,7 +12770,7 @@
     </row>
     <row r="283" spans="1:14" ht="18" customHeight="1">
       <c r="A283" s="24"/>
-      <c r="B283" s="96" t="s">
+      <c r="B283" s="44" t="s">
         <v>370</v>
       </c>
       <c r="C283" s="2" t="s">
@@ -12737,7 +12779,7 @@
       <c r="D283" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E283" s="97" t="s">
+      <c r="E283" s="42" t="s">
         <v>375</v>
       </c>
       <c r="F283" s="2" t="s">
@@ -12768,7 +12810,7 @@
     </row>
     <row r="284" spans="1:14" ht="18" customHeight="1">
       <c r="A284" s="24"/>
-      <c r="B284" s="96" t="s">
+      <c r="B284" s="44" t="s">
         <v>369</v>
       </c>
       <c r="C284" s="2" t="s">
@@ -12777,7 +12819,7 @@
       <c r="D284" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E284" s="97" t="s">
+      <c r="E284" s="42" t="s">
         <v>375</v>
       </c>
       <c r="F284" s="2" t="s">
@@ -12808,7 +12850,7 @@
     </row>
     <row r="285" spans="1:14" ht="18" customHeight="1">
       <c r="A285" s="24"/>
-      <c r="B285" s="96" t="s">
+      <c r="B285" s="44" t="s">
         <v>370</v>
       </c>
       <c r="C285" s="2" t="s">
@@ -12817,7 +12859,7 @@
       <c r="D285" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E285" s="97" t="s">
+      <c r="E285" s="42" t="s">
         <v>375</v>
       </c>
       <c r="F285" s="2" t="s">
@@ -12848,7 +12890,7 @@
     </row>
     <row r="286" spans="1:14" ht="18" customHeight="1">
       <c r="A286" s="24"/>
-      <c r="B286" s="96" t="s">
+      <c r="B286" s="44" t="s">
         <v>369</v>
       </c>
       <c r="C286" s="2" t="s">
@@ -12857,7 +12899,7 @@
       <c r="D286" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E286" s="97" t="s">
+      <c r="E286" s="42" t="s">
         <v>375</v>
       </c>
       <c r="F286" s="2" t="s">
@@ -12888,7 +12930,7 @@
     </row>
     <row r="287" spans="1:14" ht="18" customHeight="1">
       <c r="A287" s="24"/>
-      <c r="B287" s="96" t="s">
+      <c r="B287" s="44" t="s">
         <v>370</v>
       </c>
       <c r="C287" s="2" t="s">
@@ -12897,7 +12939,7 @@
       <c r="D287" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E287" s="97" t="s">
+      <c r="E287" s="42" t="s">
         <v>375</v>
       </c>
       <c r="F287" s="2" t="s">
@@ -12928,8 +12970,18 @@
     </row>
     <row r="288" spans="1:14" ht="18" customHeight="1">
       <c r="A288" s="24"/>
-      <c r="C288" s="2"/>
-      <c r="D288" s="2"/>
+      <c r="B288" s="96" t="s">
+        <v>382</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D288" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E288" s="97" t="s">
+        <v>394</v>
+      </c>
       <c r="F288" s="2"/>
       <c r="G288" s="2"/>
       <c r="H288" s="2"/>
@@ -12938,12 +12990,24 @@
       <c r="K288" s="4"/>
       <c r="L288" s="44"/>
       <c r="M288" s="44"/>
-      <c r="N288" s="44"/>
+      <c r="N288" s="44" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="289" spans="1:14" ht="18" customHeight="1">
       <c r="A289" s="24"/>
-      <c r="C289" s="2"/>
-      <c r="D289" s="2"/>
+      <c r="B289" s="96" t="s">
+        <v>383</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D289" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E289" s="97" t="s">
+        <v>394</v>
+      </c>
       <c r="F289" s="2"/>
       <c r="G289" s="2"/>
       <c r="H289" s="2"/>
@@ -12952,12 +13016,24 @@
       <c r="K289" s="4"/>
       <c r="L289" s="44"/>
       <c r="M289" s="44"/>
-      <c r="N289" s="44"/>
+      <c r="N289" s="44" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="290" spans="1:14" ht="18" customHeight="1">
       <c r="A290" s="24"/>
-      <c r="C290" s="2"/>
-      <c r="D290" s="2"/>
+      <c r="B290" s="96" t="s">
+        <v>384</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D290" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E290" s="97" t="s">
+        <v>394</v>
+      </c>
       <c r="F290" s="2"/>
       <c r="G290" s="2"/>
       <c r="H290" s="2"/>
@@ -12966,12 +13042,24 @@
       <c r="K290" s="4"/>
       <c r="L290" s="44"/>
       <c r="M290" s="44"/>
-      <c r="N290" s="44"/>
+      <c r="N290" s="44" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="291" spans="1:14" ht="18" customHeight="1">
       <c r="A291" s="24"/>
-      <c r="C291" s="2"/>
-      <c r="D291" s="2"/>
+      <c r="B291" s="96" t="s">
+        <v>385</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D291" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E291" s="97" t="s">
+        <v>394</v>
+      </c>
       <c r="F291" s="2"/>
       <c r="G291" s="2"/>
       <c r="H291" s="2"/>
@@ -12980,12 +13068,24 @@
       <c r="K291" s="4"/>
       <c r="L291" s="44"/>
       <c r="M291" s="44"/>
-      <c r="N291" s="44"/>
+      <c r="N291" s="44" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="292" spans="1:14" ht="18" customHeight="1">
       <c r="A292" s="24"/>
-      <c r="C292" s="2"/>
-      <c r="D292" s="2"/>
+      <c r="B292" s="96" t="s">
+        <v>391</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="D292" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E292" s="97" t="s">
+        <v>394</v>
+      </c>
       <c r="F292" s="2"/>
       <c r="G292" s="2"/>
       <c r="H292" s="2"/>
@@ -12994,12 +13094,24 @@
       <c r="K292" s="4"/>
       <c r="L292" s="44"/>
       <c r="M292" s="44"/>
-      <c r="N292" s="44"/>
+      <c r="N292" s="44" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="293" spans="1:14" ht="18" customHeight="1">
       <c r="A293" s="24"/>
-      <c r="C293" s="2"/>
-      <c r="D293" s="2"/>
+      <c r="B293" s="96" t="s">
+        <v>386</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D293" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E293" s="97" t="s">
+        <v>394</v>
+      </c>
       <c r="F293" s="2"/>
       <c r="G293" s="2"/>
       <c r="H293" s="2"/>
@@ -13008,12 +13120,24 @@
       <c r="K293" s="4"/>
       <c r="L293" s="44"/>
       <c r="M293" s="44"/>
-      <c r="N293" s="44"/>
+      <c r="N293" s="44" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="294" spans="1:14" ht="18" customHeight="1">
       <c r="A294" s="24"/>
-      <c r="C294" s="2"/>
-      <c r="D294" s="2"/>
+      <c r="B294" s="96" t="s">
+        <v>387</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="D294" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E294" s="97" t="s">
+        <v>394</v>
+      </c>
       <c r="F294" s="2"/>
       <c r="G294" s="2"/>
       <c r="H294" s="2"/>
@@ -13022,12 +13146,24 @@
       <c r="K294" s="4"/>
       <c r="L294" s="44"/>
       <c r="M294" s="44"/>
-      <c r="N294" s="44"/>
+      <c r="N294" s="44" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="295" spans="1:14" ht="18" customHeight="1">
       <c r="A295" s="24"/>
-      <c r="C295" s="2"/>
-      <c r="D295" s="2"/>
+      <c r="B295" s="96" t="s">
+        <v>388</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="D295" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E295" s="97" t="s">
+        <v>394</v>
+      </c>
       <c r="F295" s="2"/>
       <c r="G295" s="2"/>
       <c r="H295" s="2"/>
@@ -13036,12 +13172,24 @@
       <c r="K295" s="4"/>
       <c r="L295" s="44"/>
       <c r="M295" s="44"/>
-      <c r="N295" s="44"/>
+      <c r="N295" s="44" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="296" spans="1:14" ht="18" customHeight="1">
       <c r="A296" s="24"/>
-      <c r="C296" s="2"/>
-      <c r="D296" s="2"/>
+      <c r="B296" s="96" t="s">
+        <v>389</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D296" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E296" s="97" t="s">
+        <v>394</v>
+      </c>
       <c r="F296" s="2"/>
       <c r="G296" s="2"/>
       <c r="H296" s="2"/>
@@ -13050,7 +13198,9 @@
       <c r="K296" s="4"/>
       <c r="L296" s="44"/>
       <c r="M296" s="44"/>
-      <c r="N296" s="44"/>
+      <c r="N296" s="44" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="297" spans="1:14" ht="18" customHeight="1">
       <c r="A297" s="24"/>
@@ -14846,11 +14996,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -14865,6 +15010,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.rinp.2019.102275`; updated last data too
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B09371-8B85-5545-BDBE-E391502038C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD6DC98-42FD-BA4F-A5E8-778EED7006C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="780" windowWidth="30660" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2418" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2447" uniqueCount="402">
   <si>
     <t>Metadata</t>
   </si>
@@ -1313,6 +1313,24 @@
   </si>
   <si>
     <t>10.1016/j.physc.2019.1353520</t>
+  </si>
+  <si>
+    <t>Nb20Re20Zr20Hf20Ti20</t>
+  </si>
+  <si>
+    <t>superconducting transition temperature</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2018.08.039</t>
+  </si>
+  <si>
+    <t>Hf21Nb25Ti15V15Zr24</t>
+  </si>
+  <si>
+    <t>annealed at 1073k for 4 days in vacuum</t>
+  </si>
+  <si>
+    <t>10.1016/j.rinp.2019.102275</t>
   </si>
 </sst>
 </file>
@@ -2532,8 +2550,8 @@
   </sheetPr>
   <dimension ref="A1:T424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A266" zoomScale="89" workbookViewId="0">
-      <selection activeCell="B303" sqref="B303"/>
+    <sheetView tabSelected="1" topLeftCell="A262" zoomScale="89" workbookViewId="0">
+      <selection activeCell="H307" sqref="H307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -12982,11 +13000,17 @@
       <c r="E288" s="97" t="s">
         <v>394</v>
       </c>
-      <c r="F288" s="2"/>
-      <c r="G288" s="2"/>
+      <c r="F288" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G288" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H288" s="2"/>
       <c r="I288" s="3"/>
-      <c r="J288" s="4"/>
+      <c r="J288" s="4">
+        <v>9.1</v>
+      </c>
       <c r="K288" s="4"/>
       <c r="L288" s="44"/>
       <c r="M288" s="44"/>
@@ -13008,11 +13032,17 @@
       <c r="E289" s="97" t="s">
         <v>394</v>
       </c>
-      <c r="F289" s="2"/>
-      <c r="G289" s="2"/>
+      <c r="F289" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G289" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H289" s="2"/>
       <c r="I289" s="3"/>
-      <c r="J289" s="4"/>
+      <c r="J289" s="4">
+        <v>2.5</v>
+      </c>
       <c r="K289" s="4"/>
       <c r="L289" s="44"/>
       <c r="M289" s="44"/>
@@ -13034,11 +13064,17 @@
       <c r="E290" s="97" t="s">
         <v>394</v>
       </c>
-      <c r="F290" s="2"/>
-      <c r="G290" s="2"/>
+      <c r="F290" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G290" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H290" s="2"/>
       <c r="I290" s="3"/>
-      <c r="J290" s="4"/>
+      <c r="J290" s="4">
+        <v>3.6</v>
+      </c>
       <c r="K290" s="4"/>
       <c r="L290" s="44"/>
       <c r="M290" s="44"/>
@@ -13060,11 +13096,17 @@
       <c r="E291" s="97" t="s">
         <v>394</v>
       </c>
-      <c r="F291" s="2"/>
-      <c r="G291" s="2"/>
+      <c r="F291" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G291" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H291" s="2"/>
       <c r="I291" s="3"/>
-      <c r="J291" s="4"/>
+      <c r="J291" s="4">
+        <v>4.7</v>
+      </c>
       <c r="K291" s="4"/>
       <c r="L291" s="44"/>
       <c r="M291" s="44"/>
@@ -13090,7 +13132,6 @@
       <c r="G292" s="2"/>
       <c r="H292" s="2"/>
       <c r="I292" s="3"/>
-      <c r="J292" s="4"/>
       <c r="K292" s="4"/>
       <c r="L292" s="44"/>
       <c r="M292" s="44"/>
@@ -13112,11 +13153,17 @@
       <c r="E293" s="97" t="s">
         <v>394</v>
       </c>
-      <c r="F293" s="2"/>
-      <c r="G293" s="2"/>
+      <c r="F293" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G293" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H293" s="2"/>
       <c r="I293" s="3"/>
-      <c r="J293" s="4"/>
+      <c r="J293" s="4">
+        <v>2.1</v>
+      </c>
       <c r="K293" s="4"/>
       <c r="L293" s="44"/>
       <c r="M293" s="44"/>
@@ -13138,11 +13185,17 @@
       <c r="E294" s="97" t="s">
         <v>394</v>
       </c>
-      <c r="F294" s="2"/>
-      <c r="G294" s="2"/>
+      <c r="F294" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G294" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H294" s="2"/>
       <c r="I294" s="3"/>
-      <c r="J294" s="4"/>
+      <c r="J294" s="4">
+        <v>2.2000000000000002</v>
+      </c>
       <c r="K294" s="4"/>
       <c r="L294" s="44"/>
       <c r="M294" s="44"/>
@@ -13164,11 +13217,17 @@
       <c r="E295" s="97" t="s">
         <v>394</v>
       </c>
-      <c r="F295" s="2"/>
-      <c r="G295" s="2"/>
+      <c r="F295" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G295" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H295" s="2"/>
       <c r="I295" s="3"/>
-      <c r="J295" s="4"/>
+      <c r="J295" s="4">
+        <v>2.5</v>
+      </c>
       <c r="K295" s="4"/>
       <c r="L295" s="44"/>
       <c r="M295" s="44"/>
@@ -13190,11 +13249,17 @@
       <c r="E296" s="97" t="s">
         <v>394</v>
       </c>
-      <c r="F296" s="2"/>
-      <c r="G296" s="2"/>
+      <c r="F296" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G296" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H296" s="2"/>
       <c r="I296" s="3"/>
-      <c r="J296" s="4"/>
+      <c r="J296" s="4">
+        <v>5.5</v>
+      </c>
       <c r="K296" s="4"/>
       <c r="L296" s="44"/>
       <c r="M296" s="44"/>
@@ -13204,31 +13269,64 @@
     </row>
     <row r="297" spans="1:14" ht="18" customHeight="1">
       <c r="A297" s="24"/>
-      <c r="C297" s="2"/>
-      <c r="D297" s="2"/>
-      <c r="F297" s="2"/>
-      <c r="G297" s="2"/>
+      <c r="B297" s="96" t="s">
+        <v>396</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D297" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F297" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G297" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H297" s="2"/>
       <c r="I297" s="3"/>
-      <c r="J297" s="4"/>
+      <c r="J297" s="4">
+        <v>5.3</v>
+      </c>
       <c r="K297" s="4"/>
       <c r="L297" s="44"/>
       <c r="M297" s="44"/>
-      <c r="N297" s="44"/>
+      <c r="N297" s="44" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="298" spans="1:14" ht="18" customHeight="1">
       <c r="A298" s="24"/>
-      <c r="C298" s="2"/>
-      <c r="D298" s="2"/>
-      <c r="F298" s="2"/>
-      <c r="G298" s="2"/>
+      <c r="B298" s="96" t="s">
+        <v>399</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D298" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E298" s="97" t="s">
+        <v>400</v>
+      </c>
+      <c r="F298" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G298" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H298" s="2"/>
       <c r="I298" s="3"/>
-      <c r="J298" s="4"/>
+      <c r="J298" s="4">
+        <v>5.3</v>
+      </c>
       <c r="K298" s="4"/>
       <c r="L298" s="44"/>
       <c r="M298" s="44"/>
-      <c r="N298" s="44"/>
+      <c r="N298" s="44" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="299" spans="1:14" ht="18" customHeight="1">
       <c r="A299" s="24"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.scriptamat.2020.03.004`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD6DC98-42FD-BA4F-A5E8-778EED7006C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A03E2B-CCC8-244D-8C98-5D7F5E1AA262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="780" windowWidth="30660" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2447" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2511" uniqueCount="407">
   <si>
     <t>Metadata</t>
   </si>
@@ -1331,6 +1331,21 @@
   </si>
   <si>
     <t>10.1016/j.rinp.2019.102275</t>
+  </si>
+  <si>
+    <t>Nb10 Mo35 Ru35 Rh10 Pd10</t>
+  </si>
+  <si>
+    <t>Nb15 Mo32.5 Ru32.5 Rh10 Pd10</t>
+  </si>
+  <si>
+    <t>Nb20 Mo30 Ru30 Rh10 Pd10</t>
+  </si>
+  <si>
+    <t>elemental powders pressed into pellet in argon before arc melting in argon; no significant mass loss</t>
+  </si>
+  <si>
+    <t>10.1016/j.scriptamat.2020.03.004</t>
   </si>
 </sst>
 </file>
@@ -2550,8 +2565,8 @@
   </sheetPr>
   <dimension ref="A1:T424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" zoomScale="89" workbookViewId="0">
-      <selection activeCell="H307" sqref="H307"/>
+    <sheetView tabSelected="1" topLeftCell="B278" zoomScale="89" workbookViewId="0">
+      <selection activeCell="K321" sqref="K321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -13012,7 +13027,9 @@
         <v>9.1</v>
       </c>
       <c r="K288" s="4"/>
-      <c r="L288" s="44"/>
+      <c r="L288" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="M288" s="44"/>
       <c r="N288" s="44" t="s">
         <v>395</v>
@@ -13044,7 +13061,9 @@
         <v>2.5</v>
       </c>
       <c r="K289" s="4"/>
-      <c r="L289" s="44"/>
+      <c r="L289" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="M289" s="44"/>
       <c r="N289" s="44" t="s">
         <v>395</v>
@@ -13076,7 +13095,9 @@
         <v>3.6</v>
       </c>
       <c r="K290" s="4"/>
-      <c r="L290" s="44"/>
+      <c r="L290" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="M290" s="44"/>
       <c r="N290" s="44" t="s">
         <v>395</v>
@@ -13108,7 +13129,9 @@
         <v>4.7</v>
       </c>
       <c r="K291" s="4"/>
-      <c r="L291" s="44"/>
+      <c r="L291" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="M291" s="44"/>
       <c r="N291" s="44" t="s">
         <v>395</v>
@@ -13165,7 +13188,9 @@
         <v>2.1</v>
       </c>
       <c r="K293" s="4"/>
-      <c r="L293" s="44"/>
+      <c r="L293" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="M293" s="44"/>
       <c r="N293" s="44" t="s">
         <v>395</v>
@@ -13197,7 +13222,9 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="K294" s="4"/>
-      <c r="L294" s="44"/>
+      <c r="L294" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="M294" s="44"/>
       <c r="N294" s="44" t="s">
         <v>395</v>
@@ -13229,7 +13256,9 @@
         <v>2.5</v>
       </c>
       <c r="K295" s="4"/>
-      <c r="L295" s="44"/>
+      <c r="L295" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="M295" s="44"/>
       <c r="N295" s="44" t="s">
         <v>395</v>
@@ -13261,7 +13290,9 @@
         <v>5.5</v>
       </c>
       <c r="K296" s="4"/>
-      <c r="L296" s="44"/>
+      <c r="L296" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="M296" s="44"/>
       <c r="N296" s="44" t="s">
         <v>395</v>
@@ -13290,7 +13321,9 @@
         <v>5.3</v>
       </c>
       <c r="K297" s="4"/>
-      <c r="L297" s="44"/>
+      <c r="L297" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="M297" s="44"/>
       <c r="N297" s="44" t="s">
         <v>398</v>
@@ -13322,7 +13355,9 @@
         <v>5.3</v>
       </c>
       <c r="K298" s="4"/>
-      <c r="L298" s="44"/>
+      <c r="L298" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="M298" s="44"/>
       <c r="N298" s="44" t="s">
         <v>401</v>
@@ -13330,87 +13365,225 @@
     </row>
     <row r="299" spans="1:14" ht="18" customHeight="1">
       <c r="A299" s="24"/>
-      <c r="C299" s="2"/>
-      <c r="D299" s="2"/>
-      <c r="F299" s="2"/>
-      <c r="G299" s="2"/>
+      <c r="B299" s="96" t="s">
+        <v>402</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D299" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E299" s="97" t="s">
+        <v>405</v>
+      </c>
+      <c r="F299" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G299" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H299" s="2"/>
       <c r="I299" s="3"/>
-      <c r="J299" s="4"/>
+      <c r="J299" s="4">
+        <v>5.58</v>
+      </c>
       <c r="K299" s="4"/>
-      <c r="L299" s="44"/>
-      <c r="M299" s="44"/>
-      <c r="N299" s="44"/>
+      <c r="L299" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M299" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="N299" s="44" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="300" spans="1:14" ht="18" customHeight="1">
       <c r="A300" s="44"/>
-      <c r="C300" s="2"/>
-      <c r="D300" s="2"/>
-      <c r="F300" s="2"/>
-      <c r="G300" s="2"/>
+      <c r="B300" s="96" t="s">
+        <v>403</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D300" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E300" s="97" t="s">
+        <v>405</v>
+      </c>
+      <c r="F300" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G300" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H300" s="2"/>
       <c r="I300" s="3"/>
-      <c r="J300" s="4"/>
+      <c r="J300" s="4">
+        <v>6.19</v>
+      </c>
       <c r="K300" s="4"/>
-      <c r="L300" s="44"/>
-      <c r="M300" s="44"/>
-      <c r="N300" s="44"/>
+      <c r="L300" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M300" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="N300" s="44" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="301" spans="1:14" ht="18" customHeight="1">
       <c r="A301" s="44"/>
-      <c r="C301" s="2"/>
-      <c r="D301" s="2"/>
-      <c r="F301" s="2"/>
-      <c r="G301" s="2"/>
+      <c r="B301" s="96" t="s">
+        <v>404</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D301" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E301" s="97" t="s">
+        <v>405</v>
+      </c>
+      <c r="F301" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G301" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H301" s="2"/>
       <c r="I301" s="3"/>
-      <c r="J301" s="4"/>
+      <c r="J301" s="4">
+        <v>6.1</v>
+      </c>
       <c r="K301" s="4"/>
-      <c r="L301" s="44"/>
-      <c r="M301" s="44"/>
-      <c r="N301" s="44"/>
+      <c r="L301" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M301" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="N301" s="44" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="302" spans="1:14" ht="18" customHeight="1">
       <c r="A302" s="44"/>
-      <c r="C302" s="2"/>
-      <c r="D302" s="2"/>
-      <c r="F302" s="2"/>
-      <c r="G302" s="2"/>
+      <c r="B302" s="96" t="s">
+        <v>402</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D302" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E302" s="97" t="s">
+        <v>405</v>
+      </c>
+      <c r="F302" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G302" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H302" s="2"/>
-      <c r="I302" s="3"/>
-      <c r="J302" s="4"/>
+      <c r="I302" s="3">
+        <v>298</v>
+      </c>
+      <c r="J302" s="4">
+        <v>1.5700000000000002E-8</v>
+      </c>
       <c r="K302" s="4"/>
-      <c r="L302" s="44"/>
-      <c r="M302" s="44"/>
-      <c r="N302" s="44"/>
+      <c r="L302" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M302" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="N302" s="44" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="303" spans="1:14" ht="18" customHeight="1">
       <c r="A303" s="44"/>
-      <c r="C303" s="2"/>
-      <c r="D303" s="2"/>
-      <c r="F303" s="2"/>
-      <c r="G303" s="2"/>
+      <c r="B303" s="96" t="s">
+        <v>403</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D303" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E303" s="97" t="s">
+        <v>405</v>
+      </c>
+      <c r="F303" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G303" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H303" s="2"/>
-      <c r="I303" s="3"/>
-      <c r="J303" s="4"/>
+      <c r="I303" s="3">
+        <v>298</v>
+      </c>
+      <c r="J303" s="4">
+        <v>1.27E-8</v>
+      </c>
       <c r="K303" s="4"/>
-      <c r="L303" s="44"/>
-      <c r="M303" s="44"/>
-      <c r="N303" s="44"/>
+      <c r="L303" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M303" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="N303" s="44" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="304" spans="1:14" ht="18" customHeight="1">
       <c r="A304" s="44"/>
-      <c r="C304" s="2"/>
-      <c r="D304" s="2"/>
-      <c r="F304" s="2"/>
-      <c r="G304" s="2"/>
+      <c r="B304" s="96" t="s">
+        <v>404</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D304" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E304" s="97" t="s">
+        <v>405</v>
+      </c>
+      <c r="F304" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G304" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H304" s="2"/>
-      <c r="I304" s="3"/>
-      <c r="J304" s="4"/>
+      <c r="I304" s="3">
+        <v>298</v>
+      </c>
+      <c r="J304" s="4">
+        <v>8.8599999999999999E-8</v>
+      </c>
       <c r="K304" s="4"/>
-      <c r="L304" s="44"/>
-      <c r="M304" s="44"/>
-      <c r="N304" s="44"/>
+      <c r="L304" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M304" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="N304" s="44" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="305" spans="1:14" ht="18" customHeight="1">
       <c r="A305" s="44"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.matchar.2024.113730`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A03E2B-CCC8-244D-8C98-5D7F5E1AA262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9BE7A5-0564-6941-8EB5-02507F04552D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="780" windowWidth="30660" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3640" yWindow="920" windowWidth="30660" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2511" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2786" uniqueCount="421">
   <si>
     <t>Metadata</t>
   </si>
@@ -1346,6 +1346,48 @@
   </si>
   <si>
     <t>10.1016/j.scriptamat.2020.03.004</t>
+  </si>
+  <si>
+    <t>Al5 Sc25 Ti35 Zr35</t>
+  </si>
+  <si>
+    <t>Al10 Sc20 Ti35 Zr35</t>
+  </si>
+  <si>
+    <t>Al15 Sc15 Ti35 Zr35</t>
+  </si>
+  <si>
+    <t>AAM+A+WQ+A</t>
+  </si>
+  <si>
+    <t>annealed in vacuum at 1173K for 60min in quartz then water quenched and annealed again 773K for 30min and cooled down</t>
+  </si>
+  <si>
+    <t>HCP+BCC</t>
+  </si>
+  <si>
+    <t>BCC+HCP</t>
+  </si>
+  <si>
+    <t>annealed in vacuum at 1273K for 60min in quartz then water quenched and annealed again 773K for 30min and cooled down</t>
+  </si>
+  <si>
+    <t>Al5</t>
+  </si>
+  <si>
+    <t>Al10</t>
+  </si>
+  <si>
+    <t>Al15</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>10.1016/j.matchar.2024.113730</t>
   </si>
 </sst>
 </file>
@@ -2565,8 +2607,8 @@
   </sheetPr>
   <dimension ref="A1:T424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B278" zoomScale="89" workbookViewId="0">
-      <selection activeCell="K321" sqref="K321"/>
+    <sheetView tabSelected="1" topLeftCell="A299" zoomScale="89" workbookViewId="0">
+      <selection activeCell="N337" sqref="N337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -13586,410 +13628,1153 @@
       </c>
     </row>
     <row r="305" spans="1:14" ht="18" customHeight="1">
-      <c r="A305" s="44"/>
-      <c r="C305" s="2"/>
-      <c r="D305" s="2"/>
-      <c r="F305" s="2"/>
-      <c r="G305" s="2"/>
+      <c r="A305" s="44" t="s">
+        <v>415</v>
+      </c>
+      <c r="B305" s="96" t="s">
+        <v>407</v>
+      </c>
+      <c r="C305" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D305" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F305" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G305" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H305" s="2"/>
-      <c r="I305" s="3"/>
-      <c r="J305" s="4"/>
-      <c r="K305" s="4"/>
-      <c r="L305" s="44"/>
-      <c r="M305" s="44"/>
-      <c r="N305" s="44"/>
+      <c r="I305" s="3">
+        <v>298</v>
+      </c>
+      <c r="J305" s="4">
+        <v>1615000000</v>
+      </c>
+      <c r="K305" s="4">
+        <v>21000000</v>
+      </c>
+      <c r="L305" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M305" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N305" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="306" spans="1:14" ht="18" customHeight="1">
-      <c r="A306" s="44"/>
-      <c r="C306" s="2"/>
-      <c r="D306" s="2"/>
-      <c r="F306" s="2"/>
-      <c r="G306" s="2"/>
+      <c r="A306" s="44" t="s">
+        <v>416</v>
+      </c>
+      <c r="B306" s="96" t="s">
+        <v>408</v>
+      </c>
+      <c r="C306" s="48" t="s">
+        <v>412</v>
+      </c>
+      <c r="D306" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F306" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G306" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H306" s="2"/>
-      <c r="I306" s="3"/>
-      <c r="J306" s="4"/>
-      <c r="K306" s="4"/>
-      <c r="L306" s="44"/>
-      <c r="M306" s="44"/>
-      <c r="N306" s="44"/>
+      <c r="I306" s="3">
+        <v>298</v>
+      </c>
+      <c r="J306" s="4">
+        <v>1268000000</v>
+      </c>
+      <c r="K306" s="4">
+        <v>3000000</v>
+      </c>
+      <c r="L306" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M306" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N306" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="307" spans="1:14" ht="18" customHeight="1">
-      <c r="A307" s="44"/>
-      <c r="C307" s="2"/>
-      <c r="D307" s="2"/>
-      <c r="F307" s="2"/>
-      <c r="G307" s="2"/>
+      <c r="A307" s="44" t="s">
+        <v>417</v>
+      </c>
+      <c r="B307" s="96" t="s">
+        <v>409</v>
+      </c>
+      <c r="C307" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D307" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F307" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G307" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H307" s="2"/>
-      <c r="I307" s="3"/>
-      <c r="J307" s="4"/>
-      <c r="K307" s="4"/>
-      <c r="L307" s="44"/>
-      <c r="M307" s="44"/>
-      <c r="N307" s="44"/>
+      <c r="I307" s="3">
+        <v>298</v>
+      </c>
+      <c r="J307" s="4">
+        <v>2007000000</v>
+      </c>
+      <c r="K307" s="4">
+        <v>59000000</v>
+      </c>
+      <c r="L307" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M307" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N307" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="308" spans="1:14" ht="18" customHeight="1">
-      <c r="A308" s="44"/>
-      <c r="C308" s="2"/>
-      <c r="D308" s="2"/>
-      <c r="F308" s="2"/>
-      <c r="G308" s="2"/>
+      <c r="A308" s="44" t="s">
+        <v>415</v>
+      </c>
+      <c r="B308" s="96" t="s">
+        <v>407</v>
+      </c>
+      <c r="C308" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="D308" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E308" s="97" t="s">
+        <v>411</v>
+      </c>
+      <c r="F308" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G308" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H308" s="2"/>
-      <c r="I308" s="3"/>
-      <c r="J308" s="4"/>
-      <c r="K308" s="4"/>
-      <c r="L308" s="44"/>
-      <c r="M308" s="44"/>
-      <c r="N308" s="44"/>
+      <c r="I308" s="3">
+        <v>298</v>
+      </c>
+      <c r="J308" s="4">
+        <v>1351000000</v>
+      </c>
+      <c r="K308" s="4">
+        <v>24000000</v>
+      </c>
+      <c r="L308" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M308" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N308" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="309" spans="1:14" ht="18" customHeight="1">
-      <c r="A309" s="44"/>
-      <c r="C309" s="2"/>
-      <c r="D309" s="2"/>
-      <c r="F309" s="2"/>
-      <c r="G309" s="2"/>
+      <c r="A309" s="44" t="s">
+        <v>416</v>
+      </c>
+      <c r="B309" s="96" t="s">
+        <v>408</v>
+      </c>
+      <c r="C309" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D309" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E309" s="97" t="s">
+        <v>411</v>
+      </c>
+      <c r="F309" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G309" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H309" s="2"/>
-      <c r="I309" s="3"/>
-      <c r="J309" s="4"/>
-      <c r="K309" s="4"/>
-      <c r="L309" s="44"/>
-      <c r="M309" s="44"/>
-      <c r="N309" s="44"/>
+      <c r="I309" s="3">
+        <v>298</v>
+      </c>
+      <c r="J309" s="4">
+        <v>1517000000</v>
+      </c>
+      <c r="K309" s="4">
+        <v>30000000</v>
+      </c>
+      <c r="L309" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M309" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N309" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="310" spans="1:14" ht="18" customHeight="1">
-      <c r="A310" s="44"/>
-      <c r="C310" s="2"/>
-      <c r="D310" s="2"/>
-      <c r="F310" s="2"/>
-      <c r="G310" s="2"/>
+      <c r="A310" s="44" t="s">
+        <v>415</v>
+      </c>
+      <c r="B310" s="96" t="s">
+        <v>407</v>
+      </c>
+      <c r="C310" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D310" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F310" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G310" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H310" s="2"/>
-      <c r="I310" s="3"/>
-      <c r="J310" s="4"/>
-      <c r="K310" s="4"/>
-      <c r="L310" s="44"/>
-      <c r="M310" s="44"/>
-      <c r="N310" s="44"/>
+      <c r="I310" s="3">
+        <v>298</v>
+      </c>
+      <c r="J310" s="4">
+        <v>1861000000</v>
+      </c>
+      <c r="K310" s="4">
+        <v>46000000</v>
+      </c>
+      <c r="L310" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M310" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N310" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="311" spans="1:14" ht="18" customHeight="1">
-      <c r="A311" s="44"/>
-      <c r="C311" s="2"/>
-      <c r="D311" s="2"/>
-      <c r="F311" s="2"/>
-      <c r="G311" s="2"/>
+      <c r="A311" s="44" t="s">
+        <v>416</v>
+      </c>
+      <c r="B311" s="96" t="s">
+        <v>408</v>
+      </c>
+      <c r="C311" s="48" t="s">
+        <v>412</v>
+      </c>
+      <c r="D311" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F311" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G311" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H311" s="2"/>
-      <c r="I311" s="3"/>
-      <c r="J311" s="4"/>
-      <c r="K311" s="4"/>
-      <c r="L311" s="44"/>
-      <c r="M311" s="44"/>
-      <c r="N311" s="44"/>
+      <c r="I311" s="3">
+        <v>298</v>
+      </c>
+      <c r="J311" s="4">
+        <v>2040000000</v>
+      </c>
+      <c r="K311" s="4">
+        <v>25000000</v>
+      </c>
+      <c r="L311" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M311" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N311" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="312" spans="1:14" ht="18" customHeight="1">
-      <c r="A312" s="44"/>
-      <c r="C312" s="2"/>
-      <c r="D312" s="2"/>
-      <c r="F312" s="2"/>
-      <c r="G312" s="2"/>
+      <c r="A312" s="44" t="s">
+        <v>417</v>
+      </c>
+      <c r="B312" s="96" t="s">
+        <v>409</v>
+      </c>
+      <c r="C312" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D312" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F312" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G312" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H312" s="2"/>
-      <c r="I312" s="3"/>
-      <c r="J312" s="4"/>
-      <c r="K312" s="4"/>
-      <c r="L312" s="44"/>
-      <c r="M312" s="44"/>
-      <c r="N312" s="44"/>
+      <c r="I312" s="3">
+        <v>298</v>
+      </c>
+      <c r="J312" s="4">
+        <v>1798000000</v>
+      </c>
+      <c r="K312" s="4">
+        <v>146000000</v>
+      </c>
+      <c r="L312" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M312" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N312" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="313" spans="1:14" ht="18" customHeight="1">
-      <c r="A313" s="44"/>
-      <c r="C313" s="2"/>
-      <c r="D313" s="2"/>
-      <c r="F313" s="2"/>
-      <c r="G313" s="2"/>
+      <c r="A313" s="44" t="s">
+        <v>415</v>
+      </c>
+      <c r="B313" s="96" t="s">
+        <v>407</v>
+      </c>
+      <c r="C313" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="D313" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E313" s="97" t="s">
+        <v>411</v>
+      </c>
+      <c r="F313" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G313" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H313" s="2"/>
-      <c r="I313" s="3"/>
-      <c r="J313" s="4"/>
-      <c r="K313" s="4"/>
-      <c r="L313" s="44"/>
-      <c r="M313" s="44"/>
-      <c r="N313" s="44"/>
+      <c r="I313" s="3">
+        <v>298</v>
+      </c>
+      <c r="J313" s="4">
+        <v>1953000000</v>
+      </c>
+      <c r="K313" s="4">
+        <v>39000000</v>
+      </c>
+      <c r="L313" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M313" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N313" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="314" spans="1:14" ht="18" customHeight="1">
-      <c r="A314" s="44"/>
-      <c r="C314" s="2"/>
-      <c r="D314" s="2"/>
-      <c r="F314" s="2"/>
-      <c r="G314" s="2"/>
+      <c r="A314" s="44" t="s">
+        <v>416</v>
+      </c>
+      <c r="B314" s="96" t="s">
+        <v>408</v>
+      </c>
+      <c r="C314" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D314" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E314" s="97" t="s">
+        <v>411</v>
+      </c>
+      <c r="F314" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G314" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H314" s="2"/>
-      <c r="I314" s="3"/>
-      <c r="J314" s="4"/>
-      <c r="K314" s="4"/>
-      <c r="L314" s="44"/>
-      <c r="M314" s="44"/>
-      <c r="N314" s="44"/>
+      <c r="I314" s="3">
+        <v>298</v>
+      </c>
+      <c r="J314" s="4">
+        <v>2584000000</v>
+      </c>
+      <c r="K314" s="4">
+        <v>44000000</v>
+      </c>
+      <c r="L314" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M314" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N314" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="315" spans="1:14" ht="18" customHeight="1">
-      <c r="A315" s="44"/>
-      <c r="C315" s="2"/>
-      <c r="D315" s="2"/>
-      <c r="F315" s="2"/>
-      <c r="G315" s="2"/>
+      <c r="A315" s="44" t="s">
+        <v>417</v>
+      </c>
+      <c r="B315" s="96" t="s">
+        <v>409</v>
+      </c>
+      <c r="C315" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D315" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E315" s="97" t="s">
+        <v>414</v>
+      </c>
+      <c r="F315" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G315" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H315" s="2"/>
-      <c r="I315" s="3"/>
-      <c r="J315" s="4"/>
-      <c r="K315" s="4"/>
-      <c r="L315" s="44"/>
-      <c r="M315" s="44"/>
-      <c r="N315" s="44"/>
+      <c r="I315" s="3">
+        <v>298</v>
+      </c>
+      <c r="J315" s="4">
+        <v>1750000000</v>
+      </c>
+      <c r="K315" s="4">
+        <v>58000000</v>
+      </c>
+      <c r="L315" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M315" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N315" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="316" spans="1:14" ht="18" customHeight="1">
-      <c r="A316" s="44"/>
-      <c r="C316" s="2"/>
-      <c r="D316" s="2"/>
-      <c r="F316" s="2"/>
-      <c r="G316" s="2"/>
+      <c r="A316" s="44" t="s">
+        <v>415</v>
+      </c>
+      <c r="B316" s="96" t="s">
+        <v>407</v>
+      </c>
+      <c r="C316" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D316" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F316" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G316" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H316" s="2"/>
-      <c r="I316" s="3"/>
-      <c r="J316" s="4"/>
-      <c r="K316" s="4"/>
-      <c r="L316" s="44"/>
-      <c r="M316" s="44"/>
-      <c r="N316" s="44"/>
+      <c r="I316" s="3">
+        <v>298</v>
+      </c>
+      <c r="J316" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="K316" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="L316" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M316" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N316" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="317" spans="1:14" ht="18" customHeight="1">
-      <c r="A317" s="44"/>
-      <c r="C317" s="2"/>
-      <c r="D317" s="2"/>
-      <c r="F317" s="2"/>
-      <c r="G317" s="2"/>
+      <c r="A317" s="44" t="s">
+        <v>416</v>
+      </c>
+      <c r="B317" s="96" t="s">
+        <v>408</v>
+      </c>
+      <c r="C317" s="48" t="s">
+        <v>412</v>
+      </c>
+      <c r="D317" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F317" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G317" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H317" s="2"/>
-      <c r="I317" s="3"/>
-      <c r="J317" s="4"/>
-      <c r="K317" s="4"/>
-      <c r="L317" s="44"/>
-      <c r="M317" s="44"/>
-      <c r="N317" s="44"/>
+      <c r="I317" s="3">
+        <v>298</v>
+      </c>
+      <c r="J317" s="4">
+        <v>14.9</v>
+      </c>
+      <c r="K317" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="L317" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M317" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N317" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="318" spans="1:14" ht="18" customHeight="1">
-      <c r="A318" s="44"/>
-      <c r="C318" s="2"/>
-      <c r="D318" s="2"/>
-      <c r="F318" s="2"/>
-      <c r="G318" s="2"/>
+      <c r="A318" s="44" t="s">
+        <v>417</v>
+      </c>
+      <c r="B318" s="96" t="s">
+        <v>409</v>
+      </c>
+      <c r="C318" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D318" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F318" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G318" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H318" s="2"/>
-      <c r="I318" s="3"/>
-      <c r="J318" s="4"/>
-      <c r="K318" s="4"/>
-      <c r="L318" s="44"/>
-      <c r="M318" s="44"/>
-      <c r="N318" s="44"/>
+      <c r="I318" s="3">
+        <v>298</v>
+      </c>
+      <c r="J318" s="4">
+        <v>17</v>
+      </c>
+      <c r="K318" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="L318" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M318" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N318" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="319" spans="1:14" ht="18" customHeight="1">
-      <c r="A319" s="44"/>
-      <c r="C319" s="2"/>
-      <c r="D319" s="2"/>
-      <c r="F319" s="2"/>
-      <c r="G319" s="2"/>
+      <c r="A319" s="44" t="s">
+        <v>415</v>
+      </c>
+      <c r="B319" s="96" t="s">
+        <v>407</v>
+      </c>
+      <c r="C319" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="D319" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E319" s="97" t="s">
+        <v>411</v>
+      </c>
+      <c r="F319" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G319" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H319" s="2"/>
-      <c r="I319" s="3"/>
-      <c r="J319" s="4"/>
-      <c r="K319" s="4"/>
-      <c r="L319" s="44"/>
-      <c r="M319" s="44"/>
-      <c r="N319" s="44"/>
+      <c r="I319" s="3">
+        <v>298</v>
+      </c>
+      <c r="J319" s="4">
+        <v>7.8</v>
+      </c>
+      <c r="K319" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="L319" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M319" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N319" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="320" spans="1:14" ht="18" customHeight="1">
-      <c r="A320" s="44"/>
-      <c r="C320" s="2"/>
-      <c r="D320" s="2"/>
-      <c r="F320" s="2"/>
-      <c r="G320" s="2"/>
+      <c r="A320" s="44" t="s">
+        <v>416</v>
+      </c>
+      <c r="B320" s="96" t="s">
+        <v>408</v>
+      </c>
+      <c r="C320" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D320" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E320" s="97" t="s">
+        <v>411</v>
+      </c>
+      <c r="F320" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G320" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H320" s="2"/>
-      <c r="I320" s="3"/>
-      <c r="J320" s="4"/>
-      <c r="K320" s="4"/>
-      <c r="L320" s="44"/>
-      <c r="M320" s="44"/>
-      <c r="N320" s="44"/>
+      <c r="I320" s="3">
+        <v>298</v>
+      </c>
+      <c r="J320" s="4">
+        <v>31.9</v>
+      </c>
+      <c r="K320" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="L320" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M320" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N320" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="321" spans="1:14" ht="18" customHeight="1">
-      <c r="A321" s="44"/>
-      <c r="C321" s="2"/>
-      <c r="D321" s="2"/>
-      <c r="F321" s="2"/>
-      <c r="G321" s="2"/>
+      <c r="A321" s="44" t="s">
+        <v>417</v>
+      </c>
+      <c r="B321" s="96" t="s">
+        <v>409</v>
+      </c>
+      <c r="C321" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D321" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E321" s="97" t="s">
+        <v>414</v>
+      </c>
+      <c r="F321" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G321" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H321" s="2"/>
-      <c r="I321" s="3"/>
-      <c r="J321" s="4"/>
-      <c r="K321" s="4"/>
-      <c r="L321" s="44"/>
-      <c r="M321" s="44"/>
-      <c r="N321" s="44"/>
+      <c r="I321" s="3">
+        <v>298</v>
+      </c>
+      <c r="J321" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="K321" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="L321" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M321" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="N321" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="322" spans="1:14" ht="18" customHeight="1">
-      <c r="A322" s="44"/>
-      <c r="C322" s="2"/>
-      <c r="D322" s="2"/>
-      <c r="F322" s="2"/>
-      <c r="G322" s="2"/>
+      <c r="A322" s="44" t="s">
+        <v>415</v>
+      </c>
+      <c r="B322" s="96" t="s">
+        <v>407</v>
+      </c>
+      <c r="C322" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D322" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F322" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G322" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H322" s="2"/>
-      <c r="I322" s="3"/>
-      <c r="J322" s="4"/>
+      <c r="I322" s="3">
+        <v>298</v>
+      </c>
+      <c r="J322" s="4">
+        <v>4950</v>
+      </c>
       <c r="K322" s="4"/>
-      <c r="L322" s="44"/>
-      <c r="M322" s="44"/>
-      <c r="N322" s="44"/>
+      <c r="L322" s="44" t="s">
+        <v>418</v>
+      </c>
+      <c r="M322" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N322" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="323" spans="1:14" ht="18" customHeight="1">
-      <c r="A323" s="44"/>
-      <c r="C323" s="2"/>
-      <c r="D323" s="2"/>
-      <c r="F323" s="2"/>
-      <c r="G323" s="2"/>
+      <c r="A323" s="44" t="s">
+        <v>416</v>
+      </c>
+      <c r="B323" s="96" t="s">
+        <v>408</v>
+      </c>
+      <c r="C323" s="48" t="s">
+        <v>412</v>
+      </c>
+      <c r="D323" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F323" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G323" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H323" s="2"/>
-      <c r="I323" s="3"/>
-      <c r="J323" s="4"/>
+      <c r="I323" s="3">
+        <v>298</v>
+      </c>
+      <c r="J323" s="4">
+        <v>4954</v>
+      </c>
       <c r="K323" s="4"/>
-      <c r="L323" s="44"/>
-      <c r="M323" s="44"/>
-      <c r="N323" s="44"/>
+      <c r="L323" s="44" t="s">
+        <v>418</v>
+      </c>
+      <c r="M323" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N323" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="324" spans="1:14" ht="18" customHeight="1">
-      <c r="A324" s="44"/>
-      <c r="C324" s="2"/>
-      <c r="D324" s="2"/>
-      <c r="F324" s="2"/>
-      <c r="G324" s="2"/>
+      <c r="A324" s="44" t="s">
+        <v>417</v>
+      </c>
+      <c r="B324" s="96" t="s">
+        <v>409</v>
+      </c>
+      <c r="C324" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D324" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F324" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G324" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H324" s="2"/>
-      <c r="I324" s="3"/>
-      <c r="J324" s="4"/>
+      <c r="I324" s="3">
+        <v>298</v>
+      </c>
+      <c r="J324" s="4">
+        <v>4957</v>
+      </c>
       <c r="K324" s="4"/>
-      <c r="L324" s="44"/>
-      <c r="M324" s="44"/>
-      <c r="N324" s="44"/>
+      <c r="L324" s="44" t="s">
+        <v>418</v>
+      </c>
+      <c r="M324" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="N324" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="325" spans="1:14" ht="18" customHeight="1">
-      <c r="A325" s="44"/>
-      <c r="C325" s="2"/>
-      <c r="D325" s="2"/>
-      <c r="F325" s="2"/>
-      <c r="G325" s="2"/>
+      <c r="A325" s="44" t="s">
+        <v>417</v>
+      </c>
+      <c r="B325" s="96" t="s">
+        <v>409</v>
+      </c>
+      <c r="C325" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D325" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F325" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G325" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H325" s="2"/>
-      <c r="I325" s="3"/>
-      <c r="J325" s="4"/>
+      <c r="I325" s="3">
+        <v>873</v>
+      </c>
+      <c r="J325" s="4">
+        <v>804000000</v>
+      </c>
       <c r="K325" s="4"/>
-      <c r="L325" s="44"/>
-      <c r="M325" s="44"/>
-      <c r="N325" s="44"/>
+      <c r="L325" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M325" s="44" t="s">
+        <v>419</v>
+      </c>
+      <c r="N325" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="326" spans="1:14" ht="18" customHeight="1">
-      <c r="A326" s="44"/>
-      <c r="C326" s="2"/>
-      <c r="D326" s="2"/>
-      <c r="F326" s="2"/>
-      <c r="G326" s="2"/>
+      <c r="A326" s="44" t="s">
+        <v>415</v>
+      </c>
+      <c r="B326" s="96" t="s">
+        <v>407</v>
+      </c>
+      <c r="C326" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="D326" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E326" s="97" t="s">
+        <v>411</v>
+      </c>
+      <c r="F326" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G326" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H326" s="2"/>
-      <c r="I326" s="3"/>
-      <c r="J326" s="4"/>
+      <c r="I326" s="3">
+        <v>873</v>
+      </c>
+      <c r="J326" s="4">
+        <v>692000000</v>
+      </c>
       <c r="K326" s="4"/>
-      <c r="L326" s="44"/>
-      <c r="M326" s="44"/>
-      <c r="N326" s="44"/>
+      <c r="L326" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M326" s="44" t="s">
+        <v>419</v>
+      </c>
+      <c r="N326" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="327" spans="1:14" ht="18" customHeight="1">
-      <c r="A327" s="44"/>
-      <c r="C327" s="2"/>
-      <c r="D327" s="2"/>
-      <c r="F327" s="2"/>
-      <c r="G327" s="2"/>
+      <c r="A327" s="44" t="s">
+        <v>416</v>
+      </c>
+      <c r="B327" s="96" t="s">
+        <v>408</v>
+      </c>
+      <c r="C327" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D327" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E327" s="97" t="s">
+        <v>411</v>
+      </c>
+      <c r="F327" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G327" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H327" s="2"/>
-      <c r="I327" s="3"/>
-      <c r="J327" s="4"/>
+      <c r="I327" s="3">
+        <v>873</v>
+      </c>
+      <c r="J327" s="4">
+        <v>605000000</v>
+      </c>
       <c r="K327" s="4"/>
-      <c r="L327" s="44"/>
-      <c r="M327" s="44"/>
-      <c r="N327" s="44"/>
+      <c r="L327" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M327" s="44" t="s">
+        <v>419</v>
+      </c>
+      <c r="N327" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="328" spans="1:14" ht="18" customHeight="1">
-      <c r="A328" s="44"/>
-      <c r="C328" s="2"/>
-      <c r="D328" s="2"/>
-      <c r="F328" s="2"/>
-      <c r="G328" s="2"/>
+      <c r="A328" s="44" t="s">
+        <v>417</v>
+      </c>
+      <c r="B328" s="96" t="s">
+        <v>409</v>
+      </c>
+      <c r="C328" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D328" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F328" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G328" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H328" s="2"/>
-      <c r="I328" s="3"/>
-      <c r="J328" s="4"/>
+      <c r="I328" s="3">
+        <v>873</v>
+      </c>
+      <c r="J328" s="4">
+        <v>689000000</v>
+      </c>
       <c r="K328" s="4"/>
-      <c r="L328" s="44"/>
-      <c r="M328" s="44"/>
-      <c r="N328" s="44"/>
+      <c r="L328" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M328" s="44" t="s">
+        <v>419</v>
+      </c>
+      <c r="N328" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="329" spans="1:14" ht="18" customHeight="1">
-      <c r="A329" s="44"/>
-      <c r="C329" s="2"/>
-      <c r="D329" s="2"/>
-      <c r="F329" s="2"/>
-      <c r="G329" s="2"/>
+      <c r="A329" s="44" t="s">
+        <v>415</v>
+      </c>
+      <c r="B329" s="96" t="s">
+        <v>407</v>
+      </c>
+      <c r="C329" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="D329" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E329" s="97" t="s">
+        <v>411</v>
+      </c>
+      <c r="F329" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G329" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H329" s="2"/>
-      <c r="I329" s="3"/>
-      <c r="J329" s="4"/>
+      <c r="I329" s="3">
+        <v>873</v>
+      </c>
+      <c r="J329" s="4">
+        <v>576000000</v>
+      </c>
       <c r="K329" s="4"/>
-      <c r="L329" s="44"/>
-      <c r="M329" s="44"/>
-      <c r="N329" s="44"/>
+      <c r="L329" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M329" s="44" t="s">
+        <v>419</v>
+      </c>
+      <c r="N329" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="330" spans="1:14" ht="18" customHeight="1">
-      <c r="A330" s="44"/>
-      <c r="C330" s="2"/>
-      <c r="D330" s="2"/>
-      <c r="F330" s="2"/>
-      <c r="G330" s="2"/>
+      <c r="A330" s="44" t="s">
+        <v>416</v>
+      </c>
+      <c r="B330" s="96" t="s">
+        <v>408</v>
+      </c>
+      <c r="C330" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D330" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E330" s="97" t="s">
+        <v>411</v>
+      </c>
+      <c r="F330" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G330" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H330" s="2"/>
-      <c r="I330" s="3"/>
-      <c r="J330" s="4"/>
+      <c r="I330" s="3">
+        <v>873</v>
+      </c>
+      <c r="J330" s="4">
+        <v>442000000</v>
+      </c>
       <c r="K330" s="4"/>
-      <c r="L330" s="44"/>
-      <c r="M330" s="44"/>
-      <c r="N330" s="44"/>
+      <c r="L330" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M330" s="44" t="s">
+        <v>419</v>
+      </c>
+      <c r="N330" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="331" spans="1:14" ht="18" customHeight="1">
-      <c r="A331" s="44"/>
-      <c r="C331" s="2"/>
-      <c r="D331" s="2"/>
-      <c r="F331" s="2"/>
-      <c r="G331" s="2"/>
+      <c r="A331" s="44" t="s">
+        <v>417</v>
+      </c>
+      <c r="B331" s="96" t="s">
+        <v>409</v>
+      </c>
+      <c r="C331" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D331" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F331" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="G331" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H331" s="2"/>
-      <c r="I331" s="3"/>
-      <c r="J331" s="4"/>
+      <c r="I331" s="3">
+        <v>873</v>
+      </c>
+      <c r="J331" s="4">
+        <v>50</v>
+      </c>
       <c r="K331" s="4"/>
-      <c r="L331" s="44"/>
-      <c r="M331" s="44"/>
-      <c r="N331" s="44"/>
+      <c r="L331" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M331" s="44" t="s">
+        <v>419</v>
+      </c>
+      <c r="N331" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="332" spans="1:14" ht="18" customHeight="1">
-      <c r="A332" s="44"/>
-      <c r="C332" s="2"/>
-      <c r="D332" s="2"/>
-      <c r="F332" s="2"/>
-      <c r="G332" s="2"/>
+      <c r="A332" s="44" t="s">
+        <v>415</v>
+      </c>
+      <c r="B332" s="96" t="s">
+        <v>407</v>
+      </c>
+      <c r="C332" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="D332" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E332" s="97" t="s">
+        <v>411</v>
+      </c>
+      <c r="F332" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G332" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H332" s="2"/>
-      <c r="I332" s="3"/>
-      <c r="J332" s="4"/>
+      <c r="I332" s="3">
+        <v>873</v>
+      </c>
+      <c r="J332" s="4">
+        <v>45</v>
+      </c>
       <c r="K332" s="4"/>
-      <c r="L332" s="44"/>
-      <c r="M332" s="44"/>
-      <c r="N332" s="44"/>
+      <c r="L332" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M332" s="44" t="s">
+        <v>419</v>
+      </c>
+      <c r="N332" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="333" spans="1:14" ht="18" customHeight="1">
-      <c r="A333" s="44"/>
-      <c r="C333" s="2"/>
-      <c r="D333" s="2"/>
-      <c r="F333" s="2"/>
-      <c r="G333" s="2"/>
+      <c r="A333" s="44" t="s">
+        <v>416</v>
+      </c>
+      <c r="B333" s="96" t="s">
+        <v>408</v>
+      </c>
+      <c r="C333" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D333" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E333" s="97" t="s">
+        <v>411</v>
+      </c>
+      <c r="F333" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="G333" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H333" s="2"/>
-      <c r="I333" s="3"/>
-      <c r="J333" s="4"/>
+      <c r="I333" s="3">
+        <v>873</v>
+      </c>
+      <c r="J333" s="4">
+        <v>50</v>
+      </c>
       <c r="K333" s="4"/>
-      <c r="L333" s="44"/>
-      <c r="M333" s="44"/>
-      <c r="N333" s="44"/>
+      <c r="L333" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M333" s="44" t="s">
+        <v>419</v>
+      </c>
+      <c r="N333" s="44" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="334" spans="1:14" ht="18" customHeight="1">
       <c r="A334" s="44"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.scriptamat.2024.115986`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9BE7A5-0564-6941-8EB5-02507F04552D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F24A1D9-A882-F546-8C4A-592AB3D0A653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3640" yWindow="920" windowWidth="30660" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2786" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2814" uniqueCount="428">
   <si>
     <t>Metadata</t>
   </si>
@@ -1388,6 +1388,27 @@
   </si>
   <si>
     <t>10.1016/j.matchar.2024.113730</t>
+  </si>
+  <si>
+    <t>elemental powders pressed into pellet in argon before arc melting in argon</t>
+  </si>
+  <si>
+    <t>Mo35 W10 Re20 Ru30 Pd5</t>
+  </si>
+  <si>
+    <t>Mo35 W10 Re35 Ru15 Pd5</t>
+  </si>
+  <si>
+    <t>Mo35 W15 Re35 Ru10 Pd5</t>
+  </si>
+  <si>
+    <t>Mo35 W35 Re15 Ru10 Pd5</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>10.1016/j.scriptamat.2024.115986</t>
   </si>
 </sst>
 </file>
@@ -2607,8 +2628,8 @@
   </sheetPr>
   <dimension ref="A1:T424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A299" zoomScale="89" workbookViewId="0">
-      <selection activeCell="N337" sqref="N337"/>
+    <sheetView tabSelected="1" topLeftCell="A301" zoomScale="89" workbookViewId="0">
+      <selection activeCell="N340" sqref="N340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -14778,59 +14799,131 @@
     </row>
     <row r="334" spans="1:14" ht="18" customHeight="1">
       <c r="A334" s="44"/>
-      <c r="C334" s="2"/>
-      <c r="D334" s="2"/>
-      <c r="F334" s="2"/>
-      <c r="G334" s="2"/>
+      <c r="B334" s="96" t="s">
+        <v>422</v>
+      </c>
+      <c r="C334" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D334" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E334" t="s">
+        <v>421</v>
+      </c>
+      <c r="F334" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G334" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H334" s="2"/>
       <c r="I334" s="3"/>
-      <c r="J334" s="4"/>
+      <c r="J334" s="4">
+        <v>8.32</v>
+      </c>
       <c r="K334" s="4"/>
       <c r="L334" s="44"/>
       <c r="M334" s="44"/>
-      <c r="N334" s="44"/>
+      <c r="N334" s="44" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="335" spans="1:14" ht="18" customHeight="1">
       <c r="A335" s="44"/>
-      <c r="C335" s="2"/>
-      <c r="D335" s="2"/>
-      <c r="F335" s="2"/>
-      <c r="G335" s="2"/>
+      <c r="B335" s="96" t="s">
+        <v>423</v>
+      </c>
+      <c r="C335" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D335" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E335" t="s">
+        <v>421</v>
+      </c>
+      <c r="F335" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G335" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H335" s="2"/>
       <c r="I335" s="3"/>
-      <c r="J335" s="4"/>
+      <c r="J335" s="4">
+        <v>6.61</v>
+      </c>
       <c r="K335" s="4"/>
       <c r="L335" s="44"/>
       <c r="M335" s="44"/>
-      <c r="N335" s="44"/>
+      <c r="N335" s="44" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="336" spans="1:14" ht="18" customHeight="1">
       <c r="A336" s="44"/>
-      <c r="C336" s="2"/>
-      <c r="D336" s="2"/>
-      <c r="F336" s="2"/>
-      <c r="G336" s="2"/>
+      <c r="B336" s="96" t="s">
+        <v>424</v>
+      </c>
+      <c r="C336" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D336" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E336" t="s">
+        <v>421</v>
+      </c>
+      <c r="F336" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G336" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H336" s="2"/>
       <c r="I336" s="3"/>
-      <c r="J336" s="4"/>
+      <c r="J336" s="4">
+        <v>6.17</v>
+      </c>
       <c r="K336" s="4"/>
       <c r="L336" s="44"/>
       <c r="M336" s="44"/>
-      <c r="N336" s="44"/>
+      <c r="N336" s="44" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="337" spans="1:14" ht="18" customHeight="1">
       <c r="A337" s="44"/>
-      <c r="C337" s="2"/>
-      <c r="D337" s="2"/>
-      <c r="F337" s="2"/>
-      <c r="G337" s="2"/>
+      <c r="B337" s="96" t="s">
+        <v>425</v>
+      </c>
+      <c r="C337" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D337" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E337" t="s">
+        <v>421</v>
+      </c>
+      <c r="F337" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G337" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H337" s="2"/>
       <c r="I337" s="3"/>
-      <c r="J337" s="4"/>
+      <c r="J337" s="4">
+        <v>3.98</v>
+      </c>
       <c r="K337" s="4"/>
       <c r="L337" s="44"/>
       <c r="M337" s="44"/>
-      <c r="N337" s="44"/>
+      <c r="N337" s="44" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="338" spans="1:14" ht="18" customHeight="1">
       <c r="A338" s="44"/>

</xml_diff>

<commit_message>
- extracted data from `10.1007/s10853-024-09780-5`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F24A1D9-A882-F546-8C4A-592AB3D0A653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF861CF-E7D0-DC49-8BD9-57729E540264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="920" windowWidth="30660" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24380" yWindow="760" windowWidth="30660" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2814" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2951" uniqueCount="448">
   <si>
     <t>Metadata</t>
   </si>
@@ -1409,6 +1409,66 @@
   </si>
   <si>
     <t>10.1016/j.scriptamat.2024.115986</t>
+  </si>
+  <si>
+    <t>W3.5RhIrPt2</t>
+  </si>
+  <si>
+    <t>W3RhIrPt2</t>
+  </si>
+  <si>
+    <t>W2.65Mo0.35RhIrPt2</t>
+  </si>
+  <si>
+    <t>W2.3Mo0.7RhIrPt2</t>
+  </si>
+  <si>
+    <t>W2.5RhIrPt2</t>
+  </si>
+  <si>
+    <t>W2.175Mo0.325RhIrPt2</t>
+  </si>
+  <si>
+    <t>W1.85Mo0.65RhIrPt2</t>
+  </si>
+  <si>
+    <t>W2RhIrPt2</t>
+  </si>
+  <si>
+    <t>W1.7Mo0.3RhIrPt2</t>
+  </si>
+  <si>
+    <t>W1.4Mo0.6RhIrPt2</t>
+  </si>
+  <si>
+    <t>W2.175Ta0.325RhIrPt2</t>
+  </si>
+  <si>
+    <t>W1.7Ta0.3RhIrPt2</t>
+  </si>
+  <si>
+    <t>W2.175Nb0.325RhIrPt2</t>
+  </si>
+  <si>
+    <t>W1.7Nb0.3RhIrPt2</t>
+  </si>
+  <si>
+    <t>W2.175Re0.325RhIrPt2</t>
+  </si>
+  <si>
+    <t>W1.85Re0.65RhIrPt2</t>
+  </si>
+  <si>
+    <t>W1.7Re0.3RhIrPt2</t>
+  </si>
+  <si>
+    <t>FCC+HCP</t>
+  </si>
+  <si>
+    <t>AAM+RS</t>
+  </si>
+  <si>
+    <t>10.1007/s10853-024-09780-5</t>
   </si>
 </sst>
 </file>
@@ -2628,8 +2688,8 @@
   </sheetPr>
   <dimension ref="A1:T424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A301" zoomScale="89" workbookViewId="0">
-      <selection activeCell="N340" sqref="N340"/>
+    <sheetView tabSelected="1" topLeftCell="B324" zoomScale="89" workbookViewId="0">
+      <selection activeCell="O340" sqref="O340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -14823,7 +14883,9 @@
         <v>8.32</v>
       </c>
       <c r="K334" s="4"/>
-      <c r="L334" s="44"/>
+      <c r="L334" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="M334" s="44"/>
       <c r="N334" s="44" t="s">
         <v>427</v>
@@ -14855,7 +14917,9 @@
         <v>6.61</v>
       </c>
       <c r="K335" s="4"/>
-      <c r="L335" s="44"/>
+      <c r="L335" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="M335" s="44"/>
       <c r="N335" s="44" t="s">
         <v>427</v>
@@ -14887,7 +14951,9 @@
         <v>6.17</v>
       </c>
       <c r="K336" s="4"/>
-      <c r="L336" s="44"/>
+      <c r="L336" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="M336" s="44"/>
       <c r="N336" s="44" t="s">
         <v>427</v>
@@ -14919,7 +14985,9 @@
         <v>3.98</v>
       </c>
       <c r="K337" s="4"/>
-      <c r="L337" s="44"/>
+      <c r="L337" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="M337" s="44"/>
       <c r="N337" s="44" t="s">
         <v>427</v>
@@ -14927,241 +14995,555 @@
     </row>
     <row r="338" spans="1:14" ht="18" customHeight="1">
       <c r="A338" s="44"/>
-      <c r="C338" s="2"/>
-      <c r="D338" s="2"/>
-      <c r="F338" s="2"/>
-      <c r="G338" s="2"/>
+      <c r="B338" s="96" t="s">
+        <v>428</v>
+      </c>
+      <c r="C338" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D338" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F338" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G338" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H338" s="2"/>
       <c r="I338" s="3"/>
-      <c r="J338" s="4"/>
+      <c r="J338" s="4">
+        <v>1.56</v>
+      </c>
       <c r="K338" s="4"/>
-      <c r="L338" s="44"/>
-      <c r="M338" s="44"/>
-      <c r="N338" s="44"/>
+      <c r="L338" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M338" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N338" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="339" spans="1:14" ht="18" customHeight="1">
       <c r="A339" s="44"/>
-      <c r="C339" s="2"/>
-      <c r="D339" s="2"/>
-      <c r="F339" s="2"/>
-      <c r="G339" s="2"/>
+      <c r="B339" s="96" t="s">
+        <v>429</v>
+      </c>
+      <c r="C339" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D339" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F339" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G339" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H339" s="2"/>
       <c r="I339" s="3"/>
-      <c r="J339" s="4"/>
+      <c r="J339" s="4">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="K339" s="4"/>
-      <c r="L339" s="44"/>
-      <c r="M339" s="44"/>
-      <c r="N339" s="44"/>
+      <c r="L339" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M339" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N339" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="340" spans="1:14" ht="18" customHeight="1">
       <c r="A340" s="44"/>
-      <c r="C340" s="2"/>
-      <c r="D340" s="2"/>
-      <c r="F340" s="2"/>
-      <c r="G340" s="2"/>
+      <c r="B340" s="96" t="s">
+        <v>430</v>
+      </c>
+      <c r="C340" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D340" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F340" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G340" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H340" s="2"/>
       <c r="I340" s="3"/>
-      <c r="J340" s="4"/>
+      <c r="J340" s="4">
+        <v>1.25</v>
+      </c>
       <c r="K340" s="4"/>
-      <c r="L340" s="44"/>
-      <c r="M340" s="44"/>
-      <c r="N340" s="44"/>
+      <c r="L340" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M340" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N340" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="341" spans="1:14" ht="18" customHeight="1">
       <c r="A341" s="44"/>
-      <c r="C341" s="2"/>
-      <c r="D341" s="2"/>
+      <c r="B341" s="96" t="s">
+        <v>431</v>
+      </c>
+      <c r="C341" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="D341" s="2" t="s">
+        <v>446</v>
+      </c>
       <c r="F341" s="2"/>
-      <c r="G341" s="2"/>
+      <c r="G341" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H341" s="2"/>
       <c r="I341" s="3"/>
-      <c r="J341" s="4"/>
       <c r="K341" s="4"/>
       <c r="L341" s="44"/>
       <c r="M341" s="44"/>
-      <c r="N341" s="44"/>
+      <c r="N341" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="342" spans="1:14" ht="18" customHeight="1">
       <c r="A342" s="44"/>
-      <c r="C342" s="2"/>
-      <c r="D342" s="2"/>
-      <c r="F342" s="2"/>
-      <c r="G342" s="2"/>
+      <c r="B342" s="96" t="s">
+        <v>432</v>
+      </c>
+      <c r="C342" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D342" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F342" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G342" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H342" s="2"/>
       <c r="I342" s="3"/>
-      <c r="J342" s="4"/>
+      <c r="J342" s="4">
+        <v>0.9</v>
+      </c>
       <c r="K342" s="4"/>
-      <c r="L342" s="44"/>
-      <c r="M342" s="44"/>
-      <c r="N342" s="44"/>
+      <c r="L342" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M342" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N342" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="343" spans="1:14" ht="18" customHeight="1">
       <c r="A343" s="44"/>
-      <c r="C343" s="2"/>
-      <c r="D343" s="2"/>
-      <c r="F343" s="2"/>
-      <c r="G343" s="2"/>
+      <c r="B343" s="96" t="s">
+        <v>433</v>
+      </c>
+      <c r="C343" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D343" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F343" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G343" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H343" s="2"/>
       <c r="I343" s="3"/>
-      <c r="J343" s="4"/>
+      <c r="J343" s="4">
+        <v>0.85</v>
+      </c>
       <c r="K343" s="4"/>
-      <c r="L343" s="44"/>
-      <c r="M343" s="44"/>
-      <c r="N343" s="44"/>
+      <c r="L343" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M343" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N343" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="344" spans="1:14" ht="18" customHeight="1">
       <c r="A344" s="44"/>
-      <c r="C344" s="2"/>
-      <c r="D344" s="2"/>
-      <c r="F344" s="2"/>
-      <c r="G344" s="2"/>
+      <c r="B344" s="96" t="s">
+        <v>434</v>
+      </c>
+      <c r="C344" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D344" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F344" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G344" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H344" s="2"/>
       <c r="I344" s="3"/>
-      <c r="J344" s="4"/>
+      <c r="J344" s="4">
+        <v>0.85</v>
+      </c>
       <c r="K344" s="4"/>
-      <c r="L344" s="44"/>
-      <c r="M344" s="44"/>
-      <c r="N344" s="44"/>
+      <c r="L344" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M344" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N344" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="345" spans="1:14" ht="18" customHeight="1">
       <c r="A345" s="44"/>
-      <c r="C345" s="2"/>
-      <c r="D345" s="2"/>
-      <c r="F345" s="2"/>
-      <c r="G345" s="2"/>
+      <c r="B345" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="C345" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D345" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F345" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G345" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H345" s="2"/>
       <c r="I345" s="3"/>
-      <c r="J345" s="4"/>
+      <c r="J345" s="4">
+        <v>0.45</v>
+      </c>
       <c r="K345" s="4"/>
-      <c r="L345" s="44"/>
-      <c r="M345" s="44"/>
-      <c r="N345" s="44"/>
+      <c r="L345" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M345" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N345" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="346" spans="1:14" ht="18" customHeight="1">
       <c r="A346" s="44"/>
-      <c r="C346" s="2"/>
-      <c r="D346" s="2"/>
-      <c r="F346" s="2"/>
-      <c r="G346" s="2"/>
+      <c r="B346" s="96" t="s">
+        <v>436</v>
+      </c>
+      <c r="C346" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D346" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F346" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G346" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H346" s="2"/>
       <c r="I346" s="3"/>
-      <c r="J346" s="4"/>
+      <c r="J346" s="4">
+        <v>0.4</v>
+      </c>
       <c r="K346" s="4"/>
-      <c r="L346" s="44"/>
-      <c r="M346" s="44"/>
-      <c r="N346" s="44"/>
+      <c r="L346" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M346" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N346" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="347" spans="1:14" ht="18" customHeight="1">
       <c r="A347" s="44"/>
-      <c r="C347" s="2"/>
-      <c r="D347" s="2"/>
-      <c r="F347" s="2"/>
-      <c r="G347" s="2"/>
+      <c r="B347" s="96" t="s">
+        <v>437</v>
+      </c>
+      <c r="C347" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D347" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F347" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G347" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H347" s="2"/>
       <c r="I347" s="3"/>
-      <c r="J347" s="4"/>
+      <c r="J347" s="4">
+        <v>0.3</v>
+      </c>
       <c r="K347" s="4"/>
-      <c r="L347" s="44"/>
-      <c r="M347" s="44"/>
-      <c r="N347" s="44"/>
+      <c r="L347" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M347" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N347" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="348" spans="1:14" ht="18" customHeight="1">
       <c r="A348" s="44"/>
-      <c r="C348" s="2"/>
-      <c r="D348" s="2"/>
-      <c r="F348" s="2"/>
-      <c r="G348" s="2"/>
+      <c r="B348" s="96" t="s">
+        <v>438</v>
+      </c>
+      <c r="C348" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D348" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F348" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G348" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H348" s="2"/>
       <c r="I348" s="3"/>
-      <c r="J348" s="4"/>
+      <c r="J348" s="4">
+        <v>0.9</v>
+      </c>
       <c r="K348" s="4"/>
-      <c r="L348" s="44"/>
-      <c r="M348" s="44"/>
-      <c r="N348" s="44"/>
+      <c r="L348" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M348" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N348" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="349" spans="1:14" ht="18" customHeight="1">
       <c r="A349" s="44"/>
-      <c r="C349" s="2"/>
-      <c r="D349" s="2"/>
-      <c r="F349" s="2"/>
-      <c r="G349" s="2"/>
+      <c r="B349" s="96" t="s">
+        <v>439</v>
+      </c>
+      <c r="C349" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D349" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F349" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G349" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H349" s="2"/>
       <c r="I349" s="3"/>
-      <c r="J349" s="4"/>
+      <c r="J349" s="4">
+        <v>0.4</v>
+      </c>
       <c r="K349" s="4"/>
-      <c r="L349" s="44"/>
-      <c r="M349" s="44"/>
-      <c r="N349" s="44"/>
+      <c r="L349" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M349" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N349" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="350" spans="1:14" ht="18" customHeight="1">
       <c r="A350" s="44"/>
-      <c r="C350" s="2"/>
-      <c r="D350" s="2"/>
-      <c r="F350" s="2"/>
-      <c r="G350" s="2"/>
+      <c r="B350" s="96" t="s">
+        <v>440</v>
+      </c>
+      <c r="C350" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D350" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F350" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G350" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H350" s="2"/>
       <c r="I350" s="3"/>
-      <c r="J350" s="4"/>
+      <c r="J350" s="4">
+        <v>0.8</v>
+      </c>
       <c r="K350" s="4"/>
-      <c r="L350" s="44"/>
-      <c r="M350" s="44"/>
-      <c r="N350" s="44"/>
+      <c r="L350" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M350" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N350" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="351" spans="1:14" ht="18" customHeight="1">
       <c r="A351" s="44"/>
-      <c r="C351" s="2"/>
-      <c r="D351" s="2"/>
-      <c r="F351" s="2"/>
-      <c r="G351" s="2"/>
+      <c r="B351" s="96" t="s">
+        <v>441</v>
+      </c>
+      <c r="C351" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D351" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F351" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G351" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H351" s="2"/>
       <c r="I351" s="3"/>
-      <c r="J351" s="4"/>
+      <c r="J351" s="4">
+        <v>0.4</v>
+      </c>
       <c r="K351" s="4"/>
-      <c r="L351" s="44"/>
-      <c r="M351" s="44"/>
-      <c r="N351" s="44"/>
+      <c r="L351" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M351" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N351" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="352" spans="1:14" ht="18" customHeight="1">
       <c r="A352" s="44"/>
-      <c r="C352" s="2"/>
-      <c r="D352" s="2"/>
-      <c r="F352" s="2"/>
-      <c r="G352" s="2"/>
+      <c r="B352" s="96" t="s">
+        <v>442</v>
+      </c>
+      <c r="C352" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D352" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F352" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G352" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H352" s="2"/>
       <c r="I352" s="3"/>
-      <c r="J352" s="4"/>
+      <c r="J352" s="4">
+        <v>1</v>
+      </c>
       <c r="K352" s="4"/>
-      <c r="L352" s="44"/>
-      <c r="M352" s="44"/>
-      <c r="N352" s="44"/>
+      <c r="L352" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M352" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N352" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="353" spans="1:14" ht="18" customHeight="1">
       <c r="A353" s="44"/>
-      <c r="C353" s="2"/>
-      <c r="D353" s="2"/>
-      <c r="F353" s="2"/>
-      <c r="G353" s="2"/>
+      <c r="B353" s="96" t="s">
+        <v>443</v>
+      </c>
+      <c r="C353" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D353" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F353" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G353" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H353" s="2"/>
       <c r="I353" s="3"/>
-      <c r="J353" s="4"/>
+      <c r="J353" s="4">
+        <v>1.05</v>
+      </c>
       <c r="K353" s="4"/>
-      <c r="L353" s="44"/>
-      <c r="M353" s="44"/>
-      <c r="N353" s="44"/>
+      <c r="L353" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M353" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N353" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="354" spans="1:14" ht="18" customHeight="1">
       <c r="A354" s="44"/>
-      <c r="C354" s="2"/>
-      <c r="D354" s="2"/>
-      <c r="F354" s="2"/>
-      <c r="G354" s="2"/>
+      <c r="B354" s="96" t="s">
+        <v>444</v>
+      </c>
+      <c r="C354" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D354" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F354" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G354" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H354" s="2"/>
       <c r="I354" s="3"/>
-      <c r="J354" s="4"/>
+      <c r="J354" s="4">
+        <v>0.65</v>
+      </c>
       <c r="K354" s="4"/>
-      <c r="L354" s="44"/>
-      <c r="M354" s="44"/>
-      <c r="N354" s="44"/>
+      <c r="L354" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="M354" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="N354" s="44" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="355" spans="1:14" ht="18" customHeight="1">
       <c r="A355" s="44"/>

</xml_diff>

<commit_message>
- extracted data from `10.1103/PhysRevLett.113.107001`; typo fixes in earlier upload
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF861CF-E7D0-DC49-8BD9-57729E540264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71279368-85CD-BD48-B953-957BBCFC31CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24380" yWindow="760" windowWidth="30660" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2951" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2965" uniqueCount="450">
   <si>
     <t>Metadata</t>
   </si>
@@ -1469,6 +1469,12 @@
   </si>
   <si>
     <t>10.1007/s10853-024-09780-5</t>
+  </si>
+  <si>
+    <t>10.1103/PhysRevLett.113.107001</t>
+  </si>
+  <si>
+    <t>Ta34 Nb33 Hf8 Zr14 Ti11</t>
   </si>
 </sst>
 </file>
@@ -2688,8 +2694,8 @@
   </sheetPr>
   <dimension ref="A1:T424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B324" zoomScale="89" workbookViewId="0">
-      <selection activeCell="O340" sqref="O340"/>
+    <sheetView tabSelected="1" topLeftCell="A324" zoomScale="89" workbookViewId="0">
+      <selection activeCell="G363" sqref="G363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -13619,7 +13625,7 @@
         <v>298</v>
       </c>
       <c r="J302" s="4">
-        <v>1.5700000000000002E-8</v>
+        <v>1.57E-6</v>
       </c>
       <c r="K302" s="4"/>
       <c r="L302" s="2" t="s">
@@ -13657,7 +13663,7 @@
         <v>298</v>
       </c>
       <c r="J303" s="4">
-        <v>1.27E-8</v>
+        <v>1.2699999999999999E-6</v>
       </c>
       <c r="K303" s="4"/>
       <c r="L303" s="2" t="s">
@@ -13695,7 +13701,7 @@
         <v>298</v>
       </c>
       <c r="J304" s="4">
-        <v>8.8599999999999999E-8</v>
+        <v>8.8599999999999997E-7</v>
       </c>
       <c r="K304" s="4"/>
       <c r="L304" s="2" t="s">
@@ -15547,31 +15553,69 @@
     </row>
     <row r="355" spans="1:14" ht="18" customHeight="1">
       <c r="A355" s="44"/>
-      <c r="C355" s="2"/>
-      <c r="D355" s="2"/>
-      <c r="F355" s="2"/>
-      <c r="G355" s="2"/>
+      <c r="B355" s="96" t="s">
+        <v>449</v>
+      </c>
+      <c r="C355" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D355" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F355" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G355" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H355" s="2"/>
       <c r="I355" s="3"/>
-      <c r="J355" s="4"/>
+      <c r="J355" s="4">
+        <v>7.27</v>
+      </c>
       <c r="K355" s="4"/>
-      <c r="L355" s="44"/>
+      <c r="L355" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="M355" s="44"/>
-      <c r="N355" s="44"/>
+      <c r="N355" s="44" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="356" spans="1:14" ht="18" customHeight="1">
       <c r="A356" s="44"/>
-      <c r="C356" s="2"/>
-      <c r="D356" s="2"/>
-      <c r="F356" s="2"/>
-      <c r="G356" s="2"/>
+      <c r="B356" s="96" t="s">
+        <v>449</v>
+      </c>
+      <c r="C356" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D356" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F356" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G356" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H356" s="2"/>
-      <c r="I356" s="3"/>
-      <c r="J356" s="4"/>
-      <c r="K356" s="4"/>
-      <c r="L356" s="44"/>
+      <c r="I356" s="3">
+        <v>300</v>
+      </c>
+      <c r="J356" s="4">
+        <v>4.5999999999999999E-7</v>
+      </c>
+      <c r="K356" s="4">
+        <v>1E-8</v>
+      </c>
+      <c r="L356" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="M356" s="44"/>
-      <c r="N356" s="44"/>
+      <c r="N356" s="44" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="357" spans="1:14" ht="18" customHeight="1">
       <c r="A357" s="44"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jallcom.2024.175273`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71279368-85CD-BD48-B953-957BBCFC31CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC2B299-1765-A948-9F67-7CEB637E9B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10340" yWindow="760" windowWidth="24220" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2965" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3203" uniqueCount="468">
   <si>
     <t>Metadata</t>
   </si>
@@ -1475,6 +1475,60 @@
   </si>
   <si>
     <t>Ta34 Nb33 Hf8 Zr14 Ti11</t>
+  </si>
+  <si>
+    <t>after arc melting samples were homogenized at 0.9 homologous temperature and water quenched then deformed by rotary swaging to 0.71 true strain then recrystallized at 0.9 homologous temperature and water quenched</t>
+  </si>
+  <si>
+    <t>AAM+H+WQ+RX</t>
+  </si>
+  <si>
+    <t>Ni25(CuPdPt)25</t>
+  </si>
+  <si>
+    <t>Au2.5Ni22.5(CuPdIPt)25</t>
+  </si>
+  <si>
+    <t>Au5 Ni20 (CuPdPt)25</t>
+  </si>
+  <si>
+    <t>Au7.5 Ni17.5 (CuPdPt)25</t>
+  </si>
+  <si>
+    <t>Au10 Ni15 (CuPdPt)25</t>
+  </si>
+  <si>
+    <t>Au15 Ni10 (CuPdPt)25</t>
+  </si>
+  <si>
+    <t>Au20 Ni5 (CuPdPt)25</t>
+  </si>
+  <si>
+    <t>Au25 (CuPdPt)25</t>
+  </si>
+  <si>
+    <t>Pt25 (AuCuPd)25</t>
+  </si>
+  <si>
+    <t>Ni5 Pt20 (AuCuPd)25</t>
+  </si>
+  <si>
+    <t>Ni10 Pt15 (AuCuPd)25</t>
+  </si>
+  <si>
+    <t>Ni15 Pt10 (AuCuPd)25</t>
+  </si>
+  <si>
+    <t>Ni20 Pt5 (AuCuPd)25</t>
+  </si>
+  <si>
+    <t>Ni25 (AuCuPd)25</t>
+  </si>
+  <si>
+    <t>1e-3 strain rate</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2024.175273</t>
   </si>
 </sst>
 </file>
@@ -2694,8 +2748,8 @@
   </sheetPr>
   <dimension ref="A1:T424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A324" zoomScale="89" workbookViewId="0">
-      <selection activeCell="G363" sqref="G363"/>
+    <sheetView tabSelected="1" topLeftCell="B349" zoomScale="89" workbookViewId="0">
+      <selection activeCell="L394" sqref="L394"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10517,7 +10571,7 @@
         <v>298</v>
       </c>
       <c r="J207" s="50">
-        <f t="shared" si="5"/>
+        <f>P207*9807000</f>
         <v>5923428000</v>
       </c>
       <c r="K207" s="4"/>
@@ -15619,395 +15673,1095 @@
     </row>
     <row r="357" spans="1:14" ht="18" customHeight="1">
       <c r="A357" s="44"/>
-      <c r="C357" s="2"/>
-      <c r="D357" s="2"/>
-      <c r="F357" s="2"/>
-      <c r="G357" s="2"/>
-      <c r="H357" s="2"/>
-      <c r="I357" s="3"/>
-      <c r="J357" s="4"/>
+      <c r="B357" s="96" t="s">
+        <v>452</v>
+      </c>
+      <c r="C357" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D357" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E357" t="s">
+        <v>450</v>
+      </c>
+      <c r="F357" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G357" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H357" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I357" s="3">
+        <v>298</v>
+      </c>
+      <c r="J357" s="4">
+        <v>375000000</v>
+      </c>
       <c r="K357" s="4"/>
-      <c r="L357" s="44"/>
+      <c r="L357" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M357" s="44"/>
-      <c r="N357" s="44"/>
+      <c r="N357" s="44" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="358" spans="1:14" ht="18" customHeight="1">
       <c r="A358" s="44"/>
-      <c r="C358" s="2"/>
-      <c r="D358" s="2"/>
-      <c r="F358" s="2"/>
-      <c r="G358" s="2"/>
-      <c r="H358" s="2"/>
-      <c r="I358" s="3"/>
-      <c r="J358" s="4"/>
+      <c r="B358" s="96" t="s">
+        <v>453</v>
+      </c>
+      <c r="C358" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D358" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E358" t="s">
+        <v>450</v>
+      </c>
+      <c r="F358" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G358" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H358" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I358" s="3">
+        <v>298</v>
+      </c>
+      <c r="J358" s="4">
+        <v>432000000</v>
+      </c>
       <c r="K358" s="4"/>
-      <c r="L358" s="44"/>
+      <c r="L358" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M358" s="44"/>
-      <c r="N358" s="44"/>
+      <c r="N358" s="44" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="359" spans="1:14" ht="18" customHeight="1">
       <c r="A359" s="44"/>
-      <c r="C359" s="2"/>
-      <c r="D359" s="2"/>
-      <c r="F359" s="2"/>
-      <c r="G359" s="2"/>
-      <c r="H359" s="2"/>
-      <c r="I359" s="3"/>
-      <c r="J359" s="4"/>
+      <c r="B359" s="96" t="s">
+        <v>454</v>
+      </c>
+      <c r="C359" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D359" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E359" t="s">
+        <v>450</v>
+      </c>
+      <c r="F359" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G359" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H359" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I359" s="3">
+        <v>298</v>
+      </c>
+      <c r="J359" s="4">
+        <v>465000000</v>
+      </c>
       <c r="K359" s="4"/>
-      <c r="L359" s="44"/>
+      <c r="L359" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M359" s="44"/>
-      <c r="N359" s="44"/>
+      <c r="N359" s="44" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="360" spans="1:14" ht="18" customHeight="1">
       <c r="A360" s="44"/>
-      <c r="C360" s="2"/>
-      <c r="D360" s="2"/>
-      <c r="F360" s="2"/>
-      <c r="G360" s="2"/>
-      <c r="H360" s="2"/>
-      <c r="I360" s="3"/>
-      <c r="J360" s="4"/>
+      <c r="B360" s="96" t="s">
+        <v>455</v>
+      </c>
+      <c r="C360" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D360" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E360" t="s">
+        <v>450</v>
+      </c>
+      <c r="F360" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G360" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H360" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I360" s="3">
+        <v>298</v>
+      </c>
+      <c r="J360" s="4">
+        <v>499000000</v>
+      </c>
       <c r="K360" s="4"/>
-      <c r="L360" s="44"/>
+      <c r="L360" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M360" s="44"/>
-      <c r="N360" s="44"/>
+      <c r="N360" s="44" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="361" spans="1:14" ht="18" customHeight="1">
       <c r="A361" s="44"/>
-      <c r="C361" s="2"/>
-      <c r="D361" s="2"/>
-      <c r="F361" s="2"/>
-      <c r="G361" s="2"/>
-      <c r="H361" s="2"/>
-      <c r="I361" s="3"/>
-      <c r="J361" s="4"/>
+      <c r="B361" s="96" t="s">
+        <v>456</v>
+      </c>
+      <c r="C361" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D361" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E361" t="s">
+        <v>450</v>
+      </c>
+      <c r="F361" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G361" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H361" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I361" s="3">
+        <v>298</v>
+      </c>
+      <c r="J361" s="4">
+        <v>526000000</v>
+      </c>
       <c r="K361" s="4"/>
-      <c r="L361" s="44"/>
+      <c r="L361" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M361" s="44"/>
-      <c r="N361" s="44"/>
+      <c r="N361" s="44" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="362" spans="1:14" ht="18" customHeight="1">
       <c r="A362" s="44"/>
-      <c r="C362" s="2"/>
-      <c r="D362" s="2"/>
-      <c r="F362" s="2"/>
-      <c r="G362" s="2"/>
-      <c r="H362" s="2"/>
-      <c r="I362" s="3"/>
-      <c r="J362" s="4"/>
+      <c r="B362" s="96" t="s">
+        <v>457</v>
+      </c>
+      <c r="C362" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D362" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E362" t="s">
+        <v>450</v>
+      </c>
+      <c r="F362" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G362" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H362" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I362" s="3">
+        <v>298</v>
+      </c>
+      <c r="J362" s="4">
+        <v>524000000</v>
+      </c>
       <c r="K362" s="4"/>
-      <c r="L362" s="44"/>
+      <c r="L362" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M362" s="44"/>
-      <c r="N362" s="44"/>
+      <c r="N362" s="44" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="363" spans="1:14" ht="18" customHeight="1">
       <c r="A363" s="44"/>
-      <c r="C363" s="2"/>
-      <c r="D363" s="2"/>
-      <c r="F363" s="2"/>
-      <c r="G363" s="2"/>
-      <c r="H363" s="2"/>
-      <c r="I363" s="3"/>
-      <c r="J363" s="4"/>
+      <c r="B363" s="96" t="s">
+        <v>458</v>
+      </c>
+      <c r="C363" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D363" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E363" t="s">
+        <v>450</v>
+      </c>
+      <c r="F363" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G363" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H363" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I363" s="3">
+        <v>298</v>
+      </c>
+      <c r="J363" s="4">
+        <v>508000000</v>
+      </c>
       <c r="K363" s="4"/>
-      <c r="L363" s="44"/>
+      <c r="L363" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M363" s="44"/>
-      <c r="N363" s="44"/>
+      <c r="N363" s="44" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="364" spans="1:14" ht="18" customHeight="1">
       <c r="A364" s="44"/>
-      <c r="C364" s="2"/>
-      <c r="D364" s="2"/>
-      <c r="F364" s="2"/>
-      <c r="G364" s="2"/>
-      <c r="H364" s="2"/>
-      <c r="I364" s="3"/>
-      <c r="J364" s="4"/>
+      <c r="B364" s="96" t="s">
+        <v>459</v>
+      </c>
+      <c r="C364" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D364" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E364" t="s">
+        <v>450</v>
+      </c>
+      <c r="F364" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G364" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H364" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I364" s="3">
+        <v>298</v>
+      </c>
+      <c r="J364" s="4">
+        <v>430000000</v>
+      </c>
       <c r="K364" s="4"/>
-      <c r="L364" s="44"/>
+      <c r="L364" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M364" s="44"/>
-      <c r="N364" s="44"/>
+      <c r="N364" s="44" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="365" spans="1:14" ht="18" customHeight="1">
       <c r="A365" s="44"/>
-      <c r="C365" s="2"/>
-      <c r="D365" s="2"/>
-      <c r="F365" s="2"/>
-      <c r="G365" s="2"/>
-      <c r="H365" s="2"/>
-      <c r="I365" s="3"/>
-      <c r="J365" s="4"/>
+      <c r="B365" s="96" t="s">
+        <v>460</v>
+      </c>
+      <c r="C365" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D365" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E365" t="s">
+        <v>450</v>
+      </c>
+      <c r="F365" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G365" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H365" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I365" s="3">
+        <v>298</v>
+      </c>
+      <c r="J365" s="4">
+        <v>380000000</v>
+      </c>
       <c r="K365" s="4"/>
-      <c r="L365" s="44"/>
+      <c r="L365" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M365" s="44"/>
-      <c r="N365" s="44"/>
+      <c r="N365" s="44" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="366" spans="1:14" ht="18" customHeight="1">
       <c r="A366" s="44"/>
-      <c r="C366" s="2"/>
-      <c r="D366" s="2"/>
-      <c r="F366" s="2"/>
-      <c r="G366" s="2"/>
-      <c r="H366" s="2"/>
-      <c r="I366" s="3"/>
-      <c r="J366" s="4"/>
+      <c r="B366" s="96" t="s">
+        <v>461</v>
+      </c>
+      <c r="C366" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D366" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E366" t="s">
+        <v>450</v>
+      </c>
+      <c r="F366" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G366" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H366" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I366" s="3">
+        <v>298</v>
+      </c>
+      <c r="J366" s="4">
+        <v>474000000</v>
+      </c>
       <c r="K366" s="4"/>
-      <c r="L366" s="44"/>
+      <c r="L366" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M366" s="44"/>
-      <c r="N366" s="44"/>
+      <c r="N366" s="44" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="367" spans="1:14" ht="18" customHeight="1">
       <c r="A367" s="44"/>
-      <c r="C367" s="2"/>
-      <c r="D367" s="2"/>
-      <c r="F367" s="2"/>
-      <c r="G367" s="2"/>
-      <c r="H367" s="2"/>
-      <c r="I367" s="3"/>
-      <c r="J367" s="4"/>
+      <c r="B367" s="96" t="s">
+        <v>462</v>
+      </c>
+      <c r="C367" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D367" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E367" t="s">
+        <v>450</v>
+      </c>
+      <c r="F367" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G367" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H367" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I367" s="3">
+        <v>298</v>
+      </c>
+      <c r="J367" s="4">
+        <v>549000000</v>
+      </c>
       <c r="K367" s="4"/>
-      <c r="L367" s="44"/>
+      <c r="L367" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M367" s="44"/>
-      <c r="N367" s="44"/>
+      <c r="N367" s="44" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="368" spans="1:14" ht="18" customHeight="1">
       <c r="A368" s="44"/>
-      <c r="C368" s="2"/>
-      <c r="D368" s="2"/>
-      <c r="F368" s="2"/>
-      <c r="G368" s="2"/>
-      <c r="H368" s="2"/>
-      <c r="I368" s="3"/>
-      <c r="J368" s="4"/>
+      <c r="B368" s="96" t="s">
+        <v>463</v>
+      </c>
+      <c r="C368" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D368" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E368" t="s">
+        <v>450</v>
+      </c>
+      <c r="F368" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G368" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H368" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I368" s="3">
+        <v>298</v>
+      </c>
+      <c r="J368" s="4">
+        <v>581000000</v>
+      </c>
       <c r="K368" s="4"/>
-      <c r="L368" s="44"/>
+      <c r="L368" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M368" s="44"/>
-      <c r="N368" s="44"/>
-    </row>
-    <row r="369" spans="1:14" ht="18" customHeight="1">
+      <c r="N368" s="44" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="369" spans="1:16" ht="18" customHeight="1">
       <c r="A369" s="44"/>
-      <c r="C369" s="2"/>
-      <c r="D369" s="2"/>
-      <c r="F369" s="2"/>
-      <c r="G369" s="2"/>
-      <c r="H369" s="2"/>
-      <c r="I369" s="3"/>
-      <c r="J369" s="4"/>
+      <c r="B369" s="96" t="s">
+        <v>464</v>
+      </c>
+      <c r="C369" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D369" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E369" t="s">
+        <v>450</v>
+      </c>
+      <c r="F369" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G369" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H369" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I369" s="3">
+        <v>298</v>
+      </c>
+      <c r="J369" s="4">
+        <v>513000000</v>
+      </c>
       <c r="K369" s="4"/>
-      <c r="L369" s="44"/>
+      <c r="L369" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M369" s="44"/>
-      <c r="N369" s="44"/>
-    </row>
-    <row r="370" spans="1:14" ht="18" customHeight="1">
+      <c r="N369" s="44" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="370" spans="1:16" ht="18" customHeight="1">
       <c r="A370" s="44"/>
-      <c r="C370" s="2"/>
-      <c r="D370" s="2"/>
-      <c r="F370" s="2"/>
-      <c r="G370" s="2"/>
-      <c r="H370" s="2"/>
-      <c r="I370" s="3"/>
-      <c r="J370" s="4"/>
+      <c r="B370" s="96" t="s">
+        <v>465</v>
+      </c>
+      <c r="C370" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D370" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E370" t="s">
+        <v>450</v>
+      </c>
+      <c r="F370" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G370" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H370" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I370" s="3">
+        <v>298</v>
+      </c>
+      <c r="J370" s="4">
+        <v>472000000</v>
+      </c>
       <c r="K370" s="4"/>
-      <c r="L370" s="44"/>
+      <c r="L370" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M370" s="44"/>
-      <c r="N370" s="44"/>
-    </row>
-    <row r="371" spans="1:14" ht="18" customHeight="1">
+      <c r="N370" s="44" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="371" spans="1:16" ht="18" customHeight="1">
       <c r="A371" s="44"/>
-      <c r="C371" s="2"/>
-      <c r="D371" s="2"/>
-      <c r="F371" s="2"/>
-      <c r="G371" s="2"/>
+      <c r="B371" s="96" t="s">
+        <v>452</v>
+      </c>
+      <c r="C371" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D371" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E371" t="s">
+        <v>450</v>
+      </c>
+      <c r="F371" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G371" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H371" s="2"/>
-      <c r="I371" s="3"/>
-      <c r="J371" s="4"/>
+      <c r="I371" s="3">
+        <v>298</v>
+      </c>
+      <c r="J371" s="4">
+        <f>P371*9807000</f>
+        <v>2030049000</v>
+      </c>
       <c r="K371" s="4"/>
-      <c r="L371" s="44"/>
+      <c r="L371" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M371" s="44"/>
-      <c r="N371" s="44"/>
-    </row>
-    <row r="372" spans="1:14" ht="18" customHeight="1">
+      <c r="N371" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="P371" s="6">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="372" spans="1:16" ht="18" customHeight="1">
       <c r="A372" s="44"/>
-      <c r="C372" s="2"/>
-      <c r="D372" s="2"/>
-      <c r="F372" s="2"/>
-      <c r="G372" s="2"/>
+      <c r="B372" s="96" t="s">
+        <v>453</v>
+      </c>
+      <c r="C372" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D372" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E372" t="s">
+        <v>450</v>
+      </c>
+      <c r="F372" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G372" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H372" s="2"/>
-      <c r="I372" s="3"/>
-      <c r="J372" s="4"/>
+      <c r="I372" s="3">
+        <v>298</v>
+      </c>
+      <c r="J372" s="4">
+        <f t="shared" ref="J372:J384" si="6">P372*9807000</f>
+        <v>2177154000</v>
+      </c>
       <c r="K372" s="4"/>
-      <c r="L372" s="44"/>
+      <c r="L372" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M372" s="44"/>
-      <c r="N372" s="44"/>
-    </row>
-    <row r="373" spans="1:14" ht="18" customHeight="1">
+      <c r="N372" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="P372" s="6">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="373" spans="1:16" ht="18" customHeight="1">
       <c r="A373" s="44"/>
-      <c r="C373" s="2"/>
-      <c r="D373" s="2"/>
-      <c r="F373" s="2"/>
-      <c r="G373" s="2"/>
+      <c r="B373" s="96" t="s">
+        <v>454</v>
+      </c>
+      <c r="C373" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D373" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E373" t="s">
+        <v>450</v>
+      </c>
+      <c r="F373" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G373" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H373" s="2"/>
-      <c r="I373" s="3"/>
-      <c r="J373" s="4"/>
+      <c r="I373" s="3">
+        <v>298</v>
+      </c>
+      <c r="J373" s="4">
+        <f t="shared" si="6"/>
+        <v>2314452000</v>
+      </c>
       <c r="K373" s="4"/>
-      <c r="L373" s="44"/>
+      <c r="L373" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M373" s="44"/>
-      <c r="N373" s="44"/>
-    </row>
-    <row r="374" spans="1:14" ht="18" customHeight="1">
+      <c r="N373" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="P373" s="6">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="374" spans="1:16" ht="18" customHeight="1">
       <c r="A374" s="44"/>
-      <c r="C374" s="2"/>
-      <c r="D374" s="2"/>
-      <c r="F374" s="2"/>
-      <c r="G374" s="2"/>
+      <c r="B374" s="96" t="s">
+        <v>455</v>
+      </c>
+      <c r="C374" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D374" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E374" t="s">
+        <v>450</v>
+      </c>
+      <c r="F374" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G374" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H374" s="2"/>
-      <c r="I374" s="3"/>
-      <c r="J374" s="4"/>
+      <c r="I374" s="3">
+        <v>298</v>
+      </c>
+      <c r="J374" s="4">
+        <f t="shared" si="6"/>
+        <v>2402715000</v>
+      </c>
       <c r="K374" s="4"/>
-      <c r="L374" s="44"/>
+      <c r="L374" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M374" s="44"/>
-      <c r="N374" s="44"/>
-    </row>
-    <row r="375" spans="1:14" ht="18" customHeight="1">
+      <c r="N374" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="P374" s="6">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="375" spans="1:16" ht="18" customHeight="1">
       <c r="A375" s="44"/>
-      <c r="C375" s="2"/>
-      <c r="D375" s="2"/>
-      <c r="F375" s="2"/>
-      <c r="G375" s="2"/>
+      <c r="B375" s="96" t="s">
+        <v>456</v>
+      </c>
+      <c r="C375" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D375" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E375" t="s">
+        <v>450</v>
+      </c>
+      <c r="F375" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G375" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H375" s="2"/>
-      <c r="I375" s="3"/>
-      <c r="J375" s="4"/>
+      <c r="I375" s="3">
+        <v>298</v>
+      </c>
+      <c r="J375" s="4">
+        <f t="shared" si="6"/>
+        <v>2441943000</v>
+      </c>
       <c r="K375" s="4"/>
-      <c r="L375" s="44"/>
+      <c r="L375" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M375" s="44"/>
-      <c r="N375" s="44"/>
-    </row>
-    <row r="376" spans="1:14" ht="18" customHeight="1">
+      <c r="N375" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="P375" s="6">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="376" spans="1:16" ht="18" customHeight="1">
       <c r="A376" s="44"/>
-      <c r="C376" s="2"/>
-      <c r="D376" s="2"/>
-      <c r="F376" s="2"/>
-      <c r="G376" s="2"/>
+      <c r="B376" s="96" t="s">
+        <v>457</v>
+      </c>
+      <c r="C376" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D376" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E376" t="s">
+        <v>450</v>
+      </c>
+      <c r="F376" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G376" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H376" s="2"/>
-      <c r="I376" s="3"/>
-      <c r="J376" s="4"/>
+      <c r="I376" s="3">
+        <v>298</v>
+      </c>
+      <c r="J376" s="4">
+        <f t="shared" si="6"/>
+        <v>2412522000</v>
+      </c>
       <c r="K376" s="4"/>
-      <c r="L376" s="44"/>
+      <c r="L376" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M376" s="44"/>
-      <c r="N376" s="44"/>
-    </row>
-    <row r="377" spans="1:14" ht="18" customHeight="1">
+      <c r="N376" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="P376" s="6">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="377" spans="1:16" ht="18" customHeight="1">
       <c r="A377" s="44"/>
-      <c r="C377" s="2"/>
-      <c r="D377" s="2"/>
-      <c r="F377" s="2"/>
-      <c r="G377" s="2"/>
+      <c r="B377" s="96" t="s">
+        <v>458</v>
+      </c>
+      <c r="C377" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D377" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E377" t="s">
+        <v>450</v>
+      </c>
+      <c r="F377" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G377" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H377" s="2"/>
-      <c r="I377" s="3"/>
-      <c r="J377" s="4"/>
+      <c r="I377" s="3">
+        <v>298</v>
+      </c>
+      <c r="J377" s="4">
+        <f t="shared" si="6"/>
+        <v>2285031000</v>
+      </c>
       <c r="K377" s="4"/>
-      <c r="L377" s="44"/>
+      <c r="L377" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M377" s="44"/>
-      <c r="N377" s="44"/>
-    </row>
-    <row r="378" spans="1:14" ht="18" customHeight="1">
+      <c r="N377" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="P377" s="6">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="378" spans="1:16" ht="18" customHeight="1">
       <c r="A378" s="44"/>
-      <c r="C378" s="2"/>
-      <c r="D378" s="2"/>
-      <c r="F378" s="2"/>
-      <c r="G378" s="2"/>
+      <c r="B378" s="96" t="s">
+        <v>459</v>
+      </c>
+      <c r="C378" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D378" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E378" t="s">
+        <v>450</v>
+      </c>
+      <c r="F378" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G378" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H378" s="2"/>
-      <c r="I378" s="3"/>
-      <c r="J378" s="4"/>
+      <c r="I378" s="3">
+        <v>298</v>
+      </c>
+      <c r="J378" s="4">
+        <f t="shared" si="6"/>
+        <v>1981014000</v>
+      </c>
       <c r="K378" s="4"/>
-      <c r="L378" s="44"/>
+      <c r="L378" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M378" s="44"/>
-      <c r="N378" s="44"/>
-    </row>
-    <row r="379" spans="1:14" ht="18" customHeight="1">
+      <c r="N378" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="P378" s="6">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="379" spans="1:16" ht="18" customHeight="1">
       <c r="A379" s="44"/>
-      <c r="C379" s="2"/>
-      <c r="D379" s="2"/>
-      <c r="F379" s="2"/>
-      <c r="G379" s="2"/>
+      <c r="B379" s="96" t="s">
+        <v>460</v>
+      </c>
+      <c r="C379" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D379" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E379" t="s">
+        <v>450</v>
+      </c>
+      <c r="F379" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G379" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H379" s="2"/>
-      <c r="I379" s="3"/>
-      <c r="J379" s="4"/>
+      <c r="I379" s="3">
+        <v>298</v>
+      </c>
+      <c r="J379" s="4">
+        <f t="shared" si="6"/>
+        <v>2000628000</v>
+      </c>
       <c r="K379" s="4"/>
-      <c r="L379" s="44"/>
+      <c r="L379" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M379" s="44"/>
-      <c r="N379" s="44"/>
-    </row>
-    <row r="380" spans="1:14" ht="18" customHeight="1">
+      <c r="N379" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="P379" s="6">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="380" spans="1:16" ht="18" customHeight="1">
       <c r="A380" s="44"/>
-      <c r="C380" s="2"/>
-      <c r="D380" s="2"/>
-      <c r="F380" s="2"/>
-      <c r="G380" s="2"/>
+      <c r="B380" s="96" t="s">
+        <v>461</v>
+      </c>
+      <c r="C380" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D380" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E380" t="s">
+        <v>450</v>
+      </c>
+      <c r="F380" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G380" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H380" s="2"/>
-      <c r="I380" s="3"/>
-      <c r="J380" s="4"/>
+      <c r="I380" s="3">
+        <v>298</v>
+      </c>
+      <c r="J380" s="4">
+        <f t="shared" si="6"/>
+        <v>2275224000</v>
+      </c>
       <c r="K380" s="4"/>
-      <c r="L380" s="44"/>
+      <c r="L380" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M380" s="44"/>
-      <c r="N380" s="44"/>
-    </row>
-    <row r="381" spans="1:14" ht="18" customHeight="1">
+      <c r="N380" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="P380" s="6">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="381" spans="1:16" ht="18" customHeight="1">
       <c r="A381" s="44"/>
-      <c r="C381" s="2"/>
-      <c r="D381" s="2"/>
-      <c r="F381" s="2"/>
-      <c r="G381" s="2"/>
+      <c r="B381" s="96" t="s">
+        <v>462</v>
+      </c>
+      <c r="C381" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D381" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E381" t="s">
+        <v>450</v>
+      </c>
+      <c r="F381" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G381" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H381" s="2"/>
-      <c r="I381" s="3"/>
-      <c r="J381" s="4"/>
+      <c r="I381" s="3">
+        <v>298</v>
+      </c>
+      <c r="J381" s="4">
+        <f t="shared" si="6"/>
+        <v>2451750000</v>
+      </c>
       <c r="K381" s="4"/>
-      <c r="L381" s="44"/>
+      <c r="L381" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M381" s="44"/>
-      <c r="N381" s="44"/>
-    </row>
-    <row r="382" spans="1:14" ht="18" customHeight="1">
+      <c r="N381" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="P381" s="6">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="382" spans="1:16" ht="18" customHeight="1">
       <c r="A382" s="44"/>
-      <c r="C382" s="2"/>
-      <c r="D382" s="2"/>
-      <c r="F382" s="2"/>
-      <c r="G382" s="2"/>
+      <c r="B382" s="96" t="s">
+        <v>463</v>
+      </c>
+      <c r="C382" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D382" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E382" t="s">
+        <v>450</v>
+      </c>
+      <c r="F382" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G382" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H382" s="2"/>
-      <c r="I382" s="3"/>
-      <c r="J382" s="4"/>
+      <c r="I382" s="3">
+        <v>298</v>
+      </c>
+      <c r="J382" s="4">
+        <f t="shared" si="6"/>
+        <v>2628276000</v>
+      </c>
       <c r="K382" s="4"/>
-      <c r="L382" s="44"/>
+      <c r="L382" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M382" s="44"/>
-      <c r="N382" s="44"/>
-    </row>
-    <row r="383" spans="1:14" ht="18" customHeight="1">
+      <c r="N382" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="P382" s="6">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="383" spans="1:16" ht="18" customHeight="1">
       <c r="A383" s="44"/>
-      <c r="C383" s="2"/>
-      <c r="D383" s="2"/>
-      <c r="F383" s="2"/>
-      <c r="G383" s="2"/>
+      <c r="B383" s="96" t="s">
+        <v>464</v>
+      </c>
+      <c r="C383" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D383" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E383" t="s">
+        <v>450</v>
+      </c>
+      <c r="F383" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G383" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H383" s="2"/>
-      <c r="I383" s="3"/>
-      <c r="J383" s="4"/>
+      <c r="I383" s="3">
+        <v>298</v>
+      </c>
+      <c r="J383" s="4">
+        <f t="shared" si="6"/>
+        <v>2412522000</v>
+      </c>
       <c r="K383" s="4"/>
-      <c r="L383" s="44"/>
+      <c r="L383" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M383" s="44"/>
-      <c r="N383" s="44"/>
-    </row>
-    <row r="384" spans="1:14" ht="18" customHeight="1">
+      <c r="N383" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="P383" s="6">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="384" spans="1:16" ht="18" customHeight="1">
       <c r="A384" s="44"/>
-      <c r="C384" s="2"/>
-      <c r="D384" s="2"/>
-      <c r="F384" s="2"/>
-      <c r="G384" s="2"/>
+      <c r="B384" s="96" t="s">
+        <v>465</v>
+      </c>
+      <c r="C384" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D384" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E384" t="s">
+        <v>450</v>
+      </c>
+      <c r="F384" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G384" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H384" s="2"/>
-      <c r="I384" s="3"/>
-      <c r="J384" s="4"/>
+      <c r="I384" s="3">
+        <v>298</v>
+      </c>
+      <c r="J384" s="4">
+        <f t="shared" si="6"/>
+        <v>2177154000</v>
+      </c>
       <c r="K384" s="4"/>
-      <c r="L384" s="44"/>
+      <c r="L384" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M384" s="44"/>
-      <c r="N384" s="44"/>
+      <c r="N384" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="P384" s="6">
+        <v>222</v>
+      </c>
     </row>
     <row r="385" spans="1:14" ht="18" customHeight="1">
       <c r="A385" s="44"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.actamat.2019.12.020`; added extra data to `10.1016/j.jallcom.2024.175273`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC2B299-1765-A948-9F67-7CEB637E9B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633E6438-B589-6D44-9E7E-26197DA16F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10340" yWindow="760" windowWidth="24220" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3203" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3306" uniqueCount="481">
   <si>
     <t>Metadata</t>
   </si>
@@ -1480,9 +1480,6 @@
     <t>after arc melting samples were homogenized at 0.9 homologous temperature and water quenched then deformed by rotary swaging to 0.71 true strain then recrystallized at 0.9 homologous temperature and water quenched</t>
   </si>
   <si>
-    <t>AAM+H+WQ+RX</t>
-  </si>
-  <si>
     <t>Ni25(CuPdPt)25</t>
   </si>
   <si>
@@ -1529,6 +1526,48 @@
   </si>
   <si>
     <t>10.1016/j.jallcom.2024.175273</t>
+  </si>
+  <si>
+    <t>AuCuNiPdPt</t>
+  </si>
+  <si>
+    <t>AC+H+WQ</t>
+  </si>
+  <si>
+    <t>after arc melting samples were homogenized at 1100*C for 20h and water quenched</t>
+  </si>
+  <si>
+    <t>after arc melting samples were homogenized at 800*C for 20h and water quenched</t>
+  </si>
+  <si>
+    <t>after arc melting samples were homogenized at 900*C for 20h and water quenched; almost single phase</t>
+  </si>
+  <si>
+    <t>after arc melting samples were homogenized at 1000*C for 20h and water quenched</t>
+  </si>
+  <si>
+    <t>after arc melting samples were homogenized at 1100*C for 20h and water quenched  then deformed by rotary swaging to 0.6 true strain then recrystallized at 1100*C for 1h and water quenched</t>
+  </si>
+  <si>
+    <t>AAM+H+WQ+RX+WQ</t>
+  </si>
+  <si>
+    <t>P408</t>
+  </si>
+  <si>
+    <t>P409</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>hall-petch coefficient</t>
+  </si>
+  <si>
+    <t>Pa/m^0.5</t>
+  </si>
+  <si>
+    <t>10.1016/j.actamat.2019.12.020</t>
   </si>
 </sst>
 </file>
@@ -2748,8 +2787,8 @@
   </sheetPr>
   <dimension ref="A1:T424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B349" zoomScale="89" workbookViewId="0">
-      <selection activeCell="L394" sqref="L394"/>
+    <sheetView tabSelected="1" topLeftCell="A356" zoomScale="89" workbookViewId="0">
+      <selection activeCell="J400" sqref="J400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -15674,13 +15713,13 @@
     <row r="357" spans="1:14" ht="18" customHeight="1">
       <c r="A357" s="44"/>
       <c r="B357" s="96" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C357" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D357" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E357" t="s">
         <v>450</v>
@@ -15692,7 +15731,7 @@
         <v>29</v>
       </c>
       <c r="H357" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I357" s="3">
         <v>298</v>
@@ -15706,19 +15745,19 @@
       </c>
       <c r="M357" s="44"/>
       <c r="N357" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="358" spans="1:14" ht="18" customHeight="1">
       <c r="A358" s="44"/>
       <c r="B358" s="96" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C358" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D358" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E358" t="s">
         <v>450</v>
@@ -15730,7 +15769,7 @@
         <v>29</v>
       </c>
       <c r="H358" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I358" s="3">
         <v>298</v>
@@ -15744,19 +15783,19 @@
       </c>
       <c r="M358" s="44"/>
       <c r="N358" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="359" spans="1:14" ht="18" customHeight="1">
       <c r="A359" s="44"/>
       <c r="B359" s="96" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C359" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D359" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E359" t="s">
         <v>450</v>
@@ -15768,7 +15807,7 @@
         <v>29</v>
       </c>
       <c r="H359" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I359" s="3">
         <v>298</v>
@@ -15782,19 +15821,19 @@
       </c>
       <c r="M359" s="44"/>
       <c r="N359" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="360" spans="1:14" ht="18" customHeight="1">
       <c r="A360" s="44"/>
       <c r="B360" s="96" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C360" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D360" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E360" t="s">
         <v>450</v>
@@ -15806,7 +15845,7 @@
         <v>29</v>
       </c>
       <c r="H360" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I360" s="3">
         <v>298</v>
@@ -15820,19 +15859,19 @@
       </c>
       <c r="M360" s="44"/>
       <c r="N360" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="361" spans="1:14" ht="18" customHeight="1">
       <c r="A361" s="44"/>
       <c r="B361" s="96" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C361" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D361" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E361" t="s">
         <v>450</v>
@@ -15844,7 +15883,7 @@
         <v>29</v>
       </c>
       <c r="H361" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I361" s="3">
         <v>298</v>
@@ -15858,19 +15897,19 @@
       </c>
       <c r="M361" s="44"/>
       <c r="N361" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="362" spans="1:14" ht="18" customHeight="1">
       <c r="A362" s="44"/>
       <c r="B362" s="96" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D362" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E362" t="s">
         <v>450</v>
@@ -15882,7 +15921,7 @@
         <v>29</v>
       </c>
       <c r="H362" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I362" s="3">
         <v>298</v>
@@ -15896,19 +15935,19 @@
       </c>
       <c r="M362" s="44"/>
       <c r="N362" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="363" spans="1:14" ht="18" customHeight="1">
       <c r="A363" s="44"/>
       <c r="B363" s="96" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C363" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D363" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E363" t="s">
         <v>450</v>
@@ -15920,7 +15959,7 @@
         <v>29</v>
       </c>
       <c r="H363" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I363" s="3">
         <v>298</v>
@@ -15934,19 +15973,19 @@
       </c>
       <c r="M363" s="44"/>
       <c r="N363" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="364" spans="1:14" ht="18" customHeight="1">
       <c r="A364" s="44"/>
       <c r="B364" s="96" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D364" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E364" t="s">
         <v>450</v>
@@ -15958,7 +15997,7 @@
         <v>29</v>
       </c>
       <c r="H364" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I364" s="3">
         <v>298</v>
@@ -15972,19 +16011,19 @@
       </c>
       <c r="M364" s="44"/>
       <c r="N364" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="365" spans="1:14" ht="18" customHeight="1">
       <c r="A365" s="44"/>
       <c r="B365" s="96" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D365" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E365" t="s">
         <v>450</v>
@@ -15996,7 +16035,7 @@
         <v>29</v>
       </c>
       <c r="H365" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I365" s="3">
         <v>298</v>
@@ -16010,19 +16049,19 @@
       </c>
       <c r="M365" s="44"/>
       <c r="N365" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="366" spans="1:14" ht="18" customHeight="1">
       <c r="A366" s="44"/>
       <c r="B366" s="96" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C366" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D366" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E366" t="s">
         <v>450</v>
@@ -16034,7 +16073,7 @@
         <v>29</v>
       </c>
       <c r="H366" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I366" s="3">
         <v>298</v>
@@ -16048,19 +16087,19 @@
       </c>
       <c r="M366" s="44"/>
       <c r="N366" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="367" spans="1:14" ht="18" customHeight="1">
       <c r="A367" s="44"/>
       <c r="B367" s="96" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D367" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E367" t="s">
         <v>450</v>
@@ -16072,7 +16111,7 @@
         <v>29</v>
       </c>
       <c r="H367" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I367" s="3">
         <v>298</v>
@@ -16086,19 +16125,19 @@
       </c>
       <c r="M367" s="44"/>
       <c r="N367" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="368" spans="1:14" ht="18" customHeight="1">
       <c r="A368" s="44"/>
       <c r="B368" s="96" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C368" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D368" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E368" t="s">
         <v>450</v>
@@ -16110,7 +16149,7 @@
         <v>29</v>
       </c>
       <c r="H368" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I368" s="3">
         <v>298</v>
@@ -16124,19 +16163,19 @@
       </c>
       <c r="M368" s="44"/>
       <c r="N368" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="369" spans="1:16" ht="18" customHeight="1">
       <c r="A369" s="44"/>
       <c r="B369" s="96" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C369" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D369" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E369" t="s">
         <v>450</v>
@@ -16148,7 +16187,7 @@
         <v>29</v>
       </c>
       <c r="H369" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I369" s="3">
         <v>298</v>
@@ -16162,19 +16201,19 @@
       </c>
       <c r="M369" s="44"/>
       <c r="N369" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="370" spans="1:16" ht="18" customHeight="1">
       <c r="A370" s="44"/>
       <c r="B370" s="96" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C370" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D370" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E370" t="s">
         <v>450</v>
@@ -16186,7 +16225,7 @@
         <v>29</v>
       </c>
       <c r="H370" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I370" s="3">
         <v>298</v>
@@ -16200,19 +16239,19 @@
       </c>
       <c r="M370" s="44"/>
       <c r="N370" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="371" spans="1:16" ht="18" customHeight="1">
       <c r="A371" s="44"/>
       <c r="B371" s="96" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C371" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D371" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E371" t="s">
         <v>450</v>
@@ -16237,7 +16276,7 @@
       </c>
       <c r="M371" s="44"/>
       <c r="N371" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P371" s="6">
         <v>207</v>
@@ -16246,13 +16285,13 @@
     <row r="372" spans="1:16" ht="18" customHeight="1">
       <c r="A372" s="44"/>
       <c r="B372" s="96" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C372" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D372" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E372" t="s">
         <v>450</v>
@@ -16277,7 +16316,7 @@
       </c>
       <c r="M372" s="44"/>
       <c r="N372" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P372" s="6">
         <v>222</v>
@@ -16286,13 +16325,13 @@
     <row r="373" spans="1:16" ht="18" customHeight="1">
       <c r="A373" s="44"/>
       <c r="B373" s="96" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C373" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D373" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E373" t="s">
         <v>450</v>
@@ -16317,7 +16356,7 @@
       </c>
       <c r="M373" s="44"/>
       <c r="N373" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P373" s="6">
         <v>236</v>
@@ -16326,13 +16365,13 @@
     <row r="374" spans="1:16" ht="18" customHeight="1">
       <c r="A374" s="44"/>
       <c r="B374" s="96" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C374" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D374" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E374" t="s">
         <v>450</v>
@@ -16357,7 +16396,7 @@
       </c>
       <c r="M374" s="44"/>
       <c r="N374" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P374" s="6">
         <v>245</v>
@@ -16366,13 +16405,13 @@
     <row r="375" spans="1:16" ht="18" customHeight="1">
       <c r="A375" s="44"/>
       <c r="B375" s="96" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C375" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D375" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E375" t="s">
         <v>450</v>
@@ -16397,7 +16436,7 @@
       </c>
       <c r="M375" s="44"/>
       <c r="N375" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P375" s="6">
         <v>249</v>
@@ -16406,13 +16445,13 @@
     <row r="376" spans="1:16" ht="18" customHeight="1">
       <c r="A376" s="44"/>
       <c r="B376" s="96" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C376" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D376" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E376" t="s">
         <v>450</v>
@@ -16437,7 +16476,7 @@
       </c>
       <c r="M376" s="44"/>
       <c r="N376" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P376" s="6">
         <v>246</v>
@@ -16446,13 +16485,13 @@
     <row r="377" spans="1:16" ht="18" customHeight="1">
       <c r="A377" s="44"/>
       <c r="B377" s="96" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C377" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D377" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E377" t="s">
         <v>450</v>
@@ -16477,7 +16516,7 @@
       </c>
       <c r="M377" s="44"/>
       <c r="N377" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P377" s="6">
         <v>233</v>
@@ -16486,13 +16525,13 @@
     <row r="378" spans="1:16" ht="18" customHeight="1">
       <c r="A378" s="44"/>
       <c r="B378" s="96" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D378" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E378" t="s">
         <v>450</v>
@@ -16517,7 +16556,7 @@
       </c>
       <c r="M378" s="44"/>
       <c r="N378" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P378" s="6">
         <v>202</v>
@@ -16526,13 +16565,13 @@
     <row r="379" spans="1:16" ht="18" customHeight="1">
       <c r="A379" s="44"/>
       <c r="B379" s="96" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C379" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D379" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E379" t="s">
         <v>450</v>
@@ -16557,7 +16596,7 @@
       </c>
       <c r="M379" s="44"/>
       <c r="N379" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P379" s="6">
         <v>204</v>
@@ -16566,13 +16605,13 @@
     <row r="380" spans="1:16" ht="18" customHeight="1">
       <c r="A380" s="44"/>
       <c r="B380" s="96" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C380" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D380" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E380" t="s">
         <v>450</v>
@@ -16597,7 +16636,7 @@
       </c>
       <c r="M380" s="44"/>
       <c r="N380" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P380" s="6">
         <v>232</v>
@@ -16606,13 +16645,13 @@
     <row r="381" spans="1:16" ht="18" customHeight="1">
       <c r="A381" s="44"/>
       <c r="B381" s="96" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C381" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D381" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E381" t="s">
         <v>450</v>
@@ -16637,7 +16676,7 @@
       </c>
       <c r="M381" s="44"/>
       <c r="N381" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P381" s="6">
         <v>250</v>
@@ -16646,13 +16685,13 @@
     <row r="382" spans="1:16" ht="18" customHeight="1">
       <c r="A382" s="44"/>
       <c r="B382" s="96" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C382" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D382" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E382" t="s">
         <v>450</v>
@@ -16677,7 +16716,7 @@
       </c>
       <c r="M382" s="44"/>
       <c r="N382" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P382" s="6">
         <v>268</v>
@@ -16686,13 +16725,13 @@
     <row r="383" spans="1:16" ht="18" customHeight="1">
       <c r="A383" s="44"/>
       <c r="B383" s="96" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C383" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D383" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E383" t="s">
         <v>450</v>
@@ -16717,7 +16756,7 @@
       </c>
       <c r="M383" s="44"/>
       <c r="N383" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P383" s="6">
         <v>246</v>
@@ -16726,13 +16765,13 @@
     <row r="384" spans="1:16" ht="18" customHeight="1">
       <c r="A384" s="44"/>
       <c r="B384" s="96" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C384" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D384" s="2" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="E384" t="s">
         <v>450</v>
@@ -16757,44 +16796,104 @@
       </c>
       <c r="M384" s="44"/>
       <c r="N384" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P384" s="6">
         <v>222</v>
       </c>
     </row>
-    <row r="385" spans="1:14" ht="18" customHeight="1">
+    <row r="385" spans="1:16" ht="18" customHeight="1">
       <c r="A385" s="44"/>
-      <c r="C385" s="2"/>
-      <c r="D385" s="2"/>
-      <c r="F385" s="2"/>
-      <c r="G385" s="2"/>
-      <c r="H385" s="2"/>
-      <c r="I385" s="3"/>
-      <c r="J385" s="4"/>
-      <c r="K385" s="4"/>
-      <c r="L385" s="44"/>
-      <c r="M385" s="44"/>
-      <c r="N385" s="44"/>
-    </row>
-    <row r="386" spans="1:14" ht="18" customHeight="1">
+      <c r="B385" s="96" t="s">
+        <v>458</v>
+      </c>
+      <c r="C385" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D385" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E385" t="s">
+        <v>450</v>
+      </c>
+      <c r="F385" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="G385" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H385" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="I385" s="3">
+        <v>298</v>
+      </c>
+      <c r="J385" s="50">
+        <v>420000</v>
+      </c>
+      <c r="L385" s="44" t="s">
+        <v>479</v>
+      </c>
+      <c r="M385" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N385" s="44" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="386" spans="1:16" ht="18" customHeight="1">
       <c r="A386" s="44"/>
-      <c r="C386" s="2"/>
-      <c r="D386" s="2"/>
-      <c r="F386" s="2"/>
-      <c r="G386" s="2"/>
-      <c r="H386" s="2"/>
-      <c r="I386" s="3"/>
-      <c r="J386" s="4"/>
-      <c r="K386" s="4"/>
-      <c r="L386" s="44"/>
-      <c r="M386" s="44"/>
-      <c r="N386" s="44"/>
-    </row>
-    <row r="387" spans="1:14" ht="18" customHeight="1">
+      <c r="B386" s="96" t="s">
+        <v>461</v>
+      </c>
+      <c r="C386" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D386" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E386" t="s">
+        <v>450</v>
+      </c>
+      <c r="F386" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="G386" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H386" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="I386" s="3">
+        <v>298</v>
+      </c>
+      <c r="J386" s="50">
+        <v>328000</v>
+      </c>
+      <c r="L386" s="44" t="s">
+        <v>479</v>
+      </c>
+      <c r="M386" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N386" s="44" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="387" spans="1:16" ht="18" customHeight="1">
       <c r="A387" s="44"/>
-      <c r="C387" s="2"/>
-      <c r="D387" s="2"/>
+      <c r="B387" s="96" t="s">
+        <v>467</v>
+      </c>
+      <c r="C387" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D387" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E387" t="s">
+        <v>469</v>
+      </c>
       <c r="F387" s="2"/>
       <c r="G387" s="2"/>
       <c r="H387" s="2"/>
@@ -16803,12 +16902,24 @@
       <c r="K387" s="4"/>
       <c r="L387" s="44"/>
       <c r="M387" s="44"/>
-      <c r="N387" s="44"/>
-    </row>
-    <row r="388" spans="1:14" ht="18" customHeight="1">
+      <c r="N387" s="44" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="388" spans="1:16" ht="18" customHeight="1">
       <c r="A388" s="44"/>
-      <c r="C388" s="2"/>
-      <c r="D388" s="2"/>
+      <c r="B388" s="96" t="s">
+        <v>467</v>
+      </c>
+      <c r="C388" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D388" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E388" t="s">
+        <v>472</v>
+      </c>
       <c r="F388" s="2"/>
       <c r="G388" s="2"/>
       <c r="H388" s="2"/>
@@ -16817,12 +16928,24 @@
       <c r="K388" s="4"/>
       <c r="L388" s="44"/>
       <c r="M388" s="44"/>
-      <c r="N388" s="44"/>
-    </row>
-    <row r="389" spans="1:14" ht="18" customHeight="1">
+      <c r="N388" s="44" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="389" spans="1:16" ht="18" customHeight="1">
       <c r="A389" s="44"/>
-      <c r="C389" s="2"/>
-      <c r="D389" s="2"/>
+      <c r="B389" s="96" t="s">
+        <v>467</v>
+      </c>
+      <c r="C389" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D389" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E389" t="s">
+        <v>471</v>
+      </c>
       <c r="F389" s="2"/>
       <c r="G389" s="2"/>
       <c r="H389" s="2"/>
@@ -16831,12 +16954,24 @@
       <c r="K389" s="4"/>
       <c r="L389" s="44"/>
       <c r="M389" s="44"/>
-      <c r="N389" s="44"/>
-    </row>
-    <row r="390" spans="1:14" ht="18" customHeight="1">
+      <c r="N389" s="44" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="390" spans="1:16" ht="18" customHeight="1">
       <c r="A390" s="44"/>
-      <c r="C390" s="2"/>
-      <c r="D390" s="2"/>
+      <c r="B390" s="96" t="s">
+        <v>467</v>
+      </c>
+      <c r="C390" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D390" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E390" t="s">
+        <v>470</v>
+      </c>
       <c r="F390" s="2"/>
       <c r="G390" s="2"/>
       <c r="H390" s="2"/>
@@ -16845,107 +16980,283 @@
       <c r="K390" s="4"/>
       <c r="L390" s="44"/>
       <c r="M390" s="44"/>
-      <c r="N390" s="44"/>
-    </row>
-    <row r="391" spans="1:14" ht="18" customHeight="1">
+      <c r="N390" s="44" t="s">
+        <v>480</v>
+      </c>
+      <c r="P390" s="6">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="391" spans="1:16" ht="18" customHeight="1">
       <c r="A391" s="44"/>
-      <c r="C391" s="2"/>
-      <c r="D391" s="2"/>
-      <c r="F391" s="2"/>
-      <c r="G391" s="2"/>
+      <c r="B391" s="96" t="s">
+        <v>467</v>
+      </c>
+      <c r="C391" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D391" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E391" t="s">
+        <v>473</v>
+      </c>
+      <c r="F391" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G391" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H391" s="2"/>
-      <c r="I391" s="3"/>
-      <c r="J391" s="4"/>
-      <c r="K391" s="4"/>
-      <c r="L391" s="44"/>
-      <c r="M391" s="44"/>
-      <c r="N391" s="44"/>
-    </row>
-    <row r="392" spans="1:14" ht="18" customHeight="1">
+      <c r="I391" s="3">
+        <v>298</v>
+      </c>
+      <c r="J391" s="4">
+        <v>820000000</v>
+      </c>
+      <c r="K391" s="4">
+        <v>15000000</v>
+      </c>
+      <c r="L391" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M391" s="44" t="s">
+        <v>475</v>
+      </c>
+      <c r="N391" s="44" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="392" spans="1:16" ht="18" customHeight="1">
       <c r="A392" s="44"/>
-      <c r="C392" s="2"/>
-      <c r="D392" s="2"/>
-      <c r="F392" s="2"/>
-      <c r="G392" s="2"/>
+      <c r="B392" s="96" t="s">
+        <v>467</v>
+      </c>
+      <c r="C392" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D392" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E392" t="s">
+        <v>473</v>
+      </c>
+      <c r="F392" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G392" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H392" s="2"/>
-      <c r="I392" s="3"/>
-      <c r="J392" s="4"/>
+      <c r="I392" s="3">
+        <v>298</v>
+      </c>
+      <c r="J392" s="4">
+        <f>P390*9807000</f>
+        <v>3383415000</v>
+      </c>
       <c r="K392" s="4"/>
-      <c r="L392" s="44"/>
-      <c r="M392" s="44"/>
-      <c r="N392" s="44"/>
-    </row>
-    <row r="393" spans="1:14" ht="18" customHeight="1">
+      <c r="L392" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M392" s="44" t="s">
+        <v>475</v>
+      </c>
+      <c r="N392" s="44" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="393" spans="1:16" ht="18" customHeight="1">
       <c r="A393" s="44"/>
-      <c r="C393" s="2"/>
-      <c r="D393" s="2"/>
-      <c r="F393" s="2"/>
-      <c r="G393" s="2"/>
+      <c r="B393" s="96" t="s">
+        <v>467</v>
+      </c>
+      <c r="C393" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D393" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E393" t="s">
+        <v>473</v>
+      </c>
+      <c r="F393" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G393" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H393" s="2"/>
-      <c r="I393" s="3"/>
-      <c r="J393" s="4"/>
+      <c r="I393" s="3">
+        <v>298</v>
+      </c>
+      <c r="J393" s="4">
+        <v>830000000</v>
+      </c>
       <c r="K393" s="4"/>
-      <c r="L393" s="44"/>
-      <c r="M393" s="44"/>
-      <c r="N393" s="44"/>
-    </row>
-    <row r="394" spans="1:14" ht="18" customHeight="1">
+      <c r="L393" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M393" s="44" t="s">
+        <v>475</v>
+      </c>
+      <c r="N393" s="44" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="394" spans="1:16" ht="18" customHeight="1">
       <c r="A394" s="44"/>
-      <c r="C394" s="2"/>
-      <c r="D394" s="2"/>
-      <c r="F394" s="2"/>
-      <c r="G394" s="2"/>
+      <c r="B394" s="96" t="s">
+        <v>467</v>
+      </c>
+      <c r="C394" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D394" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E394" t="s">
+        <v>473</v>
+      </c>
+      <c r="F394" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G394" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H394" s="2"/>
-      <c r="I394" s="3"/>
-      <c r="J394" s="4"/>
+      <c r="I394" s="3">
+        <v>298</v>
+      </c>
+      <c r="J394" s="4">
+        <v>1200000000</v>
+      </c>
       <c r="K394" s="4"/>
-      <c r="L394" s="44"/>
-      <c r="M394" s="44"/>
-      <c r="N394" s="44"/>
-    </row>
-    <row r="395" spans="1:14" ht="18" customHeight="1">
+      <c r="L394" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M394" s="44" t="s">
+        <v>475</v>
+      </c>
+      <c r="N394" s="44" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="395" spans="1:16" ht="18" customHeight="1">
       <c r="A395" s="44"/>
-      <c r="C395" s="2"/>
-      <c r="D395" s="2"/>
-      <c r="F395" s="2"/>
-      <c r="G395" s="2"/>
+      <c r="B395" s="96" t="s">
+        <v>467</v>
+      </c>
+      <c r="C395" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D395" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E395" t="s">
+        <v>473</v>
+      </c>
+      <c r="F395" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="G395" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H395" s="2"/>
-      <c r="I395" s="3"/>
-      <c r="J395" s="4"/>
+      <c r="I395" s="3">
+        <v>298</v>
+      </c>
+      <c r="J395" s="4">
+        <v>50</v>
+      </c>
       <c r="K395" s="4"/>
-      <c r="L395" s="44"/>
-      <c r="M395" s="44"/>
-      <c r="N395" s="44"/>
-    </row>
-    <row r="396" spans="1:14" ht="18" customHeight="1">
+      <c r="L395" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M395" s="44" t="s">
+        <v>477</v>
+      </c>
+      <c r="N395" s="44" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="396" spans="1:16" ht="18" customHeight="1">
       <c r="A396" s="44"/>
-      <c r="C396" s="2"/>
-      <c r="D396" s="2"/>
-      <c r="F396" s="2"/>
-      <c r="G396" s="2"/>
+      <c r="B396" s="96" t="s">
+        <v>467</v>
+      </c>
+      <c r="C396" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D396" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E396" t="s">
+        <v>473</v>
+      </c>
+      <c r="F396" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G396" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H396" s="2"/>
-      <c r="I396" s="3"/>
-      <c r="J396" s="4"/>
+      <c r="I396" s="3">
+        <v>298</v>
+      </c>
+      <c r="J396" s="4">
+        <v>15</v>
+      </c>
       <c r="K396" s="4"/>
-      <c r="L396" s="44"/>
-      <c r="M396" s="44"/>
-      <c r="N396" s="44"/>
-    </row>
-    <row r="397" spans="1:14" ht="18" customHeight="1">
+      <c r="L396" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M396" s="44" t="s">
+        <v>477</v>
+      </c>
+      <c r="N396" s="44" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="397" spans="1:16" ht="18" customHeight="1">
       <c r="A397" s="44"/>
-      <c r="C397" s="2"/>
-      <c r="D397" s="2"/>
-      <c r="F397" s="2"/>
-      <c r="G397" s="2"/>
+      <c r="B397" s="96" t="s">
+        <v>467</v>
+      </c>
+      <c r="C397" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D397" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E397" t="s">
+        <v>473</v>
+      </c>
+      <c r="F397" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="G397" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H397" s="2"/>
-      <c r="I397" s="3"/>
-      <c r="J397" s="4"/>
+      <c r="I397" s="3">
+        <v>298</v>
+      </c>
+      <c r="J397" s="4">
+        <v>675000</v>
+      </c>
       <c r="K397" s="4"/>
-      <c r="L397" s="44"/>
-      <c r="M397" s="44"/>
-      <c r="N397" s="44"/>
-    </row>
-    <row r="398" spans="1:14" ht="18" customHeight="1">
+      <c r="L397" s="44" t="s">
+        <v>479</v>
+      </c>
+      <c r="M397" s="44" t="s">
+        <v>476</v>
+      </c>
+      <c r="N397" s="44" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="398" spans="1:16" ht="18" customHeight="1">
       <c r="A398" s="44"/>
       <c r="C398" s="2"/>
       <c r="D398" s="2"/>
@@ -16959,7 +17270,7 @@
       <c r="M398" s="44"/>
       <c r="N398" s="44"/>
     </row>
-    <row r="399" spans="1:14" ht="18" customHeight="1">
+    <row r="399" spans="1:16" ht="18" customHeight="1">
       <c r="A399" s="44"/>
       <c r="C399" s="2"/>
       <c r="D399" s="2"/>
@@ -16973,7 +17284,7 @@
       <c r="M399" s="44"/>
       <c r="N399" s="44"/>
     </row>
-    <row r="400" spans="1:14" ht="18" customHeight="1">
+    <row r="400" spans="1:16" ht="18" customHeight="1">
       <c r="A400" s="44"/>
       <c r="C400" s="2"/>
       <c r="D400" s="2"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.msea.2022.144271`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633E6438-B589-6D44-9E7E-26197DA16F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5261CCC8-FB81-E24C-B889-D566217EC501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3306" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3946" uniqueCount="522">
   <si>
     <t>Metadata</t>
   </si>
@@ -1568,6 +1568,129 @@
   </si>
   <si>
     <t>10.1016/j.actamat.2019.12.020</t>
+  </si>
+  <si>
+    <t>after arc melting samples were homogenized at 0.9 homologous temperature and water quenched then deformed by rotary swaging to 0.6 true strain then recrystallized at 0.9 homologous temperature and water quenched</t>
+  </si>
+  <si>
+    <t>CuNiPdPt</t>
+  </si>
+  <si>
+    <t>(CuNiPdPt)24.75 Au1</t>
+  </si>
+  <si>
+    <t>(CuNiPdPt)24.25 Au3</t>
+  </si>
+  <si>
+    <t>(CuNiPdPt)23.75 Au5</t>
+  </si>
+  <si>
+    <t>(CuNiPdPt)23.25 Au7</t>
+  </si>
+  <si>
+    <t>(CuNiPdPt)22.5 Au10</t>
+  </si>
+  <si>
+    <t>(CuNiPdPt)21.25 Au15</t>
+  </si>
+  <si>
+    <t>(CuNiPdPt)20 Au20</t>
+  </si>
+  <si>
+    <t>(AuCuPdPt)24.75 Ni1</t>
+  </si>
+  <si>
+    <t>Au</t>
+  </si>
+  <si>
+    <t>(AuCuPdPt)24.25 Ni3</t>
+  </si>
+  <si>
+    <t>(AuCuPdPt)23.75 Ni5</t>
+  </si>
+  <si>
+    <t>(AuCuPdPt)23.25 Ni7</t>
+  </si>
+  <si>
+    <t>(AuCuPdPt)22.5 Ni10</t>
+  </si>
+  <si>
+    <t>(AuCuPdPt)21.25 Ni15</t>
+  </si>
+  <si>
+    <t>(AuCuPdPt)20 Ni20</t>
+  </si>
+  <si>
+    <t>Ni</t>
+  </si>
+  <si>
+    <t>AuCuPdPt</t>
+  </si>
+  <si>
+    <t>AuCuNiPt</t>
+  </si>
+  <si>
+    <t>Pd</t>
+  </si>
+  <si>
+    <t>(AuCuNiPt)24.75 Pd1</t>
+  </si>
+  <si>
+    <t>(AuCuNiPt)24.25 Pd3</t>
+  </si>
+  <si>
+    <t>(AuCuNiPt)23.75 Pd5</t>
+  </si>
+  <si>
+    <t>(AuCuNiPt)23.25 Pd7</t>
+  </si>
+  <si>
+    <t>(AuCuNiPt)22.5 Pd10</t>
+  </si>
+  <si>
+    <t>(AuCuNiPt)21.25 Pd15</t>
+  </si>
+  <si>
+    <t>(AuCuNiPt)20 Pd20</t>
+  </si>
+  <si>
+    <t>AuCuNiPd</t>
+  </si>
+  <si>
+    <t>Pt</t>
+  </si>
+  <si>
+    <t>(AuCuNiPd)24.75 Pt1</t>
+  </si>
+  <si>
+    <t>(AuCuNiPd)24.25 Pt3</t>
+  </si>
+  <si>
+    <t>(AuCuNiPd)23.75 Pt5</t>
+  </si>
+  <si>
+    <t>(AuCuNiPd)23.25 Pt7</t>
+  </si>
+  <si>
+    <t>(AuCuNiPd)22.5 Pt10</t>
+  </si>
+  <si>
+    <t>(AuCuNiPd)21.25 Pt15</t>
+  </si>
+  <si>
+    <t>(AuCuNiPd)20 Pt20</t>
+  </si>
+  <si>
+    <t>F5a</t>
+  </si>
+  <si>
+    <t>F5c</t>
+  </si>
+  <si>
+    <t>F6a</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2022.144271</t>
   </si>
 </sst>
 </file>
@@ -2785,10 +2908,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T424"/>
+  <dimension ref="A1:T461"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A356" zoomScale="89" workbookViewId="0">
-      <selection activeCell="J400" sqref="J400"/>
+    <sheetView tabSelected="1" topLeftCell="A417" zoomScale="89" workbookViewId="0">
+      <selection activeCell="O458" sqref="O458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -16983,9 +17106,6 @@
       <c r="N390" s="44" t="s">
         <v>480</v>
       </c>
-      <c r="P390" s="6">
-        <v>345</v>
-      </c>
     </row>
     <row r="391" spans="1:16" ht="18" customHeight="1">
       <c r="A391" s="44"/>
@@ -17052,7 +17172,7 @@
         <v>298</v>
       </c>
       <c r="J392" s="4">
-        <f>P390*9807000</f>
+        <f>P392*9807000</f>
         <v>3383415000</v>
       </c>
       <c r="K392" s="4"/>
@@ -17064,6 +17184,9 @@
       </c>
       <c r="N392" s="44" t="s">
         <v>480</v>
+      </c>
+      <c r="P392" s="6">
+        <v>345</v>
       </c>
     </row>
     <row r="393" spans="1:16" ht="18" customHeight="1">
@@ -17257,382 +17380,2820 @@
       </c>
     </row>
     <row r="398" spans="1:16" ht="18" customHeight="1">
-      <c r="A398" s="44"/>
-      <c r="C398" s="2"/>
-      <c r="D398" s="2"/>
-      <c r="F398" s="2"/>
-      <c r="G398" s="2"/>
+      <c r="A398" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B398" s="96" t="s">
+        <v>482</v>
+      </c>
+      <c r="C398" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D398" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E398" t="s">
+        <v>481</v>
+      </c>
+      <c r="F398" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G398" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H398" s="2"/>
-      <c r="I398" s="3"/>
-      <c r="J398" s="4"/>
+      <c r="I398" s="3">
+        <v>298</v>
+      </c>
+      <c r="J398" s="4">
+        <f>P398*1000000</f>
+        <v>373396674.58432305</v>
+      </c>
       <c r="K398" s="4"/>
-      <c r="L398" s="44"/>
-      <c r="M398" s="44"/>
-      <c r="N398" s="44"/>
+      <c r="L398" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M398" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N398" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P398" s="6">
+        <v>373.39667458432302</v>
+      </c>
     </row>
     <row r="399" spans="1:16" ht="18" customHeight="1">
-      <c r="A399" s="44"/>
-      <c r="C399" s="2"/>
-      <c r="D399" s="2"/>
-      <c r="F399" s="2"/>
-      <c r="G399" s="2"/>
+      <c r="A399" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B399" s="96" t="s">
+        <v>483</v>
+      </c>
+      <c r="C399" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D399" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E399" t="s">
+        <v>481</v>
+      </c>
+      <c r="F399" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G399" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H399" s="2"/>
-      <c r="I399" s="3"/>
-      <c r="J399" s="4"/>
+      <c r="I399" s="3">
+        <v>298</v>
+      </c>
+      <c r="J399" s="4">
+        <f t="shared" ref="J399:J405" si="7">P399*1000000</f>
+        <v>400000000</v>
+      </c>
       <c r="K399" s="4"/>
-      <c r="L399" s="44"/>
-      <c r="M399" s="44"/>
-      <c r="N399" s="44"/>
+      <c r="L399" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M399" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N399" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P399" s="6">
+        <v>400</v>
+      </c>
     </row>
     <row r="400" spans="1:16" ht="18" customHeight="1">
-      <c r="A400" s="44"/>
-      <c r="C400" s="2"/>
-      <c r="D400" s="2"/>
-      <c r="F400" s="2"/>
-      <c r="G400" s="2"/>
+      <c r="A400" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B400" s="96" t="s">
+        <v>484</v>
+      </c>
+      <c r="C400" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D400" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E400" t="s">
+        <v>481</v>
+      </c>
+      <c r="F400" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G400" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H400" s="2"/>
-      <c r="I400" s="3"/>
-      <c r="J400" s="4"/>
+      <c r="I400" s="3">
+        <v>298</v>
+      </c>
+      <c r="J400" s="4">
+        <f t="shared" si="7"/>
+        <v>449406175.77197099</v>
+      </c>
       <c r="K400" s="4"/>
-      <c r="L400" s="44"/>
-      <c r="M400" s="44"/>
-      <c r="N400" s="44"/>
-    </row>
-    <row r="401" spans="1:14" ht="18" customHeight="1">
-      <c r="A401" s="44"/>
-      <c r="C401" s="2"/>
-      <c r="D401" s="2"/>
-      <c r="F401" s="2"/>
-      <c r="G401" s="2"/>
+      <c r="L400" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M400" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N400" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P400" s="6">
+        <v>449.40617577197099</v>
+      </c>
+    </row>
+    <row r="401" spans="1:16" ht="18" customHeight="1">
+      <c r="A401" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B401" s="96" t="s">
+        <v>485</v>
+      </c>
+      <c r="C401" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D401" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E401" t="s">
+        <v>481</v>
+      </c>
+      <c r="F401" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G401" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H401" s="2"/>
-      <c r="I401" s="3"/>
-      <c r="J401" s="4"/>
+      <c r="I401" s="3">
+        <v>298</v>
+      </c>
+      <c r="J401" s="4">
+        <f t="shared" si="7"/>
+        <v>502612826.60332501</v>
+      </c>
       <c r="K401" s="4"/>
-      <c r="L401" s="44"/>
-      <c r="M401" s="44"/>
-      <c r="N401" s="44"/>
-    </row>
-    <row r="402" spans="1:14" ht="18" customHeight="1">
-      <c r="A402" s="44"/>
-      <c r="C402" s="2"/>
-      <c r="D402" s="2"/>
-      <c r="F402" s="2"/>
-      <c r="G402" s="2"/>
+      <c r="L401" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M401" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N401" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P401" s="6">
+        <v>502.612826603325</v>
+      </c>
+    </row>
+    <row r="402" spans="1:16" ht="18" customHeight="1">
+      <c r="A402" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B402" s="96" t="s">
+        <v>486</v>
+      </c>
+      <c r="C402" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D402" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E402" t="s">
+        <v>481</v>
+      </c>
+      <c r="F402" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G402" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H402" s="2"/>
-      <c r="I402" s="3"/>
-      <c r="J402" s="4"/>
+      <c r="I402" s="3">
+        <v>298</v>
+      </c>
+      <c r="J402" s="4">
+        <f t="shared" si="7"/>
+        <v>559619952.49406099</v>
+      </c>
       <c r="K402" s="4"/>
-      <c r="L402" s="44"/>
-      <c r="M402" s="44"/>
-      <c r="N402" s="44"/>
-    </row>
-    <row r="403" spans="1:14" ht="18" customHeight="1">
-      <c r="A403" s="44"/>
-      <c r="C403" s="2"/>
-      <c r="D403" s="2"/>
-      <c r="F403" s="2"/>
-      <c r="G403" s="2"/>
+      <c r="L402" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M402" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N402" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P402" s="6">
+        <v>559.61995249406095</v>
+      </c>
+    </row>
+    <row r="403" spans="1:16" ht="18" customHeight="1">
+      <c r="A403" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B403" s="96" t="s">
+        <v>487</v>
+      </c>
+      <c r="C403" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D403" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E403" t="s">
+        <v>481</v>
+      </c>
+      <c r="F403" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G403" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H403" s="2"/>
-      <c r="I403" s="3"/>
-      <c r="J403" s="4"/>
+      <c r="I403" s="3">
+        <v>298</v>
+      </c>
+      <c r="J403" s="4">
+        <f t="shared" si="7"/>
+        <v>616627078.38479793</v>
+      </c>
       <c r="K403" s="4"/>
-      <c r="L403" s="44"/>
-      <c r="M403" s="44"/>
-      <c r="N403" s="44"/>
-    </row>
-    <row r="404" spans="1:14" ht="18" customHeight="1">
-      <c r="A404" s="44"/>
-      <c r="C404" s="2"/>
-      <c r="D404" s="2"/>
-      <c r="F404" s="2"/>
-      <c r="G404" s="2"/>
+      <c r="L403" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M403" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N403" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P403" s="6">
+        <v>616.62707838479798</v>
+      </c>
+    </row>
+    <row r="404" spans="1:16" ht="18" customHeight="1">
+      <c r="A404" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B404" s="96" t="s">
+        <v>488</v>
+      </c>
+      <c r="C404" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D404" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E404" t="s">
+        <v>481</v>
+      </c>
+      <c r="F404" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G404" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H404" s="2"/>
-      <c r="I404" s="3"/>
-      <c r="J404" s="4"/>
+      <c r="I404" s="3">
+        <v>298</v>
+      </c>
+      <c r="J404" s="4">
+        <f t="shared" si="7"/>
+        <v>715439429.92874098</v>
+      </c>
       <c r="K404" s="4"/>
-      <c r="L404" s="44"/>
-      <c r="M404" s="44"/>
-      <c r="N404" s="44"/>
-    </row>
-    <row r="405" spans="1:14" ht="18" customHeight="1">
-      <c r="A405" s="44"/>
-      <c r="C405" s="2"/>
-      <c r="D405" s="2"/>
-      <c r="F405" s="2"/>
-      <c r="G405" s="2"/>
+      <c r="L404" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M404" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N404" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P404" s="6">
+        <v>715.43942992874099</v>
+      </c>
+    </row>
+    <row r="405" spans="1:16" ht="18" customHeight="1">
+      <c r="A405" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B405" s="96" t="s">
+        <v>489</v>
+      </c>
+      <c r="C405" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D405" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E405" t="s">
+        <v>481</v>
+      </c>
+      <c r="F405" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G405" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H405" s="2"/>
-      <c r="I405" s="3"/>
-      <c r="J405" s="4"/>
+      <c r="I405" s="3">
+        <v>298</v>
+      </c>
+      <c r="J405" s="4">
+        <f t="shared" si="7"/>
+        <v>869358669.83372903</v>
+      </c>
       <c r="K405" s="4"/>
-      <c r="L405" s="44"/>
-      <c r="M405" s="44"/>
-      <c r="N405" s="44"/>
-    </row>
-    <row r="406" spans="1:14" ht="18" customHeight="1">
-      <c r="A406" s="44"/>
-      <c r="C406" s="2"/>
-      <c r="D406" s="2"/>
-      <c r="F406" s="2"/>
-      <c r="G406" s="2"/>
+      <c r="L405" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M405" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N405" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P405" s="6">
+        <v>869.35866983372898</v>
+      </c>
+    </row>
+    <row r="406" spans="1:16" ht="18" customHeight="1">
+      <c r="A406" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B406" s="96" t="s">
+        <v>482</v>
+      </c>
+      <c r="C406" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D406" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E406" t="s">
+        <v>481</v>
+      </c>
+      <c r="F406" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G406" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H406" s="2"/>
-      <c r="I406" s="3"/>
-      <c r="J406" s="4"/>
+      <c r="I406" s="3">
+        <v>298</v>
+      </c>
+      <c r="J406" s="4">
+        <f>P406*9807000</f>
+        <v>1967587381.7034659</v>
+      </c>
       <c r="K406" s="4"/>
-      <c r="L406" s="44"/>
-      <c r="M406" s="44"/>
-      <c r="N406" s="44"/>
-    </row>
-    <row r="407" spans="1:14" ht="18" customHeight="1">
-      <c r="A407" s="44"/>
-      <c r="C407" s="2"/>
-      <c r="D407" s="2"/>
-      <c r="F407" s="2"/>
-      <c r="G407" s="2"/>
+      <c r="L406" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M406" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N406" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P406" s="6">
+        <v>200.63091482649801</v>
+      </c>
+    </row>
+    <row r="407" spans="1:16" ht="18" customHeight="1">
+      <c r="A407" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B407" s="96" t="s">
+        <v>483</v>
+      </c>
+      <c r="C407" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D407" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E407" t="s">
+        <v>481</v>
+      </c>
+      <c r="F407" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G407" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H407" s="2"/>
-      <c r="I407" s="3"/>
-      <c r="J407" s="4"/>
+      <c r="I407" s="3">
+        <v>298</v>
+      </c>
+      <c r="J407" s="4">
+        <f t="shared" ref="J407:J413" si="8">P407*9807000</f>
+        <v>2029461198.7381639</v>
+      </c>
       <c r="K407" s="4"/>
-      <c r="L407" s="44"/>
-      <c r="M407" s="44"/>
-      <c r="N407" s="44"/>
-    </row>
-    <row r="408" spans="1:14" ht="18" customHeight="1">
-      <c r="A408" s="44"/>
-      <c r="C408" s="2"/>
-      <c r="D408" s="2"/>
-      <c r="F408" s="2"/>
-      <c r="G408" s="2"/>
+      <c r="L407" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M407" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N407" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P407" s="6">
+        <v>206.94006309148199</v>
+      </c>
+    </row>
+    <row r="408" spans="1:16" ht="18" customHeight="1">
+      <c r="A408" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B408" s="96" t="s">
+        <v>484</v>
+      </c>
+      <c r="C408" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D408" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E408" t="s">
+        <v>481</v>
+      </c>
+      <c r="F408" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G408" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H408" s="2"/>
-      <c r="I408" s="3"/>
-      <c r="J408" s="4"/>
+      <c r="I408" s="3">
+        <v>298</v>
+      </c>
+      <c r="J408" s="4">
+        <f t="shared" si="8"/>
+        <v>2215082649.842268</v>
+      </c>
       <c r="K408" s="4"/>
-      <c r="L408" s="44"/>
-      <c r="M408" s="44"/>
-      <c r="N408" s="44"/>
-    </row>
-    <row r="409" spans="1:14" ht="18" customHeight="1">
-      <c r="A409" s="44"/>
-      <c r="C409" s="2"/>
-      <c r="D409" s="2"/>
-      <c r="F409" s="2"/>
-      <c r="G409" s="2"/>
+      <c r="L408" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M408" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N408" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P408" s="6">
+        <v>225.86750788643499</v>
+      </c>
+    </row>
+    <row r="409" spans="1:16" ht="18" customHeight="1">
+      <c r="A409" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B409" s="96" t="s">
+        <v>485</v>
+      </c>
+      <c r="C409" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D409" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E409" t="s">
+        <v>481</v>
+      </c>
+      <c r="F409" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G409" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H409" s="2"/>
-      <c r="I409" s="3"/>
-      <c r="J409" s="4"/>
+      <c r="I409" s="3">
+        <v>298</v>
+      </c>
+      <c r="J409" s="4">
+        <f t="shared" si="8"/>
+        <v>2363579810.7255473</v>
+      </c>
       <c r="K409" s="4"/>
-      <c r="L409" s="44"/>
-      <c r="M409" s="44"/>
-      <c r="N409" s="44"/>
-    </row>
-    <row r="410" spans="1:14" ht="18" customHeight="1">
-      <c r="A410" s="44"/>
-      <c r="C410" s="2"/>
-      <c r="D410" s="2"/>
-      <c r="F410" s="2"/>
-      <c r="G410" s="2"/>
+      <c r="L409" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M409" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N409" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P409" s="6">
+        <v>241.00946372239699</v>
+      </c>
+    </row>
+    <row r="410" spans="1:16" ht="18" customHeight="1">
+      <c r="A410" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B410" s="96" t="s">
+        <v>486</v>
+      </c>
+      <c r="C410" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D410" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E410" t="s">
+        <v>481</v>
+      </c>
+      <c r="F410" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G410" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H410" s="2"/>
-      <c r="I410" s="3"/>
-      <c r="J410" s="4"/>
+      <c r="I410" s="3">
+        <v>298</v>
+      </c>
+      <c r="J410" s="4">
+        <f t="shared" si="8"/>
+        <v>2536826498.4227099</v>
+      </c>
       <c r="K410" s="4"/>
-      <c r="L410" s="44"/>
-      <c r="M410" s="44"/>
-      <c r="N410" s="44"/>
-    </row>
-    <row r="411" spans="1:14" ht="18" customHeight="1">
-      <c r="A411" s="44"/>
-      <c r="C411" s="2"/>
-      <c r="D411" s="2"/>
-      <c r="F411" s="2"/>
-      <c r="G411" s="2"/>
+      <c r="L410" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M410" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N410" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P410" s="6">
+        <v>258.675078864353</v>
+      </c>
+    </row>
+    <row r="411" spans="1:16" ht="18" customHeight="1">
+      <c r="A411" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B411" s="96" t="s">
+        <v>487</v>
+      </c>
+      <c r="C411" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D411" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E411" t="s">
+        <v>481</v>
+      </c>
+      <c r="F411" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G411" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H411" s="2"/>
-      <c r="I411" s="3"/>
-      <c r="J411" s="4"/>
+      <c r="I411" s="3">
+        <v>298</v>
+      </c>
+      <c r="J411" s="4">
+        <f t="shared" si="8"/>
+        <v>2747197476.3406873</v>
+      </c>
       <c r="K411" s="4"/>
-      <c r="L411" s="44"/>
-      <c r="M411" s="44"/>
-      <c r="N411" s="44"/>
-    </row>
-    <row r="412" spans="1:14" ht="18" customHeight="1">
-      <c r="A412" s="44"/>
-      <c r="C412" s="2"/>
-      <c r="D412" s="2"/>
-      <c r="F412" s="2"/>
-      <c r="G412" s="2"/>
+      <c r="L411" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M411" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N411" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P411" s="6">
+        <v>280.12618296529899</v>
+      </c>
+    </row>
+    <row r="412" spans="1:16" ht="18" customHeight="1">
+      <c r="A412" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B412" s="96" t="s">
+        <v>488</v>
+      </c>
+      <c r="C412" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D412" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E412" t="s">
+        <v>481</v>
+      </c>
+      <c r="F412" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G412" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H412" s="2"/>
-      <c r="I412" s="3"/>
-      <c r="J412" s="4"/>
+      <c r="I412" s="3">
+        <v>298</v>
+      </c>
+      <c r="J412" s="4">
+        <f t="shared" si="8"/>
+        <v>3174126813.8801179</v>
+      </c>
       <c r="K412" s="4"/>
-      <c r="L412" s="44"/>
-      <c r="M412" s="44"/>
-      <c r="N412" s="44"/>
-    </row>
-    <row r="413" spans="1:14" ht="18" customHeight="1">
-      <c r="A413" s="44"/>
-      <c r="C413" s="2"/>
-      <c r="D413" s="2"/>
-      <c r="F413" s="2"/>
-      <c r="G413" s="2"/>
+      <c r="L412" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M412" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N412" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P412" s="6">
+        <v>323.65930599369</v>
+      </c>
+    </row>
+    <row r="413" spans="1:16" ht="18" customHeight="1">
+      <c r="A413" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="B413" s="96" t="s">
+        <v>489</v>
+      </c>
+      <c r="C413" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D413" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E413" t="s">
+        <v>481</v>
+      </c>
+      <c r="F413" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G413" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H413" s="2"/>
-      <c r="I413" s="3"/>
-      <c r="J413" s="4"/>
+      <c r="I413" s="3">
+        <v>298</v>
+      </c>
+      <c r="J413" s="4">
+        <f t="shared" si="8"/>
+        <v>3464933753.9432106</v>
+      </c>
       <c r="K413" s="4"/>
-      <c r="L413" s="44"/>
-      <c r="M413" s="44"/>
-      <c r="N413" s="44"/>
-    </row>
-    <row r="414" spans="1:14" ht="18" customHeight="1">
-      <c r="A414" s="44"/>
-      <c r="C414" s="2"/>
-      <c r="D414" s="2"/>
-      <c r="F414" s="2"/>
-      <c r="G414" s="2"/>
+      <c r="L413" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M413" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="N413" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P413" s="6">
+        <v>353.312302839116</v>
+      </c>
+    </row>
+    <row r="414" spans="1:16" ht="18" customHeight="1">
+      <c r="A414" s="47" t="s">
+        <v>498</v>
+      </c>
+      <c r="B414" s="96" t="s">
+        <v>499</v>
+      </c>
+      <c r="C414" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D414" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E414" t="s">
+        <v>481</v>
+      </c>
+      <c r="F414" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G414" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H414" s="2"/>
-      <c r="I414" s="3"/>
-      <c r="J414" s="4"/>
+      <c r="I414" s="3">
+        <v>298</v>
+      </c>
+      <c r="J414" s="4">
+        <f t="shared" ref="J414:J421" si="9">P414*1000000</f>
+        <v>421641791.04477602</v>
+      </c>
       <c r="K414" s="4"/>
-      <c r="L414" s="44"/>
-      <c r="M414" s="44"/>
-      <c r="N414" s="44"/>
-    </row>
-    <row r="415" spans="1:14" ht="18" customHeight="1">
-      <c r="A415" s="44"/>
-      <c r="C415" s="2"/>
-      <c r="D415" s="2"/>
-      <c r="F415" s="2"/>
-      <c r="G415" s="2"/>
+      <c r="L414" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M414" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N414" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P414" s="6">
+        <v>421.64179104477603</v>
+      </c>
+    </row>
+    <row r="415" spans="1:16" ht="18" customHeight="1">
+      <c r="A415" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="B415" s="96" t="s">
+        <v>490</v>
+      </c>
+      <c r="C415" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D415" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E415" t="s">
+        <v>481</v>
+      </c>
+      <c r="F415" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G415" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H415" s="2"/>
-      <c r="I415" s="3"/>
-      <c r="J415" s="4"/>
+      <c r="I415" s="3">
+        <v>298</v>
+      </c>
+      <c r="J415" s="4">
+        <f t="shared" si="9"/>
+        <v>442537313.43283498</v>
+      </c>
       <c r="K415" s="4"/>
-      <c r="L415" s="44"/>
-      <c r="M415" s="44"/>
-      <c r="N415" s="44"/>
-    </row>
-    <row r="416" spans="1:14" ht="18" customHeight="1">
-      <c r="A416" s="44"/>
-      <c r="C416" s="2"/>
-      <c r="D416" s="2"/>
-      <c r="F416" s="2"/>
-      <c r="G416" s="2"/>
+      <c r="L415" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M415" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N415" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P415" s="6">
+        <v>442.53731343283499</v>
+      </c>
+    </row>
+    <row r="416" spans="1:16" ht="18" customHeight="1">
+      <c r="A416" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="B416" s="96" t="s">
+        <v>492</v>
+      </c>
+      <c r="C416" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D416" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E416" t="s">
+        <v>481</v>
+      </c>
+      <c r="F416" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G416" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H416" s="2"/>
-      <c r="I416" s="3"/>
-      <c r="J416" s="4"/>
+      <c r="I416" s="3">
+        <v>298</v>
+      </c>
+      <c r="J416" s="4">
+        <f t="shared" si="9"/>
+        <v>479104477.61194003</v>
+      </c>
       <c r="K416" s="4"/>
-      <c r="L416" s="44"/>
-      <c r="M416" s="44"/>
-      <c r="N416" s="44"/>
-    </row>
-    <row r="417" spans="1:14" ht="18" customHeight="1">
-      <c r="A417" s="44"/>
-      <c r="C417" s="2"/>
-      <c r="D417" s="2"/>
-      <c r="F417" s="2"/>
-      <c r="G417" s="2"/>
+      <c r="L416" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M416" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N416" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P416" s="6">
+        <v>479.10447761194001</v>
+      </c>
+    </row>
+    <row r="417" spans="1:16" ht="18" customHeight="1">
+      <c r="A417" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="B417" s="96" t="s">
+        <v>493</v>
+      </c>
+      <c r="C417" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D417" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E417" t="s">
+        <v>481</v>
+      </c>
+      <c r="F417" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G417" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H417" s="2"/>
-      <c r="I417" s="3"/>
-      <c r="J417" s="4"/>
+      <c r="I417" s="3">
+        <v>298</v>
+      </c>
+      <c r="J417" s="4">
+        <f t="shared" si="9"/>
+        <v>517412935.32338297</v>
+      </c>
       <c r="K417" s="4"/>
-      <c r="L417" s="44"/>
-      <c r="M417" s="44"/>
-      <c r="N417" s="44"/>
-    </row>
-    <row r="418" spans="1:14" ht="18" customHeight="1">
-      <c r="A418" s="44"/>
-      <c r="C418" s="2"/>
-      <c r="D418" s="2"/>
-      <c r="F418" s="2"/>
-      <c r="G418" s="2"/>
+      <c r="L417" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M417" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N417" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P417" s="6">
+        <v>517.41293532338295</v>
+      </c>
+    </row>
+    <row r="418" spans="1:16" ht="18" customHeight="1">
+      <c r="A418" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="B418" s="96" t="s">
+        <v>494</v>
+      </c>
+      <c r="C418" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D418" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E418" t="s">
+        <v>481</v>
+      </c>
+      <c r="F418" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G418" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H418" s="2"/>
-      <c r="I418" s="3"/>
-      <c r="J418" s="4"/>
+      <c r="I418" s="3">
+        <v>298</v>
+      </c>
+      <c r="J418" s="4">
+        <f t="shared" si="9"/>
+        <v>543532338.30845702</v>
+      </c>
       <c r="K418" s="4"/>
-      <c r="L418" s="44"/>
-      <c r="M418" s="44"/>
-      <c r="N418" s="44"/>
-    </row>
-    <row r="419" spans="1:14" ht="18" customHeight="1">
-      <c r="A419" s="44"/>
-      <c r="C419" s="2"/>
-      <c r="D419" s="2"/>
-      <c r="F419" s="2"/>
-      <c r="G419" s="2"/>
+      <c r="L418" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M418" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N418" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P418" s="6">
+        <v>543.53233830845704</v>
+      </c>
+    </row>
+    <row r="419" spans="1:16" ht="18" customHeight="1">
+      <c r="A419" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="B419" s="96" t="s">
+        <v>495</v>
+      </c>
+      <c r="C419" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D419" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E419" t="s">
+        <v>481</v>
+      </c>
+      <c r="F419" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G419" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H419" s="2"/>
-      <c r="I419" s="3"/>
-      <c r="J419" s="4"/>
+      <c r="I419" s="3">
+        <v>298</v>
+      </c>
+      <c r="J419" s="4">
+        <f t="shared" si="9"/>
+        <v>618407960.19900489</v>
+      </c>
       <c r="K419" s="4"/>
-      <c r="L419" s="44"/>
-      <c r="M419" s="44"/>
-      <c r="N419" s="44"/>
-    </row>
-    <row r="420" spans="1:14" ht="18" customHeight="1">
-      <c r="A420" s="44"/>
-      <c r="C420" s="2"/>
-      <c r="D420" s="2"/>
-      <c r="F420" s="2"/>
-      <c r="G420" s="2"/>
+      <c r="L419" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M419" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N419" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P419" s="6">
+        <v>618.40796019900495</v>
+      </c>
+    </row>
+    <row r="420" spans="1:16" ht="18" customHeight="1">
+      <c r="A420" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="B420" s="96" t="s">
+        <v>496</v>
+      </c>
+      <c r="C420" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D420" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E420" t="s">
+        <v>481</v>
+      </c>
+      <c r="F420" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G420" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H420" s="2"/>
-      <c r="I420" s="3"/>
-      <c r="J420" s="4"/>
+      <c r="I420" s="3">
+        <v>298</v>
+      </c>
+      <c r="J420" s="4">
+        <f t="shared" si="9"/>
+        <v>780348258.70646703</v>
+      </c>
       <c r="K420" s="4"/>
-      <c r="L420" s="44"/>
-      <c r="M420" s="44"/>
-      <c r="N420" s="44"/>
-    </row>
-    <row r="421" spans="1:14" ht="18" customHeight="1">
-      <c r="A421" s="44"/>
-      <c r="C421" s="2"/>
-      <c r="D421" s="2"/>
-      <c r="F421" s="2"/>
-      <c r="G421" s="2"/>
+      <c r="L420" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M420" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N420" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P420" s="6">
+        <v>780.34825870646705</v>
+      </c>
+    </row>
+    <row r="421" spans="1:16" ht="18" customHeight="1">
+      <c r="A421" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="B421" s="96" t="s">
+        <v>497</v>
+      </c>
+      <c r="C421" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D421" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E421" t="s">
+        <v>481</v>
+      </c>
+      <c r="F421" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G421" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H421" s="2"/>
-      <c r="I421" s="3"/>
-      <c r="J421" s="4"/>
+      <c r="I421" s="3">
+        <v>298</v>
+      </c>
+      <c r="J421" s="4">
+        <f t="shared" si="9"/>
+        <v>843034825.870646</v>
+      </c>
       <c r="K421" s="4"/>
-      <c r="L421" s="44"/>
-      <c r="M421" s="44"/>
-      <c r="N421" s="44"/>
-    </row>
-    <row r="422" spans="1:14" ht="18" customHeight="1">
-      <c r="A422" s="44"/>
-      <c r="C422" s="2"/>
-      <c r="D422" s="2"/>
-      <c r="F422" s="2"/>
-      <c r="G422" s="2"/>
+      <c r="L421" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M421" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N421" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P421" s="6">
+        <v>843.03482587064605</v>
+      </c>
+    </row>
+    <row r="422" spans="1:16" ht="18" customHeight="1">
+      <c r="A422" s="47" t="s">
+        <v>498</v>
+      </c>
+      <c r="B422" s="96" t="s">
+        <v>499</v>
+      </c>
+      <c r="C422" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D422" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E422" t="s">
+        <v>481</v>
+      </c>
+      <c r="F422" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G422" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H422" s="2"/>
-      <c r="I422" s="3"/>
-      <c r="J422" s="4"/>
+      <c r="I422" s="3">
+        <v>298</v>
+      </c>
+      <c r="J422" s="4">
+        <f t="shared" ref="J422:J429" si="10">P422*9807000</f>
+        <v>1991482822.0858827</v>
+      </c>
       <c r="K422" s="4"/>
-      <c r="L422" s="44"/>
-      <c r="M422" s="44"/>
-      <c r="N422" s="44"/>
-    </row>
-    <row r="423" spans="1:14" ht="18" customHeight="1">
-      <c r="A423" s="44"/>
-      <c r="C423" s="2"/>
-      <c r="D423" s="2"/>
-      <c r="F423" s="2"/>
-      <c r="G423" s="2"/>
+      <c r="L422" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M422" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N422" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P422" s="6">
+        <v>203.06748466257599</v>
+      </c>
+    </row>
+    <row r="423" spans="1:16" ht="18" customHeight="1">
+      <c r="A423" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="B423" s="96" t="s">
+        <v>490</v>
+      </c>
+      <c r="C423" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D423" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E423" t="s">
+        <v>481</v>
+      </c>
+      <c r="F423" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G423" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H423" s="2"/>
-      <c r="I423" s="3"/>
-      <c r="J423" s="4"/>
+      <c r="I423" s="3">
+        <v>298</v>
+      </c>
+      <c r="J423" s="4">
+        <f t="shared" si="10"/>
+        <v>2087747852.7607353</v>
+      </c>
       <c r="K423" s="4"/>
-      <c r="L423" s="44"/>
-      <c r="M423" s="44"/>
-      <c r="N423" s="44"/>
-    </row>
-    <row r="424" spans="1:14" ht="18" customHeight="1">
-      <c r="A424" s="44"/>
-      <c r="C424" s="2"/>
-      <c r="D424" s="2"/>
-      <c r="F424" s="2"/>
-      <c r="G424" s="2"/>
+      <c r="L423" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M423" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N423" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P423" s="6">
+        <v>212.88343558282199</v>
+      </c>
+    </row>
+    <row r="424" spans="1:16" ht="18" customHeight="1">
+      <c r="A424" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="B424" s="96" t="s">
+        <v>492</v>
+      </c>
+      <c r="C424" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D424" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E424" t="s">
+        <v>481</v>
+      </c>
+      <c r="F424" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G424" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H424" s="2"/>
-      <c r="I424" s="3"/>
-      <c r="J424" s="4"/>
+      <c r="I424" s="3">
+        <v>298</v>
+      </c>
+      <c r="J424" s="4">
+        <f t="shared" si="10"/>
+        <v>2196046012.269937</v>
+      </c>
       <c r="K424" s="4"/>
-      <c r="L424" s="44"/>
-      <c r="M424" s="44"/>
-      <c r="N424" s="44"/>
+      <c r="L424" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M424" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N424" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P424" s="6">
+        <v>223.92638036809799</v>
+      </c>
+    </row>
+    <row r="425" spans="1:16">
+      <c r="A425" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="B425" s="96" t="s">
+        <v>493</v>
+      </c>
+      <c r="C425" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D425" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E425" t="s">
+        <v>481</v>
+      </c>
+      <c r="F425" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G425" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H425" s="2"/>
+      <c r="I425" s="3">
+        <v>298</v>
+      </c>
+      <c r="J425" s="4">
+        <f t="shared" si="10"/>
+        <v>2370526380.3680887</v>
+      </c>
+      <c r="K425" s="4"/>
+      <c r="L425" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M425" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N425" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P425" s="6">
+        <v>241.71779141104199</v>
+      </c>
+    </row>
+    <row r="426" spans="1:16">
+      <c r="A426" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="B426" s="96" t="s">
+        <v>494</v>
+      </c>
+      <c r="C426" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D426" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E426" t="s">
+        <v>481</v>
+      </c>
+      <c r="F426" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G426" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H426" s="2"/>
+      <c r="I426" s="3">
+        <v>298</v>
+      </c>
+      <c r="J426" s="4">
+        <f t="shared" si="10"/>
+        <v>2526957055.2147169</v>
+      </c>
+      <c r="K426" s="4"/>
+      <c r="L426" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M426" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N426" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P426" s="6">
+        <v>257.66871165644102</v>
+      </c>
+    </row>
+    <row r="427" spans="1:16">
+      <c r="A427" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="B427" s="96" t="s">
+        <v>495</v>
+      </c>
+      <c r="C427" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D427" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E427" t="s">
+        <v>481</v>
+      </c>
+      <c r="F427" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G427" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H427" s="2"/>
+      <c r="I427" s="3">
+        <v>298</v>
+      </c>
+      <c r="J427" s="4">
+        <f t="shared" si="10"/>
+        <v>2725503680.9815869</v>
+      </c>
+      <c r="K427" s="4"/>
+      <c r="L427" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M427" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N427" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P427" s="6">
+        <v>277.91411042944702</v>
+      </c>
+    </row>
+    <row r="428" spans="1:16">
+      <c r="A428" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="B428" s="96" t="s">
+        <v>496</v>
+      </c>
+      <c r="C428" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D428" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E428" t="s">
+        <v>481</v>
+      </c>
+      <c r="F428" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G428" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H428" s="2"/>
+      <c r="I428" s="3">
+        <v>298</v>
+      </c>
+      <c r="J428" s="4">
+        <f t="shared" si="10"/>
+        <v>3092514110.4294438</v>
+      </c>
+      <c r="K428" s="4"/>
+      <c r="L428" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M428" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N428" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P428" s="6">
+        <v>315.337423312883</v>
+      </c>
+    </row>
+    <row r="429" spans="1:16">
+      <c r="A429" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="B429" s="96" t="s">
+        <v>497</v>
+      </c>
+      <c r="C429" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D429" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E429" t="s">
+        <v>481</v>
+      </c>
+      <c r="F429" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G429" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H429" s="2"/>
+      <c r="I429" s="3">
+        <v>298</v>
+      </c>
+      <c r="J429" s="4">
+        <f t="shared" si="10"/>
+        <v>3381309202.4539814</v>
+      </c>
+      <c r="K429" s="4"/>
+      <c r="L429" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M429" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N429" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P429" s="6">
+        <v>344.785276073619</v>
+      </c>
+    </row>
+    <row r="430" spans="1:16">
+      <c r="A430" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B430" s="96" t="s">
+        <v>500</v>
+      </c>
+      <c r="C430" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D430" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E430" t="s">
+        <v>481</v>
+      </c>
+      <c r="F430" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G430" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H430" s="2"/>
+      <c r="I430" s="3">
+        <v>298</v>
+      </c>
+      <c r="J430" s="4">
+        <f t="shared" ref="J430:J437" si="11">P430*1000000</f>
+        <v>469010416.66666603</v>
+      </c>
+      <c r="K430" s="4"/>
+      <c r="L430" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M430" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N430" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P430" s="6">
+        <v>469.010416666666</v>
+      </c>
+    </row>
+    <row r="431" spans="1:16">
+      <c r="A431" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B431" s="96" t="s">
+        <v>502</v>
+      </c>
+      <c r="C431" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D431" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E431" t="s">
+        <v>481</v>
+      </c>
+      <c r="F431" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G431" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H431" s="2"/>
+      <c r="I431" s="3">
+        <v>298</v>
+      </c>
+      <c r="J431" s="4">
+        <f t="shared" si="11"/>
+        <v>494531250</v>
+      </c>
+      <c r="K431" s="4"/>
+      <c r="L431" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M431" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N431" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P431" s="6">
+        <v>494.53125</v>
+      </c>
+    </row>
+    <row r="432" spans="1:16">
+      <c r="A432" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B432" s="96" t="s">
+        <v>503</v>
+      </c>
+      <c r="C432" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D432" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E432" t="s">
+        <v>481</v>
+      </c>
+      <c r="F432" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G432" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H432" s="2"/>
+      <c r="I432" s="3">
+        <v>298</v>
+      </c>
+      <c r="J432" s="4">
+        <f t="shared" si="11"/>
+        <v>556510416.66666591</v>
+      </c>
+      <c r="K432" s="4"/>
+      <c r="L432" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M432" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N432" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P432" s="6">
+        <v>556.51041666666595</v>
+      </c>
+    </row>
+    <row r="433" spans="1:16">
+      <c r="A433" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B433" s="96" t="s">
+        <v>504</v>
+      </c>
+      <c r="C433" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D433" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E433" t="s">
+        <v>481</v>
+      </c>
+      <c r="F433" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G433" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H433" s="2"/>
+      <c r="I433" s="3">
+        <v>298</v>
+      </c>
+      <c r="J433" s="4">
+        <f t="shared" si="11"/>
+        <v>582031250</v>
+      </c>
+      <c r="K433" s="4"/>
+      <c r="L433" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M433" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N433" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P433" s="6">
+        <v>582.03125</v>
+      </c>
+    </row>
+    <row r="434" spans="1:16">
+      <c r="A434" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B434" s="96" t="s">
+        <v>505</v>
+      </c>
+      <c r="C434" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D434" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E434" t="s">
+        <v>481</v>
+      </c>
+      <c r="F434" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G434" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H434" s="2"/>
+      <c r="I434" s="3">
+        <v>298</v>
+      </c>
+      <c r="J434" s="4">
+        <f t="shared" si="11"/>
+        <v>625781250</v>
+      </c>
+      <c r="K434" s="4"/>
+      <c r="L434" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M434" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N434" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P434" s="6">
+        <v>625.78125</v>
+      </c>
+    </row>
+    <row r="435" spans="1:16">
+      <c r="A435" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B435" s="96" t="s">
+        <v>506</v>
+      </c>
+      <c r="C435" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D435" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E435" t="s">
+        <v>481</v>
+      </c>
+      <c r="F435" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G435" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H435" s="2"/>
+      <c r="I435" s="3">
+        <v>298</v>
+      </c>
+      <c r="J435" s="4">
+        <f t="shared" si="11"/>
+        <v>711458333.33333302</v>
+      </c>
+      <c r="K435" s="4"/>
+      <c r="L435" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M435" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N435" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P435" s="6">
+        <v>711.45833333333303</v>
+      </c>
+    </row>
+    <row r="436" spans="1:16">
+      <c r="A436" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B436" s="96" t="s">
+        <v>507</v>
+      </c>
+      <c r="C436" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D436" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E436" t="s">
+        <v>481</v>
+      </c>
+      <c r="F436" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G436" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H436" s="2"/>
+      <c r="I436" s="3">
+        <v>298</v>
+      </c>
+      <c r="J436" s="4">
+        <f t="shared" si="11"/>
+        <v>797135416.66666591</v>
+      </c>
+      <c r="K436" s="4"/>
+      <c r="L436" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M436" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N436" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P436" s="6">
+        <v>797.13541666666595</v>
+      </c>
+    </row>
+    <row r="437" spans="1:16">
+      <c r="A437" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B437" s="96" t="s">
+        <v>508</v>
+      </c>
+      <c r="C437" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D437" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E437" t="s">
+        <v>481</v>
+      </c>
+      <c r="F437" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G437" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H437" s="2"/>
+      <c r="I437" s="3">
+        <v>298</v>
+      </c>
+      <c r="J437" s="4">
+        <f t="shared" si="11"/>
+        <v>880989583.33333302</v>
+      </c>
+      <c r="K437" s="4"/>
+      <c r="L437" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M437" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N437" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P437" s="6">
+        <v>880.98958333333303</v>
+      </c>
+    </row>
+    <row r="438" spans="1:16">
+      <c r="A438" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B438" s="96" t="s">
+        <v>500</v>
+      </c>
+      <c r="C438" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D438" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E438" t="s">
+        <v>481</v>
+      </c>
+      <c r="F438" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G438" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H438" s="2"/>
+      <c r="I438" s="3">
+        <v>298</v>
+      </c>
+      <c r="J438" s="4">
+        <f t="shared" ref="J438:J445" si="12">P438*9807000</f>
+        <v>2239170520.2312107</v>
+      </c>
+      <c r="K438" s="4"/>
+      <c r="L438" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M438" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N438" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P438" s="6">
+        <v>228.32369942196499</v>
+      </c>
+    </row>
+    <row r="439" spans="1:16">
+      <c r="A439" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B439" s="96" t="s">
+        <v>502</v>
+      </c>
+      <c r="C439" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D439" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E439" t="s">
+        <v>481</v>
+      </c>
+      <c r="F439" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G439" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H439" s="2"/>
+      <c r="I439" s="3">
+        <v>298</v>
+      </c>
+      <c r="J439" s="4">
+        <f t="shared" si="12"/>
+        <v>2341208670.5202217</v>
+      </c>
+      <c r="K439" s="4"/>
+      <c r="L439" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M439" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N439" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P439" s="6">
+        <v>238.728323699421</v>
+      </c>
+    </row>
+    <row r="440" spans="1:16">
+      <c r="A440" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B440" s="96" t="s">
+        <v>503</v>
+      </c>
+      <c r="C440" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D440" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E440" t="s">
+        <v>481</v>
+      </c>
+      <c r="F440" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G440" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H440" s="2"/>
+      <c r="I440" s="3">
+        <v>298</v>
+      </c>
+      <c r="J440" s="4">
+        <f t="shared" si="12"/>
+        <v>2499934682.0809164</v>
+      </c>
+      <c r="K440" s="4"/>
+      <c r="L440" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M440" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N440" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P440" s="6">
+        <v>254.913294797687</v>
+      </c>
+    </row>
+    <row r="441" spans="1:16">
+      <c r="A441" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B441" s="96" t="s">
+        <v>504</v>
+      </c>
+      <c r="C441" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D441" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E441" t="s">
+        <v>481</v>
+      </c>
+      <c r="F441" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G441" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H441" s="2"/>
+      <c r="I441" s="3">
+        <v>298</v>
+      </c>
+      <c r="J441" s="4">
+        <f t="shared" si="12"/>
+        <v>2573628901.7340956</v>
+      </c>
+      <c r="K441" s="4"/>
+      <c r="L441" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M441" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N441" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P441" s="6">
+        <v>262.42774566473901</v>
+      </c>
+    </row>
+    <row r="442" spans="1:16">
+      <c r="A442" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B442" s="96" t="s">
+        <v>505</v>
+      </c>
+      <c r="C442" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D442" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E442" t="s">
+        <v>481</v>
+      </c>
+      <c r="F442" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G442" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H442" s="2"/>
+      <c r="I442" s="3">
+        <v>298</v>
+      </c>
+      <c r="J442" s="4">
+        <f t="shared" si="12"/>
+        <v>2783373988.4393058</v>
+      </c>
+      <c r="K442" s="4"/>
+      <c r="L442" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M442" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N442" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P442" s="6">
+        <v>283.81502890173402</v>
+      </c>
+    </row>
+    <row r="443" spans="1:16">
+      <c r="A443" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B443" s="96" t="s">
+        <v>506</v>
+      </c>
+      <c r="C443" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D443" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E443" t="s">
+        <v>481</v>
+      </c>
+      <c r="F443" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G443" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H443" s="2"/>
+      <c r="I443" s="3">
+        <v>298</v>
+      </c>
+      <c r="J443" s="4">
+        <f t="shared" si="12"/>
+        <v>3027131791.907506</v>
+      </c>
+      <c r="K443" s="4"/>
+      <c r="L443" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M443" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N443" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P443" s="6">
+        <v>308.670520231213</v>
+      </c>
+    </row>
+    <row r="444" spans="1:16">
+      <c r="A444" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B444" s="96" t="s">
+        <v>507</v>
+      </c>
+      <c r="C444" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D444" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E444" t="s">
+        <v>481</v>
+      </c>
+      <c r="F444" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G444" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H444" s="2"/>
+      <c r="I444" s="3">
+        <v>298</v>
+      </c>
+      <c r="J444" s="4">
+        <f t="shared" si="12"/>
+        <v>3367258959.5375686</v>
+      </c>
+      <c r="K444" s="4"/>
+      <c r="L444" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M444" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N444" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P444" s="6">
+        <v>343.352601156069</v>
+      </c>
+    </row>
+    <row r="445" spans="1:16">
+      <c r="A445" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B445" s="96" t="s">
+        <v>508</v>
+      </c>
+      <c r="C445" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D445" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E445" t="s">
+        <v>481</v>
+      </c>
+      <c r="F445" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G445" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H445" s="2"/>
+      <c r="I445" s="3">
+        <v>298</v>
+      </c>
+      <c r="J445" s="4">
+        <f t="shared" si="12"/>
+        <v>3673373410.4046211</v>
+      </c>
+      <c r="K445" s="4"/>
+      <c r="L445" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M445" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="N445" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P445" s="6">
+        <v>374.56647398843899</v>
+      </c>
+    </row>
+    <row r="446" spans="1:16">
+      <c r="A446" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B446" s="96" t="s">
+        <v>509</v>
+      </c>
+      <c r="C446" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D446" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E446" t="s">
+        <v>481</v>
+      </c>
+      <c r="F446" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G446" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H446" s="2"/>
+      <c r="I446" s="3">
+        <v>298</v>
+      </c>
+      <c r="J446" s="4">
+        <f t="shared" ref="J446:J453" si="13">P446*1000000</f>
+        <v>872493573.264781</v>
+      </c>
+      <c r="K446" s="4"/>
+      <c r="L446" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M446" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N446" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P446" s="6">
+        <v>872.49357326478105</v>
+      </c>
+    </row>
+    <row r="447" spans="1:16">
+      <c r="A447" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B447" s="96" t="s">
+        <v>511</v>
+      </c>
+      <c r="C447" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D447" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E447" t="s">
+        <v>481</v>
+      </c>
+      <c r="F447" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G447" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H447" s="2"/>
+      <c r="I447" s="3">
+        <v>298</v>
+      </c>
+      <c r="J447" s="4">
+        <f t="shared" si="13"/>
+        <v>820308483.290488</v>
+      </c>
+      <c r="K447" s="4"/>
+      <c r="L447" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M447" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N447" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P447" s="6">
+        <v>820.30848329048797</v>
+      </c>
+    </row>
+    <row r="448" spans="1:16">
+      <c r="A448" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B448" s="96" t="s">
+        <v>512</v>
+      </c>
+      <c r="C448" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D448" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E448" t="s">
+        <v>481</v>
+      </c>
+      <c r="F448" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G448" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H448" s="2"/>
+      <c r="I448" s="3">
+        <v>298</v>
+      </c>
+      <c r="J448" s="4">
+        <f t="shared" si="13"/>
+        <v>894087403.59897101</v>
+      </c>
+      <c r="K448" s="4"/>
+      <c r="L448" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M448" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N448" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P448" s="6">
+        <v>894.08740359897104</v>
+      </c>
+    </row>
+    <row r="449" spans="1:16">
+      <c r="A449" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B449" s="96" t="s">
+        <v>513</v>
+      </c>
+      <c r="C449" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D449" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E449" t="s">
+        <v>481</v>
+      </c>
+      <c r="F449" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G449" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H449" s="2"/>
+      <c r="I449" s="3">
+        <v>298</v>
+      </c>
+      <c r="J449" s="4">
+        <f t="shared" si="13"/>
+        <v>976863753.21336699</v>
+      </c>
+      <c r="K449" s="4"/>
+      <c r="L449" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M449" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N449" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P449" s="6">
+        <v>976.86375321336698</v>
+      </c>
+    </row>
+    <row r="450" spans="1:16">
+      <c r="A450" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B450" s="96" t="s">
+        <v>514</v>
+      </c>
+      <c r="C450" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D450" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E450" t="s">
+        <v>481</v>
+      </c>
+      <c r="F450" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G450" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H450" s="2"/>
+      <c r="I450" s="3">
+        <v>298</v>
+      </c>
+      <c r="J450" s="4">
+        <f t="shared" si="13"/>
+        <v>955269922.87917697</v>
+      </c>
+      <c r="K450" s="4"/>
+      <c r="L450" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M450" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N450" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P450" s="6">
+        <v>955.26992287917699</v>
+      </c>
+    </row>
+    <row r="451" spans="1:16">
+      <c r="A451" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B451" s="96" t="s">
+        <v>515</v>
+      </c>
+      <c r="C451" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D451" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E451" t="s">
+        <v>481</v>
+      </c>
+      <c r="F451" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G451" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H451" s="2"/>
+      <c r="I451" s="3">
+        <v>298</v>
+      </c>
+      <c r="J451" s="4">
+        <f t="shared" si="13"/>
+        <v>942673521.85089898</v>
+      </c>
+      <c r="K451" s="4"/>
+      <c r="L451" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M451" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N451" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P451" s="6">
+        <v>942.67352185089896</v>
+      </c>
+    </row>
+    <row r="452" spans="1:16">
+      <c r="A452" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B452" s="96" t="s">
+        <v>516</v>
+      </c>
+      <c r="C452" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D452" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E452" t="s">
+        <v>481</v>
+      </c>
+      <c r="F452" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G452" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H452" s="2"/>
+      <c r="I452" s="3">
+        <v>298</v>
+      </c>
+      <c r="J452" s="4">
+        <f t="shared" si="13"/>
+        <v>921079691.51670897</v>
+      </c>
+      <c r="K452" s="4"/>
+      <c r="L452" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M452" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N452" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P452" s="6">
+        <v>921.07969151670898</v>
+      </c>
+    </row>
+    <row r="453" spans="1:16">
+      <c r="A453" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B453" s="96" t="s">
+        <v>517</v>
+      </c>
+      <c r="C453" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D453" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E453" t="s">
+        <v>481</v>
+      </c>
+      <c r="F453" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G453" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H453" s="2"/>
+      <c r="I453" s="3">
+        <v>298</v>
+      </c>
+      <c r="J453" s="4">
+        <f t="shared" si="13"/>
+        <v>895886889.46015394</v>
+      </c>
+      <c r="K453" s="4"/>
+      <c r="L453" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M453" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N453" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P453" s="6">
+        <v>895.88688946015395</v>
+      </c>
+    </row>
+    <row r="454" spans="1:16">
+      <c r="A454" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B454" s="96" t="s">
+        <v>509</v>
+      </c>
+      <c r="C454" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D454" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E454" t="s">
+        <v>481</v>
+      </c>
+      <c r="F454" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G454" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H454" s="2"/>
+      <c r="I454" s="3">
+        <v>298</v>
+      </c>
+      <c r="J454" s="4">
+        <f t="shared" ref="J454:J461" si="14">P454*9807000</f>
+        <v>3531213074.2049384</v>
+      </c>
+      <c r="K454" s="4"/>
+      <c r="L454" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M454" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N454" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P454" s="6">
+        <v>360.07067137809099</v>
+      </c>
+    </row>
+    <row r="455" spans="1:16">
+      <c r="A455" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B455" s="96" t="s">
+        <v>511</v>
+      </c>
+      <c r="C455" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D455" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E455" t="s">
+        <v>481</v>
+      </c>
+      <c r="F455" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G455" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H455" s="2"/>
+      <c r="I455" s="3">
+        <v>298</v>
+      </c>
+      <c r="J455" s="4">
+        <f t="shared" si="14"/>
+        <v>3655966431.0954065</v>
+      </c>
+      <c r="K455" s="4"/>
+      <c r="L455" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M455" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N455" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P455" s="6">
+        <v>372.79151943462898</v>
+      </c>
+    </row>
+    <row r="456" spans="1:16">
+      <c r="A456" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B456" s="96" t="s">
+        <v>512</v>
+      </c>
+      <c r="C456" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D456" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E456" t="s">
+        <v>481</v>
+      </c>
+      <c r="F456" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G456" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H456" s="2"/>
+      <c r="I456" s="3">
+        <v>298</v>
+      </c>
+      <c r="J456" s="4">
+        <f t="shared" si="14"/>
+        <v>3541609187.2791519</v>
+      </c>
+      <c r="K456" s="4"/>
+      <c r="L456" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M456" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N456" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P456" s="6">
+        <v>361.13074204946997</v>
+      </c>
+    </row>
+    <row r="457" spans="1:16">
+      <c r="A457" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B457" s="96" t="s">
+        <v>513</v>
+      </c>
+      <c r="C457" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D457" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E457" t="s">
+        <v>481</v>
+      </c>
+      <c r="F457" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G457" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H457" s="2"/>
+      <c r="I457" s="3">
+        <v>298</v>
+      </c>
+      <c r="J457" s="4">
+        <f t="shared" si="14"/>
+        <v>3619580035.3356824</v>
+      </c>
+      <c r="K457" s="4"/>
+      <c r="L457" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M457" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N457" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P457" s="6">
+        <v>369.08127208480499</v>
+      </c>
+    </row>
+    <row r="458" spans="1:16">
+      <c r="A458" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B458" s="96" t="s">
+        <v>514</v>
+      </c>
+      <c r="C458" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D458" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E458" t="s">
+        <v>481</v>
+      </c>
+      <c r="F458" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G458" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H458" s="2"/>
+      <c r="I458" s="3">
+        <v>298</v>
+      </c>
+      <c r="J458" s="4">
+        <f t="shared" si="14"/>
+        <v>3713145053.0035286</v>
+      </c>
+      <c r="K458" s="4"/>
+      <c r="L458" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M458" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N458" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P458" s="6">
+        <v>378.62190812720797</v>
+      </c>
+    </row>
+    <row r="459" spans="1:16">
+      <c r="A459" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B459" s="96" t="s">
+        <v>515</v>
+      </c>
+      <c r="C459" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D459" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E459" t="s">
+        <v>481</v>
+      </c>
+      <c r="F459" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G459" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H459" s="2"/>
+      <c r="I459" s="3">
+        <v>298</v>
+      </c>
+      <c r="J459" s="4">
+        <f t="shared" si="14"/>
+        <v>3697550883.3922224</v>
+      </c>
+      <c r="K459" s="4"/>
+      <c r="L459" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M459" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N459" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P459" s="6">
+        <v>377.03180212014098</v>
+      </c>
+    </row>
+    <row r="460" spans="1:16">
+      <c r="A460" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B460" s="96" t="s">
+        <v>516</v>
+      </c>
+      <c r="C460" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D460" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E460" t="s">
+        <v>481</v>
+      </c>
+      <c r="F460" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G460" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H460" s="2"/>
+      <c r="I460" s="3">
+        <v>298</v>
+      </c>
+      <c r="J460" s="4">
+        <f t="shared" si="14"/>
+        <v>3645570318.0211926</v>
+      </c>
+      <c r="K460" s="4"/>
+      <c r="L460" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M460" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N460" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P460" s="6">
+        <v>371.73144876325</v>
+      </c>
+    </row>
+    <row r="461" spans="1:16">
+      <c r="A461" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="B461" s="96" t="s">
+        <v>517</v>
+      </c>
+      <c r="C461" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D461" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E461" t="s">
+        <v>481</v>
+      </c>
+      <c r="F461" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G461" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H461" s="2"/>
+      <c r="I461" s="3">
+        <v>298</v>
+      </c>
+      <c r="J461" s="4">
+        <f t="shared" si="14"/>
+        <v>3531213074.2049384</v>
+      </c>
+      <c r="K461" s="4"/>
+      <c r="L461" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M461" s="44" t="s">
+        <v>378</v>
+      </c>
+      <c r="N461" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="P461" s="6">
+        <v>360.07067137809099</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>

<commit_message>
- extracted data from `10.1038/s41598-020-61666-z` and `10.1016/j.matlet.2021.130822`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5261CCC8-FB81-E24C-B889-D566217EC501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0421A65-A2D9-9142-826F-F88E51EF0B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3946" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3979" uniqueCount="527">
   <si>
     <t>Metadata</t>
   </si>
@@ -1691,6 +1691,21 @@
   </si>
   <si>
     <t>10.1016/j.msea.2022.144271</t>
+  </si>
+  <si>
+    <t>UHfNbTi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimum ultimate compressive strength </t>
+  </si>
+  <si>
+    <t>10.1016/j.matlet.2021.130822</t>
+  </si>
+  <si>
+    <t>(TaNb)0.155 (TiUHf)0.23</t>
+  </si>
+  <si>
+    <t>10.1038/s41598-020-61666-z</t>
   </si>
 </sst>
 </file>
@@ -2908,10 +2923,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T461"/>
+  <dimension ref="A1:T466"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A417" zoomScale="89" workbookViewId="0">
-      <selection activeCell="O458" sqref="O458"/>
+    <sheetView tabSelected="1" topLeftCell="A434" zoomScale="89" workbookViewId="0">
+      <selection activeCell="H484" sqref="H484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -20195,6 +20210,145 @@
         <v>360.07067137809099</v>
       </c>
     </row>
+    <row r="462" spans="1:16">
+      <c r="B462" s="96" t="s">
+        <v>522</v>
+      </c>
+      <c r="C462" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D462" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F462" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G462" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H462" s="2"/>
+      <c r="I462" s="3">
+        <v>298</v>
+      </c>
+      <c r="J462" s="50">
+        <v>755000000</v>
+      </c>
+      <c r="L462" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="N462" s="51" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="463" spans="1:16">
+      <c r="B463" s="96" t="s">
+        <v>522</v>
+      </c>
+      <c r="C463" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D463" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F463" s="48" t="s">
+        <v>315</v>
+      </c>
+      <c r="G463" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H463" s="2"/>
+      <c r="I463" s="3">
+        <v>298</v>
+      </c>
+      <c r="J463" s="50">
+        <v>60</v>
+      </c>
+      <c r="L463" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="N463" s="51" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="464" spans="1:16">
+      <c r="B464" s="96" t="s">
+        <v>522</v>
+      </c>
+      <c r="C464" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D464" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F464" s="48" t="s">
+        <v>523</v>
+      </c>
+      <c r="G464" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H464" s="2"/>
+      <c r="I464" s="3">
+        <v>298</v>
+      </c>
+      <c r="J464" s="50">
+        <v>1502000000</v>
+      </c>
+      <c r="L464" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="N464" s="51" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="465" spans="2:14">
+      <c r="B465" s="96" t="s">
+        <v>525</v>
+      </c>
+      <c r="C465" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D465" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="F465" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="J465" s="50">
+        <v>3.2</v>
+      </c>
+      <c r="L465" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="N465" s="51" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="466" spans="2:14">
+      <c r="B466" s="96" t="s">
+        <v>525</v>
+      </c>
+      <c r="C466" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D466" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="F466" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="I466" s="49">
+        <v>300</v>
+      </c>
+      <c r="J466" s="50">
+        <v>1.8369999999999999E-6</v>
+      </c>
+      <c r="L466" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N466" s="51" t="s">
+        <v>526</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="D2:E3"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jallcom.2020.158295`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0421A65-A2D9-9142-826F-F88E51EF0B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BA395E-6163-8F40-B9DE-0D7138E612EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3979" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4068" uniqueCount="532">
   <si>
     <t>Metadata</t>
   </si>
@@ -1706,6 +1706,21 @@
   </si>
   <si>
     <t>10.1038/s41598-020-61666-z</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2020.158295</t>
+  </si>
+  <si>
+    <t>UMoNbTaHf</t>
+  </si>
+  <si>
+    <t>Hf</t>
+  </si>
+  <si>
+    <t>Ti</t>
+  </si>
+  <si>
+    <t>UMoNbTaTi</t>
   </si>
 </sst>
 </file>
@@ -2923,10 +2938,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T466"/>
+  <dimension ref="A1:T472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A434" zoomScale="89" workbookViewId="0">
-      <selection activeCell="H484" sqref="H484"/>
+    <sheetView tabSelected="1" topLeftCell="A426" zoomScale="89" workbookViewId="0">
+      <selection activeCell="N477" sqref="N477"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -17416,7 +17431,9 @@
       <c r="G398" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H398" s="2"/>
+      <c r="H398" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I398" s="3">
         <v>298</v>
       </c>
@@ -17460,7 +17477,9 @@
       <c r="G399" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H399" s="2"/>
+      <c r="H399" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I399" s="3">
         <v>298</v>
       </c>
@@ -17504,7 +17523,9 @@
       <c r="G400" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H400" s="2"/>
+      <c r="H400" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I400" s="3">
         <v>298</v>
       </c>
@@ -17548,7 +17569,9 @@
       <c r="G401" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H401" s="2"/>
+      <c r="H401" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I401" s="3">
         <v>298</v>
       </c>
@@ -17592,7 +17615,9 @@
       <c r="G402" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H402" s="2"/>
+      <c r="H402" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I402" s="3">
         <v>298</v>
       </c>
@@ -17636,7 +17661,9 @@
       <c r="G403" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H403" s="2"/>
+      <c r="H403" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I403" s="3">
         <v>298</v>
       </c>
@@ -17680,7 +17707,9 @@
       <c r="G404" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H404" s="2"/>
+      <c r="H404" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I404" s="3">
         <v>298</v>
       </c>
@@ -17724,7 +17753,9 @@
       <c r="G405" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H405" s="2"/>
+      <c r="H405" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I405" s="3">
         <v>298</v>
       </c>
@@ -18120,7 +18151,9 @@
       <c r="G414" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H414" s="2"/>
+      <c r="H414" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I414" s="3">
         <v>298</v>
       </c>
@@ -18164,7 +18197,9 @@
       <c r="G415" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H415" s="2"/>
+      <c r="H415" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I415" s="3">
         <v>298</v>
       </c>
@@ -18208,7 +18243,9 @@
       <c r="G416" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H416" s="2"/>
+      <c r="H416" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I416" s="3">
         <v>298</v>
       </c>
@@ -18252,7 +18289,9 @@
       <c r="G417" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H417" s="2"/>
+      <c r="H417" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I417" s="3">
         <v>298</v>
       </c>
@@ -18296,7 +18335,9 @@
       <c r="G418" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H418" s="2"/>
+      <c r="H418" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I418" s="3">
         <v>298</v>
       </c>
@@ -18340,7 +18381,9 @@
       <c r="G419" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H419" s="2"/>
+      <c r="H419" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I419" s="3">
         <v>298</v>
       </c>
@@ -18384,7 +18427,9 @@
       <c r="G420" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H420" s="2"/>
+      <c r="H420" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I420" s="3">
         <v>298</v>
       </c>
@@ -18428,7 +18473,9 @@
       <c r="G421" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H421" s="2"/>
+      <c r="H421" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I421" s="3">
         <v>298</v>
       </c>
@@ -18824,7 +18871,9 @@
       <c r="G430" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H430" s="2"/>
+      <c r="H430" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I430" s="3">
         <v>298</v>
       </c>
@@ -18868,7 +18917,9 @@
       <c r="G431" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H431" s="2"/>
+      <c r="H431" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I431" s="3">
         <v>298</v>
       </c>
@@ -18912,7 +18963,9 @@
       <c r="G432" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H432" s="2"/>
+      <c r="H432" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I432" s="3">
         <v>298</v>
       </c>
@@ -18956,7 +19009,9 @@
       <c r="G433" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H433" s="2"/>
+      <c r="H433" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I433" s="3">
         <v>298</v>
       </c>
@@ -19000,7 +19055,9 @@
       <c r="G434" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H434" s="2"/>
+      <c r="H434" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I434" s="3">
         <v>298</v>
       </c>
@@ -19044,7 +19101,9 @@
       <c r="G435" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H435" s="2"/>
+      <c r="H435" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I435" s="3">
         <v>298</v>
       </c>
@@ -19088,7 +19147,9 @@
       <c r="G436" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H436" s="2"/>
+      <c r="H436" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I436" s="3">
         <v>298</v>
       </c>
@@ -19132,7 +19193,9 @@
       <c r="G437" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H437" s="2"/>
+      <c r="H437" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I437" s="3">
         <v>298</v>
       </c>
@@ -19528,7 +19591,9 @@
       <c r="G446" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H446" s="2"/>
+      <c r="H446" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I446" s="3">
         <v>298</v>
       </c>
@@ -19572,7 +19637,9 @@
       <c r="G447" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H447" s="2"/>
+      <c r="H447" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I447" s="3">
         <v>298</v>
       </c>
@@ -19616,7 +19683,9 @@
       <c r="G448" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H448" s="2"/>
+      <c r="H448" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I448" s="3">
         <v>298</v>
       </c>
@@ -19660,7 +19729,9 @@
       <c r="G449" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H449" s="2"/>
+      <c r="H449" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I449" s="3">
         <v>298</v>
       </c>
@@ -19704,7 +19775,9 @@
       <c r="G450" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H450" s="2"/>
+      <c r="H450" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I450" s="3">
         <v>298</v>
       </c>
@@ -19748,7 +19821,9 @@
       <c r="G451" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H451" s="2"/>
+      <c r="H451" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I451" s="3">
         <v>298</v>
       </c>
@@ -19792,7 +19867,9 @@
       <c r="G452" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H452" s="2"/>
+      <c r="H452" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I452" s="3">
         <v>298</v>
       </c>
@@ -19836,7 +19913,9 @@
       <c r="G453" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H453" s="2"/>
+      <c r="H453" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I453" s="3">
         <v>298</v>
       </c>
@@ -20226,7 +20305,9 @@
       <c r="G462" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H462" s="2"/>
+      <c r="H462" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I462" s="3">
         <v>298</v>
       </c>
@@ -20256,7 +20337,9 @@
       <c r="G463" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H463" s="2"/>
+      <c r="H463" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I463" s="3">
         <v>298</v>
       </c>
@@ -20286,7 +20369,9 @@
       <c r="G464" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H464" s="2"/>
+      <c r="H464" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="I464" s="3">
         <v>298</v>
       </c>
@@ -20300,7 +20385,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="465" spans="2:14">
+    <row r="465" spans="1:14">
       <c r="B465" s="96" t="s">
         <v>525</v>
       </c>
@@ -20323,7 +20408,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="466" spans="2:14">
+    <row r="466" spans="1:14">
       <c r="B466" s="96" t="s">
         <v>525</v>
       </c>
@@ -20347,6 +20432,216 @@
       </c>
       <c r="N466" s="51" t="s">
         <v>526</v>
+      </c>
+    </row>
+    <row r="467" spans="1:14">
+      <c r="A467" s="47" t="s">
+        <v>529</v>
+      </c>
+      <c r="B467" s="96" t="s">
+        <v>528</v>
+      </c>
+      <c r="C467" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D467" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F467" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="H467" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="I467" s="49">
+        <v>298</v>
+      </c>
+      <c r="J467" s="50">
+        <v>1147000000</v>
+      </c>
+      <c r="L467" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M467" s="51" t="s">
+        <v>419</v>
+      </c>
+      <c r="N467" s="51" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="468" spans="1:14">
+      <c r="A468" s="47" t="s">
+        <v>529</v>
+      </c>
+      <c r="B468" s="96" t="s">
+        <v>528</v>
+      </c>
+      <c r="C468" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D468" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F468" s="48" t="s">
+        <v>306</v>
+      </c>
+      <c r="H468" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="I468" s="49">
+        <v>298</v>
+      </c>
+      <c r="J468" s="50">
+        <v>1505000000</v>
+      </c>
+      <c r="L468" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M468" s="51" t="s">
+        <v>419</v>
+      </c>
+      <c r="N468" s="51" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="469" spans="1:14">
+      <c r="A469" s="47" t="s">
+        <v>529</v>
+      </c>
+      <c r="B469" s="96" t="s">
+        <v>528</v>
+      </c>
+      <c r="C469" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D469" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F469" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="H469" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="I469" s="49">
+        <v>298</v>
+      </c>
+      <c r="J469" s="50">
+        <v>7.7</v>
+      </c>
+      <c r="L469" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M469" s="51" t="s">
+        <v>419</v>
+      </c>
+      <c r="N469" s="51" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="470" spans="1:14">
+      <c r="A470" s="47" t="s">
+        <v>530</v>
+      </c>
+      <c r="B470" s="96" t="s">
+        <v>531</v>
+      </c>
+      <c r="C470" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D470" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F470" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="H470" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="I470" s="49">
+        <v>298</v>
+      </c>
+      <c r="J470" s="50">
+        <v>985000000</v>
+      </c>
+      <c r="L470" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M470" s="51" t="s">
+        <v>419</v>
+      </c>
+      <c r="N470" s="51" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="471" spans="1:14">
+      <c r="A471" s="47" t="s">
+        <v>530</v>
+      </c>
+      <c r="B471" s="96" t="s">
+        <v>531</v>
+      </c>
+      <c r="C471" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D471" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F471" s="48" t="s">
+        <v>306</v>
+      </c>
+      <c r="H471" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="I471" s="49">
+        <v>298</v>
+      </c>
+      <c r="J471" s="50">
+        <v>1812000000</v>
+      </c>
+      <c r="L471" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M471" s="51" t="s">
+        <v>419</v>
+      </c>
+      <c r="N471" s="51" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="472" spans="1:14">
+      <c r="A472" s="47" t="s">
+        <v>530</v>
+      </c>
+      <c r="B472" s="96" t="s">
+        <v>531</v>
+      </c>
+      <c r="C472" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D472" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F472" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="H472" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="I472" s="49">
+        <v>298</v>
+      </c>
+      <c r="J472" s="50">
+        <v>39.5</v>
+      </c>
+      <c r="L472" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M472" s="51" t="s">
+        <v>419</v>
+      </c>
+      <c r="N472" s="51" t="s">
+        <v>527</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- extracted additional data from `10.1016/j.jallcom.2020.158295`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BA395E-6163-8F40-B9DE-0D7138E612EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5950F2A3-949D-7E43-B24C-E5693A03EF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4068" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4101" uniqueCount="532">
   <si>
     <t>Metadata</t>
   </si>
@@ -2938,10 +2938,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T472"/>
+  <dimension ref="A1:T475"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A426" zoomScale="89" workbookViewId="0">
-      <selection activeCell="N477" sqref="N477"/>
+    <sheetView tabSelected="1" topLeftCell="B431" zoomScale="89" workbookViewId="0">
+      <selection activeCell="I480" sqref="I480"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -20385,7 +20385,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="465" spans="1:14">
+    <row r="465" spans="1:16">
       <c r="B465" s="96" t="s">
         <v>525</v>
       </c>
@@ -20398,6 +20398,9 @@
       <c r="F465" s="48" t="s">
         <v>397</v>
       </c>
+      <c r="G465" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="J465" s="50">
         <v>3.2</v>
       </c>
@@ -20408,7 +20411,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="466" spans="1:14">
+    <row r="466" spans="1:16">
       <c r="B466" s="96" t="s">
         <v>525</v>
       </c>
@@ -20421,6 +20424,9 @@
       <c r="F466" s="48" t="s">
         <v>80</v>
       </c>
+      <c r="G466" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="I466" s="49">
         <v>300</v>
       </c>
@@ -20434,7 +20440,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="467" spans="1:14">
+    <row r="467" spans="1:16">
       <c r="A467" s="47" t="s">
         <v>529</v>
       </c>
@@ -20450,6 +20456,9 @@
       <c r="F467" s="48" t="s">
         <v>82</v>
       </c>
+      <c r="G467" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H467" s="2" t="s">
         <v>465</v>
       </c>
@@ -20469,7 +20478,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="468" spans="1:14">
+    <row r="468" spans="1:16">
       <c r="A468" s="47" t="s">
         <v>529</v>
       </c>
@@ -20485,6 +20494,9 @@
       <c r="F468" s="48" t="s">
         <v>306</v>
       </c>
+      <c r="G468" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H468" s="2" t="s">
         <v>465</v>
       </c>
@@ -20504,7 +20516,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="469" spans="1:14">
+    <row r="469" spans="1:16">
       <c r="A469" s="47" t="s">
         <v>529</v>
       </c>
@@ -20520,6 +20532,9 @@
       <c r="F469" s="48" t="s">
         <v>67</v>
       </c>
+      <c r="G469" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H469" s="2" t="s">
         <v>465</v>
       </c>
@@ -20539,7 +20554,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="470" spans="1:14">
+    <row r="470" spans="1:16">
       <c r="A470" s="47" t="s">
         <v>530</v>
       </c>
@@ -20555,6 +20570,9 @@
       <c r="F470" s="48" t="s">
         <v>82</v>
       </c>
+      <c r="G470" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H470" s="2" t="s">
         <v>465</v>
       </c>
@@ -20574,7 +20592,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="471" spans="1:14">
+    <row r="471" spans="1:16">
       <c r="A471" s="47" t="s">
         <v>530</v>
       </c>
@@ -20590,6 +20608,9 @@
       <c r="F471" s="48" t="s">
         <v>306</v>
       </c>
+      <c r="G471" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H471" s="2" t="s">
         <v>465</v>
       </c>
@@ -20609,7 +20630,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="472" spans="1:14">
+    <row r="472" spans="1:16">
       <c r="A472" s="47" t="s">
         <v>530</v>
       </c>
@@ -20625,6 +20646,9 @@
       <c r="F472" s="48" t="s">
         <v>67</v>
       </c>
+      <c r="G472" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H472" s="2" t="s">
         <v>465</v>
       </c>
@@ -20641,6 +20665,109 @@
         <v>419</v>
       </c>
       <c r="N472" s="51" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="473" spans="1:16">
+      <c r="A473" s="47" t="s">
+        <v>529</v>
+      </c>
+      <c r="B473" s="96" t="s">
+        <v>528</v>
+      </c>
+      <c r="C473" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D473" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F473" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G473" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I473" s="49">
+        <v>298</v>
+      </c>
+      <c r="J473" s="4">
+        <f t="shared" ref="J473" si="15">P473*9807000</f>
+        <v>5187903000</v>
+      </c>
+      <c r="L473" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M473" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="N473" s="51" t="s">
+        <v>527</v>
+      </c>
+      <c r="P473" s="6">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="474" spans="1:16">
+      <c r="B474" s="96" t="s">
+        <v>528</v>
+      </c>
+      <c r="C474" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D474" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F474" s="48" t="s">
+        <v>245</v>
+      </c>
+      <c r="G474" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I474" s="49">
+        <v>298</v>
+      </c>
+      <c r="J474" s="50">
+        <v>8440000000</v>
+      </c>
+      <c r="L474" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M474" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="N474" s="51" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="475" spans="1:16">
+      <c r="B475" s="96" t="s">
+        <v>528</v>
+      </c>
+      <c r="C475" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D475" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F475" s="48" t="s">
+        <v>246</v>
+      </c>
+      <c r="G475" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I475" s="49">
+        <v>298</v>
+      </c>
+      <c r="J475" s="50">
+        <v>171100000000</v>
+      </c>
+      <c r="L475" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M475" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="N475" s="51" t="s">
         <v>527</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- extracted structural data from `10.1080/00295450.2023.2236796`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43288FCF-284F-614F-BF4C-2A6EEECF8D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918551AC-049C-9349-8DB8-E78BA608B08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4317" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4337" uniqueCount="560">
   <si>
     <t>Metadata</t>
   </si>
@@ -1775,6 +1775,36 @@
   </si>
   <si>
     <t>UNb0.5Zr0.5Ti0.5Mo0.5</t>
+  </si>
+  <si>
+    <t>10.1080/00295450.2023.2236796</t>
+  </si>
+  <si>
+    <t>MoNbTaU2</t>
+  </si>
+  <si>
+    <t>MoNbTiU2</t>
+  </si>
+  <si>
+    <t>NbTiVU2</t>
+  </si>
+  <si>
+    <t>NbTaVU2</t>
+  </si>
+  <si>
+    <t>BCC+BCC+BCC</t>
+  </si>
+  <si>
+    <t>Mo-rich BCC, MoNbTa-rich BCC, and U-rich BCC</t>
+  </si>
+  <si>
+    <t>MoNbTi-rich BCC and U-rich BCC</t>
+  </si>
+  <si>
+    <t>MoTiV-rich BCC and U-rich BCC</t>
+  </si>
+  <si>
+    <t>MoTaV-rich BCC and U-rich BCC</t>
   </si>
 </sst>
 </file>
@@ -2992,10 +3022,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T502"/>
+  <dimension ref="A1:T506"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A459" zoomScale="89" workbookViewId="0">
-      <selection activeCell="M507" sqref="M507"/>
+      <selection activeCell="N513" sqref="N513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -21745,6 +21775,74 @@
         <v>535</v>
       </c>
     </row>
+    <row r="503" spans="2:16">
+      <c r="B503" s="96" t="s">
+        <v>551</v>
+      </c>
+      <c r="C503" s="48" t="s">
+        <v>555</v>
+      </c>
+      <c r="D503" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="F503" s="48" t="s">
+        <v>556</v>
+      </c>
+      <c r="N503" s="51" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="504" spans="2:16">
+      <c r="B504" s="96" t="s">
+        <v>552</v>
+      </c>
+      <c r="C504" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D504" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="F504" s="48" t="s">
+        <v>557</v>
+      </c>
+      <c r="N504" s="51" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="505" spans="2:16">
+      <c r="B505" s="96" t="s">
+        <v>553</v>
+      </c>
+      <c r="C505" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D505" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="F505" s="48" t="s">
+        <v>558</v>
+      </c>
+      <c r="N505" s="51" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="506" spans="2:16">
+      <c r="B506" s="96" t="s">
+        <v>554</v>
+      </c>
+      <c r="C506" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D506" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="F506" s="48" t="s">
+        <v>559</v>
+      </c>
+      <c r="N506" s="51" t="s">
+        <v>550</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="D2:E3"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1016/j.nanoso.2024.101391`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918551AC-049C-9349-8DB8-E78BA608B08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71260EE-7E36-3B42-BDBB-1AAFF47AA551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4337" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4342" uniqueCount="563">
   <si>
     <t>Metadata</t>
   </si>
@@ -1805,6 +1805,15 @@
   </si>
   <si>
     <t>MoTaV-rich BCC and U-rich BCC</t>
+  </si>
+  <si>
+    <t>Cu40Zn24Ni24Ag8Hg4</t>
+  </si>
+  <si>
+    <t>high purity Hg amalgamed with Ag and then ball milled with other powders for 12h (single phase after 6h); interesting based on antimicrobial properties</t>
+  </si>
+  <si>
+    <t>10.1016/j.nanoso.2024.101391</t>
   </si>
 </sst>
 </file>
@@ -3022,10 +3031,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T506"/>
+  <dimension ref="A1:T507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A459" zoomScale="89" workbookViewId="0">
-      <selection activeCell="N513" sqref="N513"/>
+    <sheetView tabSelected="1" topLeftCell="A471" zoomScale="89" workbookViewId="0">
+      <selection activeCell="G524" sqref="G524"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -21843,6 +21852,23 @@
         <v>550</v>
       </c>
     </row>
+    <row r="507" spans="2:16">
+      <c r="B507" s="96" t="s">
+        <v>560</v>
+      </c>
+      <c r="C507" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D507" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="F507" s="48" t="s">
+        <v>561</v>
+      </c>
+      <c r="N507" s="51" t="s">
+        <v>562</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="D2:E3"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1016/j.intermet.2021.107167`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71260EE-7E36-3B42-BDBB-1AAFF47AA551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E96B49-57BD-5E43-BC54-8B63727AD3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4342" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4538" uniqueCount="572">
   <si>
     <t>Metadata</t>
   </si>
@@ -1814,6 +1814,33 @@
   </si>
   <si>
     <t>10.1016/j.nanoso.2024.101391</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2021.107167</t>
+  </si>
+  <si>
+    <t>VAM+H+WQ</t>
+  </si>
+  <si>
+    <t>homogenized at 1273K for 24h and water quenched</t>
+  </si>
+  <si>
+    <t>CoCrFeNi</t>
+  </si>
+  <si>
+    <t>CoCrFeNiGe0.1</t>
+  </si>
+  <si>
+    <t>CoCrFeNiGe0.2</t>
+  </si>
+  <si>
+    <t>CoCrFeNiGe0.3</t>
+  </si>
+  <si>
+    <t>youngs modulus</t>
+  </si>
+  <si>
+    <t>tensile yield stress</t>
   </si>
 </sst>
 </file>
@@ -3031,10 +3058,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T507"/>
+  <dimension ref="A1:T527"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A471" zoomScale="89" workbookViewId="0">
-      <selection activeCell="G524" sqref="G524"/>
+    <sheetView tabSelected="1" topLeftCell="A481" zoomScale="89" workbookViewId="0">
+      <selection activeCell="K535" sqref="K535"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -21584,7 +21611,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="497" spans="2:16">
+    <row r="497" spans="2:17">
       <c r="B497" s="96" t="s">
         <v>546</v>
       </c>
@@ -21616,7 +21643,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="498" spans="2:16">
+    <row r="498" spans="2:17">
       <c r="B498" s="96" t="s">
         <v>547</v>
       </c>
@@ -21648,7 +21675,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="499" spans="2:16">
+    <row r="499" spans="2:17">
       <c r="B499" s="96" t="s">
         <v>548</v>
       </c>
@@ -21684,7 +21711,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="500" spans="2:16">
+    <row r="500" spans="2:17">
       <c r="B500" s="96" t="s">
         <v>549</v>
       </c>
@@ -21720,7 +21747,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="501" spans="2:16">
+    <row r="501" spans="2:17">
       <c r="B501" s="96" t="s">
         <v>548</v>
       </c>
@@ -21752,7 +21779,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="502" spans="2:16">
+    <row r="502" spans="2:17">
       <c r="B502" s="96" t="s">
         <v>549</v>
       </c>
@@ -21784,7 +21811,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="503" spans="2:16">
+    <row r="503" spans="2:17">
       <c r="B503" s="96" t="s">
         <v>551</v>
       </c>
@@ -21794,14 +21821,14 @@
       <c r="D503" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="F503" s="48" t="s">
+      <c r="E503" s="48" t="s">
         <v>556</v>
       </c>
       <c r="N503" s="51" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="504" spans="2:16">
+    <row r="504" spans="2:17">
       <c r="B504" s="96" t="s">
         <v>552</v>
       </c>
@@ -21811,14 +21838,14 @@
       <c r="D504" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="F504" s="48" t="s">
+      <c r="E504" s="48" t="s">
         <v>557</v>
       </c>
       <c r="N504" s="51" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="505" spans="2:16">
+    <row r="505" spans="2:17">
       <c r="B505" s="96" t="s">
         <v>553</v>
       </c>
@@ -21828,14 +21855,14 @@
       <c r="D505" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="F505" s="48" t="s">
+      <c r="E505" s="48" t="s">
         <v>558</v>
       </c>
       <c r="N505" s="51" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="506" spans="2:16">
+    <row r="506" spans="2:17">
       <c r="B506" s="96" t="s">
         <v>554</v>
       </c>
@@ -21845,14 +21872,14 @@
       <c r="D506" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="F506" s="48" t="s">
+      <c r="E506" s="48" t="s">
         <v>559</v>
       </c>
       <c r="N506" s="51" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="507" spans="2:16">
+    <row r="507" spans="2:17">
       <c r="B507" s="96" t="s">
         <v>560</v>
       </c>
@@ -21862,11 +21889,851 @@
       <c r="D507" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="F507" s="48" t="s">
+      <c r="E507" s="48" t="s">
         <v>561</v>
       </c>
       <c r="N507" s="51" t="s">
         <v>562</v>
+      </c>
+    </row>
+    <row r="508" spans="2:17">
+      <c r="B508" s="96" t="s">
+        <v>566</v>
+      </c>
+      <c r="C508" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D508" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E508" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F508" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G508" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I508" s="49">
+        <v>298</v>
+      </c>
+      <c r="J508" s="4">
+        <f t="shared" ref="J508:K511" si="19">P508*9807000</f>
+        <v>1078770000</v>
+      </c>
+      <c r="K508" s="4">
+        <f t="shared" si="19"/>
+        <v>29421000</v>
+      </c>
+      <c r="L508" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M508" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N508" s="51" t="s">
+        <v>563</v>
+      </c>
+      <c r="P508" s="6">
+        <v>110</v>
+      </c>
+      <c r="Q508" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="509" spans="2:17">
+      <c r="B509" t="s">
+        <v>567</v>
+      </c>
+      <c r="C509" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D509" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E509" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F509" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G509" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I509" s="49">
+        <v>298</v>
+      </c>
+      <c r="J509" s="4">
+        <f t="shared" si="19"/>
+        <v>1108191000</v>
+      </c>
+      <c r="K509" s="4">
+        <f t="shared" si="19"/>
+        <v>29421000</v>
+      </c>
+      <c r="L509" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M509" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N509" s="51" t="s">
+        <v>563</v>
+      </c>
+      <c r="P509" s="6">
+        <v>113</v>
+      </c>
+      <c r="Q509" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="510" spans="2:17">
+      <c r="B510" t="s">
+        <v>568</v>
+      </c>
+      <c r="C510" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D510" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E510" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F510" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G510" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I510" s="49">
+        <v>298</v>
+      </c>
+      <c r="J510" s="4">
+        <f t="shared" si="19"/>
+        <v>1157226000</v>
+      </c>
+      <c r="K510" s="4">
+        <f t="shared" si="19"/>
+        <v>29421000</v>
+      </c>
+      <c r="L510" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M510" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N510" s="51" t="s">
+        <v>563</v>
+      </c>
+      <c r="P510" s="6">
+        <v>118</v>
+      </c>
+      <c r="Q510" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="511" spans="2:17">
+      <c r="B511" t="s">
+        <v>569</v>
+      </c>
+      <c r="C511" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D511" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E511" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F511" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G511" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I511" s="49">
+        <v>298</v>
+      </c>
+      <c r="J511" s="4">
+        <f t="shared" si="19"/>
+        <v>1167033000</v>
+      </c>
+      <c r="K511" s="4">
+        <f t="shared" si="19"/>
+        <v>19614000</v>
+      </c>
+      <c r="L511" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M511" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N511" s="51" t="s">
+        <v>563</v>
+      </c>
+      <c r="P511" s="6">
+        <v>119</v>
+      </c>
+      <c r="Q511" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="512" spans="2:17">
+      <c r="B512" s="96" t="s">
+        <v>566</v>
+      </c>
+      <c r="C512" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D512" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E512" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F512" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="G512" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H512" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I512" s="49">
+        <v>298</v>
+      </c>
+      <c r="J512" s="50">
+        <v>214000000000</v>
+      </c>
+      <c r="K512" s="50">
+        <v>11000000000</v>
+      </c>
+      <c r="L512" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M512" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N512" s="51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="513" spans="2:14">
+      <c r="B513" t="s">
+        <v>567</v>
+      </c>
+      <c r="C513" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D513" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E513" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F513" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="G513" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H513" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I513" s="49">
+        <v>298</v>
+      </c>
+      <c r="J513" s="50">
+        <v>217000000000</v>
+      </c>
+      <c r="K513" s="50">
+        <v>8000000000</v>
+      </c>
+      <c r="L513" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M513" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N513" s="51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="514" spans="2:14">
+      <c r="B514" t="s">
+        <v>568</v>
+      </c>
+      <c r="C514" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D514" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E514" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F514" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="G514" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H514" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I514" s="49">
+        <v>298</v>
+      </c>
+      <c r="J514" s="50">
+        <v>218000000000</v>
+      </c>
+      <c r="K514" s="50">
+        <v>10000000000</v>
+      </c>
+      <c r="L514" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M514" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N514" s="51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="515" spans="2:14">
+      <c r="B515" t="s">
+        <v>569</v>
+      </c>
+      <c r="C515" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D515" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E515" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F515" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="G515" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H515" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I515" s="49">
+        <v>298</v>
+      </c>
+      <c r="J515" s="50">
+        <v>217000000000</v>
+      </c>
+      <c r="K515" s="50">
+        <v>13000000000</v>
+      </c>
+      <c r="L515" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M515" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N515" s="51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="516" spans="2:14">
+      <c r="B516" s="96" t="s">
+        <v>566</v>
+      </c>
+      <c r="C516" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D516" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E516" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F516" s="48" t="s">
+        <v>571</v>
+      </c>
+      <c r="G516" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H516" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I516" s="49">
+        <v>298</v>
+      </c>
+      <c r="J516" s="50">
+        <v>209000000</v>
+      </c>
+      <c r="K516" s="50">
+        <v>8000000</v>
+      </c>
+      <c r="L516" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M516" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N516" s="51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="517" spans="2:14">
+      <c r="B517" t="s">
+        <v>567</v>
+      </c>
+      <c r="C517" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D517" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E517" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F517" s="48" t="s">
+        <v>571</v>
+      </c>
+      <c r="G517" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H517" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I517" s="49">
+        <v>298</v>
+      </c>
+      <c r="J517" s="50">
+        <v>213000000</v>
+      </c>
+      <c r="K517" s="50">
+        <v>9000000</v>
+      </c>
+      <c r="L517" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M517" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N517" s="51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="518" spans="2:14">
+      <c r="B518" t="s">
+        <v>568</v>
+      </c>
+      <c r="C518" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D518" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E518" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F518" s="48" t="s">
+        <v>571</v>
+      </c>
+      <c r="G518" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H518" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I518" s="49">
+        <v>298</v>
+      </c>
+      <c r="J518" s="50">
+        <v>218000000</v>
+      </c>
+      <c r="K518" s="50">
+        <v>12000000</v>
+      </c>
+      <c r="L518" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M518" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N518" s="51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="519" spans="2:14">
+      <c r="B519" t="s">
+        <v>569</v>
+      </c>
+      <c r="C519" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D519" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E519" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F519" s="48" t="s">
+        <v>571</v>
+      </c>
+      <c r="G519" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H519" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I519" s="49">
+        <v>298</v>
+      </c>
+      <c r="J519" s="50">
+        <v>223000000</v>
+      </c>
+      <c r="K519" s="50">
+        <v>3000000</v>
+      </c>
+      <c r="L519" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M519" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N519" s="51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="520" spans="2:14">
+      <c r="B520" s="96" t="s">
+        <v>566</v>
+      </c>
+      <c r="C520" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D520" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E520" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F520" s="48" t="s">
+        <v>229</v>
+      </c>
+      <c r="G520" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H520" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I520" s="49">
+        <v>298</v>
+      </c>
+      <c r="J520" s="50">
+        <v>590000000</v>
+      </c>
+      <c r="K520" s="50">
+        <v>16000000</v>
+      </c>
+      <c r="L520" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M520" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N520" s="51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="521" spans="2:14">
+      <c r="B521" t="s">
+        <v>567</v>
+      </c>
+      <c r="C521" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D521" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E521" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F521" s="48" t="s">
+        <v>229</v>
+      </c>
+      <c r="G521" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H521" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I521" s="49">
+        <v>298</v>
+      </c>
+      <c r="J521" s="50">
+        <v>592000000</v>
+      </c>
+      <c r="K521" s="50">
+        <v>20000000</v>
+      </c>
+      <c r="L521" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M521" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N521" s="51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="522" spans="2:14">
+      <c r="B522" t="s">
+        <v>568</v>
+      </c>
+      <c r="C522" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D522" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E522" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F522" s="48" t="s">
+        <v>229</v>
+      </c>
+      <c r="G522" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H522" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I522" s="49">
+        <v>298</v>
+      </c>
+      <c r="J522" s="50">
+        <v>596000000</v>
+      </c>
+      <c r="K522" s="50">
+        <v>13000000</v>
+      </c>
+      <c r="L522" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M522" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N522" s="51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="523" spans="2:14">
+      <c r="B523" t="s">
+        <v>569</v>
+      </c>
+      <c r="C523" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D523" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E523" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F523" s="48" t="s">
+        <v>229</v>
+      </c>
+      <c r="G523" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H523" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I523" s="49">
+        <v>298</v>
+      </c>
+      <c r="J523" s="50">
+        <v>617000000</v>
+      </c>
+      <c r="K523" s="50">
+        <v>17000000</v>
+      </c>
+      <c r="L523" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M523" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N523" s="51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="524" spans="2:14">
+      <c r="B524" s="96" t="s">
+        <v>566</v>
+      </c>
+      <c r="C524" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D524" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E524" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F524" s="48" t="s">
+        <v>230</v>
+      </c>
+      <c r="G524" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H524" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I524" s="49">
+        <v>298</v>
+      </c>
+      <c r="J524" s="50">
+        <v>60</v>
+      </c>
+      <c r="K524" s="50">
+        <v>3.2</v>
+      </c>
+      <c r="L524" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M524" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N524" s="51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="525" spans="2:14">
+      <c r="B525" t="s">
+        <v>567</v>
+      </c>
+      <c r="C525" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D525" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E525" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F525" s="48" t="s">
+        <v>230</v>
+      </c>
+      <c r="G525" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H525" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I525" s="49">
+        <v>298</v>
+      </c>
+      <c r="J525" s="50">
+        <v>60.2</v>
+      </c>
+      <c r="K525" s="50">
+        <v>2.5</v>
+      </c>
+      <c r="L525" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M525" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N525" s="51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="526" spans="2:14">
+      <c r="B526" t="s">
+        <v>568</v>
+      </c>
+      <c r="C526" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D526" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E526" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F526" s="48" t="s">
+        <v>230</v>
+      </c>
+      <c r="G526" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H526" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I526" s="49">
+        <v>298</v>
+      </c>
+      <c r="J526" s="50">
+        <v>62.8</v>
+      </c>
+      <c r="K526" s="50">
+        <v>2.1</v>
+      </c>
+      <c r="L526" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M526" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N526" s="51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="527" spans="2:14">
+      <c r="B527" t="s">
+        <v>569</v>
+      </c>
+      <c r="C527" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D527" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="E527" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F527" s="48" t="s">
+        <v>230</v>
+      </c>
+      <c r="G527" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H527" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I527" s="49">
+        <v>298</v>
+      </c>
+      <c r="J527" s="50">
+        <v>63.2</v>
+      </c>
+      <c r="K527" s="50">
+        <v>4.5</v>
+      </c>
+      <c r="L527" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M527" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N527" s="51" t="s">
+        <v>563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.intermet.2021.107167`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E96B49-57BD-5E43-BC54-8B63727AD3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507F0D1B-00F1-494D-8720-59469A39173D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3061,7 +3061,7 @@
   <dimension ref="A1:T527"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A481" zoomScale="89" workbookViewId="0">
-      <selection activeCell="K535" sqref="K535"/>
+      <selection activeCell="E534" sqref="E534"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
- letter typo fix in `10.1007/s42243-024-01338-8`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FCA6D6-DABB-944F-8723-14AB48996C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFA8109-5FEF-024B-8D81-7EC6965F9B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4538" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4760" uniqueCount="593">
   <si>
     <t>Metadata</t>
   </si>
@@ -1841,6 +1841,69 @@
   </si>
   <si>
     <t>Au2.5Ni22.5(CuPdPt)25</t>
+  </si>
+  <si>
+    <t>SnBiIn</t>
+  </si>
+  <si>
+    <t>SnBiInSb0.1</t>
+  </si>
+  <si>
+    <t>SnBiInSb0.2</t>
+  </si>
+  <si>
+    <t>SnBiInSb0.3</t>
+  </si>
+  <si>
+    <t>SnBiInSb0.4</t>
+  </si>
+  <si>
+    <t>SnBiInSb0.5</t>
+  </si>
+  <si>
+    <t>BCT+BiIn+Bi</t>
+  </si>
+  <si>
+    <t>BCT+BiIn+Bi+SbIn</t>
+  </si>
+  <si>
+    <t>induction melt in atmospheric conditions; Sn-rich BCT; BiIn is solid solution with Sn; Bi is pure Bi</t>
+  </si>
+  <si>
+    <t>induction melt in atmospheric conditions; Sn-rich BCT; BiIn is solid solution with Sn; Bi is pure Bi; SbIn is stoichiometric Sb1In1</t>
+  </si>
+  <si>
+    <t>induction melt in atmospheric conditions; Sn-rich BCT; BiIn is solid solution with Sn; Bi is pure Bi; SbIn is stoichiometric Sb1In2</t>
+  </si>
+  <si>
+    <t>induction melt in atmospheric conditions; Sn-rich BCT; BiIn is solid solution with Sn; Bi is pure Bi; SbIn is stoichiometric Sb1In3</t>
+  </si>
+  <si>
+    <t>induction melt in atmospheric conditions; Sn-rich BCT; BiIn is solid solution with Sn; Bi is pure Bi; SbIn is stoichiometric Sb1In4</t>
+  </si>
+  <si>
+    <t>induction melt in atmospheric conditions; Sn-rich BCT; BiIn is solid solution with Sn; Bi is pure Bi; SbIn is stoichiometric Sb1In5</t>
+  </si>
+  <si>
+    <t>melting temperature</t>
+  </si>
+  <si>
+    <t>DTA heating rate of 10K/min</t>
+  </si>
+  <si>
+    <t>F6b</t>
+  </si>
+  <si>
+    <t>10.1007/s42243-024-01338-8</t>
+  </si>
+  <si>
+    <t>F8b</t>
+  </si>
+  <si>
+    <t>F8c</t>
+  </si>
+  <si>
+    <t>F8a</t>
   </si>
 </sst>
 </file>
@@ -2464,7 +2527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2630,6 +2693,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2696,55 +2810,8 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3052,10 +3119,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T527"/>
+  <dimension ref="A1:T551"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A348" zoomScale="89" workbookViewId="0">
-      <selection activeCell="K355" sqref="K355"/>
+    <sheetView tabSelected="1" topLeftCell="A499" zoomScale="89" workbookViewId="0">
+      <selection activeCell="J560" sqref="J560"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3104,19 +3171,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="58"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="65"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="82"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1">
@@ -3127,17 +3194,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="69"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="86"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1">
@@ -3166,43 +3233,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="70" t="s">
+      <c r="C5" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="72" t="s">
+      <c r="D5" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="72" t="s">
+      <c r="F5" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="72" t="s">
+      <c r="G5" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="75" t="s">
+      <c r="I5" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="77" t="s">
+      <c r="J5" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="77" t="s">
+      <c r="K5" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="72" t="s">
+      <c r="L5" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="72" t="s">
+      <c r="M5" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="72" t="s">
+      <c r="N5" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="79" t="s">
+      <c r="O5" s="57" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3213,19 +3280,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="80"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="93"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="88"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="58"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1">
       <c r="A7" s="17" t="s">
@@ -3270,7 +3337,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="81"/>
+      <c r="O7" s="59"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -3283,35 +3350,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="82" t="s">
+      <c r="B8" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="85" t="s">
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="86"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="87"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="90" t="s">
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="91"/>
+      <c r="N8" s="69"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="92" t="s">
+      <c r="P8" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="93"/>
-      <c r="R8" s="94"/>
-      <c r="S8" s="94"/>
-      <c r="T8" s="95"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="72"/>
+      <c r="S8" s="72"/>
+      <c r="T8" s="73"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="26" t="s">
@@ -22115,7 +22182,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="513" spans="2:14">
+    <row r="513" spans="2:16">
       <c r="B513" t="s">
         <v>566</v>
       </c>
@@ -22156,7 +22223,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="514" spans="2:14">
+    <row r="514" spans="2:16">
       <c r="B514" t="s">
         <v>567</v>
       </c>
@@ -22197,7 +22264,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="515" spans="2:14">
+    <row r="515" spans="2:16">
       <c r="B515" t="s">
         <v>568</v>
       </c>
@@ -22238,7 +22305,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="516" spans="2:14">
+    <row r="516" spans="2:16">
       <c r="B516" s="44" t="s">
         <v>565</v>
       </c>
@@ -22279,7 +22346,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="517" spans="2:14">
+    <row r="517" spans="2:16">
       <c r="B517" t="s">
         <v>566</v>
       </c>
@@ -22320,7 +22387,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="518" spans="2:14">
+    <row r="518" spans="2:16">
       <c r="B518" t="s">
         <v>567</v>
       </c>
@@ -22361,7 +22428,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="519" spans="2:14">
+    <row r="519" spans="2:16">
       <c r="B519" t="s">
         <v>568</v>
       </c>
@@ -22402,7 +22469,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="520" spans="2:14">
+    <row r="520" spans="2:16">
       <c r="B520" s="44" t="s">
         <v>565</v>
       </c>
@@ -22443,7 +22510,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="521" spans="2:14">
+    <row r="521" spans="2:16">
       <c r="B521" t="s">
         <v>566</v>
       </c>
@@ -22484,7 +22551,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="522" spans="2:14">
+    <row r="522" spans="2:16">
       <c r="B522" t="s">
         <v>567</v>
       </c>
@@ -22525,7 +22592,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="523" spans="2:14">
+    <row r="523" spans="2:16">
       <c r="B523" t="s">
         <v>568</v>
       </c>
@@ -22566,7 +22633,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="524" spans="2:14">
+    <row r="524" spans="2:16">
       <c r="B524" s="44" t="s">
         <v>565</v>
       </c>
@@ -22607,7 +22674,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="525" spans="2:14">
+    <row r="525" spans="2:16">
       <c r="B525" t="s">
         <v>566</v>
       </c>
@@ -22648,7 +22715,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="526" spans="2:14">
+    <row r="526" spans="2:16">
       <c r="B526" t="s">
         <v>567</v>
       </c>
@@ -22689,7 +22756,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="527" spans="2:14">
+    <row r="527" spans="2:16">
       <c r="B527" t="s">
         <v>568</v>
       </c>
@@ -22730,13 +22797,938 @@
         <v>562</v>
       </c>
     </row>
+    <row r="528" spans="2:16">
+      <c r="B528" t="s">
+        <v>572</v>
+      </c>
+      <c r="C528" s="48" t="s">
+        <v>578</v>
+      </c>
+      <c r="D528" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E528" s="48" t="s">
+        <v>580</v>
+      </c>
+      <c r="F528" s="48" t="s">
+        <v>586</v>
+      </c>
+      <c r="G528" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H528" s="48" t="s">
+        <v>587</v>
+      </c>
+      <c r="J528" s="50">
+        <f>P528+273.15</f>
+        <v>361.65</v>
+      </c>
+      <c r="L528" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M528" s="51" t="s">
+        <v>588</v>
+      </c>
+      <c r="N528" s="51" t="s">
+        <v>589</v>
+      </c>
+      <c r="P528" s="6">
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="529" spans="2:17">
+      <c r="B529" t="s">
+        <v>573</v>
+      </c>
+      <c r="C529" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D529" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E529" s="48" t="s">
+        <v>581</v>
+      </c>
+      <c r="F529" s="48" t="s">
+        <v>586</v>
+      </c>
+      <c r="G529" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H529" s="48" t="s">
+        <v>587</v>
+      </c>
+      <c r="J529" s="50">
+        <f t="shared" ref="J529:J533" si="20">P529+273.15</f>
+        <v>365.45</v>
+      </c>
+      <c r="L529" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M529" s="51" t="s">
+        <v>588</v>
+      </c>
+      <c r="N529" s="51" t="s">
+        <v>589</v>
+      </c>
+      <c r="P529" s="6">
+        <v>92.3</v>
+      </c>
+    </row>
+    <row r="530" spans="2:17">
+      <c r="B530" t="s">
+        <v>574</v>
+      </c>
+      <c r="C530" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D530" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E530" s="48" t="s">
+        <v>582</v>
+      </c>
+      <c r="F530" s="48" t="s">
+        <v>586</v>
+      </c>
+      <c r="G530" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H530" s="48" t="s">
+        <v>587</v>
+      </c>
+      <c r="J530" s="50">
+        <f t="shared" si="20"/>
+        <v>366.75</v>
+      </c>
+      <c r="L530" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M530" s="51" t="s">
+        <v>588</v>
+      </c>
+      <c r="N530" s="51" t="s">
+        <v>589</v>
+      </c>
+      <c r="P530" s="6">
+        <v>93.6</v>
+      </c>
+    </row>
+    <row r="531" spans="2:17">
+      <c r="B531" t="s">
+        <v>575</v>
+      </c>
+      <c r="C531" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D531" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E531" s="48" t="s">
+        <v>583</v>
+      </c>
+      <c r="F531" s="48" t="s">
+        <v>586</v>
+      </c>
+      <c r="G531" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H531" s="48" t="s">
+        <v>587</v>
+      </c>
+      <c r="J531" s="50">
+        <f t="shared" si="20"/>
+        <v>370.95</v>
+      </c>
+      <c r="L531" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M531" s="51" t="s">
+        <v>588</v>
+      </c>
+      <c r="N531" s="51" t="s">
+        <v>589</v>
+      </c>
+      <c r="P531" s="6">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="532" spans="2:17">
+      <c r="B532" t="s">
+        <v>576</v>
+      </c>
+      <c r="C532" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D532" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E532" s="48" t="s">
+        <v>584</v>
+      </c>
+      <c r="F532" s="48" t="s">
+        <v>586</v>
+      </c>
+      <c r="G532" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H532" s="48" t="s">
+        <v>587</v>
+      </c>
+      <c r="J532" s="50">
+        <f t="shared" si="20"/>
+        <v>374.34999999999997</v>
+      </c>
+      <c r="L532" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M532" s="51" t="s">
+        <v>588</v>
+      </c>
+      <c r="N532" s="51" t="s">
+        <v>589</v>
+      </c>
+      <c r="P532" s="6">
+        <v>101.2</v>
+      </c>
+    </row>
+    <row r="533" spans="2:17">
+      <c r="B533" t="s">
+        <v>577</v>
+      </c>
+      <c r="C533" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D533" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E533" s="48" t="s">
+        <v>585</v>
+      </c>
+      <c r="F533" s="48" t="s">
+        <v>586</v>
+      </c>
+      <c r="G533" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H533" s="48" t="s">
+        <v>587</v>
+      </c>
+      <c r="J533" s="50">
+        <f t="shared" si="20"/>
+        <v>380.45</v>
+      </c>
+      <c r="L533" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M533" s="51" t="s">
+        <v>588</v>
+      </c>
+      <c r="N533" s="51" t="s">
+        <v>589</v>
+      </c>
+      <c r="P533" s="6">
+        <v>107.3</v>
+      </c>
+    </row>
+    <row r="534" spans="2:17">
+      <c r="B534" t="s">
+        <v>572</v>
+      </c>
+      <c r="C534" s="48" t="s">
+        <v>578</v>
+      </c>
+      <c r="D534" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E534" s="48" t="s">
+        <v>580</v>
+      </c>
+      <c r="F534" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G534" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I534" s="49">
+        <v>298</v>
+      </c>
+      <c r="J534" s="50">
+        <v>38800000</v>
+      </c>
+      <c r="L534" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M534" s="51" t="s">
+        <v>590</v>
+      </c>
+      <c r="N534" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="535" spans="2:17">
+      <c r="B535" t="s">
+        <v>573</v>
+      </c>
+      <c r="C535" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D535" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E535" s="48" t="s">
+        <v>581</v>
+      </c>
+      <c r="F535" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G535" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I535" s="49">
+        <v>298</v>
+      </c>
+      <c r="J535" s="50">
+        <v>48600000</v>
+      </c>
+      <c r="L535" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M535" s="51" t="s">
+        <v>590</v>
+      </c>
+      <c r="N535" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="536" spans="2:17">
+      <c r="B536" t="s">
+        <v>574</v>
+      </c>
+      <c r="C536" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D536" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E536" s="48" t="s">
+        <v>582</v>
+      </c>
+      <c r="F536" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G536" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I536" s="49">
+        <v>298</v>
+      </c>
+      <c r="J536" s="50">
+        <v>51600000</v>
+      </c>
+      <c r="L536" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M536" s="51" t="s">
+        <v>590</v>
+      </c>
+      <c r="N536" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="537" spans="2:17">
+      <c r="B537" t="s">
+        <v>575</v>
+      </c>
+      <c r="C537" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D537" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E537" s="48" t="s">
+        <v>583</v>
+      </c>
+      <c r="F537" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G537" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I537" s="49">
+        <v>298</v>
+      </c>
+      <c r="J537" s="50">
+        <v>67500000</v>
+      </c>
+      <c r="L537" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M537" s="51" t="s">
+        <v>590</v>
+      </c>
+      <c r="N537" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="538" spans="2:17">
+      <c r="B538" t="s">
+        <v>576</v>
+      </c>
+      <c r="C538" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D538" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E538" s="48" t="s">
+        <v>584</v>
+      </c>
+      <c r="F538" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G538" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I538" s="49">
+        <v>298</v>
+      </c>
+      <c r="J538" s="50">
+        <v>63100000</v>
+      </c>
+      <c r="L538" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M538" s="51" t="s">
+        <v>590</v>
+      </c>
+      <c r="N538" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="539" spans="2:17">
+      <c r="B539" t="s">
+        <v>577</v>
+      </c>
+      <c r="C539" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D539" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E539" s="48" t="s">
+        <v>585</v>
+      </c>
+      <c r="F539" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G539" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I539" s="49">
+        <v>298</v>
+      </c>
+      <c r="J539" s="50">
+        <v>55200000</v>
+      </c>
+      <c r="L539" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M539" s="51" t="s">
+        <v>590</v>
+      </c>
+      <c r="N539" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="540" spans="2:17">
+      <c r="B540" t="s">
+        <v>572</v>
+      </c>
+      <c r="C540" s="48" t="s">
+        <v>578</v>
+      </c>
+      <c r="D540" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E540" s="48" t="s">
+        <v>580</v>
+      </c>
+      <c r="F540" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G540" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I540" s="49">
+        <v>298</v>
+      </c>
+      <c r="J540" s="4">
+        <f t="shared" ref="J540:K540" si="21">P540*9807000</f>
+        <v>59528490</v>
+      </c>
+      <c r="K540" s="4">
+        <f t="shared" si="21"/>
+        <v>1961400</v>
+      </c>
+      <c r="L540" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M540" s="51" t="s">
+        <v>591</v>
+      </c>
+      <c r="N540" s="51" t="s">
+        <v>589</v>
+      </c>
+      <c r="P540" s="6">
+        <v>6.07</v>
+      </c>
+      <c r="Q540" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="541" spans="2:17">
+      <c r="B541" t="s">
+        <v>573</v>
+      </c>
+      <c r="C541" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D541" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E541" s="48" t="s">
+        <v>581</v>
+      </c>
+      <c r="F541" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G541" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I541" s="49">
+        <v>298</v>
+      </c>
+      <c r="J541" s="4">
+        <f t="shared" ref="J541:J545" si="22">P541*9807000</f>
+        <v>66001110.000000007</v>
+      </c>
+      <c r="K541" s="4">
+        <f t="shared" ref="K541:K545" si="23">Q541*9807000</f>
+        <v>1961400</v>
+      </c>
+      <c r="L541" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M541" s="51" t="s">
+        <v>591</v>
+      </c>
+      <c r="N541" s="51" t="s">
+        <v>589</v>
+      </c>
+      <c r="P541" s="6">
+        <v>6.73</v>
+      </c>
+      <c r="Q541" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="542" spans="2:17">
+      <c r="B542" t="s">
+        <v>574</v>
+      </c>
+      <c r="C542" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D542" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E542" s="48" t="s">
+        <v>582</v>
+      </c>
+      <c r="F542" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G542" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I542" s="49">
+        <v>298</v>
+      </c>
+      <c r="J542" s="4">
+        <f t="shared" si="22"/>
+        <v>67668300</v>
+      </c>
+      <c r="K542" s="4">
+        <f t="shared" si="23"/>
+        <v>2451750</v>
+      </c>
+      <c r="L542" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M542" s="51" t="s">
+        <v>591</v>
+      </c>
+      <c r="N542" s="51" t="s">
+        <v>589</v>
+      </c>
+      <c r="P542" s="6">
+        <v>6.9</v>
+      </c>
+      <c r="Q542" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="543" spans="2:17">
+      <c r="B543" t="s">
+        <v>575</v>
+      </c>
+      <c r="C543" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D543" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E543" s="48" t="s">
+        <v>583</v>
+      </c>
+      <c r="F543" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G543" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I543" s="49">
+        <v>298</v>
+      </c>
+      <c r="J543" s="4">
+        <f t="shared" si="22"/>
+        <v>75513900</v>
+      </c>
+      <c r="K543" s="4">
+        <f t="shared" si="23"/>
+        <v>1961400</v>
+      </c>
+      <c r="L543" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M543" s="51" t="s">
+        <v>591</v>
+      </c>
+      <c r="N543" s="51" t="s">
+        <v>589</v>
+      </c>
+      <c r="P543" s="6">
+        <v>7.7</v>
+      </c>
+      <c r="Q543" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="544" spans="2:17">
+      <c r="B544" t="s">
+        <v>576</v>
+      </c>
+      <c r="C544" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D544" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E544" s="48" t="s">
+        <v>584</v>
+      </c>
+      <c r="F544" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G544" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I544" s="49">
+        <v>298</v>
+      </c>
+      <c r="J544" s="4">
+        <f t="shared" si="22"/>
+        <v>77867580</v>
+      </c>
+      <c r="K544" s="4">
+        <f t="shared" si="23"/>
+        <v>1471050</v>
+      </c>
+      <c r="L544" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M544" s="51" t="s">
+        <v>591</v>
+      </c>
+      <c r="N544" s="51" t="s">
+        <v>589</v>
+      </c>
+      <c r="P544" s="6">
+        <v>7.94</v>
+      </c>
+      <c r="Q544" s="6">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="545" spans="2:17">
+      <c r="B545" t="s">
+        <v>577</v>
+      </c>
+      <c r="C545" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D545" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E545" s="48" t="s">
+        <v>585</v>
+      </c>
+      <c r="F545" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G545" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I545" s="49">
+        <v>298</v>
+      </c>
+      <c r="J545" s="4">
+        <f t="shared" si="22"/>
+        <v>85320900</v>
+      </c>
+      <c r="K545" s="4">
+        <f t="shared" si="23"/>
+        <v>2451750</v>
+      </c>
+      <c r="L545" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M545" s="51" t="s">
+        <v>591</v>
+      </c>
+      <c r="N545" s="51" t="s">
+        <v>589</v>
+      </c>
+      <c r="P545" s="6">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="Q545" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="546" spans="2:17">
+      <c r="B546" s="96" t="s">
+        <v>572</v>
+      </c>
+      <c r="C546" s="97" t="s">
+        <v>578</v>
+      </c>
+      <c r="D546" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E546" s="97" t="s">
+        <v>580</v>
+      </c>
+      <c r="F546" s="48" t="s">
+        <v>315</v>
+      </c>
+      <c r="G546" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I546" s="49">
+        <v>298</v>
+      </c>
+      <c r="J546" s="50">
+        <v>50</v>
+      </c>
+      <c r="L546" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M546" s="51" t="s">
+        <v>592</v>
+      </c>
+      <c r="N546" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="547" spans="2:17">
+      <c r="B547" s="96" t="s">
+        <v>573</v>
+      </c>
+      <c r="C547" s="97" t="s">
+        <v>579</v>
+      </c>
+      <c r="D547" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E547" s="97" t="s">
+        <v>581</v>
+      </c>
+      <c r="F547" s="48" t="s">
+        <v>315</v>
+      </c>
+      <c r="G547" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I547" s="49">
+        <v>298</v>
+      </c>
+      <c r="J547" s="50">
+        <v>50</v>
+      </c>
+      <c r="L547" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M547" s="51" t="s">
+        <v>592</v>
+      </c>
+      <c r="N547" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="548" spans="2:17">
+      <c r="B548" s="96" t="s">
+        <v>574</v>
+      </c>
+      <c r="C548" s="97" t="s">
+        <v>579</v>
+      </c>
+      <c r="D548" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E548" s="97" t="s">
+        <v>582</v>
+      </c>
+      <c r="F548" s="48" t="s">
+        <v>315</v>
+      </c>
+      <c r="G548" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I548" s="49">
+        <v>298</v>
+      </c>
+      <c r="J548" s="50">
+        <v>50</v>
+      </c>
+      <c r="L548" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M548" s="51" t="s">
+        <v>592</v>
+      </c>
+      <c r="N548" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="549" spans="2:17">
+      <c r="B549" s="96" t="s">
+        <v>575</v>
+      </c>
+      <c r="C549" s="97" t="s">
+        <v>579</v>
+      </c>
+      <c r="D549" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E549" s="97" t="s">
+        <v>583</v>
+      </c>
+      <c r="F549" s="48" t="s">
+        <v>315</v>
+      </c>
+      <c r="G549" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I549" s="49">
+        <v>298</v>
+      </c>
+      <c r="J549" s="50">
+        <v>50</v>
+      </c>
+      <c r="L549" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M549" s="51" t="s">
+        <v>592</v>
+      </c>
+      <c r="N549" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="550" spans="2:17">
+      <c r="B550" s="96" t="s">
+        <v>576</v>
+      </c>
+      <c r="C550" s="97" t="s">
+        <v>579</v>
+      </c>
+      <c r="D550" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E550" s="97" t="s">
+        <v>584</v>
+      </c>
+      <c r="F550" s="48" t="s">
+        <v>315</v>
+      </c>
+      <c r="G550" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I550" s="49">
+        <v>298</v>
+      </c>
+      <c r="J550" s="50">
+        <v>50</v>
+      </c>
+      <c r="L550" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M550" s="51" t="s">
+        <v>592</v>
+      </c>
+      <c r="N550" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="551" spans="2:17">
+      <c r="B551" s="96" t="s">
+        <v>577</v>
+      </c>
+      <c r="C551" s="97" t="s">
+        <v>579</v>
+      </c>
+      <c r="D551" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E551" s="97" t="s">
+        <v>585</v>
+      </c>
+      <c r="F551" s="48" t="s">
+        <v>315</v>
+      </c>
+      <c r="G551" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I551" s="49">
+        <v>298</v>
+      </c>
+      <c r="J551" s="50">
+        <v>50</v>
+      </c>
+      <c r="L551" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M551" s="51" t="s">
+        <v>592</v>
+      </c>
+      <c r="N551" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -22751,6 +23743,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- additional data from `10.1007/s42243-024-01338-8`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFA8109-5FEF-024B-8D81-7EC6965F9B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E594DFC-4CAB-ED4D-9436-8FC34023F884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4760" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4814" uniqueCount="596">
   <si>
     <t>Metadata</t>
   </si>
@@ -1904,6 +1904,15 @@
   </si>
   <si>
     <t>F8a</t>
+  </si>
+  <si>
+    <t>contact angle on copper</t>
+  </si>
+  <si>
+    <t>degree</t>
+  </si>
+  <si>
+    <t>F7a</t>
   </si>
 </sst>
 </file>
@@ -3119,10 +3128,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T551"/>
+  <dimension ref="A1:T557"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A499" zoomScale="89" workbookViewId="0">
-      <selection activeCell="J560" sqref="J560"/>
+    <sheetView tabSelected="1" topLeftCell="A516" zoomScale="89" workbookViewId="0">
+      <selection activeCell="N563" sqref="N563"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -23727,6 +23736,234 @@
         <v>589</v>
       </c>
     </row>
+    <row r="552" spans="2:17">
+      <c r="B552" s="96" t="s">
+        <v>572</v>
+      </c>
+      <c r="C552" s="97" t="s">
+        <v>578</v>
+      </c>
+      <c r="D552" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E552" s="97" t="s">
+        <v>580</v>
+      </c>
+      <c r="F552" s="48" t="s">
+        <v>593</v>
+      </c>
+      <c r="G552" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I552" s="49">
+        <v>298</v>
+      </c>
+      <c r="J552" s="50">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="K552" s="50">
+        <v>0.6</v>
+      </c>
+      <c r="L552" s="51" t="s">
+        <v>594</v>
+      </c>
+      <c r="M552" s="51" t="s">
+        <v>595</v>
+      </c>
+      <c r="N552" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="553" spans="2:17">
+      <c r="B553" s="96" t="s">
+        <v>573</v>
+      </c>
+      <c r="C553" s="97" t="s">
+        <v>579</v>
+      </c>
+      <c r="D553" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E553" s="97" t="s">
+        <v>581</v>
+      </c>
+      <c r="F553" s="48" t="s">
+        <v>593</v>
+      </c>
+      <c r="G553" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I553" s="49">
+        <v>298</v>
+      </c>
+      <c r="J553" s="50">
+        <v>40.9</v>
+      </c>
+      <c r="K553" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="L553" s="51" t="s">
+        <v>594</v>
+      </c>
+      <c r="M553" s="51" t="s">
+        <v>595</v>
+      </c>
+      <c r="N553" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="554" spans="2:17">
+      <c r="B554" s="96" t="s">
+        <v>574</v>
+      </c>
+      <c r="C554" s="97" t="s">
+        <v>579</v>
+      </c>
+      <c r="D554" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E554" s="97" t="s">
+        <v>582</v>
+      </c>
+      <c r="F554" s="48" t="s">
+        <v>593</v>
+      </c>
+      <c r="G554" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I554" s="49">
+        <v>298</v>
+      </c>
+      <c r="J554" s="50">
+        <v>42.6</v>
+      </c>
+      <c r="K554" s="50">
+        <v>0.3</v>
+      </c>
+      <c r="L554" s="51" t="s">
+        <v>594</v>
+      </c>
+      <c r="M554" s="51" t="s">
+        <v>595</v>
+      </c>
+      <c r="N554" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="555" spans="2:17">
+      <c r="B555" s="96" t="s">
+        <v>575</v>
+      </c>
+      <c r="C555" s="97" t="s">
+        <v>579</v>
+      </c>
+      <c r="D555" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E555" s="97" t="s">
+        <v>583</v>
+      </c>
+      <c r="F555" s="48" t="s">
+        <v>593</v>
+      </c>
+      <c r="G555" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I555" s="49">
+        <v>298</v>
+      </c>
+      <c r="J555" s="50">
+        <v>48.3</v>
+      </c>
+      <c r="K555" s="50">
+        <v>0.4</v>
+      </c>
+      <c r="L555" s="51" t="s">
+        <v>594</v>
+      </c>
+      <c r="M555" s="51" t="s">
+        <v>595</v>
+      </c>
+      <c r="N555" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="556" spans="2:17">
+      <c r="B556" s="96" t="s">
+        <v>576</v>
+      </c>
+      <c r="C556" s="97" t="s">
+        <v>579</v>
+      </c>
+      <c r="D556" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E556" s="97" t="s">
+        <v>584</v>
+      </c>
+      <c r="F556" s="48" t="s">
+        <v>593</v>
+      </c>
+      <c r="G556" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I556" s="49">
+        <v>298</v>
+      </c>
+      <c r="J556" s="50">
+        <v>57</v>
+      </c>
+      <c r="K556" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="L556" s="51" t="s">
+        <v>594</v>
+      </c>
+      <c r="M556" s="51" t="s">
+        <v>595</v>
+      </c>
+      <c r="N556" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="557" spans="2:17">
+      <c r="B557" s="96" t="s">
+        <v>577</v>
+      </c>
+      <c r="C557" s="97" t="s">
+        <v>579</v>
+      </c>
+      <c r="D557" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E557" s="97" t="s">
+        <v>585</v>
+      </c>
+      <c r="F557" s="48" t="s">
+        <v>593</v>
+      </c>
+      <c r="G557" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I557" s="49">
+        <v>298</v>
+      </c>
+      <c r="J557" s="50">
+        <v>61.5</v>
+      </c>
+      <c r="K557" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="L557" s="51" t="s">
+        <v>594</v>
+      </c>
+      <c r="M557" s="51" t="s">
+        <v>595</v>
+      </c>
+      <c r="N557" s="51" t="s">
+        <v>589</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="D2:E3"/>

</xml_diff>

<commit_message>
- extracted data from `10.1109/LMAG.2019.2955667`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E594DFC-4CAB-ED4D-9436-8FC34023F884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A81D305-65F2-3049-9033-358C5783961B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4814" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4831" uniqueCount="601">
   <si>
     <t>Metadata</t>
   </si>
@@ -1913,6 +1913,21 @@
   </si>
   <si>
     <t>F7a</t>
+  </si>
+  <si>
+    <t>Mn27 Cr7 Ni33 Ge25 Si8</t>
+  </si>
+  <si>
+    <t>orthorhombic</t>
+  </si>
+  <si>
+    <t>single unidentified orthorhombic phase (Pnma)</t>
+  </si>
+  <si>
+    <t>1.5T</t>
+  </si>
+  <si>
+    <t>10.1109/LMAG.2019.2955667</t>
   </si>
 </sst>
 </file>
@@ -2536,7 +2551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2821,6 +2836,10 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3128,10 +3147,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T557"/>
+  <dimension ref="A1:T559"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A516" zoomScale="89" workbookViewId="0">
-      <selection activeCell="N563" sqref="N563"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="I561" sqref="I561"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -23964,6 +23983,67 @@
         <v>589</v>
       </c>
     </row>
+    <row r="558" spans="2:17">
+      <c r="B558" s="98" t="s">
+        <v>596</v>
+      </c>
+      <c r="C558" s="48" t="s">
+        <v>597</v>
+      </c>
+      <c r="D558" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="E558" s="99" t="s">
+        <v>598</v>
+      </c>
+      <c r="F558" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="G558" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H558" s="48" t="s">
+        <v>599</v>
+      </c>
+      <c r="J558" s="50">
+        <v>1.99</v>
+      </c>
+      <c r="L558" s="51" t="s">
+        <v>282</v>
+      </c>
+      <c r="N558" s="51" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="559" spans="2:17">
+      <c r="B559" s="98" t="s">
+        <v>596</v>
+      </c>
+      <c r="C559" s="48" t="s">
+        <v>597</v>
+      </c>
+      <c r="D559" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="E559" s="99" t="s">
+        <v>598</v>
+      </c>
+      <c r="F559" s="48" t="s">
+        <v>280</v>
+      </c>
+      <c r="G559" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J559" s="50">
+        <v>413</v>
+      </c>
+      <c r="L559" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="N559" s="51" t="s">
+        <v>600</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="D2:E3"/>

</xml_diff>

<commit_message>
- minor adjustment in `10.1016/j.jallcom.2021.159918`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A81D305-65F2-3049-9033-358C5783961B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342AED5F-2A90-CE4F-8CE3-D32A1C9BCE84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4831" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4836" uniqueCount="602">
   <si>
     <t>Metadata</t>
   </si>
@@ -1928,6 +1928,9 @@
   </si>
   <si>
     <t>10.1109/LMAG.2019.2955667</t>
+  </si>
+  <si>
+    <t>5T</t>
   </si>
 </sst>
 </file>
@@ -3149,8 +3152,8 @@
   </sheetPr>
   <dimension ref="A1:T559"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="I561" sqref="I561"/>
+    <sheetView tabSelected="1" topLeftCell="A516" zoomScale="89" workbookViewId="0">
+      <selection activeCell="I564" sqref="I564"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9562,7 +9565,9 @@
       <c r="G169" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H169" s="42"/>
+      <c r="H169" s="42" t="s">
+        <v>601</v>
+      </c>
       <c r="I169" s="3"/>
       <c r="J169" s="4">
         <v>8.64</v>
@@ -9595,7 +9600,9 @@
       <c r="G170" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H170" s="42"/>
+      <c r="H170" s="42" t="s">
+        <v>601</v>
+      </c>
       <c r="I170" s="3"/>
       <c r="J170" s="4">
         <v>5.92</v>
@@ -9629,7 +9636,9 @@
       <c r="G171" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H171" s="42"/>
+      <c r="H171" s="42" t="s">
+        <v>601</v>
+      </c>
       <c r="I171" s="3"/>
       <c r="J171" s="4">
         <v>5.85</v>
@@ -9663,7 +9672,9 @@
       <c r="G172" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H172" s="42"/>
+      <c r="H172" s="42" t="s">
+        <v>601</v>
+      </c>
       <c r="I172" s="3"/>
       <c r="J172" s="4">
         <v>6.92</v>
@@ -9819,7 +9830,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="18" customHeight="1">
+    <row r="177" spans="1:16" ht="18" customHeight="1">
       <c r="A177" s="24"/>
       <c r="B177" s="44" t="s">
         <v>287</v>
@@ -9857,7 +9868,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="18" customHeight="1">
+    <row r="178" spans="1:16" ht="18" customHeight="1">
       <c r="A178" s="24"/>
       <c r="B178" s="44" t="s">
         <v>288</v>
@@ -9895,7 +9906,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="18" customHeight="1">
+    <row r="179" spans="1:16" ht="18" customHeight="1">
       <c r="A179" s="24"/>
       <c r="B179" s="44" t="s">
         <v>289</v>
@@ -9933,7 +9944,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="18" customHeight="1">
+    <row r="180" spans="1:16" ht="18" customHeight="1">
       <c r="A180" s="24"/>
       <c r="B180" s="44" t="s">
         <v>287</v>
@@ -9971,7 +9982,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="181" spans="1:14" ht="18" customHeight="1">
+    <row r="181" spans="1:16" ht="18" customHeight="1">
       <c r="A181" s="24"/>
       <c r="B181" s="44" t="s">
         <v>288</v>
@@ -10009,7 +10020,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="182" spans="1:14" ht="18" customHeight="1">
+    <row r="182" spans="1:16" ht="18" customHeight="1">
       <c r="A182" s="24"/>
       <c r="B182" s="44" t="s">
         <v>289</v>
@@ -10046,8 +10057,11 @@
       <c r="N182" s="44" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="183" spans="1:14" ht="18" customHeight="1">
+      <c r="P182" s="6">
+        <v>2.3228176700000001</v>
+      </c>
+    </row>
+    <row r="183" spans="1:16" ht="18" customHeight="1">
       <c r="A183" s="24"/>
       <c r="B183" s="44" t="s">
         <v>287</v>
@@ -10085,7 +10099,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="184" spans="1:14" ht="18" customHeight="1">
+    <row r="184" spans="1:16" ht="18" customHeight="1">
       <c r="A184" s="24"/>
       <c r="B184" s="44" t="s">
         <v>288</v>
@@ -10123,7 +10137,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="185" spans="1:14" ht="18" customHeight="1">
+    <row r="185" spans="1:16" ht="18" customHeight="1">
       <c r="A185" s="24"/>
       <c r="B185" s="44" t="s">
         <v>289</v>
@@ -10161,7 +10175,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="186" spans="1:14" ht="18" customHeight="1">
+    <row r="186" spans="1:16" ht="18" customHeight="1">
       <c r="A186" s="24"/>
       <c r="B186" s="44" t="s">
         <v>293</v>
@@ -10199,7 +10213,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="18" customHeight="1">
+    <row r="187" spans="1:16" ht="18" customHeight="1">
       <c r="A187" s="24"/>
       <c r="B187" s="44" t="s">
         <v>293</v>
@@ -10239,7 +10253,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="188" spans="1:14" ht="18" customHeight="1">
+    <row r="188" spans="1:16" ht="18" customHeight="1">
       <c r="A188" s="24"/>
       <c r="B188" s="44" t="s">
         <v>293</v>
@@ -10279,7 +10293,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="189" spans="1:14" ht="18" customHeight="1">
+    <row r="189" spans="1:16" ht="18" customHeight="1">
       <c r="A189" s="24"/>
       <c r="B189" s="44" t="s">
         <v>297</v>
@@ -10315,7 +10329,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="190" spans="1:14" ht="18" customHeight="1">
+    <row r="190" spans="1:16" ht="18" customHeight="1">
       <c r="A190" s="24"/>
       <c r="B190" s="44" t="s">
         <v>297</v>
@@ -10353,7 +10367,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="191" spans="1:14" ht="18" customHeight="1">
+    <row r="191" spans="1:16" ht="18" customHeight="1">
       <c r="A191" s="24"/>
       <c r="B191" s="44" t="s">
         <v>297</v>
@@ -10391,7 +10405,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="192" spans="1:14" ht="18" customHeight="1">
+    <row r="192" spans="1:16" ht="18" customHeight="1">
       <c r="A192" s="24"/>
       <c r="B192" s="44" t="s">
         <v>297</v>
@@ -24033,6 +24047,9 @@
       </c>
       <c r="G559" s="48" t="s">
         <v>29</v>
+      </c>
+      <c r="H559" s="48" t="s">
+        <v>599</v>
       </c>
       <c r="J559" s="50">
         <v>413</v>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.cap.2019.09.019`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342AED5F-2A90-CE4F-8CE3-D32A1C9BCE84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F06EF88-D5BD-B647-A9C4-AF09C165388D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4836" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4869" uniqueCount="606">
   <si>
     <t>Metadata</t>
   </si>
@@ -1931,6 +1931,18 @@
   </si>
   <si>
     <t>5T</t>
+  </si>
+  <si>
+    <t>Fe26.7 Ni26.7 Ga15.6 Mn20 Si11</t>
+  </si>
+  <si>
+    <t>AAM+A</t>
+  </si>
+  <si>
+    <t>annealed at 973K for 1h in Ar and slowly cooled</t>
+  </si>
+  <si>
+    <t>10.1016/j.cap.2019.09.019</t>
   </si>
 </sst>
 </file>
@@ -3150,10 +3162,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T559"/>
+  <dimension ref="A1:T563"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A516" zoomScale="89" workbookViewId="0">
-      <selection activeCell="I564" sqref="I564"/>
+    <sheetView tabSelected="1" topLeftCell="A531" zoomScale="89" workbookViewId="0">
+      <selection activeCell="M576" sqref="M576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -24048,9 +24060,6 @@
       <c r="G559" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="H559" s="48" t="s">
-        <v>599</v>
-      </c>
       <c r="J559" s="50">
         <v>413</v>
       </c>
@@ -24059,6 +24068,128 @@
       </c>
       <c r="N559" s="51" t="s">
         <v>600</v>
+      </c>
+    </row>
+    <row r="560" spans="2:17">
+      <c r="B560" s="98" t="s">
+        <v>602</v>
+      </c>
+      <c r="C560" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D560" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="E560" s="99" t="s">
+        <v>604</v>
+      </c>
+      <c r="F560" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="G560" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H560" s="48" t="s">
+        <v>599</v>
+      </c>
+      <c r="J560" s="50">
+        <v>0.504</v>
+      </c>
+      <c r="L560" s="51" t="s">
+        <v>282</v>
+      </c>
+      <c r="N560" s="51" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="561" spans="2:14">
+      <c r="B561" s="98" t="s">
+        <v>602</v>
+      </c>
+      <c r="C561" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D561" s="48" t="s">
+        <v>603</v>
+      </c>
+      <c r="E561" s="99" t="s">
+        <v>604</v>
+      </c>
+      <c r="F561" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="G561" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H561" s="48" t="s">
+        <v>599</v>
+      </c>
+      <c r="J561" s="50">
+        <v>1.26</v>
+      </c>
+      <c r="L561" s="51" t="s">
+        <v>282</v>
+      </c>
+      <c r="N561" s="51" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="562" spans="2:14">
+      <c r="B562" s="98" t="s">
+        <v>602</v>
+      </c>
+      <c r="C562" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D562" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="E562" s="99" t="s">
+        <v>604</v>
+      </c>
+      <c r="F562" s="48" t="s">
+        <v>280</v>
+      </c>
+      <c r="G562" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J562" s="50">
+        <v>322</v>
+      </c>
+      <c r="L562" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="N562" s="51" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="563" spans="2:14">
+      <c r="B563" s="98" t="s">
+        <v>602</v>
+      </c>
+      <c r="C563" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D563" s="48" t="s">
+        <v>603</v>
+      </c>
+      <c r="E563" s="99" t="s">
+        <v>604</v>
+      </c>
+      <c r="F563" s="48" t="s">
+        <v>280</v>
+      </c>
+      <c r="G563" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J563" s="50">
+        <v>334</v>
+      </c>
+      <c r="L563" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="N563" s="51" t="s">
+        <v>605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- extracted data from `10.1002/adem.202201831`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F06EF88-D5BD-B647-A9C4-AF09C165388D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4E74F6-BE8F-4E45-81D6-5B4C77AAC27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4869" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4914" uniqueCount="623">
   <si>
     <t>Metadata</t>
   </si>
@@ -1943,6 +1943,57 @@
   </si>
   <si>
     <t>10.1016/j.cap.2019.09.019</t>
+  </si>
+  <si>
+    <t>10.1002/adem.202201831</t>
+  </si>
+  <si>
+    <t>GaInSnZn</t>
+  </si>
+  <si>
+    <t>GaInSnZn1.5</t>
+  </si>
+  <si>
+    <t>GaInSnZn2</t>
+  </si>
+  <si>
+    <t>GaInSnZn2.5</t>
+  </si>
+  <si>
+    <t>GaInSnZn3</t>
+  </si>
+  <si>
+    <t>Zn1</t>
+  </si>
+  <si>
+    <t>Zn1.5</t>
+  </si>
+  <si>
+    <t>Zn2</t>
+  </si>
+  <si>
+    <t>Zn2.5</t>
+  </si>
+  <si>
+    <t>Zn3</t>
+  </si>
+  <si>
+    <t>monoclinic+HCP+In3Sn</t>
+  </si>
+  <si>
+    <t>monoclinic+HCP+amorphous+InSn4+In3Sn</t>
+  </si>
+  <si>
+    <t>monoclinic+HCP+amorphous+InSn4+In`</t>
+  </si>
+  <si>
+    <t>monoclinic+HCP</t>
+  </si>
+  <si>
+    <t>monoclinic+HCP+InSn4</t>
+  </si>
+  <si>
+    <t>induction metling in Ar in quartz tube; Ga-based monoclinic SS (C2/c), Zn-based HCP, γ phase InSn4 (P6/mmm), and β phase In3Sn (P4/mmm)</t>
   </si>
 </sst>
 </file>
@@ -3162,10 +3213,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T563"/>
+  <dimension ref="A1:T568"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A531" zoomScale="89" workbookViewId="0">
-      <selection activeCell="M576" sqref="M576"/>
+    <sheetView tabSelected="1" topLeftCell="A530" zoomScale="89" workbookViewId="0">
+      <selection activeCell="J583" sqref="J583"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -24102,7 +24153,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="561" spans="2:14">
+    <row r="561" spans="1:16">
       <c r="B561" s="98" t="s">
         <v>602</v>
       </c>
@@ -24134,7 +24185,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="562" spans="2:14">
+    <row r="562" spans="1:16">
       <c r="B562" s="98" t="s">
         <v>602</v>
       </c>
@@ -24163,7 +24214,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="563" spans="2:14">
+    <row r="563" spans="1:16">
       <c r="B563" s="98" t="s">
         <v>602</v>
       </c>
@@ -24190,6 +24241,201 @@
       </c>
       <c r="N563" s="51" t="s">
         <v>605</v>
+      </c>
+    </row>
+    <row r="564" spans="1:16">
+      <c r="A564" s="47" t="s">
+        <v>612</v>
+      </c>
+      <c r="B564" s="98" t="s">
+        <v>607</v>
+      </c>
+      <c r="C564" s="48" t="s">
+        <v>617</v>
+      </c>
+      <c r="D564" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E564" s="99" t="s">
+        <v>622</v>
+      </c>
+      <c r="F564" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="G564" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I564" s="49">
+        <v>298</v>
+      </c>
+      <c r="J564" s="50">
+        <f>(1/P564)*0.000001</f>
+        <v>2.1383928571428609E-7</v>
+      </c>
+      <c r="L564" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N564" s="51" t="s">
+        <v>606</v>
+      </c>
+      <c r="P564" s="6">
+        <v>4.6764091858037498</v>
+      </c>
+    </row>
+    <row r="565" spans="1:16">
+      <c r="A565" s="47" t="s">
+        <v>613</v>
+      </c>
+      <c r="B565" s="98" t="s">
+        <v>608</v>
+      </c>
+      <c r="C565" s="48" t="s">
+        <v>618</v>
+      </c>
+      <c r="D565" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E565" s="99" t="s">
+        <v>622</v>
+      </c>
+      <c r="F565" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="G565" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I565" s="49">
+        <v>298</v>
+      </c>
+      <c r="J565" s="50">
+        <f t="shared" ref="J565:J568" si="24">(1/P565)*0.000001</f>
+        <v>2.0789930555555562E-7</v>
+      </c>
+      <c r="L565" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N565" s="51" t="s">
+        <v>606</v>
+      </c>
+      <c r="P565" s="6">
+        <v>4.8100208768267203</v>
+      </c>
+    </row>
+    <row r="566" spans="1:16">
+      <c r="A566" s="47" t="s">
+        <v>614</v>
+      </c>
+      <c r="B566" s="98" t="s">
+        <v>609</v>
+      </c>
+      <c r="C566" s="48" t="s">
+        <v>620</v>
+      </c>
+      <c r="D566" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E566" s="99" t="s">
+        <v>622</v>
+      </c>
+      <c r="F566" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="G566" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I566" s="49">
+        <v>298</v>
+      </c>
+      <c r="J566" s="50">
+        <f t="shared" si="24"/>
+        <v>1.7819940476190474E-7</v>
+      </c>
+      <c r="L566" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N566" s="51" t="s">
+        <v>606</v>
+      </c>
+      <c r="P566" s="6">
+        <v>5.6116910229645098</v>
+      </c>
+    </row>
+    <row r="567" spans="1:16">
+      <c r="A567" s="47" t="s">
+        <v>615</v>
+      </c>
+      <c r="B567" s="96" t="s">
+        <v>610</v>
+      </c>
+      <c r="C567" s="48" t="s">
+        <v>621</v>
+      </c>
+      <c r="D567" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E567" s="99" t="s">
+        <v>622</v>
+      </c>
+      <c r="F567" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="G567" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I567" s="49">
+        <v>298</v>
+      </c>
+      <c r="J567" s="50">
+        <f t="shared" si="24"/>
+        <v>1.7009943181818207E-7</v>
+      </c>
+      <c r="L567" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N567" s="51" t="s">
+        <v>606</v>
+      </c>
+      <c r="P567" s="6">
+        <v>5.8789144050104296</v>
+      </c>
+    </row>
+    <row r="568" spans="1:16">
+      <c r="A568" s="47" t="s">
+        <v>616</v>
+      </c>
+      <c r="B568" s="96" t="s">
+        <v>611</v>
+      </c>
+      <c r="C568" s="48" t="s">
+        <v>619</v>
+      </c>
+      <c r="D568" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E568" s="99" t="s">
+        <v>622</v>
+      </c>
+      <c r="F568" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="G568" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I568" s="49">
+        <v>298</v>
+      </c>
+      <c r="J568" s="50">
+        <f t="shared" si="24"/>
+        <v>1.5839947089947098E-7</v>
+      </c>
+      <c r="L568" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N568" s="51" t="s">
+        <v>606</v>
+      </c>
+      <c r="P568" s="6">
+        <v>6.3131524008350697</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- extracted data from `10.1109/ICEPT63120.2024.10668666`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4E74F6-BE8F-4E45-81D6-5B4C77AAC27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16032BA-6752-5143-9490-16545E59F46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4914" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4949" uniqueCount="626">
   <si>
     <t>Metadata</t>
   </si>
@@ -1994,6 +1994,15 @@
   </si>
   <si>
     <t>induction metling in Ar in quartz tube; Ga-based monoclinic SS (C2/c), Zn-based HCP, γ phase InSn4 (P6/mmm), and β phase In3Sn (P4/mmm)</t>
+  </si>
+  <si>
+    <t>Sn37 In22 Bi36 Zn5</t>
+  </si>
+  <si>
+    <t>smolten in Ar at 680*C for 120min and stirred</t>
+  </si>
+  <si>
+    <t>BCT+BiIn</t>
   </si>
 </sst>
 </file>
@@ -3213,10 +3222,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T568"/>
+  <dimension ref="A1:T572"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A530" zoomScale="89" workbookViewId="0">
-      <selection activeCell="J583" sqref="J583"/>
+    <sheetView tabSelected="1" topLeftCell="A528" zoomScale="89" workbookViewId="0">
+      <selection activeCell="N576" sqref="N576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -24438,6 +24447,147 @@
         <v>6.3131524008350697</v>
       </c>
     </row>
+    <row r="569" spans="1:16">
+      <c r="B569" s="98" t="s">
+        <v>623</v>
+      </c>
+      <c r="C569" s="48" t="s">
+        <v>625</v>
+      </c>
+      <c r="D569" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E569" s="99" t="s">
+        <v>624</v>
+      </c>
+      <c r="F569" s="48" t="s">
+        <v>586</v>
+      </c>
+      <c r="G569" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J569" s="50">
+        <f>81.5+273.15</f>
+        <v>354.65</v>
+      </c>
+      <c r="L569" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M569" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="N569" s="51" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="570" spans="1:16">
+      <c r="B570" s="98" t="s">
+        <v>623</v>
+      </c>
+      <c r="C570" s="48" t="s">
+        <v>625</v>
+      </c>
+      <c r="D570" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E570" s="99" t="s">
+        <v>624</v>
+      </c>
+      <c r="F570" s="48" t="s">
+        <v>229</v>
+      </c>
+      <c r="G570" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I570" s="49">
+        <v>298</v>
+      </c>
+      <c r="J570" s="50">
+        <v>38400000</v>
+      </c>
+      <c r="L570" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M570" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="N570" s="51" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="571" spans="1:16">
+      <c r="B571" s="98" t="s">
+        <v>623</v>
+      </c>
+      <c r="C571" s="48" t="s">
+        <v>625</v>
+      </c>
+      <c r="D571" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E571" s="99" t="s">
+        <v>624</v>
+      </c>
+      <c r="F571" s="48" t="s">
+        <v>230</v>
+      </c>
+      <c r="G571" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I571" s="49">
+        <v>298</v>
+      </c>
+      <c r="J571" s="50">
+        <v>65</v>
+      </c>
+      <c r="K571" s="50">
+        <v>5</v>
+      </c>
+      <c r="L571" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M571" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="N571" s="51" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="572" spans="1:16">
+      <c r="B572" s="98" t="s">
+        <v>623</v>
+      </c>
+      <c r="C572" s="48" t="s">
+        <v>625</v>
+      </c>
+      <c r="D572" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E572" s="99" t="s">
+        <v>624</v>
+      </c>
+      <c r="F572" s="48" t="s">
+        <v>593</v>
+      </c>
+      <c r="G572" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I572" s="49">
+        <v>298</v>
+      </c>
+      <c r="J572" s="50">
+        <v>40</v>
+      </c>
+      <c r="K572" s="50">
+        <v>1</v>
+      </c>
+      <c r="L572" s="51" t="s">
+        <v>594</v>
+      </c>
+      <c r="N572" s="51" t="s">
+        <v>233</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="D2:E3"/>

</xml_diff>

<commit_message>
- noticed earlier partial data extraction  from `10.1109/ICEPT63120.2024.10668666` and adjusted the upload to merge smoothly
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16032BA-6752-5143-9490-16545E59F46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FED86DE-7B8E-7146-8FF9-262DAD03FB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4949" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4949" uniqueCount="625">
   <si>
     <t>Metadata</t>
   </si>
@@ -2000,9 +2000,6 @@
   </si>
   <si>
     <t>smolten in Ar at 680*C for 120min and stirred</t>
-  </si>
-  <si>
-    <t>BCT+BiIn</t>
   </si>
 </sst>
 </file>
@@ -3224,8 +3221,8 @@
   </sheetPr>
   <dimension ref="A1:T572"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A528" zoomScale="89" workbookViewId="0">
-      <selection activeCell="N576" sqref="N576"/>
+    <sheetView tabSelected="1" topLeftCell="A534" zoomScale="89" workbookViewId="0">
+      <selection activeCell="J580" sqref="J580"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -24452,7 +24449,7 @@
         <v>623</v>
       </c>
       <c r="C569" s="48" t="s">
-        <v>625</v>
+        <v>231</v>
       </c>
       <c r="D569" s="48" t="s">
         <v>64</v>
@@ -24485,7 +24482,7 @@
         <v>623</v>
       </c>
       <c r="C570" s="48" t="s">
-        <v>625</v>
+        <v>231</v>
       </c>
       <c r="D570" s="48" t="s">
         <v>64</v>
@@ -24520,7 +24517,7 @@
         <v>623</v>
       </c>
       <c r="C571" s="48" t="s">
-        <v>625</v>
+        <v>231</v>
       </c>
       <c r="D571" s="48" t="s">
         <v>64</v>
@@ -24558,7 +24555,7 @@
         <v>623</v>
       </c>
       <c r="C572" s="48" t="s">
-        <v>625</v>
+        <v>231</v>
       </c>
       <c r="D572" s="48" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.surfcoat.2024.130707`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FED86DE-7B8E-7146-8FF9-262DAD03FB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B83E469-D0CD-124D-BE35-0FDDB9074A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4949" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5069" uniqueCount="640">
   <si>
     <t>Metadata</t>
   </si>
@@ -2000,6 +2000,51 @@
   </si>
   <si>
     <t>smolten in Ar at 680*C for 120min and stirred</t>
+  </si>
+  <si>
+    <t>MEAF</t>
+  </si>
+  <si>
+    <t>Nd0</t>
+  </si>
+  <si>
+    <t>Nd25</t>
+  </si>
+  <si>
+    <t>Nd50</t>
+  </si>
+  <si>
+    <t>Nd75</t>
+  </si>
+  <si>
+    <t>Nd100</t>
+  </si>
+  <si>
+    <t>FCC+amorphous</t>
+  </si>
+  <si>
+    <t>RF sputtering deposition from B, Nd, and equiatomic CoCrNi targets</t>
+  </si>
+  <si>
+    <t>Co0.96 Cr0.97 Ni1.07</t>
+  </si>
+  <si>
+    <t>(Co0.96 Cr0.97 Ni1.07)33.02 B0.94</t>
+  </si>
+  <si>
+    <t>(Co0.96 Cr0.97 Ni1.07)32.38 B1.5 Nd1.37</t>
+  </si>
+  <si>
+    <t>(Co0.96 Cr0.97 Ni1.07)31.39 B1.59 Nd4.25</t>
+  </si>
+  <si>
+    <t>(Co0.96 Cr0.97 Ni1.07)30.6 B1.05 Nd7.15</t>
+  </si>
+  <si>
+    <t>(Co0.96 Cr0.97 Ni1.07)29.84 B0.77 Nd9.7</t>
+  </si>
+  <si>
+    <t>10.1016/j.surfcoat.2024.130707</t>
   </si>
 </sst>
 </file>
@@ -3219,10 +3264,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T572"/>
+  <dimension ref="A1:T584"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A534" zoomScale="89" workbookViewId="0">
-      <selection activeCell="J580" sqref="J580"/>
+    <sheetView tabSelected="1" topLeftCell="A538" zoomScale="89" workbookViewId="0">
+      <selection activeCell="N588" sqref="N588"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -24585,6 +24630,498 @@
         <v>233</v>
       </c>
     </row>
+    <row r="573" spans="1:16">
+      <c r="A573" s="47" t="s">
+        <v>625</v>
+      </c>
+      <c r="B573" s="98" t="s">
+        <v>633</v>
+      </c>
+      <c r="C573" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D573" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="E573" s="99" t="s">
+        <v>632</v>
+      </c>
+      <c r="F573" s="48" t="s">
+        <v>245</v>
+      </c>
+      <c r="G573" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I573" s="49">
+        <v>298</v>
+      </c>
+      <c r="J573" s="50">
+        <v>9110000000</v>
+      </c>
+      <c r="K573" s="50">
+        <v>400000000</v>
+      </c>
+      <c r="L573" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M573" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N573" s="51" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="574" spans="1:16">
+      <c r="A574" s="47" t="s">
+        <v>626</v>
+      </c>
+      <c r="B574" s="98" t="s">
+        <v>634</v>
+      </c>
+      <c r="C574" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D574" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="E574" s="99" t="s">
+        <v>632</v>
+      </c>
+      <c r="F574" s="48" t="s">
+        <v>245</v>
+      </c>
+      <c r="G574" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I574" s="49">
+        <v>298</v>
+      </c>
+      <c r="J574" s="50">
+        <v>13280000000</v>
+      </c>
+      <c r="K574" s="50">
+        <v>230000000</v>
+      </c>
+      <c r="L574" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M574" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N574" s="51" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="575" spans="1:16">
+      <c r="A575" s="47" t="s">
+        <v>627</v>
+      </c>
+      <c r="B575" s="98" t="s">
+        <v>635</v>
+      </c>
+      <c r="C575" s="48" t="s">
+        <v>631</v>
+      </c>
+      <c r="D575" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="E575" s="99" t="s">
+        <v>632</v>
+      </c>
+      <c r="F575" s="48" t="s">
+        <v>245</v>
+      </c>
+      <c r="G575" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I575" s="49">
+        <v>298</v>
+      </c>
+      <c r="J575" s="50">
+        <v>9810000000</v>
+      </c>
+      <c r="K575" s="50">
+        <v>30000000</v>
+      </c>
+      <c r="L575" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M575" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N575" s="51" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="576" spans="1:16">
+      <c r="A576" s="47" t="s">
+        <v>628</v>
+      </c>
+      <c r="B576" s="98" t="s">
+        <v>636</v>
+      </c>
+      <c r="C576" s="48" t="s">
+        <v>244</v>
+      </c>
+      <c r="D576" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="E576" s="99" t="s">
+        <v>632</v>
+      </c>
+      <c r="F576" s="48" t="s">
+        <v>245</v>
+      </c>
+      <c r="G576" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I576" s="49">
+        <v>298</v>
+      </c>
+      <c r="J576" s="50">
+        <v>9660000000</v>
+      </c>
+      <c r="K576" s="50">
+        <v>170000000</v>
+      </c>
+      <c r="L576" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M576" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N576" s="51" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="577" spans="1:14">
+      <c r="A577" s="47" t="s">
+        <v>629</v>
+      </c>
+      <c r="B577" s="98" t="s">
+        <v>637</v>
+      </c>
+      <c r="C577" s="48" t="s">
+        <v>244</v>
+      </c>
+      <c r="D577" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="E577" s="99" t="s">
+        <v>632</v>
+      </c>
+      <c r="F577" s="48" t="s">
+        <v>245</v>
+      </c>
+      <c r="G577" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I577" s="49">
+        <v>298</v>
+      </c>
+      <c r="J577" s="50">
+        <v>9600000000</v>
+      </c>
+      <c r="K577" s="50">
+        <v>60000000</v>
+      </c>
+      <c r="L577" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M577" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N577" s="51" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="578" spans="1:14">
+      <c r="A578" s="47" t="s">
+        <v>630</v>
+      </c>
+      <c r="B578" s="98" t="s">
+        <v>638</v>
+      </c>
+      <c r="C578" s="48" t="s">
+        <v>244</v>
+      </c>
+      <c r="D578" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="E578" s="99" t="s">
+        <v>632</v>
+      </c>
+      <c r="F578" s="48" t="s">
+        <v>245</v>
+      </c>
+      <c r="G578" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I578" s="49">
+        <v>298</v>
+      </c>
+      <c r="J578" s="50">
+        <v>9630000000</v>
+      </c>
+      <c r="K578" s="50">
+        <v>160000000</v>
+      </c>
+      <c r="L578" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M578" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N578" s="51" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="579" spans="1:14">
+      <c r="A579" s="47" t="s">
+        <v>625</v>
+      </c>
+      <c r="B579" s="98" t="s">
+        <v>633</v>
+      </c>
+      <c r="C579" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D579" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="E579" s="99" t="s">
+        <v>632</v>
+      </c>
+      <c r="F579" s="48" t="s">
+        <v>246</v>
+      </c>
+      <c r="G579" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I579" s="49">
+        <v>298</v>
+      </c>
+      <c r="J579" s="50">
+        <v>199300000000</v>
+      </c>
+      <c r="K579" s="50">
+        <v>3400000000</v>
+      </c>
+      <c r="L579" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M579" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N579" s="51" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="580" spans="1:14">
+      <c r="A580" s="47" t="s">
+        <v>626</v>
+      </c>
+      <c r="B580" s="98" t="s">
+        <v>634</v>
+      </c>
+      <c r="C580" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D580" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="E580" s="99" t="s">
+        <v>632</v>
+      </c>
+      <c r="F580" s="48" t="s">
+        <v>246</v>
+      </c>
+      <c r="G580" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I580" s="49">
+        <v>298</v>
+      </c>
+      <c r="J580" s="50">
+        <v>212300000000</v>
+      </c>
+      <c r="K580" s="50">
+        <v>900000000</v>
+      </c>
+      <c r="L580" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M580" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N580" s="51" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="581" spans="1:14">
+      <c r="A581" s="47" t="s">
+        <v>627</v>
+      </c>
+      <c r="B581" s="98" t="s">
+        <v>635</v>
+      </c>
+      <c r="C581" s="48" t="s">
+        <v>631</v>
+      </c>
+      <c r="D581" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="E581" s="99" t="s">
+        <v>632</v>
+      </c>
+      <c r="F581" s="48" t="s">
+        <v>246</v>
+      </c>
+      <c r="G581" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I581" s="49">
+        <v>298</v>
+      </c>
+      <c r="J581" s="50">
+        <v>173700000000</v>
+      </c>
+      <c r="K581" s="50">
+        <v>3000000000</v>
+      </c>
+      <c r="L581" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M581" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N581" s="51" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="582" spans="1:14">
+      <c r="A582" s="47" t="s">
+        <v>628</v>
+      </c>
+      <c r="B582" s="98" t="s">
+        <v>636</v>
+      </c>
+      <c r="C582" s="48" t="s">
+        <v>244</v>
+      </c>
+      <c r="D582" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="E582" s="99" t="s">
+        <v>632</v>
+      </c>
+      <c r="F582" s="48" t="s">
+        <v>246</v>
+      </c>
+      <c r="G582" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I582" s="49">
+        <v>298</v>
+      </c>
+      <c r="J582" s="50">
+        <v>166400000000</v>
+      </c>
+      <c r="K582" s="50">
+        <v>2500000000</v>
+      </c>
+      <c r="L582" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M582" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N582" s="51" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="583" spans="1:14">
+      <c r="A583" s="47" t="s">
+        <v>629</v>
+      </c>
+      <c r="B583" s="98" t="s">
+        <v>637</v>
+      </c>
+      <c r="C583" s="48" t="s">
+        <v>244</v>
+      </c>
+      <c r="D583" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="E583" s="99" t="s">
+        <v>632</v>
+      </c>
+      <c r="F583" s="48" t="s">
+        <v>246</v>
+      </c>
+      <c r="G583" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I583" s="49">
+        <v>298</v>
+      </c>
+      <c r="J583" s="50">
+        <v>158900000000</v>
+      </c>
+      <c r="K583" s="50">
+        <v>1300000000</v>
+      </c>
+      <c r="L583" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M583" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N583" s="51" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="584" spans="1:14">
+      <c r="A584" s="47" t="s">
+        <v>630</v>
+      </c>
+      <c r="B584" s="98" t="s">
+        <v>638</v>
+      </c>
+      <c r="C584" s="48" t="s">
+        <v>244</v>
+      </c>
+      <c r="D584" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="E584" s="99" t="s">
+        <v>632</v>
+      </c>
+      <c r="F584" s="48" t="s">
+        <v>246</v>
+      </c>
+      <c r="G584" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I584" s="49">
+        <v>298</v>
+      </c>
+      <c r="J584" s="50">
+        <v>152100000000</v>
+      </c>
+      <c r="K584" s="50">
+        <v>2200000000</v>
+      </c>
+      <c r="L584" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M584" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N584" s="51" t="s">
+        <v>639</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="D2:E3"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jssc.2023.123881`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B83E469-D0CD-124D-BE35-0FDDB9074A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253AFE08-677A-054A-95A5-16FCED41516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5069" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5156" uniqueCount="660">
   <si>
     <t>Metadata</t>
   </si>
@@ -2045,6 +2045,66 @@
   </si>
   <si>
     <t>10.1016/j.surfcoat.2024.130707</t>
+  </si>
+  <si>
+    <t>arc melted in Ar from powders with small excesses compensating for mass loss</t>
+  </si>
+  <si>
+    <t>MoReRuRhPt</t>
+  </si>
+  <si>
+    <t>MoReRuIrPt</t>
+  </si>
+  <si>
+    <t>MoReRuRhPd</t>
+  </si>
+  <si>
+    <t>MoReRuIrPd</t>
+  </si>
+  <si>
+    <t>NbMoRuPtAu</t>
+  </si>
+  <si>
+    <t>NbMoReRuRhPt</t>
+  </si>
+  <si>
+    <t>NbMoReRuIrPt</t>
+  </si>
+  <si>
+    <t>NbMoReRuRh</t>
+  </si>
+  <si>
+    <t>NbMoReRuIr</t>
+  </si>
+  <si>
+    <t>ZrNbMoReRu</t>
+  </si>
+  <si>
+    <t>YZrNbMoRe</t>
+  </si>
+  <si>
+    <t>arc melted in Ar from powders with small excesses compensating for mass loss; Pd-rich FCC</t>
+  </si>
+  <si>
+    <t>C11b+sigma+FCC</t>
+  </si>
+  <si>
+    <t>arc melted in Ar from powders with small excesses compensating for mass loss; C11b is MoPt2-type and FCC is Au-rich</t>
+  </si>
+  <si>
+    <t>HCP+sigma</t>
+  </si>
+  <si>
+    <t>BCC+B2+C14</t>
+  </si>
+  <si>
+    <t>BCC+BCC+C15+HCP+sigma</t>
+  </si>
+  <si>
+    <t>arc melted in Ar from powders with small excesses compensating for mass loss; BCC2 is Mo-rich and HCP is Y-rich</t>
+  </si>
+  <si>
+    <t>10.1016/j.jssc.2023.123881</t>
   </si>
 </sst>
 </file>
@@ -3264,10 +3324,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T584"/>
+  <dimension ref="A1:T595"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A538" zoomScale="89" workbookViewId="0">
-      <selection activeCell="N588" sqref="N588"/>
+    <sheetView tabSelected="1" topLeftCell="A553" zoomScale="89" workbookViewId="0">
+      <selection activeCell="J606" sqref="J606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -25122,6 +25182,313 @@
         <v>639</v>
       </c>
     </row>
+    <row r="585" spans="1:14">
+      <c r="B585" s="98" t="s">
+        <v>641</v>
+      </c>
+      <c r="C585" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D585" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E585" s="99" t="s">
+        <v>640</v>
+      </c>
+      <c r="F585" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="G585" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J585" s="50">
+        <v>0.82</v>
+      </c>
+      <c r="L585" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M585" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="N585" s="51" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="586" spans="1:14">
+      <c r="B586" s="98" t="s">
+        <v>642</v>
+      </c>
+      <c r="C586" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D586" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E586" s="99" t="s">
+        <v>640</v>
+      </c>
+      <c r="F586" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="G586" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J586" s="50">
+        <v>1.06</v>
+      </c>
+      <c r="L586" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M586" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="N586" s="51" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="587" spans="1:14">
+      <c r="B587" s="98" t="s">
+        <v>643</v>
+      </c>
+      <c r="C587" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="D587" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E587" s="99" t="s">
+        <v>652</v>
+      </c>
+      <c r="F587" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="G587" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J587" s="50">
+        <v>1.38</v>
+      </c>
+      <c r="L587" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M587" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="N587" s="51" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="588" spans="1:14">
+      <c r="B588" s="98" t="s">
+        <v>644</v>
+      </c>
+      <c r="C588" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="D588" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E588" s="99" t="s">
+        <v>640</v>
+      </c>
+      <c r="F588" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="G588" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J588" s="50">
+        <v>1.61</v>
+      </c>
+      <c r="L588" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M588" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="N588" s="51" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="589" spans="1:14">
+      <c r="B589" s="98" t="s">
+        <v>645</v>
+      </c>
+      <c r="C589" s="48" t="s">
+        <v>653</v>
+      </c>
+      <c r="D589" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E589" s="99" t="s">
+        <v>654</v>
+      </c>
+      <c r="N589" s="51" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="590" spans="1:14">
+      <c r="B590" s="98" t="s">
+        <v>646</v>
+      </c>
+      <c r="C590" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="D590" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E590" s="99" t="s">
+        <v>640</v>
+      </c>
+      <c r="F590" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="G590" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J590" s="50">
+        <v>2.96</v>
+      </c>
+      <c r="L590" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M590" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="N590" s="51" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="591" spans="1:14">
+      <c r="B591" s="98" t="s">
+        <v>647</v>
+      </c>
+      <c r="C591" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="D591" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E591" s="99" t="s">
+        <v>640</v>
+      </c>
+      <c r="F591" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="G591" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J591" s="50">
+        <v>2.84</v>
+      </c>
+      <c r="L591" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M591" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="N591" s="51" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="592" spans="1:14">
+      <c r="B592" s="98" t="s">
+        <v>648</v>
+      </c>
+      <c r="C592" s="48" t="s">
+        <v>655</v>
+      </c>
+      <c r="D592" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E592" s="99" t="s">
+        <v>640</v>
+      </c>
+      <c r="F592" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="G592" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J592" s="50">
+        <v>6.13</v>
+      </c>
+      <c r="L592" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M592" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="N592" s="51" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="593" spans="2:14">
+      <c r="B593" s="98" t="s">
+        <v>649</v>
+      </c>
+      <c r="C593" s="48" t="s">
+        <v>655</v>
+      </c>
+      <c r="D593" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E593" s="99" t="s">
+        <v>640</v>
+      </c>
+      <c r="F593" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="G593" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J593" s="50">
+        <v>5.51</v>
+      </c>
+      <c r="L593" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M593" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="N593" s="51" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="594" spans="2:14">
+      <c r="B594" s="98" t="s">
+        <v>650</v>
+      </c>
+      <c r="C594" s="48" t="s">
+        <v>656</v>
+      </c>
+      <c r="D594" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E594" s="99" t="s">
+        <v>640</v>
+      </c>
+      <c r="N594" s="51" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="595" spans="2:14">
+      <c r="B595" s="98" t="s">
+        <v>651</v>
+      </c>
+      <c r="C595" s="48" t="s">
+        <v>657</v>
+      </c>
+      <c r="D595" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E595" s="99" t="s">
+        <v>658</v>
+      </c>
+      <c r="N595" s="51" t="s">
+        <v>659</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="D2:E3"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.mtcomm.2024.109690`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253AFE08-677A-054A-95A5-16FCED41516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9C6305-F8C1-B24C-B2BC-906F1565CB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5156" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5244" uniqueCount="666">
   <si>
     <t>Metadata</t>
   </si>
@@ -2105,6 +2105,24 @@
   </si>
   <si>
     <t>10.1016/j.jssc.2023.123881</t>
+  </si>
+  <si>
+    <t>10.1016/j.mtcomm.2024.109690</t>
+  </si>
+  <si>
+    <t>NbScTiZr</t>
+  </si>
+  <si>
+    <t>annealed at 673K for 4 days in Ar</t>
+  </si>
+  <si>
+    <t>annealed at 873K for 4 days in Ar</t>
+  </si>
+  <si>
+    <t>annealed at 1073K for 4 days in Ar</t>
+  </si>
+  <si>
+    <t>annealed at 1273K for 4 days in Ar</t>
   </si>
 </sst>
 </file>
@@ -3324,10 +3342,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T595"/>
+  <dimension ref="A1:T605"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A553" zoomScale="89" workbookViewId="0">
-      <selection activeCell="J606" sqref="J606"/>
+    <sheetView tabSelected="1" topLeftCell="A571" zoomScale="89" workbookViewId="0">
+      <selection activeCell="J615" sqref="J615"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -25423,7 +25441,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="593" spans="2:14">
+    <row r="593" spans="2:17">
       <c r="B593" s="98" t="s">
         <v>649</v>
       </c>
@@ -25455,7 +25473,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="594" spans="2:14">
+    <row r="594" spans="2:17">
       <c r="B594" s="98" t="s">
         <v>650</v>
       </c>
@@ -25472,7 +25490,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="595" spans="2:14">
+    <row r="595" spans="2:17">
       <c r="B595" s="98" t="s">
         <v>651</v>
       </c>
@@ -25487,6 +25505,390 @@
       </c>
       <c r="N595" s="51" t="s">
         <v>659</v>
+      </c>
+    </row>
+    <row r="596" spans="2:17">
+      <c r="B596" s="98" t="s">
+        <v>661</v>
+      </c>
+      <c r="C596" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D596" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F596" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="G596" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J596" s="50">
+        <v>8.11</v>
+      </c>
+      <c r="L596" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M596" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N596" s="51" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="597" spans="2:17">
+      <c r="B597" s="98" t="s">
+        <v>661</v>
+      </c>
+      <c r="C597" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D597" s="48" t="s">
+        <v>603</v>
+      </c>
+      <c r="E597" s="99" t="s">
+        <v>662</v>
+      </c>
+      <c r="F597" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="G597" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J597" s="50">
+        <v>8.7100000000000009</v>
+      </c>
+      <c r="L597" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M597" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N597" s="51" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="598" spans="2:17">
+      <c r="B598" s="98" t="s">
+        <v>661</v>
+      </c>
+      <c r="C598" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D598" s="48" t="s">
+        <v>603</v>
+      </c>
+      <c r="E598" s="99" t="s">
+        <v>663</v>
+      </c>
+      <c r="F598" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="G598" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J598" s="50">
+        <v>9.36</v>
+      </c>
+      <c r="L598" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M598" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N598" s="51" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="599" spans="2:17">
+      <c r="B599" s="98" t="s">
+        <v>661</v>
+      </c>
+      <c r="C599" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D599" s="48" t="s">
+        <v>603</v>
+      </c>
+      <c r="E599" s="99" t="s">
+        <v>664</v>
+      </c>
+      <c r="F599" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="G599" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J599" s="50">
+        <v>9.1300000000000008</v>
+      </c>
+      <c r="L599" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M599" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N599" s="51" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="600" spans="2:17">
+      <c r="B600" s="98" t="s">
+        <v>661</v>
+      </c>
+      <c r="C600" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D600" s="48" t="s">
+        <v>603</v>
+      </c>
+      <c r="E600" s="99" t="s">
+        <v>665</v>
+      </c>
+      <c r="F600" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="G600" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J600" s="50">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="L600" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="M600" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N600" s="51" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="601" spans="2:17">
+      <c r="B601" s="98" t="s">
+        <v>661</v>
+      </c>
+      <c r="C601" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D601" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F601" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G601" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I601" s="49">
+        <v>298</v>
+      </c>
+      <c r="J601" s="4">
+        <f t="shared" ref="J601:K605" si="25">P601*9807000</f>
+        <v>3295152000</v>
+      </c>
+      <c r="K601" s="4">
+        <f t="shared" si="25"/>
+        <v>9807000</v>
+      </c>
+      <c r="L601" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M601" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N601" s="51" t="s">
+        <v>660</v>
+      </c>
+      <c r="P601" s="6">
+        <v>336</v>
+      </c>
+      <c r="Q601" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="602" spans="2:17">
+      <c r="B602" s="98" t="s">
+        <v>661</v>
+      </c>
+      <c r="C602" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D602" s="48" t="s">
+        <v>603</v>
+      </c>
+      <c r="E602" s="99" t="s">
+        <v>662</v>
+      </c>
+      <c r="F602" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G602" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I602" s="49">
+        <v>298</v>
+      </c>
+      <c r="J602" s="4">
+        <f t="shared" si="25"/>
+        <v>3383415000</v>
+      </c>
+      <c r="K602" s="4">
+        <f t="shared" si="25"/>
+        <v>39228000</v>
+      </c>
+      <c r="L602" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M602" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N602" s="51" t="s">
+        <v>660</v>
+      </c>
+      <c r="P602" s="6">
+        <v>345</v>
+      </c>
+      <c r="Q602" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="603" spans="2:17">
+      <c r="B603" s="98" t="s">
+        <v>661</v>
+      </c>
+      <c r="C603" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D603" s="48" t="s">
+        <v>603</v>
+      </c>
+      <c r="E603" s="99" t="s">
+        <v>663</v>
+      </c>
+      <c r="F603" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G603" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I603" s="49">
+        <v>298</v>
+      </c>
+      <c r="J603" s="4">
+        <f t="shared" si="25"/>
+        <v>2589048000</v>
+      </c>
+      <c r="K603" s="4">
+        <f t="shared" si="25"/>
+        <v>58842000</v>
+      </c>
+      <c r="L603" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M603" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N603" s="51" t="s">
+        <v>660</v>
+      </c>
+      <c r="P603" s="6">
+        <v>264</v>
+      </c>
+      <c r="Q603" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="604" spans="2:17">
+      <c r="B604" s="98" t="s">
+        <v>661</v>
+      </c>
+      <c r="C604" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D604" s="48" t="s">
+        <v>603</v>
+      </c>
+      <c r="E604" s="99" t="s">
+        <v>664</v>
+      </c>
+      <c r="F604" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G604" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I604" s="49">
+        <v>298</v>
+      </c>
+      <c r="J604" s="4">
+        <f t="shared" si="25"/>
+        <v>2343873000</v>
+      </c>
+      <c r="K604" s="4">
+        <f t="shared" si="25"/>
+        <v>19614000</v>
+      </c>
+      <c r="L604" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M604" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N604" s="51" t="s">
+        <v>660</v>
+      </c>
+      <c r="P604" s="6">
+        <v>239</v>
+      </c>
+      <c r="Q604" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="605" spans="2:17">
+      <c r="B605" s="98" t="s">
+        <v>661</v>
+      </c>
+      <c r="C605" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D605" s="48" t="s">
+        <v>603</v>
+      </c>
+      <c r="E605" s="99" t="s">
+        <v>665</v>
+      </c>
+      <c r="F605" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G605" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I605" s="49">
+        <v>298</v>
+      </c>
+      <c r="J605" s="4">
+        <f t="shared" si="25"/>
+        <v>2255610000</v>
+      </c>
+      <c r="K605" s="4">
+        <f t="shared" si="25"/>
+        <v>19614000</v>
+      </c>
+      <c r="L605" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M605" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="N605" s="51" t="s">
+        <v>660</v>
+      </c>
+      <c r="P605" s="6">
+        <v>230</v>
+      </c>
+      <c r="Q605" s="6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- extracted structural data from `10.2320/matertrans.MT-M2022213`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9C6305-F8C1-B24C-B2BC-906F1565CB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20277D3-27A0-164D-8140-998693DF2880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5244" uniqueCount="666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5268" uniqueCount="674">
   <si>
     <t>Metadata</t>
   </si>
@@ -2123,6 +2123,30 @@
   </si>
   <si>
     <t>annealed at 1273K for 4 days in Ar</t>
+  </si>
+  <si>
+    <t>Mo35Ni15Rh15Ru35</t>
+  </si>
+  <si>
+    <t>Fe14Mo35Ni15Rh15Ru21</t>
+  </si>
+  <si>
+    <t>Mo25Ni25Rh25Ru25</t>
+  </si>
+  <si>
+    <t>Fe20Mo20Ni20Rh20Ru20</t>
+  </si>
+  <si>
+    <t>annealed at 1700K for 1h in Ar then water quenched</t>
+  </si>
+  <si>
+    <t>VAM+A+WQ</t>
+  </si>
+  <si>
+    <t>HCP+?</t>
+  </si>
+  <si>
+    <t>10.2320/matertrans.MT-M2022213</t>
   </si>
 </sst>
 </file>
@@ -3342,10 +3366,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T605"/>
+  <dimension ref="A1:T609"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A571" zoomScale="89" workbookViewId="0">
-      <selection activeCell="J615" sqref="J615"/>
+    <sheetView tabSelected="1" topLeftCell="A572" zoomScale="89" workbookViewId="0">
+      <selection activeCell="M613" sqref="M613"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -25891,6 +25915,86 @@
         <v>2</v>
       </c>
     </row>
+    <row r="606" spans="2:17">
+      <c r="B606" s="98" t="s">
+        <v>666</v>
+      </c>
+      <c r="C606" s="48" t="s">
+        <v>672</v>
+      </c>
+      <c r="D606" s="48" t="s">
+        <v>671</v>
+      </c>
+      <c r="E606" s="99" t="s">
+        <v>670</v>
+      </c>
+      <c r="M606" s="51" t="s">
+        <v>225</v>
+      </c>
+      <c r="N606" s="51" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="607" spans="2:17">
+      <c r="B607" s="98" t="s">
+        <v>667</v>
+      </c>
+      <c r="C607" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D607" s="48" t="s">
+        <v>671</v>
+      </c>
+      <c r="E607" s="99" t="s">
+        <v>670</v>
+      </c>
+      <c r="M607" s="51" t="s">
+        <v>225</v>
+      </c>
+      <c r="N607" s="51" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="608" spans="2:17">
+      <c r="B608" s="98" t="s">
+        <v>668</v>
+      </c>
+      <c r="C608" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D608" s="48" t="s">
+        <v>671</v>
+      </c>
+      <c r="E608" s="99" t="s">
+        <v>670</v>
+      </c>
+      <c r="M608" s="51" t="s">
+        <v>225</v>
+      </c>
+      <c r="N608" s="51" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="609" spans="2:14">
+      <c r="B609" s="98" t="s">
+        <v>669</v>
+      </c>
+      <c r="C609" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D609" s="48" t="s">
+        <v>671</v>
+      </c>
+      <c r="E609" s="99" t="s">
+        <v>670</v>
+      </c>
+      <c r="M609" s="51" t="s">
+        <v>225</v>
+      </c>
+      <c r="N609" s="51" t="s">
+        <v>673</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="D2:E3"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1557/adv.2019.114`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20277D3-27A0-164D-8140-998693DF2880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76701051-4D10-6340-9AC8-F7EEEBC8C78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5268" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5277" uniqueCount="678">
   <si>
     <t>Metadata</t>
   </si>
@@ -2147,6 +2147,18 @@
   </si>
   <si>
     <t>10.2320/matertrans.MT-M2022213</t>
+  </si>
+  <si>
+    <t>Os24Ru14W25Mo23Re14</t>
+  </si>
+  <si>
+    <t>HCP+orthorhombic</t>
+  </si>
+  <si>
+    <t>magnetron sputtering onto Si; 8 more datapoints available with XRD lacking interpretation</t>
+  </si>
+  <si>
+    <t>10.1557/adv.2019.114</t>
   </si>
 </sst>
 </file>
@@ -3366,10 +3378,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T609"/>
+  <dimension ref="A1:T611"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A572" zoomScale="89" workbookViewId="0">
-      <selection activeCell="M613" sqref="M613"/>
+      <selection activeCell="K612" sqref="K612"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -25995,6 +26007,37 @@
         <v>673</v>
       </c>
     </row>
+    <row r="610" spans="2:14">
+      <c r="B610" s="98" t="s">
+        <v>674</v>
+      </c>
+      <c r="C610" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D610" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="E610" s="99" t="s">
+        <v>676</v>
+      </c>
+      <c r="N610" s="51" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="611" spans="2:14">
+      <c r="B611" s="98" t="s">
+        <v>674</v>
+      </c>
+      <c r="C611" s="48" t="s">
+        <v>675</v>
+      </c>
+      <c r="D611" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="N611" s="51" t="s">
+        <v>677</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="D2:E3"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.15330/pcss.25.3.506-512`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76701051-4D10-6340-9AC8-F7EEEBC8C78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB68D532-9B9B-F144-8884-2C9417C5872B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5277" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5295" uniqueCount="684">
   <si>
     <t>Metadata</t>
   </si>
@@ -2160,6 +2160,24 @@
   <si>
     <t>10.1557/adv.2019.114</t>
   </si>
+  <si>
+    <t>CoCrFeMnNiBe</t>
+  </si>
+  <si>
+    <t>FCC+BCC+B2</t>
+  </si>
+  <si>
+    <t>B2 was BeNi(Co)</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>CoCrFeMnNi</t>
+  </si>
+  <si>
+    <t>10.15330/pcss.25.3.506-512</t>
+  </si>
 </sst>
 </file>
 
@@ -2169,7 +2187,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2271,6 +2289,12 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="-webkit-standard"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2782,7 +2806,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3073,6 +3097,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3378,10 +3403,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T611"/>
+  <dimension ref="A1:T615"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A572" zoomScale="89" workbookViewId="0">
-      <selection activeCell="K612" sqref="K612"/>
+      <selection activeCell="M619" sqref="M619"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -26038,6 +26063,68 @@
         <v>677</v>
       </c>
     </row>
+    <row r="612" spans="2:14">
+      <c r="B612" s="100" t="s">
+        <v>682</v>
+      </c>
+      <c r="C612" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D612" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="N612" s="51" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="613" spans="2:14">
+      <c r="B613" s="100" t="s">
+        <v>682</v>
+      </c>
+      <c r="C613" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D613" s="48" t="s">
+        <v>681</v>
+      </c>
+      <c r="N613" s="51" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="614" spans="2:14">
+      <c r="B614" s="98" t="s">
+        <v>678</v>
+      </c>
+      <c r="C614" s="48" t="s">
+        <v>679</v>
+      </c>
+      <c r="D614" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E614" s="99" t="s">
+        <v>680</v>
+      </c>
+      <c r="N614" s="51" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="615" spans="2:14">
+      <c r="B615" s="98" t="s">
+        <v>678</v>
+      </c>
+      <c r="C615" s="48" t="s">
+        <v>679</v>
+      </c>
+      <c r="D615" s="48" t="s">
+        <v>681</v>
+      </c>
+      <c r="E615" s="99" t="s">
+        <v>680</v>
+      </c>
+      <c r="N615" s="51" t="s">
+        <v>683</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="D2:E3"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.matdes.2024.113260`
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB68D532-9B9B-F144-8884-2C9417C5872B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EFE7F5-10F4-F04B-93C6-BCBDD5DC192F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5295" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5365" uniqueCount="693">
   <si>
     <t>Metadata</t>
   </si>
@@ -2177,6 +2177,33 @@
   </si>
   <si>
     <t>10.15330/pcss.25.3.506-512</t>
+  </si>
+  <si>
+    <t>Nb28Ti20V32Zr20</t>
+  </si>
+  <si>
+    <t>V32</t>
+  </si>
+  <si>
+    <t>Nb25Ti35V5Zr35</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>NbTiVZr</t>
+  </si>
+  <si>
+    <t>V25</t>
+  </si>
+  <si>
+    <t>BCC+C14+C15</t>
+  </si>
+  <si>
+    <t>F14a</t>
+  </si>
+  <si>
+    <t>10.1016/j.matdes.2024.113260</t>
   </si>
 </sst>
 </file>
@@ -3403,10 +3430,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T615"/>
+  <dimension ref="A1:T622"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A572" zoomScale="89" workbookViewId="0">
-      <selection activeCell="M619" sqref="M619"/>
+    <sheetView tabSelected="1" topLeftCell="A583" zoomScale="89" workbookViewId="0">
+      <selection activeCell="F639" sqref="F639"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -26012,7 +26039,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="609" spans="2:14">
+    <row r="609" spans="1:14">
       <c r="B609" s="98" t="s">
         <v>669</v>
       </c>
@@ -26032,7 +26059,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="610" spans="2:14">
+    <row r="610" spans="1:14">
       <c r="B610" s="98" t="s">
         <v>674</v>
       </c>
@@ -26049,7 +26076,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="611" spans="2:14">
+    <row r="611" spans="1:14">
       <c r="B611" s="98" t="s">
         <v>674</v>
       </c>
@@ -26063,7 +26090,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="612" spans="2:14">
+    <row r="612" spans="1:14">
       <c r="B612" s="100" t="s">
         <v>682</v>
       </c>
@@ -26077,7 +26104,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="613" spans="2:14">
+    <row r="613" spans="1:14">
       <c r="B613" s="100" t="s">
         <v>682</v>
       </c>
@@ -26091,7 +26118,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="614" spans="2:14">
+    <row r="614" spans="1:14">
       <c r="B614" s="98" t="s">
         <v>678</v>
       </c>
@@ -26108,7 +26135,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="615" spans="2:14">
+    <row r="615" spans="1:14">
       <c r="B615" s="98" t="s">
         <v>678</v>
       </c>
@@ -26123,6 +26150,272 @@
       </c>
       <c r="N615" s="51" t="s">
         <v>683</v>
+      </c>
+    </row>
+    <row r="616" spans="1:14">
+      <c r="A616" s="47" t="s">
+        <v>687</v>
+      </c>
+      <c r="B616" s="98" t="s">
+        <v>686</v>
+      </c>
+      <c r="C616" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D616" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F616" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G616" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H616" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I616" s="49">
+        <v>298</v>
+      </c>
+      <c r="J616" s="50">
+        <v>855000000</v>
+      </c>
+      <c r="L616" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M616" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N616" s="51" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="617" spans="1:14">
+      <c r="A617" s="47" t="s">
+        <v>689</v>
+      </c>
+      <c r="B617" s="98" t="s">
+        <v>688</v>
+      </c>
+      <c r="C617" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D617" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F617" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G617" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H617" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I617" s="49">
+        <v>298</v>
+      </c>
+      <c r="J617" s="50">
+        <v>944000000</v>
+      </c>
+      <c r="L617" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M617" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N617" s="51" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="618" spans="1:14">
+      <c r="A618" s="47" t="s">
+        <v>685</v>
+      </c>
+      <c r="B618" s="98" t="s">
+        <v>684</v>
+      </c>
+      <c r="C618" s="48" t="s">
+        <v>690</v>
+      </c>
+      <c r="D618" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F618" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G618" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H618" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I618" s="49">
+        <v>298</v>
+      </c>
+      <c r="J618" s="50">
+        <v>1402000000</v>
+      </c>
+      <c r="L618" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M618" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N618" s="51" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="619" spans="1:14">
+      <c r="A619" s="47" t="s">
+        <v>687</v>
+      </c>
+      <c r="B619" s="98" t="s">
+        <v>686</v>
+      </c>
+      <c r="C619" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D619" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F619" s="48" t="s">
+        <v>315</v>
+      </c>
+      <c r="G619" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H619" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I619" s="49">
+        <v>298</v>
+      </c>
+      <c r="J619" s="50">
+        <v>50</v>
+      </c>
+      <c r="L619" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M619" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N619" s="51" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="620" spans="1:14">
+      <c r="A620" s="47" t="s">
+        <v>689</v>
+      </c>
+      <c r="B620" s="98" t="s">
+        <v>688</v>
+      </c>
+      <c r="C620" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D620" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F620" s="48" t="s">
+        <v>315</v>
+      </c>
+      <c r="G620" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H620" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I620" s="49">
+        <v>298</v>
+      </c>
+      <c r="J620" s="50">
+        <v>50</v>
+      </c>
+      <c r="L620" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M620" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N620" s="51" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="621" spans="1:14">
+      <c r="A621" s="47" t="s">
+        <v>685</v>
+      </c>
+      <c r="B621" s="98" t="s">
+        <v>684</v>
+      </c>
+      <c r="C621" s="48" t="s">
+        <v>690</v>
+      </c>
+      <c r="D621" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F621" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="G621" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H621" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I621" s="49">
+        <v>298</v>
+      </c>
+      <c r="J621" s="50">
+        <v>29.3</v>
+      </c>
+      <c r="L621" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="M621" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="N621" s="51" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="622" spans="1:14">
+      <c r="A622" s="47" t="s">
+        <v>685</v>
+      </c>
+      <c r="B622" s="98" t="s">
+        <v>684</v>
+      </c>
+      <c r="C622" s="48" t="s">
+        <v>690</v>
+      </c>
+      <c r="D622" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F622" s="48" t="s">
+        <v>306</v>
+      </c>
+      <c r="G622" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H622" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="I622" s="49">
+        <v>298</v>
+      </c>
+      <c r="J622" s="50">
+        <v>2483000000</v>
+      </c>
+      <c r="L622" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M622" s="51" t="s">
+        <v>691</v>
+      </c>
+      <c r="N622" s="51" t="s">
+        <v>692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jallcom.2013.12.210` Marcia and MPEA missed
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAE6F62-DB17-BE43-A4EE-D7509963E1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298C3B46-9042-7047-9814-2A933376A5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="760" windowWidth="34240" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2998,6 +2998,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3063,57 +3114,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3422,8 +3422,8 @@
   </sheetPr>
   <dimension ref="A1:T622"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="89" workbookViewId="0">
-      <selection activeCell="F95" sqref="F95"/>
+    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="89" workbookViewId="0">
+      <selection activeCell="H252" sqref="H252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3472,19 +3472,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="61"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="68"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="85"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1">
@@ -3495,17 +3495,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="72"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="89"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1">
@@ -3534,43 +3534,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="75" t="s">
+      <c r="F5" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="75" t="s">
+      <c r="G5" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="76" t="s">
+      <c r="H5" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="78" t="s">
+      <c r="I5" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="80" t="s">
+      <c r="J5" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="80" t="s">
+      <c r="K5" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="75" t="s">
+      <c r="L5" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="75" t="s">
+      <c r="M5" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="75" t="s">
+      <c r="N5" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="82" t="s">
+      <c r="O5" s="60" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3581,19 +3581,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="79"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="81"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
-      <c r="O6" s="83"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+      <c r="O6" s="61"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1">
       <c r="A7" s="17" t="s">
@@ -3638,7 +3638,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="84"/>
+      <c r="O7" s="62"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -3651,35 +3651,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="88" t="s">
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="91"/>
-      <c r="K8" s="91"/>
-      <c r="L8" s="92"/>
-      <c r="M8" s="93" t="s">
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="70"/>
+      <c r="M8" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="94"/>
+      <c r="N8" s="72"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="95" t="s">
+      <c r="P8" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="96"/>
-      <c r="R8" s="97"/>
-      <c r="S8" s="97"/>
-      <c r="T8" s="98"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="75"/>
+      <c r="S8" s="75"/>
+      <c r="T8" s="76"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="26" t="s">
@@ -26410,11 +26410,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -26429,6 +26424,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- adjust 4 units (no data changes)
</commit_message>
<xml_diff>
--- a/LessCommonElements_Nov2024.xlsx
+++ b/LessCommonElements_Nov2024.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298C3B46-9042-7047-9814-2A933376A5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A417C0-0661-4643-9BF3-6E4703C657A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2998,57 +2998,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3114,6 +3063,57 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3422,8 +3422,8 @@
   </sheetPr>
   <dimension ref="A1:T622"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="89" workbookViewId="0">
-      <selection activeCell="H252" sqref="H252"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="89" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3472,19 +3472,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="85"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="68"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1">
@@ -3495,17 +3495,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="89"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="72"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1">
@@ -3534,43 +3534,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="90" t="s">
+      <c r="C5" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="92" t="s">
+      <c r="D5" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="92" t="s">
+      <c r="E5" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="92" t="s">
+      <c r="F5" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="92" t="s">
+      <c r="G5" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="93" t="s">
+      <c r="H5" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="95" t="s">
+      <c r="I5" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="97" t="s">
+      <c r="J5" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="97" t="s">
+      <c r="K5" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="92" t="s">
+      <c r="L5" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="92" t="s">
+      <c r="M5" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="92" t="s">
+      <c r="N5" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="60" t="s">
+      <c r="O5" s="82" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3581,19 +3581,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="94"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
-      <c r="O6" s="61"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="74"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="83"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1">
       <c r="A7" s="17" t="s">
@@ -3638,7 +3638,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="62"/>
+      <c r="O7" s="84"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -3651,35 +3651,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="66" t="s">
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="71" t="s">
+      <c r="G8" s="89"/>
+      <c r="H8" s="89"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="91"/>
+      <c r="L8" s="92"/>
+      <c r="M8" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="72"/>
+      <c r="N8" s="94"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="74"/>
-      <c r="R8" s="75"/>
-      <c r="S8" s="75"/>
-      <c r="T8" s="76"/>
+      <c r="Q8" s="96"/>
+      <c r="R8" s="97"/>
+      <c r="S8" s="97"/>
+      <c r="T8" s="98"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="26" t="s">
@@ -4696,7 +4696,7 @@
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="9" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="M34" s="9" t="s">
         <v>102</v>
@@ -4736,7 +4736,7 @@
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="9" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="M35" s="9" t="s">
         <v>102</v>
@@ -4776,7 +4776,7 @@
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="9" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="M36" s="9" t="s">
         <v>103</v>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="9" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="M37" s="9" t="s">
         <v>102</v>
@@ -26410,6 +26410,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -26424,11 +26429,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>